<commit_message>
ws: Recipe ws made with placeholders
</commit_message>
<xml_diff>
--- a/MealPrepTracker.xlsx
+++ b/MealPrepTracker.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/quinnreams/Documents/GitHub/Personal-Growth-Planner/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0386C48B-4FB5-6E4D-A290-0ECBFE7CD9CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F1DBEB7B-77CC-734C-A04E-5749D301E275}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="660" windowWidth="38080" windowHeight="19300" xr2:uid="{D3DA68F7-6D5A-0240-8F01-44B1910C5B1F}"/>
+    <workbookView xWindow="160" yWindow="660" windowWidth="38080" windowHeight="19260" activeTab="1" xr2:uid="{D3DA68F7-6D5A-0240-8F01-44B1910C5B1F}"/>
   </bookViews>
   <sheets>
-    <sheet name="Meal Calender" sheetId="1" r:id="rId1"/>
+    <sheet name="Meal Calendar" sheetId="1" r:id="rId1"/>
+    <sheet name="Recipes" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Monday</t>
   </si>
@@ -75,6 +76,27 @@
   </si>
   <si>
     <t>Week</t>
+  </si>
+  <si>
+    <t>Meal Name</t>
+  </si>
+  <si>
+    <t>Salad</t>
+  </si>
+  <si>
+    <t>Soup</t>
+  </si>
+  <si>
+    <t>Egg</t>
+  </si>
+  <si>
+    <t>Beef</t>
+  </si>
+  <si>
+    <t>Chicken</t>
+  </si>
+  <si>
+    <t>PlaceHolder</t>
   </si>
 </sst>
 </file>
@@ -516,7 +538,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16B2BAA0-4794-6143-A848-FEE0CEBAF496}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H16" sqref="H16"/>
     </sheetView>
@@ -588,4 +610,54 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFFEA0BD-4E22-FC49-A8B4-AF7211BE5BFB}">
+  <dimension ref="A1:A7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
wb: week 2 added
</commit_message>
<xml_diff>
--- a/MealPrepTracker.xlsx
+++ b/MealPrepTracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/quinnreams/Documents/GitHub/Personal-Growth-Planner/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F010AC1D-213F-764C-BCAB-B9991EA01C85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E3F073A-FF73-6948-9806-81883ADAB9B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="160" yWindow="660" windowWidth="38080" windowHeight="19260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="172">
   <si>
     <t>Week</t>
   </si>
@@ -48,6 +48,9 @@
   </si>
   <si>
     <t>Week 1</t>
+  </si>
+  <si>
+    <t>Week 2</t>
   </si>
   <si>
     <t>Recipe Name</t>
@@ -686,8 +689,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:F22" totalsRowShown="0" headerRowDxfId="3">
-  <autoFilter ref="A1:F22" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:F43" totalsRowShown="0" headerRowDxfId="3">
+  <autoFilter ref="A1:F43" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Week"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Day"/>
@@ -1017,11 +1020,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C22" sqref="C22"/>
+      <selection pane="bottomLeft" activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1038,19 +1041,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="30" customHeight="1">
@@ -1061,17 +1064,17 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="30" customHeight="1">
       <c r="C3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="30" customHeight="1">
       <c r="C4" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="30" customHeight="1">
@@ -1079,17 +1082,17 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="30" customHeight="1">
       <c r="C6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="30" customHeight="1">
       <c r="C7" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="30" customHeight="1">
@@ -1097,17 +1100,17 @@
         <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="30" customHeight="1">
       <c r="C9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="30" customHeight="1">
       <c r="C10" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="30" customHeight="1">
@@ -1115,17 +1118,17 @@
         <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="30" customHeight="1">
       <c r="C12" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="30" customHeight="1">
       <c r="C13" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="30" customHeight="1">
@@ -1133,53 +1136,182 @@
         <v>5</v>
       </c>
       <c r="C14" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="30" customHeight="1">
       <c r="C15" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="30" customHeight="1">
       <c r="C16" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" ht="30" customHeight="1">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="30" customHeight="1">
       <c r="B17" t="s">
         <v>6</v>
       </c>
       <c r="C17" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" ht="30" customHeight="1">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="30" customHeight="1">
       <c r="C18" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" ht="30" customHeight="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="30" customHeight="1">
       <c r="C19" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" ht="30" customHeight="1">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="30" customHeight="1">
       <c r="B20" t="s">
         <v>7</v>
       </c>
       <c r="C20" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3" ht="30" customHeight="1">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="30" customHeight="1">
       <c r="C21" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3" ht="30" customHeight="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="30" customHeight="1">
       <c r="C22" t="s">
-        <v>90</v>
+        <v>91</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="30" customHeight="1">
+      <c r="A23" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="30" customHeight="1">
+      <c r="C24" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="30" customHeight="1">
+      <c r="C25" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="30" customHeight="1">
+      <c r="B26" t="s">
+        <v>2</v>
+      </c>
+      <c r="C26" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="30" customHeight="1">
+      <c r="C27" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="30" customHeight="1">
+      <c r="C28" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="30" customHeight="1">
+      <c r="B29" t="s">
+        <v>3</v>
+      </c>
+      <c r="C29" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="30" customHeight="1">
+      <c r="C30" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="30" customHeight="1">
+      <c r="C31" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="30" customHeight="1">
+      <c r="B32" t="s">
+        <v>4</v>
+      </c>
+      <c r="C32" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" ht="30" customHeight="1">
+      <c r="C33" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" ht="30" customHeight="1">
+      <c r="C34" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" ht="30" customHeight="1">
+      <c r="B35" t="s">
+        <v>5</v>
+      </c>
+      <c r="C35" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" ht="30" customHeight="1">
+      <c r="C36" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" ht="30" customHeight="1">
+      <c r="C37" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" ht="30" customHeight="1">
+      <c r="B38" t="s">
+        <v>6</v>
+      </c>
+      <c r="C38" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" ht="30" customHeight="1">
+      <c r="C39" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" ht="30" customHeight="1">
+      <c r="C40" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3" ht="30" customHeight="1">
+      <c r="B41" t="s">
+        <v>7</v>
+      </c>
+      <c r="C41" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3" ht="30" customHeight="1">
+      <c r="C42" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3" ht="30" customHeight="1">
+      <c r="C43" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -1200,716 +1332,716 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D11" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C12" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D12" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D13" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D14" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C15" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D15" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B16" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D16" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B17" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C17" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D17" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B18" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C18" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D18" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B19" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C19" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D19" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B20" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C20" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D20" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B21" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C21" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D21" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B22" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C22" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D22" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B23" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C23" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D23" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B24" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C24" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D24" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B25" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C25" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D25" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B26" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C26" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D26" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B27" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C27" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D27" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B28" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C28" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D28" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B29" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C29" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D29" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B30" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C30" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D30" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B31" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C31" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D31" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B32" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C32" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D32" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B33" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C33" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D33" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B34" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C34" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D34" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B35" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C35" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D35" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B36" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C36" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D36" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B37" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C37" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D37" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B38" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C38" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D38" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B39" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C39" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D39" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B40" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C40" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D40" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B41" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C41" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D41" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B42" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C42" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D42" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B43" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C43" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D43" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B44" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C44" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D44" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B45" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C45" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D45" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B46" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C46" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D46" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B47" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C47" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D47" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B48" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C48" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D48" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B49" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C49" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D49" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B50" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C50" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D50" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B51" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C51" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D51" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
wb: weeks 3 and 4 added
</commit_message>
<xml_diff>
--- a/MealPrepTracker.xlsx
+++ b/MealPrepTracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/quinnreams/Documents/GitHub/Personal-Growth-Planner/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E3F073A-FF73-6948-9806-81883ADAB9B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9647AFAA-27C2-514D-ABB6-F42CC325CF00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="160" yWindow="660" windowWidth="38080" windowHeight="19260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,10 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="172">
-  <si>
-    <t>Week</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="174">
   <si>
     <t>Monday</t>
   </si>
@@ -53,6 +50,12 @@
     <t>Week 2</t>
   </si>
   <si>
+    <t>Week 3</t>
+  </si>
+  <si>
+    <t>Week 4</t>
+  </si>
+  <si>
     <t>Recipe Name</t>
   </si>
   <si>
@@ -537,6 +540,9 @@
   </si>
   <si>
     <t>Breakfast</t>
+  </si>
+  <si>
+    <t>Weeks</t>
   </si>
 </sst>
 </file>
@@ -554,19 +560,18 @@
     <font>
       <b/>
       <sz val="12"/>
-      <color rgb="FF707070"/>
-      <name val="Aptos Narrow"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
       <name val="Aptos Narrow"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color rgb="FF707070"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -613,13 +618,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -627,11 +631,21 @@
   <dxfs count="4">
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF707070"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
       </font>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF00B0F0"/>
         </patternFill>
       </fill>
     </dxf>
@@ -692,12 +706,27 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:F43" totalsRowShown="0" headerRowDxfId="3">
   <autoFilter ref="A1:F43" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Week"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Weeks"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Day"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Meal"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Meal Name"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Calories"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Cost"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{06E1EBF5-7EB8-F845-A946-ABCBE0D03A8F}" name="Table13" displayName="Table13" ref="G1:L43" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="G1:L43" xr:uid="{06E1EBF5-7EB8-F845-A946-ABCBE0D03A8F}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{306D6AD0-64AE-3343-8DB9-BD5DE32F72CB}" name="Weeks"/>
+    <tableColumn id="2" xr3:uid="{844E6CC4-4122-B843-82BC-5EC1EDB17702}" name="Day"/>
+    <tableColumn id="3" xr3:uid="{DF154DD6-1E1E-4443-B749-826CEB950EC4}" name="Meal"/>
+    <tableColumn id="4" xr3:uid="{12E8841E-70B3-A34D-B938-AADCC6B67F37}" name="Meal Name"/>
+    <tableColumn id="5" xr3:uid="{01D1ABEC-7C45-C14D-BF14-EF859C0632CA}" name="Calories"/>
+    <tableColumn id="6" xr3:uid="{06F1FAD0-750A-0546-9EFC-4B07C20142E6}" name="Cost"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1020,11 +1049,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F43"/>
+  <dimension ref="A1:L43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C44" sqref="C44"/>
+      <selection pane="bottomLeft" activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1033,291 +1062,489 @@
     <col min="2" max="2" width="18.83203125" customWidth="1"/>
     <col min="3" max="3" width="20.83203125" customWidth="1"/>
     <col min="4" max="4" width="30.83203125" customWidth="1"/>
-    <col min="5" max="6" width="15.83203125" customWidth="1"/>
+    <col min="5" max="7" width="15.83203125" customWidth="1"/>
+    <col min="8" max="8" width="18.83203125" customWidth="1"/>
+    <col min="9" max="9" width="20.83203125" customWidth="1"/>
+    <col min="10" max="10" width="30.83203125" customWidth="1"/>
+    <col min="11" max="12" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="25" customHeight="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:12" ht="25" customHeight="1">
+      <c r="A1" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="30" customHeight="1">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="30" customHeight="1">
-      <c r="A2" t="s">
+      <c r="C2" t="s">
+        <v>172</v>
+      </c>
+      <c r="G2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="30" customHeight="1">
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="30" customHeight="1">
+      <c r="C4" t="s">
+        <v>92</v>
+      </c>
+      <c r="I4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="30" customHeight="1">
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>172</v>
+      </c>
+      <c r="H5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I5" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="30" customHeight="1">
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="30" customHeight="1">
+      <c r="C7" t="s">
+        <v>92</v>
+      </c>
+      <c r="I7" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="30" customHeight="1">
+      <c r="B8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>172</v>
+      </c>
+      <c r="H8" t="s">
+        <v>2</v>
+      </c>
+      <c r="I8" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="30" customHeight="1">
+      <c r="C9" t="s">
+        <v>16</v>
+      </c>
+      <c r="I9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="30" customHeight="1">
+      <c r="C10" t="s">
+        <v>92</v>
+      </c>
+      <c r="I10" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="30" customHeight="1">
+      <c r="B11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" t="s">
+        <v>172</v>
+      </c>
+      <c r="H11" t="s">
+        <v>3</v>
+      </c>
+      <c r="I11" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="30" customHeight="1">
+      <c r="C12" t="s">
+        <v>16</v>
+      </c>
+      <c r="I12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="30" customHeight="1">
+      <c r="C13" t="s">
+        <v>92</v>
+      </c>
+      <c r="I13" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="30" customHeight="1">
+      <c r="B14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" t="s">
+        <v>172</v>
+      </c>
+      <c r="H14" t="s">
+        <v>4</v>
+      </c>
+      <c r="I14" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="30" customHeight="1">
+      <c r="C15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="30" customHeight="1">
+      <c r="C16" t="s">
+        <v>92</v>
+      </c>
+      <c r="I16" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="30" customHeight="1">
+      <c r="B17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" t="s">
+        <v>172</v>
+      </c>
+      <c r="H17" t="s">
+        <v>5</v>
+      </c>
+      <c r="I17" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="30" customHeight="1">
+      <c r="C18" t="s">
+        <v>16</v>
+      </c>
+      <c r="I18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="30" customHeight="1">
+      <c r="C19" t="s">
+        <v>92</v>
+      </c>
+      <c r="I19" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="30" customHeight="1">
+      <c r="B20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" t="s">
+        <v>172</v>
+      </c>
+      <c r="H20" t="s">
+        <v>6</v>
+      </c>
+      <c r="I20" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="30" customHeight="1">
+      <c r="C21" t="s">
+        <v>16</v>
+      </c>
+      <c r="I21" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="30" customHeight="1">
+      <c r="C22" t="s">
+        <v>92</v>
+      </c>
+      <c r="I22" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="30" customHeight="1">
+      <c r="A23" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C23" t="s">
+        <v>172</v>
+      </c>
+      <c r="G23" t="s">
+        <v>10</v>
+      </c>
+      <c r="H23" t="s">
+        <v>0</v>
+      </c>
+      <c r="I23" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="30" customHeight="1">
+      <c r="C24" t="s">
+        <v>16</v>
+      </c>
+      <c r="I24" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="30" customHeight="1">
+      <c r="C25" t="s">
+        <v>92</v>
+      </c>
+      <c r="I25" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="30" customHeight="1">
+      <c r="B26" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="30" customHeight="1">
-      <c r="C3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="30" customHeight="1">
-      <c r="C4" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="30" customHeight="1">
-      <c r="B5" t="s">
+      <c r="C26" t="s">
+        <v>172</v>
+      </c>
+      <c r="H26" t="s">
+        <v>1</v>
+      </c>
+      <c r="I26" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="30" customHeight="1">
+      <c r="C27" t="s">
+        <v>16</v>
+      </c>
+      <c r="I27" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="30" customHeight="1">
+      <c r="C28" t="s">
+        <v>92</v>
+      </c>
+      <c r="I28" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="30" customHeight="1">
+      <c r="B29" t="s">
         <v>2</v>
       </c>
-      <c r="C5" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="30" customHeight="1">
-      <c r="C6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="30" customHeight="1">
-      <c r="C7" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="30" customHeight="1">
-      <c r="B8" t="s">
+      <c r="C29" t="s">
+        <v>172</v>
+      </c>
+      <c r="H29" t="s">
+        <v>2</v>
+      </c>
+      <c r="I29" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="30" customHeight="1">
+      <c r="C30" t="s">
+        <v>16</v>
+      </c>
+      <c r="I30" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="30" customHeight="1">
+      <c r="C31" t="s">
+        <v>92</v>
+      </c>
+      <c r="I31" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="30" customHeight="1">
+      <c r="B32" t="s">
         <v>3</v>
       </c>
-      <c r="C8" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="30" customHeight="1">
-      <c r="C9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="30" customHeight="1">
-      <c r="C10" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="30" customHeight="1">
-      <c r="B11" t="s">
+      <c r="C32" t="s">
+        <v>172</v>
+      </c>
+      <c r="H32" t="s">
+        <v>3</v>
+      </c>
+      <c r="I32" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" ht="30" customHeight="1">
+      <c r="C33" t="s">
+        <v>16</v>
+      </c>
+      <c r="I33" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" ht="30" customHeight="1">
+      <c r="C34" t="s">
+        <v>92</v>
+      </c>
+      <c r="I34" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9" ht="30" customHeight="1">
+      <c r="B35" t="s">
         <v>4</v>
       </c>
-      <c r="C11" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="30" customHeight="1">
-      <c r="C12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="30" customHeight="1">
-      <c r="C13" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="30" customHeight="1">
-      <c r="B14" t="s">
+      <c r="C35" t="s">
+        <v>172</v>
+      </c>
+      <c r="H35" t="s">
+        <v>4</v>
+      </c>
+      <c r="I35" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9" ht="30" customHeight="1">
+      <c r="C36" t="s">
+        <v>16</v>
+      </c>
+      <c r="I36" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9" ht="30" customHeight="1">
+      <c r="C37" t="s">
+        <v>92</v>
+      </c>
+      <c r="I37" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="38" spans="2:9" ht="30" customHeight="1">
+      <c r="B38" t="s">
         <v>5</v>
       </c>
-      <c r="C14" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="30" customHeight="1">
-      <c r="C15" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="30" customHeight="1">
-      <c r="C16" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="30" customHeight="1">
-      <c r="B17" t="s">
+      <c r="C38" t="s">
+        <v>172</v>
+      </c>
+      <c r="H38" t="s">
+        <v>5</v>
+      </c>
+      <c r="I38" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="39" spans="2:9" ht="30" customHeight="1">
+      <c r="C39" t="s">
+        <v>16</v>
+      </c>
+      <c r="I39" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="40" spans="2:9" ht="30" customHeight="1">
+      <c r="C40" t="s">
+        <v>92</v>
+      </c>
+      <c r="I40" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="41" spans="2:9" ht="30" customHeight="1">
+      <c r="B41" t="s">
         <v>6</v>
       </c>
-      <c r="C17" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="30" customHeight="1">
-      <c r="C18" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="30" customHeight="1">
-      <c r="C19" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="30" customHeight="1">
-      <c r="B20" t="s">
-        <v>7</v>
-      </c>
-      <c r="C20" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="30" customHeight="1">
-      <c r="C21" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="30" customHeight="1">
-      <c r="C22" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="30" customHeight="1">
-      <c r="A23" t="s">
-        <v>9</v>
-      </c>
-      <c r="B23" t="s">
-        <v>1</v>
-      </c>
-      <c r="C23" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="30" customHeight="1">
-      <c r="C24" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="30" customHeight="1">
-      <c r="C25" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="30" customHeight="1">
-      <c r="B26" t="s">
-        <v>2</v>
-      </c>
-      <c r="C26" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="30" customHeight="1">
-      <c r="C27" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="30" customHeight="1">
-      <c r="C28" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="30" customHeight="1">
-      <c r="B29" t="s">
-        <v>3</v>
-      </c>
-      <c r="C29" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="30" customHeight="1">
-      <c r="C30" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="30" customHeight="1">
-      <c r="C31" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="30" customHeight="1">
-      <c r="B32" t="s">
-        <v>4</v>
-      </c>
-      <c r="C32" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="33" spans="2:3" ht="30" customHeight="1">
-      <c r="C33" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="34" spans="2:3" ht="30" customHeight="1">
-      <c r="C34" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="35" spans="2:3" ht="30" customHeight="1">
-      <c r="B35" t="s">
-        <v>5</v>
-      </c>
-      <c r="C35" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="36" spans="2:3" ht="30" customHeight="1">
-      <c r="C36" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="37" spans="2:3" ht="30" customHeight="1">
-      <c r="C37" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="38" spans="2:3" ht="30" customHeight="1">
-      <c r="B38" t="s">
+      <c r="C41" t="s">
+        <v>172</v>
+      </c>
+      <c r="H41" t="s">
         <v>6</v>
       </c>
-      <c r="C38" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="39" spans="2:3" ht="30" customHeight="1">
-      <c r="C39" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="40" spans="2:3" ht="30" customHeight="1">
-      <c r="C40" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="41" spans="2:3" ht="30" customHeight="1">
-      <c r="B41" t="s">
-        <v>7</v>
-      </c>
-      <c r="C41" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="42" spans="2:3" ht="30" customHeight="1">
+      <c r="I41" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="42" spans="2:9" ht="30" customHeight="1">
       <c r="C42" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="43" spans="2:3" ht="30" customHeight="1">
+        <v>16</v>
+      </c>
+      <c r="I42" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="43" spans="2:9" ht="30" customHeight="1">
       <c r="C43" t="s">
-        <v>91</v>
+        <v>92</v>
+      </c>
+      <c r="I43" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
+  <tableParts count="2">
     <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -1331,717 +1558,717 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>13</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D10" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C11" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D11" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C12" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D12" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C13" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D13" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C14" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C15" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D15" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B16" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C16" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D16" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B17" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D17" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B18" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C18" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D18" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B19" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C19" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D19" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B20" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C20" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D20" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B21" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C21" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D21" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B22" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C22" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D22" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B23" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C23" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D23" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B24" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C24" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D24" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B25" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C25" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D25" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B26" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C26" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D26" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B27" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C27" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D27" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B28" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C28" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D28" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B29" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C29" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D29" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B30" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C30" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D30" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B31" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C31" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D31" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B32" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C32" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D32" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B33" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C33" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D33" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B34" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C34" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D34" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B35" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C35" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D35" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B36" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C36" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D36" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B37" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C37" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D37" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B38" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C38" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D38" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B39" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C39" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D39" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B40" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C40" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D40" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B41" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C41" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D41" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B42" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C42" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D42" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B43" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C43" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D43" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B44" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C44" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D44" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B45" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C45" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D45" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B46" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C46" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D46" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B47" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C47" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D47" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B48" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C48" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D48" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B49" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C49" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D49" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B50" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C50" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D50" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B51" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C51" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D51" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
wb:dropdowns made for meal selection
</commit_message>
<xml_diff>
--- a/MealPrepTracker.xlsx
+++ b/MealPrepTracker.xlsx
@@ -8,14 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/quinnreams/Documents/GitHub/Personal-Growth-Planner/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72A0C03A-A03D-2C49-8ED5-A8DA4A0BC531}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E508B7A-7FC2-9848-AF70-43B2B1D14112}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="660" windowWidth="38080" windowHeight="19260" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="160" yWindow="660" windowWidth="38080" windowHeight="19260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Meal Calendar" sheetId="1" r:id="rId1"/>
     <sheet name="Recipes" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="RecipeList">OFFSET(Recipes!$A$2, 0, 0, COUNTA(Recipes!$A$2:$A$1000), 1)</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -618,17 +621,29 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="5">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -693,13 +708,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:F43" totalsRowShown="0" headerRowDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:F43" totalsRowShown="0" headerRowDxfId="4">
   <autoFilter ref="A1:F43" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Week"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Day"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Meal"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Meal Name"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Meal Name" dataDxfId="0"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Calories"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Cost"/>
   </tableColumns>
@@ -708,13 +723,13 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{06E1EBF5-7EB8-F845-A946-ABCBE0D03A8F}" name="Table13" displayName="Table13" ref="G1:L43" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{06E1EBF5-7EB8-F845-A946-ABCBE0D03A8F}" name="Table13" displayName="Table13" ref="G1:L43" totalsRowShown="0" headerRowDxfId="2">
   <autoFilter ref="G1:L43" xr:uid="{06E1EBF5-7EB8-F845-A946-ABCBE0D03A8F}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{306D6AD0-64AE-3343-8DB9-BD5DE32F72CB}" name="Week"/>
     <tableColumn id="2" xr3:uid="{844E6CC4-4122-B843-82BC-5EC1EDB17702}" name="Day"/>
     <tableColumn id="3" xr3:uid="{DF154DD6-1E1E-4443-B749-826CEB950EC4}" name="Meal"/>
-    <tableColumn id="4" xr3:uid="{12E8841E-70B3-A34D-B938-AADCC6B67F37}" name="Meal Name"/>
+    <tableColumn id="4" xr3:uid="{12E8841E-70B3-A34D-B938-AADCC6B67F37}" name="Meal Name" dataDxfId="1"/>
     <tableColumn id="5" xr3:uid="{01D1ABEC-7C45-C14D-BF14-EF859C0632CA}" name="Calories"/>
     <tableColumn id="6" xr3:uid="{06F1FAD0-750A-0546-9EFC-4B07C20142E6}" name="Cost"/>
   </tableColumns>
@@ -1041,9 +1056,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L43"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1051,11 +1066,11 @@
     <col min="1" max="1" width="15.83203125" customWidth="1"/>
     <col min="2" max="2" width="18.83203125" customWidth="1"/>
     <col min="3" max="3" width="20.83203125" customWidth="1"/>
-    <col min="4" max="4" width="30.83203125" customWidth="1"/>
+    <col min="4" max="4" width="30.83203125" style="4" customWidth="1"/>
     <col min="5" max="7" width="15.83203125" customWidth="1"/>
     <col min="8" max="8" width="18.83203125" customWidth="1"/>
     <col min="9" max="9" width="20.83203125" customWidth="1"/>
-    <col min="10" max="10" width="30.83203125" customWidth="1"/>
+    <col min="10" max="10" width="30.83203125" style="4" customWidth="1"/>
     <col min="11" max="12" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1069,7 +1084,7 @@
       <c r="C1" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>170</v>
       </c>
       <c r="E1" s="2" t="s">
@@ -1087,7 +1102,7 @@
       <c r="I1" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="3" t="s">
         <v>170</v>
       </c>
       <c r="K1" s="2" t="s">
@@ -1531,6 +1546,11 @@
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D43 J2:J43" xr:uid="{317D4B3D-4DBF-2749-B892-0E6482D4EC8A}">
+      <formula1>RecipeList</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="2">
     <tablePart r:id="rId1"/>
@@ -1543,13 +1563,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A14" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="75.83203125" customWidth="1"/>
+    <col min="1" max="1" width="70.83203125" customWidth="1"/>
     <col min="2" max="2" width="15.83203125" customWidth="1"/>
     <col min="3" max="3" width="50.83203125" customWidth="1"/>
     <col min="4" max="4" width="40.83203125" customWidth="1"/>

</xml_diff>

<commit_message>
wb: vlookup codes started for calories and cost
</commit_message>
<xml_diff>
--- a/MealPrepTracker.xlsx
+++ b/MealPrepTracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/quinnreams/Documents/GitHub/Personal-Growth-Planner/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E508B7A-7FC2-9848-AF70-43B2B1D14112}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A698EFE0-DA77-1C48-8A43-E20A78EC64C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="160" yWindow="660" windowWidth="38080" windowHeight="19260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,7 +19,20 @@
   <definedNames>
     <definedName name="RecipeList">OFFSET(Recipes!$A$2, 0, 0, COUNTA(Recipes!$A$2:$A$1000), 1)</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -552,7 +565,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -578,6 +591,17 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
+      <name val="Inherit"/>
     </font>
   </fonts>
   <fills count="3">
@@ -621,7 +645,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -633,11 +657,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="9">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -708,30 +746,38 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:F43" totalsRowShown="0" headerRowDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:F43" totalsRowShown="0" headerRowDxfId="8">
   <autoFilter ref="A1:F43" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Week"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Day"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Meal"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Meal Name" dataDxfId="0"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Calories"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Cost"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Meal Name" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Calories" dataDxfId="3">
+      <calculatedColumnFormula>IFERROR(VLOOKUP(C2, Recipes!$A$2:$C$1000, 2, FALSE), "")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Cost" dataDxfId="2">
+      <calculatedColumnFormula>IFERROR(VLOOKUP(C2, Recipes!$A$2:$C$1000, 3, FALSE), "")</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{06E1EBF5-7EB8-F845-A946-ABCBE0D03A8F}" name="Table13" displayName="Table13" ref="G1:L43" totalsRowShown="0" headerRowDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{06E1EBF5-7EB8-F845-A946-ABCBE0D03A8F}" name="Table13" displayName="Table13" ref="G1:L43" totalsRowShown="0" headerRowDxfId="6">
   <autoFilter ref="G1:L43" xr:uid="{06E1EBF5-7EB8-F845-A946-ABCBE0D03A8F}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{306D6AD0-64AE-3343-8DB9-BD5DE32F72CB}" name="Week"/>
     <tableColumn id="2" xr3:uid="{844E6CC4-4122-B843-82BC-5EC1EDB17702}" name="Day"/>
     <tableColumn id="3" xr3:uid="{DF154DD6-1E1E-4443-B749-826CEB950EC4}" name="Meal"/>
-    <tableColumn id="4" xr3:uid="{12E8841E-70B3-A34D-B938-AADCC6B67F37}" name="Meal Name" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{01D1ABEC-7C45-C14D-BF14-EF859C0632CA}" name="Calories"/>
-    <tableColumn id="6" xr3:uid="{06F1FAD0-750A-0546-9EFC-4B07C20142E6}" name="Cost"/>
+    <tableColumn id="4" xr3:uid="{12E8841E-70B3-A34D-B938-AADCC6B67F37}" name="Meal Name" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{01D1ABEC-7C45-C14D-BF14-EF859C0632CA}" name="Calories" dataDxfId="1">
+      <calculatedColumnFormula>IFERROR(VLOOKUP(J2, Recipes!$A$2:$C$1000, 2, FALSE), "")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{06F1FAD0-750A-0546-9EFC-4B07C20142E6}" name="Cost" dataDxfId="0">
+      <calculatedColumnFormula>IFERROR(VLOOKUP(J2, Recipes!$A$2:$C$1000, 3, FALSE), "")</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1057,8 +1103,8 @@
   <dimension ref="A1:L43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1122,6 +1168,14 @@
       <c r="C2" t="s">
         <v>173</v>
       </c>
+      <c r="E2" s="5" t="str">
+        <f>IFERROR(VLOOKUP(C2, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="F2" s="6" t="str">
+        <f>IFERROR(VLOOKUP(C2, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <v/>
+      </c>
       <c r="G2" t="s">
         <v>10</v>
       </c>
@@ -1131,21 +1185,61 @@
       <c r="I2" t="s">
         <v>173</v>
       </c>
+      <c r="K2" s="6" t="str">
+        <f>IFERROR(VLOOKUP(J2, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="L2" s="6" t="str">
+        <f>IFERROR(VLOOKUP(J2, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <v/>
+      </c>
     </row>
     <row r="3" spans="1:12" ht="30" customHeight="1">
       <c r="C3" t="s">
         <v>17</v>
       </c>
+      <c r="E3" t="str">
+        <f>IFERROR(VLOOKUP(C3, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="F3" t="str">
+        <f>IFERROR(VLOOKUP(C3, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <v/>
+      </c>
       <c r="I3" t="s">
         <v>17</v>
+      </c>
+      <c r="K3" t="str">
+        <f>IFERROR(VLOOKUP(J3, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="L3" t="str">
+        <f>IFERROR(VLOOKUP(J3, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <v/>
       </c>
     </row>
     <row r="4" spans="1:12" ht="30" customHeight="1">
       <c r="C4" t="s">
         <v>93</v>
       </c>
+      <c r="E4" t="str">
+        <f>IFERROR(VLOOKUP(C4, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="F4" t="str">
+        <f>IFERROR(VLOOKUP(C4, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <v/>
+      </c>
       <c r="I4" t="s">
         <v>93</v>
+      </c>
+      <c r="K4" t="str">
+        <f>IFERROR(VLOOKUP(J4, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="L4" t="str">
+        <f>IFERROR(VLOOKUP(J4, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <v/>
       </c>
     </row>
     <row r="5" spans="1:12" ht="30" customHeight="1">
@@ -1155,27 +1249,75 @@
       <c r="C5" t="s">
         <v>173</v>
       </c>
+      <c r="E5" t="str">
+        <f>IFERROR(VLOOKUP(C5, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="F5" t="str">
+        <f>IFERROR(VLOOKUP(C5, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <v/>
+      </c>
       <c r="H5" t="s">
         <v>2</v>
       </c>
       <c r="I5" t="s">
         <v>173</v>
       </c>
+      <c r="K5" t="str">
+        <f>IFERROR(VLOOKUP(J5, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="L5" t="str">
+        <f>IFERROR(VLOOKUP(J5, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <v/>
+      </c>
     </row>
     <row r="6" spans="1:12" ht="30" customHeight="1">
       <c r="C6" t="s">
         <v>17</v>
       </c>
+      <c r="E6" t="str">
+        <f>IFERROR(VLOOKUP(C6, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="F6" t="str">
+        <f>IFERROR(VLOOKUP(C6, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <v/>
+      </c>
       <c r="I6" t="s">
         <v>17</v>
+      </c>
+      <c r="K6" t="str">
+        <f>IFERROR(VLOOKUP(J6, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="L6" t="str">
+        <f>IFERROR(VLOOKUP(J6, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <v/>
       </c>
     </row>
     <row r="7" spans="1:12" ht="30" customHeight="1">
       <c r="C7" t="s">
         <v>93</v>
       </c>
+      <c r="E7" t="str">
+        <f>IFERROR(VLOOKUP(C7, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="F7" t="str">
+        <f>IFERROR(VLOOKUP(C7, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <v/>
+      </c>
       <c r="I7" t="s">
         <v>93</v>
+      </c>
+      <c r="K7" t="str">
+        <f>IFERROR(VLOOKUP(J7, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="L7" t="str">
+        <f>IFERROR(VLOOKUP(J7, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <v/>
       </c>
     </row>
     <row r="8" spans="1:12" ht="30" customHeight="1">
@@ -1185,27 +1327,75 @@
       <c r="C8" t="s">
         <v>173</v>
       </c>
+      <c r="E8" t="str">
+        <f>IFERROR(VLOOKUP(C8, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="F8" t="str">
+        <f>IFERROR(VLOOKUP(C8, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <v/>
+      </c>
       <c r="H8" t="s">
         <v>3</v>
       </c>
       <c r="I8" t="s">
         <v>173</v>
       </c>
+      <c r="K8" t="str">
+        <f>IFERROR(VLOOKUP(J8, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="L8" t="str">
+        <f>IFERROR(VLOOKUP(J8, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <v/>
+      </c>
     </row>
     <row r="9" spans="1:12" ht="30" customHeight="1">
       <c r="C9" t="s">
         <v>17</v>
       </c>
+      <c r="E9" t="str">
+        <f>IFERROR(VLOOKUP(C9, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="F9" t="str">
+        <f>IFERROR(VLOOKUP(C9, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <v/>
+      </c>
       <c r="I9" t="s">
         <v>17</v>
+      </c>
+      <c r="K9" t="str">
+        <f>IFERROR(VLOOKUP(J9, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="L9" t="str">
+        <f>IFERROR(VLOOKUP(J9, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <v/>
       </c>
     </row>
     <row r="10" spans="1:12" ht="30" customHeight="1">
       <c r="C10" t="s">
         <v>93</v>
       </c>
+      <c r="E10" t="str">
+        <f>IFERROR(VLOOKUP(C10, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="F10" t="str">
+        <f>IFERROR(VLOOKUP(C10, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <v/>
+      </c>
       <c r="I10" t="s">
         <v>93</v>
+      </c>
+      <c r="K10" t="str">
+        <f>IFERROR(VLOOKUP(J10, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="L10" t="str">
+        <f>IFERROR(VLOOKUP(J10, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <v/>
       </c>
     </row>
     <row r="11" spans="1:12" ht="30" customHeight="1">
@@ -1215,27 +1405,75 @@
       <c r="C11" t="s">
         <v>173</v>
       </c>
+      <c r="E11" t="str">
+        <f>IFERROR(VLOOKUP(C11, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="F11" t="str">
+        <f>IFERROR(VLOOKUP(C11, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <v/>
+      </c>
       <c r="H11" t="s">
         <v>4</v>
       </c>
       <c r="I11" t="s">
         <v>173</v>
       </c>
+      <c r="K11" t="str">
+        <f>IFERROR(VLOOKUP(J11, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="L11" t="str">
+        <f>IFERROR(VLOOKUP(J11, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <v/>
+      </c>
     </row>
     <row r="12" spans="1:12" ht="30" customHeight="1">
       <c r="C12" t="s">
         <v>17</v>
       </c>
+      <c r="E12" t="str">
+        <f>IFERROR(VLOOKUP(C12, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="F12" t="str">
+        <f>IFERROR(VLOOKUP(C12, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <v/>
+      </c>
       <c r="I12" t="s">
         <v>17</v>
+      </c>
+      <c r="K12" t="str">
+        <f>IFERROR(VLOOKUP(J12, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="L12" t="str">
+        <f>IFERROR(VLOOKUP(J12, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <v/>
       </c>
     </row>
     <row r="13" spans="1:12" ht="30" customHeight="1">
       <c r="C13" t="s">
         <v>93</v>
       </c>
+      <c r="E13" t="str">
+        <f>IFERROR(VLOOKUP(C13, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="F13" t="str">
+        <f>IFERROR(VLOOKUP(C13, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <v/>
+      </c>
       <c r="I13" t="s">
         <v>93</v>
+      </c>
+      <c r="K13" t="str">
+        <f>IFERROR(VLOOKUP(J13, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="L13" t="str">
+        <f>IFERROR(VLOOKUP(J13, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <v/>
       </c>
     </row>
     <row r="14" spans="1:12" ht="30" customHeight="1">
@@ -1245,90 +1483,234 @@
       <c r="C14" t="s">
         <v>173</v>
       </c>
+      <c r="E14" t="str">
+        <f>IFERROR(VLOOKUP(C14, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="F14" t="str">
+        <f>IFERROR(VLOOKUP(C14, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <v/>
+      </c>
       <c r="H14" t="s">
         <v>5</v>
       </c>
       <c r="I14" t="s">
         <v>173</v>
       </c>
+      <c r="K14" t="str">
+        <f>IFERROR(VLOOKUP(J14, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="L14" t="str">
+        <f>IFERROR(VLOOKUP(J14, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <v/>
+      </c>
     </row>
     <row r="15" spans="1:12" ht="30" customHeight="1">
       <c r="C15" t="s">
         <v>17</v>
       </c>
+      <c r="E15" t="str">
+        <f>IFERROR(VLOOKUP(C15, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="F15" t="str">
+        <f>IFERROR(VLOOKUP(C15, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <v/>
+      </c>
       <c r="I15" t="s">
         <v>17</v>
+      </c>
+      <c r="K15" t="str">
+        <f>IFERROR(VLOOKUP(J15, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="L15" t="str">
+        <f>IFERROR(VLOOKUP(J15, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <v/>
       </c>
     </row>
     <row r="16" spans="1:12" ht="30" customHeight="1">
       <c r="C16" t="s">
         <v>93</v>
       </c>
+      <c r="E16" t="str">
+        <f>IFERROR(VLOOKUP(C16, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="F16" t="str">
+        <f>IFERROR(VLOOKUP(C16, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <v/>
+      </c>
       <c r="I16" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" ht="30" customHeight="1">
+      <c r="K16" t="str">
+        <f>IFERROR(VLOOKUP(J16, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="L16" t="str">
+        <f>IFERROR(VLOOKUP(J16, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="30" customHeight="1">
       <c r="B17" t="s">
         <v>6</v>
       </c>
       <c r="C17" t="s">
         <v>173</v>
       </c>
+      <c r="E17" t="str">
+        <f>IFERROR(VLOOKUP(C17, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="F17" t="str">
+        <f>IFERROR(VLOOKUP(C17, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <v/>
+      </c>
       <c r="H17" t="s">
         <v>6</v>
       </c>
       <c r="I17" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" ht="30" customHeight="1">
+      <c r="K17" t="str">
+        <f>IFERROR(VLOOKUP(J17, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="L17" t="str">
+        <f>IFERROR(VLOOKUP(J17, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="C18" t="s">
         <v>17</v>
       </c>
+      <c r="E18" t="str">
+        <f>IFERROR(VLOOKUP(C18, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="F18" t="str">
+        <f>IFERROR(VLOOKUP(C18, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <v/>
+      </c>
       <c r="I18" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" ht="30" customHeight="1">
+      <c r="K18" t="str">
+        <f>IFERROR(VLOOKUP(J18, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="L18" t="str">
+        <f>IFERROR(VLOOKUP(J18, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="30" customHeight="1">
       <c r="C19" t="s">
         <v>93</v>
       </c>
+      <c r="E19" t="str">
+        <f>IFERROR(VLOOKUP(C19, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="F19" t="str">
+        <f>IFERROR(VLOOKUP(C19, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <v/>
+      </c>
       <c r="I19" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" ht="30" customHeight="1">
+      <c r="K19" t="str">
+        <f>IFERROR(VLOOKUP(J19, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="L19" t="str">
+        <f>IFERROR(VLOOKUP(J19, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="30" customHeight="1">
       <c r="B20" t="s">
         <v>7</v>
       </c>
       <c r="C20" t="s">
         <v>173</v>
       </c>
+      <c r="E20" t="str">
+        <f>IFERROR(VLOOKUP(C20, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="F20" t="str">
+        <f>IFERROR(VLOOKUP(C20, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <v/>
+      </c>
       <c r="H20" t="s">
         <v>7</v>
       </c>
       <c r="I20" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" ht="30" customHeight="1">
+      <c r="K20" t="str">
+        <f>IFERROR(VLOOKUP(J20, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="L20" t="str">
+        <f>IFERROR(VLOOKUP(J20, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="30" customHeight="1">
       <c r="C21" t="s">
         <v>17</v>
       </c>
+      <c r="E21" t="str">
+        <f>IFERROR(VLOOKUP(C21, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="F21" t="str">
+        <f>IFERROR(VLOOKUP(C21, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <v/>
+      </c>
       <c r="I21" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" ht="30" customHeight="1">
+      <c r="K21" t="str">
+        <f>IFERROR(VLOOKUP(J21, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="L21" t="str">
+        <f>IFERROR(VLOOKUP(J21, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="30" customHeight="1">
       <c r="C22" t="s">
         <v>93</v>
       </c>
+      <c r="E22" t="str">
+        <f>IFERROR(VLOOKUP(C22, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="F22" t="str">
+        <f>IFERROR(VLOOKUP(C22, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <v/>
+      </c>
       <c r="I22" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" ht="30" customHeight="1">
+      <c r="K22" t="str">
+        <f>IFERROR(VLOOKUP(J22, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="L22" t="str">
+        <f>IFERROR(VLOOKUP(J22, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="30" customHeight="1">
       <c r="A23" t="s">
         <v>9</v>
       </c>
@@ -1338,6 +1720,14 @@
       <c r="C23" t="s">
         <v>173</v>
       </c>
+      <c r="E23" t="str">
+        <f>IFERROR(VLOOKUP(C23, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="F23" t="str">
+        <f>IFERROR(VLOOKUP(C23, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <v/>
+      </c>
       <c r="G23" t="s">
         <v>11</v>
       </c>
@@ -1347,201 +1737,529 @@
       <c r="I23" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" ht="30" customHeight="1">
+      <c r="K23" t="str">
+        <f>IFERROR(VLOOKUP(J23, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="L23" t="str">
+        <f>IFERROR(VLOOKUP(J23, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="30" customHeight="1">
       <c r="C24" t="s">
         <v>17</v>
       </c>
+      <c r="E24" t="str">
+        <f>IFERROR(VLOOKUP(C24, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="F24" t="str">
+        <f>IFERROR(VLOOKUP(C24, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <v/>
+      </c>
       <c r="I24" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" ht="30" customHeight="1">
+      <c r="K24" t="str">
+        <f>IFERROR(VLOOKUP(J24, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="L24" t="str">
+        <f>IFERROR(VLOOKUP(J24, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="30" customHeight="1">
       <c r="C25" t="s">
         <v>93</v>
       </c>
+      <c r="E25" t="str">
+        <f>IFERROR(VLOOKUP(C25, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="F25" t="str">
+        <f>IFERROR(VLOOKUP(C25, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <v/>
+      </c>
       <c r="I25" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" ht="30" customHeight="1">
+      <c r="K25" t="str">
+        <f>IFERROR(VLOOKUP(J25, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="L25" t="str">
+        <f>IFERROR(VLOOKUP(J25, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="30" customHeight="1">
       <c r="B26" t="s">
         <v>2</v>
       </c>
       <c r="C26" t="s">
         <v>173</v>
       </c>
+      <c r="E26" t="str">
+        <f>IFERROR(VLOOKUP(C26, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="F26" t="str">
+        <f>IFERROR(VLOOKUP(C26, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <v/>
+      </c>
       <c r="H26" t="s">
         <v>2</v>
       </c>
       <c r="I26" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" ht="30" customHeight="1">
+      <c r="K26" t="str">
+        <f>IFERROR(VLOOKUP(J26, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="L26" t="str">
+        <f>IFERROR(VLOOKUP(J26, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="30" customHeight="1">
       <c r="C27" t="s">
         <v>17</v>
       </c>
+      <c r="E27" t="str">
+        <f>IFERROR(VLOOKUP(C27, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="F27" t="str">
+        <f>IFERROR(VLOOKUP(C27, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <v/>
+      </c>
       <c r="I27" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" ht="30" customHeight="1">
+      <c r="K27" t="str">
+        <f>IFERROR(VLOOKUP(J27, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="L27" t="str">
+        <f>IFERROR(VLOOKUP(J27, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="30" customHeight="1">
       <c r="C28" t="s">
         <v>93</v>
       </c>
+      <c r="E28" t="str">
+        <f>IFERROR(VLOOKUP(C28, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="F28" t="str">
+        <f>IFERROR(VLOOKUP(C28, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <v/>
+      </c>
       <c r="I28" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" ht="30" customHeight="1">
+      <c r="K28" t="str">
+        <f>IFERROR(VLOOKUP(J28, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="L28" t="str">
+        <f>IFERROR(VLOOKUP(J28, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="30" customHeight="1">
       <c r="B29" t="s">
         <v>3</v>
       </c>
       <c r="C29" t="s">
         <v>173</v>
       </c>
+      <c r="E29" t="str">
+        <f>IFERROR(VLOOKUP(C29, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="F29" t="str">
+        <f>IFERROR(VLOOKUP(C29, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <v/>
+      </c>
       <c r="H29" t="s">
         <v>3</v>
       </c>
       <c r="I29" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" ht="30" customHeight="1">
+      <c r="K29" t="str">
+        <f>IFERROR(VLOOKUP(J29, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="L29" t="str">
+        <f>IFERROR(VLOOKUP(J29, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="30" customHeight="1">
       <c r="C30" t="s">
         <v>17</v>
       </c>
+      <c r="E30" t="str">
+        <f>IFERROR(VLOOKUP(C30, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="F30" t="str">
+        <f>IFERROR(VLOOKUP(C30, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <v/>
+      </c>
       <c r="I30" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" ht="30" customHeight="1">
+      <c r="K30" t="str">
+        <f>IFERROR(VLOOKUP(J30, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="L30" t="str">
+        <f>IFERROR(VLOOKUP(J30, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="30" customHeight="1">
       <c r="C31" t="s">
         <v>93</v>
       </c>
+      <c r="E31" t="str">
+        <f>IFERROR(VLOOKUP(C31, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="F31" t="str">
+        <f>IFERROR(VLOOKUP(C31, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <v/>
+      </c>
       <c r="I31" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" ht="30" customHeight="1">
+      <c r="K31" t="str">
+        <f>IFERROR(VLOOKUP(J31, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="L31" t="str">
+        <f>IFERROR(VLOOKUP(J31, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="30" customHeight="1">
       <c r="B32" t="s">
         <v>4</v>
       </c>
       <c r="C32" t="s">
         <v>173</v>
       </c>
+      <c r="E32" t="str">
+        <f>IFERROR(VLOOKUP(C32, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="F32" t="str">
+        <f>IFERROR(VLOOKUP(C32, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <v/>
+      </c>
       <c r="H32" t="s">
         <v>4</v>
       </c>
       <c r="I32" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="33" spans="2:9" ht="30" customHeight="1">
+      <c r="K32" t="str">
+        <f>IFERROR(VLOOKUP(J32, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="L32" t="str">
+        <f>IFERROR(VLOOKUP(J32, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="33" spans="2:12" ht="30" customHeight="1">
       <c r="C33" t="s">
         <v>17</v>
       </c>
+      <c r="E33" t="str">
+        <f>IFERROR(VLOOKUP(C33, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="F33" t="str">
+        <f>IFERROR(VLOOKUP(C33, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <v/>
+      </c>
       <c r="I33" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="34" spans="2:9" ht="30" customHeight="1">
+      <c r="K33" t="str">
+        <f>IFERROR(VLOOKUP(J33, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="L33" t="str">
+        <f>IFERROR(VLOOKUP(J33, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="2:12" ht="30" customHeight="1">
       <c r="C34" t="s">
         <v>93</v>
       </c>
+      <c r="E34" t="str">
+        <f>IFERROR(VLOOKUP(C34, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="F34" t="str">
+        <f>IFERROR(VLOOKUP(C34, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <v/>
+      </c>
       <c r="I34" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="35" spans="2:9" ht="30" customHeight="1">
+      <c r="K34" t="str">
+        <f>IFERROR(VLOOKUP(J34, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="L34" t="str">
+        <f>IFERROR(VLOOKUP(J34, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="35" spans="2:12" ht="30" customHeight="1">
       <c r="B35" t="s">
         <v>5</v>
       </c>
       <c r="C35" t="s">
         <v>173</v>
       </c>
+      <c r="E35" t="str">
+        <f>IFERROR(VLOOKUP(C35, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="F35" t="str">
+        <f>IFERROR(VLOOKUP(C35, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <v/>
+      </c>
       <c r="H35" t="s">
         <v>5</v>
       </c>
       <c r="I35" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="36" spans="2:9" ht="30" customHeight="1">
+      <c r="K35" t="str">
+        <f>IFERROR(VLOOKUP(J35, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="L35" t="str">
+        <f>IFERROR(VLOOKUP(J35, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="36" spans="2:12" ht="30" customHeight="1">
       <c r="C36" t="s">
         <v>17</v>
       </c>
+      <c r="E36" t="str">
+        <f>IFERROR(VLOOKUP(C36, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="F36" t="str">
+        <f>IFERROR(VLOOKUP(C36, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <v/>
+      </c>
       <c r="I36" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="37" spans="2:9" ht="30" customHeight="1">
+      <c r="K36" t="str">
+        <f>IFERROR(VLOOKUP(J36, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="L36" t="str">
+        <f>IFERROR(VLOOKUP(J36, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="37" spans="2:12" ht="30" customHeight="1">
       <c r="C37" t="s">
         <v>93</v>
       </c>
+      <c r="E37" t="str">
+        <f>IFERROR(VLOOKUP(C37, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="F37" t="str">
+        <f>IFERROR(VLOOKUP(C37, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <v/>
+      </c>
       <c r="I37" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="38" spans="2:9" ht="30" customHeight="1">
+      <c r="K37" t="str">
+        <f>IFERROR(VLOOKUP(J37, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="L37" t="str">
+        <f>IFERROR(VLOOKUP(J37, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="38" spans="2:12" ht="30" customHeight="1">
       <c r="B38" t="s">
         <v>6</v>
       </c>
       <c r="C38" t="s">
         <v>173</v>
       </c>
+      <c r="E38" t="str">
+        <f>IFERROR(VLOOKUP(C38, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="F38" t="str">
+        <f>IFERROR(VLOOKUP(C38, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <v/>
+      </c>
       <c r="H38" t="s">
         <v>6</v>
       </c>
       <c r="I38" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="39" spans="2:9" ht="30" customHeight="1">
+      <c r="K38" t="str">
+        <f>IFERROR(VLOOKUP(J38, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="L38" t="str">
+        <f>IFERROR(VLOOKUP(J38, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="39" spans="2:12" ht="30" customHeight="1">
       <c r="C39" t="s">
         <v>17</v>
       </c>
+      <c r="E39" t="str">
+        <f>IFERROR(VLOOKUP(C39, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="F39" t="str">
+        <f>IFERROR(VLOOKUP(C39, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <v/>
+      </c>
       <c r="I39" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="40" spans="2:9" ht="30" customHeight="1">
+      <c r="K39" t="str">
+        <f>IFERROR(VLOOKUP(J39, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="L39" t="str">
+        <f>IFERROR(VLOOKUP(J39, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="40" spans="2:12" ht="30" customHeight="1">
       <c r="C40" t="s">
         <v>93</v>
       </c>
+      <c r="E40" t="str">
+        <f>IFERROR(VLOOKUP(C40, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="F40" t="str">
+        <f>IFERROR(VLOOKUP(C40, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <v/>
+      </c>
       <c r="I40" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="41" spans="2:9" ht="30" customHeight="1">
+      <c r="K40" t="str">
+        <f>IFERROR(VLOOKUP(J40, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="L40" t="str">
+        <f>IFERROR(VLOOKUP(J40, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="41" spans="2:12" ht="30" customHeight="1">
       <c r="B41" t="s">
         <v>7</v>
       </c>
       <c r="C41" t="s">
         <v>173</v>
       </c>
+      <c r="E41" t="str">
+        <f>IFERROR(VLOOKUP(C41, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="F41" t="str">
+        <f>IFERROR(VLOOKUP(C41, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <v/>
+      </c>
       <c r="H41" t="s">
         <v>7</v>
       </c>
       <c r="I41" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="42" spans="2:9" ht="30" customHeight="1">
+      <c r="K41" t="str">
+        <f>IFERROR(VLOOKUP(J41, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="L41" t="str">
+        <f>IFERROR(VLOOKUP(J41, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="42" spans="2:12" ht="30" customHeight="1">
       <c r="C42" t="s">
         <v>17</v>
       </c>
+      <c r="E42" t="str">
+        <f>IFERROR(VLOOKUP(C42, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="F42" t="str">
+        <f>IFERROR(VLOOKUP(C42, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <v/>
+      </c>
       <c r="I42" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="43" spans="2:9" ht="30" customHeight="1">
+      <c r="K42" t="str">
+        <f>IFERROR(VLOOKUP(J42, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="L42" t="str">
+        <f>IFERROR(VLOOKUP(J42, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="43" spans="2:12" ht="30" customHeight="1">
       <c r="C43" t="s">
         <v>93</v>
       </c>
+      <c r="E43" t="str">
+        <f>IFERROR(VLOOKUP(C43, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="F43" t="str">
+        <f>IFERROR(VLOOKUP(C43, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <v/>
+      </c>
       <c r="I43" t="s">
         <v>93</v>
+      </c>
+      <c r="K43" t="str">
+        <f>IFERROR(VLOOKUP(J43, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="L43" t="str">
+        <f>IFERROR(VLOOKUP(J43, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <v/>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
wb: totals row added
</commit_message>
<xml_diff>
--- a/MealPrepTracker.xlsx
+++ b/MealPrepTracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/quinnreams/Documents/GitHub/Personal-Growth-Planner/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A698EFE0-DA77-1C48-8A43-E20A78EC64C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2FDE25C-CF74-7D4D-BF10-9F3391891A53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="160" yWindow="660" windowWidth="38080" windowHeight="19260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="175">
   <si>
     <t>Week</t>
   </si>
@@ -559,6 +559,9 @@
   </si>
   <si>
     <t>Breakfast</t>
+  </si>
+  <si>
+    <t>Totals</t>
   </si>
 </sst>
 </file>
@@ -645,7 +648,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -659,6 +662,7 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -671,13 +675,33 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF707070"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -712,26 +736,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF707070"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -746,17 +750,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:F43" totalsRowShown="0" headerRowDxfId="8">
-  <autoFilter ref="A1:F43" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:F45" totalsRowShown="0" headerRowDxfId="3">
+  <autoFilter ref="A1:F45" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Week"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Day"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Meal"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Meal Name" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Calories" dataDxfId="3">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Meal Name" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Calories" dataDxfId="1">
       <calculatedColumnFormula>IFERROR(VLOOKUP(C2, Recipes!$A$2:$C$1000, 2, FALSE), "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Cost" dataDxfId="2">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Cost" dataDxfId="0">
       <calculatedColumnFormula>IFERROR(VLOOKUP(C2, Recipes!$A$2:$C$1000, 3, FALSE), "")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -765,17 +769,17 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{06E1EBF5-7EB8-F845-A946-ABCBE0D03A8F}" name="Table13" displayName="Table13" ref="G1:L43" totalsRowShown="0" headerRowDxfId="6">
-  <autoFilter ref="G1:L43" xr:uid="{06E1EBF5-7EB8-F845-A946-ABCBE0D03A8F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{06E1EBF5-7EB8-F845-A946-ABCBE0D03A8F}" name="Table13" displayName="Table13" ref="G1:L45" totalsRowShown="0" headerRowDxfId="7">
+  <autoFilter ref="G1:L45" xr:uid="{06E1EBF5-7EB8-F845-A946-ABCBE0D03A8F}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{306D6AD0-64AE-3343-8DB9-BD5DE32F72CB}" name="Week"/>
     <tableColumn id="2" xr3:uid="{844E6CC4-4122-B843-82BC-5EC1EDB17702}" name="Day"/>
     <tableColumn id="3" xr3:uid="{DF154DD6-1E1E-4443-B749-826CEB950EC4}" name="Meal"/>
-    <tableColumn id="4" xr3:uid="{12E8841E-70B3-A34D-B938-AADCC6B67F37}" name="Meal Name" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{01D1ABEC-7C45-C14D-BF14-EF859C0632CA}" name="Calories" dataDxfId="1">
+    <tableColumn id="4" xr3:uid="{12E8841E-70B3-A34D-B938-AADCC6B67F37}" name="Meal Name" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{01D1ABEC-7C45-C14D-BF14-EF859C0632CA}" name="Calories" dataDxfId="5">
       <calculatedColumnFormula>IFERROR(VLOOKUP(J2, Recipes!$A$2:$C$1000, 2, FALSE), "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{06F1FAD0-750A-0546-9EFC-4B07C20142E6}" name="Cost" dataDxfId="0">
+    <tableColumn id="6" xr3:uid="{06F1FAD0-750A-0546-9EFC-4B07C20142E6}" name="Cost" dataDxfId="4">
       <calculatedColumnFormula>IFERROR(VLOOKUP(J2, Recipes!$A$2:$C$1000, 3, FALSE), "")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1100,11 +1104,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L43"/>
+  <dimension ref="A1:L45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L3" sqref="L3"/>
+      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M45" sqref="M45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1712,43 +1716,37 @@
     </row>
     <row r="23" spans="1:12" ht="30" customHeight="1">
       <c r="A23" t="s">
+        <v>174</v>
+      </c>
+      <c r="E23" s="7" t="str">
+        <f>IFERROR(VLOOKUP(C23, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="F23" s="7" t="str">
+        <f>IFERROR(VLOOKUP(C23, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="G23" t="s">
+        <v>174</v>
+      </c>
+      <c r="K23" s="7" t="str">
+        <f>IFERROR(VLOOKUP(J23, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="L23" s="7" t="str">
+        <f>IFERROR(VLOOKUP(J23, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="30" customHeight="1">
+      <c r="A24" t="s">
         <v>9</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B24" t="s">
         <v>1</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C24" t="s">
         <v>173</v>
-      </c>
-      <c r="E23" t="str">
-        <f>IFERROR(VLOOKUP(C23, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
-        <v/>
-      </c>
-      <c r="F23" t="str">
-        <f>IFERROR(VLOOKUP(C23, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
-        <v/>
-      </c>
-      <c r="G23" t="s">
-        <v>11</v>
-      </c>
-      <c r="H23" t="s">
-        <v>1</v>
-      </c>
-      <c r="I23" t="s">
-        <v>173</v>
-      </c>
-      <c r="K23" t="str">
-        <f>IFERROR(VLOOKUP(J23, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
-        <v/>
-      </c>
-      <c r="L23" t="str">
-        <f>IFERROR(VLOOKUP(J23, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="24" spans="1:12" ht="30" customHeight="1">
-      <c r="C24" t="s">
-        <v>17</v>
       </c>
       <c r="E24" t="str">
         <f>IFERROR(VLOOKUP(C24, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
@@ -1758,8 +1756,14 @@
         <f>IFERROR(VLOOKUP(C24, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
         <v/>
       </c>
+      <c r="G24" t="s">
+        <v>11</v>
+      </c>
+      <c r="H24" t="s">
+        <v>1</v>
+      </c>
       <c r="I24" t="s">
-        <v>17</v>
+        <v>173</v>
       </c>
       <c r="K24" t="str">
         <f>IFERROR(VLOOKUP(J24, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
@@ -1772,7 +1776,7 @@
     </row>
     <row r="25" spans="1:12" ht="30" customHeight="1">
       <c r="C25" t="s">
-        <v>93</v>
+        <v>17</v>
       </c>
       <c r="E25" t="str">
         <f>IFERROR(VLOOKUP(C25, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
@@ -1783,7 +1787,7 @@
         <v/>
       </c>
       <c r="I25" t="s">
-        <v>93</v>
+        <v>17</v>
       </c>
       <c r="K25" t="str">
         <f>IFERROR(VLOOKUP(J25, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
@@ -1795,11 +1799,8 @@
       </c>
     </row>
     <row r="26" spans="1:12" ht="30" customHeight="1">
-      <c r="B26" t="s">
-        <v>2</v>
-      </c>
       <c r="C26" t="s">
-        <v>173</v>
+        <v>93</v>
       </c>
       <c r="E26" t="str">
         <f>IFERROR(VLOOKUP(C26, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
@@ -1809,11 +1810,8 @@
         <f>IFERROR(VLOOKUP(C26, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
         <v/>
       </c>
-      <c r="H26" t="s">
-        <v>2</v>
-      </c>
       <c r="I26" t="s">
-        <v>173</v>
+        <v>93</v>
       </c>
       <c r="K26" t="str">
         <f>IFERROR(VLOOKUP(J26, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
@@ -1825,8 +1823,11 @@
       </c>
     </row>
     <row r="27" spans="1:12" ht="30" customHeight="1">
+      <c r="B27" t="s">
+        <v>2</v>
+      </c>
       <c r="C27" t="s">
-        <v>17</v>
+        <v>173</v>
       </c>
       <c r="E27" t="str">
         <f>IFERROR(VLOOKUP(C27, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
@@ -1836,8 +1837,11 @@
         <f>IFERROR(VLOOKUP(C27, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
         <v/>
       </c>
+      <c r="H27" t="s">
+        <v>2</v>
+      </c>
       <c r="I27" t="s">
-        <v>17</v>
+        <v>173</v>
       </c>
       <c r="K27" t="str">
         <f>IFERROR(VLOOKUP(J27, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
@@ -1850,7 +1854,7 @@
     </row>
     <row r="28" spans="1:12" ht="30" customHeight="1">
       <c r="C28" t="s">
-        <v>93</v>
+        <v>17</v>
       </c>
       <c r="E28" t="str">
         <f>IFERROR(VLOOKUP(C28, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
@@ -1861,7 +1865,7 @@
         <v/>
       </c>
       <c r="I28" t="s">
-        <v>93</v>
+        <v>17</v>
       </c>
       <c r="K28" t="str">
         <f>IFERROR(VLOOKUP(J28, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
@@ -1873,11 +1877,8 @@
       </c>
     </row>
     <row r="29" spans="1:12" ht="30" customHeight="1">
-      <c r="B29" t="s">
-        <v>3</v>
-      </c>
       <c r="C29" t="s">
-        <v>173</v>
+        <v>93</v>
       </c>
       <c r="E29" t="str">
         <f>IFERROR(VLOOKUP(C29, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
@@ -1887,11 +1888,8 @@
         <f>IFERROR(VLOOKUP(C29, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
         <v/>
       </c>
-      <c r="H29" t="s">
-        <v>3</v>
-      </c>
       <c r="I29" t="s">
-        <v>173</v>
+        <v>93</v>
       </c>
       <c r="K29" t="str">
         <f>IFERROR(VLOOKUP(J29, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
@@ -1903,8 +1901,11 @@
       </c>
     </row>
     <row r="30" spans="1:12" ht="30" customHeight="1">
+      <c r="B30" t="s">
+        <v>3</v>
+      </c>
       <c r="C30" t="s">
-        <v>17</v>
+        <v>173</v>
       </c>
       <c r="E30" t="str">
         <f>IFERROR(VLOOKUP(C30, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
@@ -1914,8 +1915,11 @@
         <f>IFERROR(VLOOKUP(C30, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
         <v/>
       </c>
+      <c r="H30" t="s">
+        <v>3</v>
+      </c>
       <c r="I30" t="s">
-        <v>17</v>
+        <v>173</v>
       </c>
       <c r="K30" t="str">
         <f>IFERROR(VLOOKUP(J30, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
@@ -1928,7 +1932,7 @@
     </row>
     <row r="31" spans="1:12" ht="30" customHeight="1">
       <c r="C31" t="s">
-        <v>93</v>
+        <v>17</v>
       </c>
       <c r="E31" t="str">
         <f>IFERROR(VLOOKUP(C31, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
@@ -1939,7 +1943,7 @@
         <v/>
       </c>
       <c r="I31" t="s">
-        <v>93</v>
+        <v>17</v>
       </c>
       <c r="K31" t="str">
         <f>IFERROR(VLOOKUP(J31, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
@@ -1951,11 +1955,8 @@
       </c>
     </row>
     <row r="32" spans="1:12" ht="30" customHeight="1">
-      <c r="B32" t="s">
-        <v>4</v>
-      </c>
       <c r="C32" t="s">
-        <v>173</v>
+        <v>93</v>
       </c>
       <c r="E32" t="str">
         <f>IFERROR(VLOOKUP(C32, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
@@ -1965,11 +1966,8 @@
         <f>IFERROR(VLOOKUP(C32, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
         <v/>
       </c>
-      <c r="H32" t="s">
-        <v>4</v>
-      </c>
       <c r="I32" t="s">
-        <v>173</v>
+        <v>93</v>
       </c>
       <c r="K32" t="str">
         <f>IFERROR(VLOOKUP(J32, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
@@ -1980,9 +1978,12 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="2:12" ht="30" customHeight="1">
+    <row r="33" spans="1:12" ht="30" customHeight="1">
+      <c r="B33" t="s">
+        <v>4</v>
+      </c>
       <c r="C33" t="s">
-        <v>17</v>
+        <v>173</v>
       </c>
       <c r="E33" t="str">
         <f>IFERROR(VLOOKUP(C33, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
@@ -1992,8 +1993,11 @@
         <f>IFERROR(VLOOKUP(C33, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
         <v/>
       </c>
+      <c r="H33" t="s">
+        <v>4</v>
+      </c>
       <c r="I33" t="s">
-        <v>17</v>
+        <v>173</v>
       </c>
       <c r="K33" t="str">
         <f>IFERROR(VLOOKUP(J33, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
@@ -2004,9 +2008,9 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="2:12" ht="30" customHeight="1">
+    <row r="34" spans="1:12" ht="30" customHeight="1">
       <c r="C34" t="s">
-        <v>93</v>
+        <v>17</v>
       </c>
       <c r="E34" t="str">
         <f>IFERROR(VLOOKUP(C34, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
@@ -2017,7 +2021,7 @@
         <v/>
       </c>
       <c r="I34" t="s">
-        <v>93</v>
+        <v>17</v>
       </c>
       <c r="K34" t="str">
         <f>IFERROR(VLOOKUP(J34, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
@@ -2028,12 +2032,9 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="2:12" ht="30" customHeight="1">
-      <c r="B35" t="s">
-        <v>5</v>
-      </c>
+    <row r="35" spans="1:12" ht="30" customHeight="1">
       <c r="C35" t="s">
-        <v>173</v>
+        <v>93</v>
       </c>
       <c r="E35" t="str">
         <f>IFERROR(VLOOKUP(C35, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
@@ -2043,11 +2044,8 @@
         <f>IFERROR(VLOOKUP(C35, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
         <v/>
       </c>
-      <c r="H35" t="s">
-        <v>5</v>
-      </c>
       <c r="I35" t="s">
-        <v>173</v>
+        <v>93</v>
       </c>
       <c r="K35" t="str">
         <f>IFERROR(VLOOKUP(J35, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
@@ -2058,9 +2056,12 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="2:12" ht="30" customHeight="1">
+    <row r="36" spans="1:12" ht="30" customHeight="1">
+      <c r="B36" t="s">
+        <v>5</v>
+      </c>
       <c r="C36" t="s">
-        <v>17</v>
+        <v>173</v>
       </c>
       <c r="E36" t="str">
         <f>IFERROR(VLOOKUP(C36, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
@@ -2070,8 +2071,11 @@
         <f>IFERROR(VLOOKUP(C36, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
         <v/>
       </c>
+      <c r="H36" t="s">
+        <v>5</v>
+      </c>
       <c r="I36" t="s">
-        <v>17</v>
+        <v>173</v>
       </c>
       <c r="K36" t="str">
         <f>IFERROR(VLOOKUP(J36, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
@@ -2082,9 +2086,9 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="2:12" ht="30" customHeight="1">
+    <row r="37" spans="1:12" ht="30" customHeight="1">
       <c r="C37" t="s">
-        <v>93</v>
+        <v>17</v>
       </c>
       <c r="E37" t="str">
         <f>IFERROR(VLOOKUP(C37, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
@@ -2095,7 +2099,7 @@
         <v/>
       </c>
       <c r="I37" t="s">
-        <v>93</v>
+        <v>17</v>
       </c>
       <c r="K37" t="str">
         <f>IFERROR(VLOOKUP(J37, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
@@ -2106,12 +2110,9 @@
         <v/>
       </c>
     </row>
-    <row r="38" spans="2:12" ht="30" customHeight="1">
-      <c r="B38" t="s">
-        <v>6</v>
-      </c>
+    <row r="38" spans="1:12" ht="30" customHeight="1">
       <c r="C38" t="s">
-        <v>173</v>
+        <v>93</v>
       </c>
       <c r="E38" t="str">
         <f>IFERROR(VLOOKUP(C38, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
@@ -2121,11 +2122,8 @@
         <f>IFERROR(VLOOKUP(C38, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
         <v/>
       </c>
-      <c r="H38" t="s">
-        <v>6</v>
-      </c>
       <c r="I38" t="s">
-        <v>173</v>
+        <v>93</v>
       </c>
       <c r="K38" t="str">
         <f>IFERROR(VLOOKUP(J38, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
@@ -2136,9 +2134,12 @@
         <v/>
       </c>
     </row>
-    <row r="39" spans="2:12" ht="30" customHeight="1">
+    <row r="39" spans="1:12" ht="30" customHeight="1">
+      <c r="B39" t="s">
+        <v>6</v>
+      </c>
       <c r="C39" t="s">
-        <v>17</v>
+        <v>173</v>
       </c>
       <c r="E39" t="str">
         <f>IFERROR(VLOOKUP(C39, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
@@ -2148,8 +2149,11 @@
         <f>IFERROR(VLOOKUP(C39, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
         <v/>
       </c>
+      <c r="H39" t="s">
+        <v>6</v>
+      </c>
       <c r="I39" t="s">
-        <v>17</v>
+        <v>173</v>
       </c>
       <c r="K39" t="str">
         <f>IFERROR(VLOOKUP(J39, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
@@ -2160,9 +2164,9 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="2:12" ht="30" customHeight="1">
+    <row r="40" spans="1:12" ht="30" customHeight="1">
       <c r="C40" t="s">
-        <v>93</v>
+        <v>17</v>
       </c>
       <c r="E40" t="str">
         <f>IFERROR(VLOOKUP(C40, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
@@ -2173,7 +2177,7 @@
         <v/>
       </c>
       <c r="I40" t="s">
-        <v>93</v>
+        <v>17</v>
       </c>
       <c r="K40" t="str">
         <f>IFERROR(VLOOKUP(J40, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
@@ -2184,12 +2188,9 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="2:12" ht="30" customHeight="1">
-      <c r="B41" t="s">
-        <v>7</v>
-      </c>
+    <row r="41" spans="1:12" ht="30" customHeight="1">
       <c r="C41" t="s">
-        <v>173</v>
+        <v>93</v>
       </c>
       <c r="E41" t="str">
         <f>IFERROR(VLOOKUP(C41, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
@@ -2199,11 +2200,8 @@
         <f>IFERROR(VLOOKUP(C41, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
         <v/>
       </c>
-      <c r="H41" t="s">
-        <v>7</v>
-      </c>
       <c r="I41" t="s">
-        <v>173</v>
+        <v>93</v>
       </c>
       <c r="K41" t="str">
         <f>IFERROR(VLOOKUP(J41, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
@@ -2214,9 +2212,12 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="2:12" ht="30" customHeight="1">
+    <row r="42" spans="1:12" ht="30" customHeight="1">
+      <c r="B42" t="s">
+        <v>7</v>
+      </c>
       <c r="C42" t="s">
-        <v>17</v>
+        <v>173</v>
       </c>
       <c r="E42" t="str">
         <f>IFERROR(VLOOKUP(C42, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
@@ -2226,8 +2227,11 @@
         <f>IFERROR(VLOOKUP(C42, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
         <v/>
       </c>
+      <c r="H42" t="s">
+        <v>7</v>
+      </c>
       <c r="I42" t="s">
-        <v>17</v>
+        <v>173</v>
       </c>
       <c r="K42" t="str">
         <f>IFERROR(VLOOKUP(J42, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
@@ -2238,9 +2242,9 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="2:12" ht="30" customHeight="1">
+    <row r="43" spans="1:12" ht="30" customHeight="1">
       <c r="C43" t="s">
-        <v>93</v>
+        <v>17</v>
       </c>
       <c r="E43" t="str">
         <f>IFERROR(VLOOKUP(C43, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
@@ -2251,7 +2255,7 @@
         <v/>
       </c>
       <c r="I43" t="s">
-        <v>93</v>
+        <v>17</v>
       </c>
       <c r="K43" t="str">
         <f>IFERROR(VLOOKUP(J43, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
@@ -2259,13 +2263,61 @@
       </c>
       <c r="L43" t="str">
         <f>IFERROR(VLOOKUP(J43, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="44" spans="1:12" ht="30" customHeight="1">
+      <c r="C44" t="s">
+        <v>93</v>
+      </c>
+      <c r="E44" t="str">
+        <f>IFERROR(VLOOKUP(C44, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="F44" t="str">
+        <f>IFERROR(VLOOKUP(C44, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="I44" t="s">
+        <v>93</v>
+      </c>
+      <c r="K44" t="str">
+        <f>IFERROR(VLOOKUP(J44, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="L44" t="str">
+        <f>IFERROR(VLOOKUP(J44, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="45" spans="1:12" ht="30" customHeight="1">
+      <c r="A45" t="s">
+        <v>174</v>
+      </c>
+      <c r="E45" s="7" t="str">
+        <f>IFERROR(VLOOKUP(C45, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="F45" s="7" t="str">
+        <f>IFERROR(VLOOKUP(C45, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="G45" t="s">
+        <v>174</v>
+      </c>
+      <c r="K45" s="7" t="str">
+        <f>IFERROR(VLOOKUP(J45, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="L45" s="7" t="str">
+        <f>IFERROR(VLOOKUP(J45, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
         <v/>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D43 J2:J43" xr:uid="{317D4B3D-4DBF-2749-B892-0E6482D4EC8A}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D45 J2:J45" xr:uid="{317D4B3D-4DBF-2749-B892-0E6482D4EC8A}">
       <formula1>RecipeList</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
wb: totals added and formula-ed for cost and calories
</commit_message>
<xml_diff>
--- a/MealPrepTracker.xlsx
+++ b/MealPrepTracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/quinnreams/Documents/GitHub/Personal-Growth-Planner/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2FDE25C-CF74-7D4D-BF10-9F3391891A53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A38F931-92F9-CC40-A9BC-8DA4F8D4A2D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="160" yWindow="660" windowWidth="38080" windowHeight="19260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -561,7 +561,7 @@
     <t>Breakfast</t>
   </si>
   <si>
-    <t>Totals</t>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -1108,7 +1108,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M45" sqref="M45"/>
+      <selection pane="bottomLeft" activeCell="L46" sqref="L46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1715,27 +1715,27 @@
       </c>
     </row>
     <row r="23" spans="1:12" ht="30" customHeight="1">
-      <c r="A23" t="s">
+      <c r="B23" t="s">
         <v>174</v>
       </c>
-      <c r="E23" s="7" t="str">
-        <f>IFERROR(VLOOKUP(C23, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
-        <v/>
-      </c>
-      <c r="F23" s="7" t="str">
-        <f>IFERROR(VLOOKUP(C23, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
-        <v/>
-      </c>
-      <c r="G23" t="s">
+      <c r="E23" s="7">
+        <f>SUM(E2:E22)</f>
+        <v>0</v>
+      </c>
+      <c r="F23" s="7">
+        <f>SUM(F2:F22)</f>
+        <v>0</v>
+      </c>
+      <c r="H23" t="s">
         <v>174</v>
       </c>
-      <c r="K23" s="7" t="str">
-        <f>IFERROR(VLOOKUP(J23, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
-        <v/>
-      </c>
-      <c r="L23" s="7" t="str">
-        <f>IFERROR(VLOOKUP(J23, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
-        <v/>
+      <c r="K23" s="7">
+        <f>SUM(K2:K22)</f>
+        <v>0</v>
+      </c>
+      <c r="L23" s="7">
+        <f>SUM(L2:L22)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="30" customHeight="1">
@@ -1978,7 +1978,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="30" customHeight="1">
+    <row r="33" spans="2:12" ht="30" customHeight="1">
       <c r="B33" t="s">
         <v>4</v>
       </c>
@@ -2008,7 +2008,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:12" ht="30" customHeight="1">
+    <row r="34" spans="2:12" ht="30" customHeight="1">
       <c r="C34" t="s">
         <v>17</v>
       </c>
@@ -2032,7 +2032,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:12" ht="30" customHeight="1">
+    <row r="35" spans="2:12" ht="30" customHeight="1">
       <c r="C35" t="s">
         <v>93</v>
       </c>
@@ -2056,7 +2056,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="30" customHeight="1">
+    <row r="36" spans="2:12" ht="30" customHeight="1">
       <c r="B36" t="s">
         <v>5</v>
       </c>
@@ -2086,7 +2086,7 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="1:12" ht="30" customHeight="1">
+    <row r="37" spans="2:12" ht="30" customHeight="1">
       <c r="C37" t="s">
         <v>17</v>
       </c>
@@ -2110,7 +2110,7 @@
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="30" customHeight="1">
+    <row r="38" spans="2:12" ht="30" customHeight="1">
       <c r="C38" t="s">
         <v>93</v>
       </c>
@@ -2134,7 +2134,7 @@
         <v/>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="30" customHeight="1">
+    <row r="39" spans="2:12" ht="30" customHeight="1">
       <c r="B39" t="s">
         <v>6</v>
       </c>
@@ -2164,7 +2164,7 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:12" ht="30" customHeight="1">
+    <row r="40" spans="2:12" ht="30" customHeight="1">
       <c r="C40" t="s">
         <v>17</v>
       </c>
@@ -2188,7 +2188,7 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:12" ht="30" customHeight="1">
+    <row r="41" spans="2:12" ht="30" customHeight="1">
       <c r="C41" t="s">
         <v>93</v>
       </c>
@@ -2212,7 +2212,7 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="1:12" ht="30" customHeight="1">
+    <row r="42" spans="2:12" ht="30" customHeight="1">
       <c r="B42" t="s">
         <v>7</v>
       </c>
@@ -2242,7 +2242,7 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:12" ht="30" customHeight="1">
+    <row r="43" spans="2:12" ht="30" customHeight="1">
       <c r="C43" t="s">
         <v>17</v>
       </c>
@@ -2266,7 +2266,7 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:12" ht="30" customHeight="1">
+    <row r="44" spans="2:12" ht="30" customHeight="1">
       <c r="C44" t="s">
         <v>93</v>
       </c>
@@ -2290,28 +2290,28 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:12" ht="30" customHeight="1">
-      <c r="A45" t="s">
+    <row r="45" spans="2:12" ht="30" customHeight="1">
+      <c r="B45" t="s">
         <v>174</v>
       </c>
-      <c r="E45" s="7" t="str">
-        <f>IFERROR(VLOOKUP(C45, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
-        <v/>
-      </c>
-      <c r="F45" s="7" t="str">
-        <f>IFERROR(VLOOKUP(C45, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
-        <v/>
-      </c>
-      <c r="G45" t="s">
+      <c r="E45" s="7">
+        <f>SUM(E24:E44)</f>
+        <v>0</v>
+      </c>
+      <c r="F45" s="7">
+        <f>SUM(F24:F44)</f>
+        <v>0</v>
+      </c>
+      <c r="H45" t="s">
         <v>174</v>
       </c>
-      <c r="K45" s="7" t="str">
-        <f>IFERROR(VLOOKUP(J45, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
-        <v/>
-      </c>
-      <c r="L45" s="7" t="str">
-        <f>IFERROR(VLOOKUP(J45, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
-        <v/>
+      <c r="K45" s="7">
+        <f>SUM(K24:K44)</f>
+        <v>0</v>
+      </c>
+      <c r="L45" s="7">
+        <f>SUM(L24:L44)</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
WB: conditioning format rule for my personal goal limits
</commit_message>
<xml_diff>
--- a/MealPrepTracker.xlsx
+++ b/MealPrepTracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/quinnreams/Documents/GitHub/Personal-Growth-Planner/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A38F931-92F9-CC40-A9BC-8DA4F8D4A2D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C5DFB77-376B-F144-A6D6-91F353EAAB8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="160" yWindow="660" windowWidth="38080" windowHeight="19260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -667,7 +667,347 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="42">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -723,16 +1063,6 @@
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -750,17 +1080,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:F45" totalsRowShown="0" headerRowDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:F45" totalsRowShown="0" headerRowDxfId="37">
   <autoFilter ref="A1:F45" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Week"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Day"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Meal"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Meal Name" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Calories" dataDxfId="1">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Meal Name" dataDxfId="36"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Calories" dataDxfId="35">
       <calculatedColumnFormula>IFERROR(VLOOKUP(C2, Recipes!$A$2:$C$1000, 2, FALSE), "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Cost" dataDxfId="0">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Cost" dataDxfId="34">
       <calculatedColumnFormula>IFERROR(VLOOKUP(C2, Recipes!$A$2:$C$1000, 3, FALSE), "")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -769,17 +1099,17 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{06E1EBF5-7EB8-F845-A946-ABCBE0D03A8F}" name="Table13" displayName="Table13" ref="G1:L45" totalsRowShown="0" headerRowDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{06E1EBF5-7EB8-F845-A946-ABCBE0D03A8F}" name="Table13" displayName="Table13" ref="G1:L45" totalsRowShown="0" headerRowDxfId="41">
   <autoFilter ref="G1:L45" xr:uid="{06E1EBF5-7EB8-F845-A946-ABCBE0D03A8F}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{306D6AD0-64AE-3343-8DB9-BD5DE32F72CB}" name="Week"/>
     <tableColumn id="2" xr3:uid="{844E6CC4-4122-B843-82BC-5EC1EDB17702}" name="Day"/>
     <tableColumn id="3" xr3:uid="{DF154DD6-1E1E-4443-B749-826CEB950EC4}" name="Meal"/>
-    <tableColumn id="4" xr3:uid="{12E8841E-70B3-A34D-B938-AADCC6B67F37}" name="Meal Name" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{01D1ABEC-7C45-C14D-BF14-EF859C0632CA}" name="Calories" dataDxfId="5">
+    <tableColumn id="4" xr3:uid="{12E8841E-70B3-A34D-B938-AADCC6B67F37}" name="Meal Name" dataDxfId="40"/>
+    <tableColumn id="5" xr3:uid="{01D1ABEC-7C45-C14D-BF14-EF859C0632CA}" name="Calories" dataDxfId="39">
       <calculatedColumnFormula>IFERROR(VLOOKUP(J2, Recipes!$A$2:$C$1000, 2, FALSE), "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{06F1FAD0-750A-0546-9EFC-4B07C20142E6}" name="Cost" dataDxfId="4">
+    <tableColumn id="6" xr3:uid="{06F1FAD0-750A-0546-9EFC-4B07C20142E6}" name="Cost" dataDxfId="38">
       <calculatedColumnFormula>IFERROR(VLOOKUP(J2, Recipes!$A$2:$C$1000, 3, FALSE), "")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1107,8 +1437,8 @@
   <dimension ref="A1:L45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L46" sqref="L46"/>
+      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L39" sqref="L39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1331,14 +1661,6 @@
       <c r="C8" t="s">
         <v>173</v>
       </c>
-      <c r="E8" t="str">
-        <f>IFERROR(VLOOKUP(C8, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
-        <v/>
-      </c>
-      <c r="F8" t="str">
-        <f>IFERROR(VLOOKUP(C8, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
-        <v/>
-      </c>
       <c r="H8" t="s">
         <v>3</v>
       </c>
@@ -1627,10 +1949,6 @@
       <c r="I19" t="s">
         <v>93</v>
       </c>
-      <c r="K19" t="str">
-        <f>IFERROR(VLOOKUP(J19, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
-        <v/>
-      </c>
       <c r="L19" t="str">
         <f>IFERROR(VLOOKUP(J19, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
         <v/>
@@ -1657,10 +1975,6 @@
       <c r="I20" t="s">
         <v>173</v>
       </c>
-      <c r="K20" t="str">
-        <f>IFERROR(VLOOKUP(J20, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
-        <v/>
-      </c>
       <c r="L20" t="str">
         <f>IFERROR(VLOOKUP(J20, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
         <v/>
@@ -1670,10 +1984,6 @@
       <c r="C21" t="s">
         <v>17</v>
       </c>
-      <c r="E21" t="str">
-        <f>IFERROR(VLOOKUP(C21, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
-        <v/>
-      </c>
       <c r="F21" t="str">
         <f>IFERROR(VLOOKUP(C21, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
         <v/>
@@ -1693,10 +2003,6 @@
     <row r="22" spans="1:12" ht="30" customHeight="1">
       <c r="C22" t="s">
         <v>93</v>
-      </c>
-      <c r="E22" t="str">
-        <f>IFERROR(VLOOKUP(C22, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
-        <v/>
       </c>
       <c r="F22" t="str">
         <f>IFERROR(VLOOKUP(C22, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
@@ -2155,14 +2461,6 @@
       <c r="I39" t="s">
         <v>173</v>
       </c>
-      <c r="K39" t="str">
-        <f>IFERROR(VLOOKUP(J39, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
-        <v/>
-      </c>
-      <c r="L39" t="str">
-        <f>IFERROR(VLOOKUP(J39, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
-        <v/>
-      </c>
     </row>
     <row r="40" spans="2:12" ht="30" customHeight="1">
       <c r="C40" t="s">
@@ -2191,10 +2489,6 @@
     <row r="41" spans="2:12" ht="30" customHeight="1">
       <c r="C41" t="s">
         <v>93</v>
-      </c>
-      <c r="E41" t="str">
-        <f>IFERROR(VLOOKUP(C41, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
-        <v/>
       </c>
       <c r="F41" t="str">
         <f>IFERROR(VLOOKUP(C41, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
@@ -2316,6 +2610,46 @@
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
+  <conditionalFormatting sqref="E23">
+    <cfRule type="cellIs" dxfId="15" priority="8" operator="greaterThan">
+      <formula>14000</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F23">
+    <cfRule type="cellIs" dxfId="14" priority="7" operator="greaterThan">
+      <formula>100</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K23">
+    <cfRule type="cellIs" dxfId="8" priority="6" stopIfTrue="1" operator="greaterThan">
+      <formula>14000</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L23">
+    <cfRule type="cellIs" dxfId="13" priority="5" operator="greaterThan">
+      <formula>100</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E45">
+    <cfRule type="cellIs" dxfId="12" priority="4" stopIfTrue="1" operator="greaterThan">
+      <formula>14000</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F45">
+    <cfRule type="cellIs" dxfId="11" priority="3" operator="greaterThan">
+      <formula>100</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K45">
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="greaterThan">
+      <formula>14000</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L45">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="greaterThan">
+      <formula>100</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D45 J2:J45" xr:uid="{317D4B3D-4DBF-2749-B892-0E6482D4EC8A}">
       <formula1>RecipeList</formula1>

</xml_diff>

<commit_message>
fix: cleaning script up after debugging
</commit_message>
<xml_diff>
--- a/MealPrepTracker.xlsx
+++ b/MealPrepTracker.xlsx
@@ -2192,7 +2192,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2240,7 +2240,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Lunch</t>
+          <t>Dinner</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -2258,11 +2258,7 @@
           <t>additional toppings: diced avocado, micro greens, chopped basil), 3 medium carrots, peeled and diced, 3 celery stalks, diced, 2 cups fully-cooked chicken breast, shredded (may be omitted for a vegetarian version), ½ cup flat leaf Italian parsley, chopped (plus extra for garnish), 6 cloves of garlic, finely minced, 2 tablespoons olive oil, 28 ounce-can plum tomatoes, drained and rinsed, chopped, 2 cups dried red lentils, rinsed, salt and black pepper, to taste, 1 large turnip, peeled and diced, 8 cups vegetable stock, 1 medium yellow onion, diced</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="F2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -2272,7 +2268,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Lunch</t>
+          <t>Dinner</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -2290,11 +2286,127 @@
           <t>1 14.5oz can of Beef Broth, 2 large carrots, chopped, 2 stalks celery, chopped, 1 26oz can Cream of Mushroom Soup, 3 green onions, chopped, 10 new (red)potatoes, 1 small onion chopped, ½ cup Dale's Seasoning, 2 pounds stew meat, 2 cups water</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="F3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Asparagus and Pea Soup: Real Convenience Food</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Breakfastr</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>https://spoonacular.com/recipes/716406</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>1 bag of frozen organic asparagus (preferably thawed), 1T EVOO (extra virgin olive oil), a couple of garlic cloves, 1/2 onion, 2-3c of frozen organic peas, 1 box low-sodium vegetable broth</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Garlicky Kale</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Breakfastr</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>https://spoonacular.com/recipes/644387</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>3 tablespoons balsamic vinegar, 1 clove garlic, minced, 1 bunch curly kale, stems removed and chopped, Olive oil</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Powerhouse Almond Matcha Superfood Smoothie</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Breakfast</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>https://spoonacular.com/recipes/756814</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>2 tablespoons unsalted natural almond butter, 1 1/2 cups unsweetened almond milk, 1 medium frozen banana, 2 teaspoons chia seeds, 1 cup baby kale, packed, 1/2 cup frozen mango pieces, 1 tablespoon matcha green tea powder, 3/4 cup frozen pineapple, 1/2 teaspoon vanilla extract</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Butternut Squash Frittata</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Breakfast</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>https://spoonacular.com/recipes/636589</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>1 large butternut squash, peeled, seeded, thinly sliced (with a mandoline), 1/2 oz goat cheese, 1/2 cup liquid egg substitute, 2 tbsp. non-fat milk, Pepper to taste</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Doughnuts</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Breakfast</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>https://spoonacular.com/recipes/716276</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>1.5 cups of flour, 30 ml honey, 1 tablespoon of powdered milk, 1/2 teaspoon salt, 150 ml warm water, 1 teaspoon yeast</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
feat: script updated for edamam instead
</commit_message>
<xml_diff>
--- a/MealPrepTracker.xlsx
+++ b/MealPrepTracker.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Recipes" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="RecipeList">OFFSET(Recipes!$A$2, 0, 0, COUNTA(Recipes!$A$2:$A$1000), 1)</definedName>
+    <definedName name="RecipeList">OFFSET(#REF!, 0, 0, COUNTA(#REF!), 1)</definedName>
   </definedNames>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
 </workbook>
@@ -19,7 +19,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <name val="Aptos Narrow"/>
       <family val="2"/>
@@ -47,11 +47,6 @@
       <sz val="16"/>
     </font>
     <font>
-      <name val="Aptos Narrow"/>
-      <b val="1"/>
-      <sz val="12"/>
-    </font>
-    <font>
       <b val="1"/>
     </font>
   </fonts>
@@ -69,27 +64,12 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -102,7 +82,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -114,9 +94,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -344,10 +321,10 @@
     <tableColumn id="3" name="Meal"/>
     <tableColumn id="4" name="Meal Name" dataDxfId="14"/>
     <tableColumn id="5" name="Calories" dataDxfId="13">
-      <calculatedColumnFormula>IFERROR(VLOOKUP(C2, Recipes!$A$2:$C$1000, 2, FALSE), "")</calculatedColumnFormula>
+      <calculatedColumnFormula>IFERROR(VLOOKUP(C2,#REF!, 2, FALSE), "")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" name="Cost" dataDxfId="12">
-      <calculatedColumnFormula>IFERROR(VLOOKUP(C2, Recipes!$A$2:$C$1000, 3, FALSE), "")</calculatedColumnFormula>
+      <calculatedColumnFormula>IFERROR(VLOOKUP(C2,#REF!, 3, FALSE), "")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -363,10 +340,10 @@
     <tableColumn id="3" name="Meal"/>
     <tableColumn id="4" name="Meal Name" dataDxfId="10"/>
     <tableColumn id="5" name="Calories" dataDxfId="9">
-      <calculatedColumnFormula>IFERROR(VLOOKUP(J2, Recipes!$A$2:$C$1000, 2, FALSE), "")</calculatedColumnFormula>
+      <calculatedColumnFormula>IFERROR(VLOOKUP(J2,#REF!, 2, FALSE), "")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" name="Cost" dataDxfId="8">
-      <calculatedColumnFormula>IFERROR(VLOOKUP(J2, Recipes!$A$2:$C$1000, 3, FALSE), "")</calculatedColumnFormula>
+      <calculatedColumnFormula>IFERROR(VLOOKUP(J2,#REF!, 3, FALSE), "")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -793,11 +770,11 @@
         </is>
       </c>
       <c r="E2" s="4">
-        <f>IFERROR(VLOOKUP(C2, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(C2,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
       <c r="F2" s="5">
-        <f>IFERROR(VLOOKUP(C2, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(C2,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
       <c r="G2" t="inlineStr">
@@ -816,11 +793,11 @@
         </is>
       </c>
       <c r="K2" s="5">
-        <f>IFERROR(VLOOKUP(J2, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(J2,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
       <c r="L2" s="5">
-        <f>IFERROR(VLOOKUP(J2, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(J2,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
     </row>
@@ -831,11 +808,11 @@
         </is>
       </c>
       <c r="E3">
-        <f>IFERROR(VLOOKUP(C3, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(C3,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
       <c r="F3">
-        <f>IFERROR(VLOOKUP(C3, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(C3,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
       <c r="I3" t="inlineStr">
@@ -844,11 +821,11 @@
         </is>
       </c>
       <c r="K3">
-        <f>IFERROR(VLOOKUP(J3, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(J3,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
       <c r="L3">
-        <f>IFERROR(VLOOKUP(J3, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(J3,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
     </row>
@@ -859,11 +836,11 @@
         </is>
       </c>
       <c r="E4">
-        <f>IFERROR(VLOOKUP(C4, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(C4,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
       <c r="F4">
-        <f>IFERROR(VLOOKUP(C4, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(C4,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
       <c r="I4" t="inlineStr">
@@ -872,11 +849,11 @@
         </is>
       </c>
       <c r="K4">
-        <f>IFERROR(VLOOKUP(J4, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(J4,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
       <c r="L4">
-        <f>IFERROR(VLOOKUP(J4, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(J4,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
     </row>
@@ -892,11 +869,11 @@
         </is>
       </c>
       <c r="E5">
-        <f>IFERROR(VLOOKUP(C5, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(C5,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
       <c r="F5">
-        <f>IFERROR(VLOOKUP(C5, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(C5,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
       <c r="H5" t="inlineStr">
@@ -910,11 +887,11 @@
         </is>
       </c>
       <c r="K5">
-        <f>IFERROR(VLOOKUP(J5, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(J5,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
       <c r="L5">
-        <f>IFERROR(VLOOKUP(J5, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(J5,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
     </row>
@@ -925,11 +902,11 @@
         </is>
       </c>
       <c r="E6">
-        <f>IFERROR(VLOOKUP(C6, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(C6,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
       <c r="F6">
-        <f>IFERROR(VLOOKUP(C6, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(C6,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
       <c r="I6" t="inlineStr">
@@ -938,11 +915,11 @@
         </is>
       </c>
       <c r="K6">
-        <f>IFERROR(VLOOKUP(J6, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(J6,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
       <c r="L6">
-        <f>IFERROR(VLOOKUP(J6, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(J6,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
     </row>
@@ -953,11 +930,11 @@
         </is>
       </c>
       <c r="E7">
-        <f>IFERROR(VLOOKUP(C7, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(C7,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
       <c r="F7">
-        <f>IFERROR(VLOOKUP(C7, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(C7,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
       <c r="I7" t="inlineStr">
@@ -966,11 +943,11 @@
         </is>
       </c>
       <c r="K7">
-        <f>IFERROR(VLOOKUP(J7, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(J7,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
       <c r="L7">
-        <f>IFERROR(VLOOKUP(J7, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(J7,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
     </row>
@@ -996,11 +973,11 @@
         </is>
       </c>
       <c r="K8">
-        <f>IFERROR(VLOOKUP(J8, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(J8,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
       <c r="L8">
-        <f>IFERROR(VLOOKUP(J8, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(J8,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
     </row>
@@ -1011,11 +988,11 @@
         </is>
       </c>
       <c r="E9">
-        <f>IFERROR(VLOOKUP(C9, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(C9,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
       <c r="F9">
-        <f>IFERROR(VLOOKUP(C9, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(C9,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
       <c r="I9" t="inlineStr">
@@ -1024,11 +1001,11 @@
         </is>
       </c>
       <c r="K9">
-        <f>IFERROR(VLOOKUP(J9, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(J9,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
       <c r="L9">
-        <f>IFERROR(VLOOKUP(J9, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(J9,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
     </row>
@@ -1039,11 +1016,11 @@
         </is>
       </c>
       <c r="E10">
-        <f>IFERROR(VLOOKUP(C10, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(C10,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
       <c r="F10">
-        <f>IFERROR(VLOOKUP(C10, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(C10,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
       <c r="I10" t="inlineStr">
@@ -1052,11 +1029,11 @@
         </is>
       </c>
       <c r="K10">
-        <f>IFERROR(VLOOKUP(J10, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(J10,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
       <c r="L10">
-        <f>IFERROR(VLOOKUP(J10, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(J10,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
     </row>
@@ -1072,11 +1049,11 @@
         </is>
       </c>
       <c r="E11">
-        <f>IFERROR(VLOOKUP(C11, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(C11,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
       <c r="F11">
-        <f>IFERROR(VLOOKUP(C11, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(C11,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
       <c r="H11" t="inlineStr">
@@ -1090,11 +1067,11 @@
         </is>
       </c>
       <c r="K11">
-        <f>IFERROR(VLOOKUP(J11, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(J11,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
       <c r="L11">
-        <f>IFERROR(VLOOKUP(J11, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(J11,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
     </row>
@@ -1105,11 +1082,11 @@
         </is>
       </c>
       <c r="E12">
-        <f>IFERROR(VLOOKUP(C12, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(C12,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
       <c r="F12">
-        <f>IFERROR(VLOOKUP(C12, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(C12,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
       <c r="I12" t="inlineStr">
@@ -1118,11 +1095,11 @@
         </is>
       </c>
       <c r="K12">
-        <f>IFERROR(VLOOKUP(J12, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(J12,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
       <c r="L12">
-        <f>IFERROR(VLOOKUP(J12, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(J12,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
     </row>
@@ -1133,11 +1110,11 @@
         </is>
       </c>
       <c r="E13">
-        <f>IFERROR(VLOOKUP(C13, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(C13,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
       <c r="F13">
-        <f>IFERROR(VLOOKUP(C13, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(C13,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
       <c r="I13" t="inlineStr">
@@ -1146,11 +1123,11 @@
         </is>
       </c>
       <c r="K13">
-        <f>IFERROR(VLOOKUP(J13, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(J13,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
       <c r="L13">
-        <f>IFERROR(VLOOKUP(J13, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(J13,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
     </row>
@@ -1166,11 +1143,11 @@
         </is>
       </c>
       <c r="E14">
-        <f>IFERROR(VLOOKUP(C14, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(C14,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
       <c r="F14">
-        <f>IFERROR(VLOOKUP(C14, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(C14,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
       <c r="H14" t="inlineStr">
@@ -1184,11 +1161,11 @@
         </is>
       </c>
       <c r="K14">
-        <f>IFERROR(VLOOKUP(J14, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(J14,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
       <c r="L14">
-        <f>IFERROR(VLOOKUP(J14, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(J14,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
     </row>
@@ -1199,11 +1176,11 @@
         </is>
       </c>
       <c r="E15">
-        <f>IFERROR(VLOOKUP(C15, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(C15,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
       <c r="F15">
-        <f>IFERROR(VLOOKUP(C15, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(C15,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
       <c r="I15" t="inlineStr">
@@ -1212,11 +1189,11 @@
         </is>
       </c>
       <c r="K15">
-        <f>IFERROR(VLOOKUP(J15, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(J15,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
       <c r="L15">
-        <f>IFERROR(VLOOKUP(J15, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(J15,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
     </row>
@@ -1227,11 +1204,11 @@
         </is>
       </c>
       <c r="E16">
-        <f>IFERROR(VLOOKUP(C16, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(C16,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
       <c r="F16">
-        <f>IFERROR(VLOOKUP(C16, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(C16,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
       <c r="I16" t="inlineStr">
@@ -1240,11 +1217,11 @@
         </is>
       </c>
       <c r="K16">
-        <f>IFERROR(VLOOKUP(J16, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(J16,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
       <c r="L16">
-        <f>IFERROR(VLOOKUP(J16, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(J16,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
     </row>
@@ -1260,11 +1237,11 @@
         </is>
       </c>
       <c r="E17">
-        <f>IFERROR(VLOOKUP(C17, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(C17,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
       <c r="F17">
-        <f>IFERROR(VLOOKUP(C17, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(C17,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
       <c r="H17" t="inlineStr">
@@ -1278,11 +1255,11 @@
         </is>
       </c>
       <c r="K17">
-        <f>IFERROR(VLOOKUP(J17, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(J17,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
       <c r="L17">
-        <f>IFERROR(VLOOKUP(J17, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(J17,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
     </row>
@@ -1293,11 +1270,11 @@
         </is>
       </c>
       <c r="E18">
-        <f>IFERROR(VLOOKUP(C18, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(C18,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
       <c r="F18">
-        <f>IFERROR(VLOOKUP(C18, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(C18,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
       <c r="I18" t="inlineStr">
@@ -1306,11 +1283,11 @@
         </is>
       </c>
       <c r="K18">
-        <f>IFERROR(VLOOKUP(J18, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(J18,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
       <c r="L18">
-        <f>IFERROR(VLOOKUP(J18, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(J18,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
     </row>
@@ -1321,11 +1298,11 @@
         </is>
       </c>
       <c r="E19">
-        <f>IFERROR(VLOOKUP(C19, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(C19,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
       <c r="F19">
-        <f>IFERROR(VLOOKUP(C19, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(C19,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
       <c r="I19" t="inlineStr">
@@ -1334,7 +1311,7 @@
         </is>
       </c>
       <c r="L19">
-        <f>IFERROR(VLOOKUP(J19, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(J19,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
     </row>
@@ -1350,11 +1327,11 @@
         </is>
       </c>
       <c r="E20">
-        <f>IFERROR(VLOOKUP(C20, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(C20,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
       <c r="F20">
-        <f>IFERROR(VLOOKUP(C20, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(C20,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
       <c r="H20" t="inlineStr">
@@ -1368,7 +1345,7 @@
         </is>
       </c>
       <c r="L20">
-        <f>IFERROR(VLOOKUP(J20, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(J20,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
     </row>
@@ -1379,7 +1356,7 @@
         </is>
       </c>
       <c r="F21">
-        <f>IFERROR(VLOOKUP(C21, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(C21,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
       <c r="I21" t="inlineStr">
@@ -1388,11 +1365,11 @@
         </is>
       </c>
       <c r="K21">
-        <f>IFERROR(VLOOKUP(J21, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(J21,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
       <c r="L21">
-        <f>IFERROR(VLOOKUP(J21, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(J21,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
     </row>
@@ -1403,7 +1380,7 @@
         </is>
       </c>
       <c r="F22">
-        <f>IFERROR(VLOOKUP(C22, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(C22,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
       <c r="I22" t="inlineStr">
@@ -1412,11 +1389,11 @@
         </is>
       </c>
       <c r="K22">
-        <f>IFERROR(VLOOKUP(J22, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(J22,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
       <c r="L22">
-        <f>IFERROR(VLOOKUP(J22, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(J22,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
     </row>
@@ -1465,11 +1442,11 @@
         </is>
       </c>
       <c r="E24">
-        <f>IFERROR(VLOOKUP(C24, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(C24,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
       <c r="F24">
-        <f>IFERROR(VLOOKUP(C24, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(C24,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
       <c r="G24" t="inlineStr">
@@ -1488,11 +1465,11 @@
         </is>
       </c>
       <c r="K24">
-        <f>IFERROR(VLOOKUP(J24, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(J24,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
       <c r="L24">
-        <f>IFERROR(VLOOKUP(J24, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(J24,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
     </row>
@@ -1503,11 +1480,11 @@
         </is>
       </c>
       <c r="E25">
-        <f>IFERROR(VLOOKUP(C25, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(C25,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
       <c r="F25">
-        <f>IFERROR(VLOOKUP(C25, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(C25,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
       <c r="I25" t="inlineStr">
@@ -1516,11 +1493,11 @@
         </is>
       </c>
       <c r="K25">
-        <f>IFERROR(VLOOKUP(J25, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(J25,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
       <c r="L25">
-        <f>IFERROR(VLOOKUP(J25, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(J25,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
     </row>
@@ -1531,11 +1508,11 @@
         </is>
       </c>
       <c r="E26">
-        <f>IFERROR(VLOOKUP(C26, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(C26,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
       <c r="F26">
-        <f>IFERROR(VLOOKUP(C26, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(C26,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
       <c r="I26" t="inlineStr">
@@ -1544,11 +1521,11 @@
         </is>
       </c>
       <c r="K26">
-        <f>IFERROR(VLOOKUP(J26, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(J26,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
       <c r="L26">
-        <f>IFERROR(VLOOKUP(J26, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(J26,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
     </row>
@@ -1564,11 +1541,11 @@
         </is>
       </c>
       <c r="E27">
-        <f>IFERROR(VLOOKUP(C27, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(C27,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
       <c r="F27">
-        <f>IFERROR(VLOOKUP(C27, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(C27,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
       <c r="H27" t="inlineStr">
@@ -1582,11 +1559,11 @@
         </is>
       </c>
       <c r="K27">
-        <f>IFERROR(VLOOKUP(J27, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(J27,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
       <c r="L27">
-        <f>IFERROR(VLOOKUP(J27, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(J27,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
     </row>
@@ -1597,11 +1574,11 @@
         </is>
       </c>
       <c r="E28">
-        <f>IFERROR(VLOOKUP(C28, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(C28,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
       <c r="F28">
-        <f>IFERROR(VLOOKUP(C28, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(C28,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
       <c r="I28" t="inlineStr">
@@ -1610,11 +1587,11 @@
         </is>
       </c>
       <c r="K28">
-        <f>IFERROR(VLOOKUP(J28, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(J28,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
       <c r="L28">
-        <f>IFERROR(VLOOKUP(J28, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(J28,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
     </row>
@@ -1625,11 +1602,11 @@
         </is>
       </c>
       <c r="E29">
-        <f>IFERROR(VLOOKUP(C29, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(C29,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
       <c r="F29">
-        <f>IFERROR(VLOOKUP(C29, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(C29,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
       <c r="I29" t="inlineStr">
@@ -1638,11 +1615,11 @@
         </is>
       </c>
       <c r="K29">
-        <f>IFERROR(VLOOKUP(J29, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(J29,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
       <c r="L29">
-        <f>IFERROR(VLOOKUP(J29, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(J29,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
     </row>
@@ -1658,11 +1635,11 @@
         </is>
       </c>
       <c r="E30">
-        <f>IFERROR(VLOOKUP(C30, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(C30,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
       <c r="F30">
-        <f>IFERROR(VLOOKUP(C30, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(C30,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
       <c r="H30" t="inlineStr">
@@ -1676,11 +1653,11 @@
         </is>
       </c>
       <c r="K30">
-        <f>IFERROR(VLOOKUP(J30, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(J30,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
       <c r="L30">
-        <f>IFERROR(VLOOKUP(J30, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(J30,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
     </row>
@@ -1691,11 +1668,11 @@
         </is>
       </c>
       <c r="E31">
-        <f>IFERROR(VLOOKUP(C31, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(C31,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
       <c r="F31">
-        <f>IFERROR(VLOOKUP(C31, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(C31,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
       <c r="I31" t="inlineStr">
@@ -1704,11 +1681,11 @@
         </is>
       </c>
       <c r="K31">
-        <f>IFERROR(VLOOKUP(J31, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(J31,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
       <c r="L31">
-        <f>IFERROR(VLOOKUP(J31, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(J31,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
     </row>
@@ -1719,11 +1696,11 @@
         </is>
       </c>
       <c r="E32">
-        <f>IFERROR(VLOOKUP(C32, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(C32,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
       <c r="F32">
-        <f>IFERROR(VLOOKUP(C32, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(C32,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
       <c r="I32" t="inlineStr">
@@ -1732,11 +1709,11 @@
         </is>
       </c>
       <c r="K32">
-        <f>IFERROR(VLOOKUP(J32, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(J32,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
       <c r="L32">
-        <f>IFERROR(VLOOKUP(J32, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(J32,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
     </row>
@@ -1752,11 +1729,11 @@
         </is>
       </c>
       <c r="E33">
-        <f>IFERROR(VLOOKUP(C33, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(C33,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
       <c r="F33">
-        <f>IFERROR(VLOOKUP(C33, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(C33,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
       <c r="H33" t="inlineStr">
@@ -1770,11 +1747,11 @@
         </is>
       </c>
       <c r="K33">
-        <f>IFERROR(VLOOKUP(J33, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(J33,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
       <c r="L33">
-        <f>IFERROR(VLOOKUP(J33, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(J33,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
     </row>
@@ -1785,11 +1762,11 @@
         </is>
       </c>
       <c r="E34">
-        <f>IFERROR(VLOOKUP(C34, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(C34,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
       <c r="F34">
-        <f>IFERROR(VLOOKUP(C34, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(C34,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
       <c r="I34" t="inlineStr">
@@ -1798,11 +1775,11 @@
         </is>
       </c>
       <c r="K34">
-        <f>IFERROR(VLOOKUP(J34, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(J34,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
       <c r="L34">
-        <f>IFERROR(VLOOKUP(J34, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(J34,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
     </row>
@@ -1813,11 +1790,11 @@
         </is>
       </c>
       <c r="E35">
-        <f>IFERROR(VLOOKUP(C35, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(C35,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
       <c r="F35">
-        <f>IFERROR(VLOOKUP(C35, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(C35,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
       <c r="I35" t="inlineStr">
@@ -1826,11 +1803,11 @@
         </is>
       </c>
       <c r="K35">
-        <f>IFERROR(VLOOKUP(J35, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(J35,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
       <c r="L35">
-        <f>IFERROR(VLOOKUP(J35, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(J35,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
     </row>
@@ -1846,11 +1823,11 @@
         </is>
       </c>
       <c r="E36">
-        <f>IFERROR(VLOOKUP(C36, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(C36,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
       <c r="F36">
-        <f>IFERROR(VLOOKUP(C36, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(C36,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
       <c r="H36" t="inlineStr">
@@ -1864,11 +1841,11 @@
         </is>
       </c>
       <c r="K36">
-        <f>IFERROR(VLOOKUP(J36, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(J36,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
       <c r="L36">
-        <f>IFERROR(VLOOKUP(J36, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(J36,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
     </row>
@@ -1879,11 +1856,11 @@
         </is>
       </c>
       <c r="E37">
-        <f>IFERROR(VLOOKUP(C37, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(C37,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
       <c r="F37">
-        <f>IFERROR(VLOOKUP(C37, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(C37,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
       <c r="I37" t="inlineStr">
@@ -1892,11 +1869,11 @@
         </is>
       </c>
       <c r="K37">
-        <f>IFERROR(VLOOKUP(J37, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(J37,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
       <c r="L37">
-        <f>IFERROR(VLOOKUP(J37, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(J37,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
     </row>
@@ -1907,11 +1884,11 @@
         </is>
       </c>
       <c r="E38">
-        <f>IFERROR(VLOOKUP(C38, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(C38,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
       <c r="F38">
-        <f>IFERROR(VLOOKUP(C38, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(C38,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
       <c r="I38" t="inlineStr">
@@ -1920,11 +1897,11 @@
         </is>
       </c>
       <c r="K38">
-        <f>IFERROR(VLOOKUP(J38, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(J38,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
       <c r="L38">
-        <f>IFERROR(VLOOKUP(J38, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(J38,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
     </row>
@@ -1940,11 +1917,11 @@
         </is>
       </c>
       <c r="E39">
-        <f>IFERROR(VLOOKUP(C39, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(C39,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
       <c r="F39">
-        <f>IFERROR(VLOOKUP(C39, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(C39,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
       <c r="H39" t="inlineStr">
@@ -1965,11 +1942,11 @@
         </is>
       </c>
       <c r="E40">
-        <f>IFERROR(VLOOKUP(C40, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(C40,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
       <c r="F40">
-        <f>IFERROR(VLOOKUP(C40, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(C40,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
       <c r="I40" t="inlineStr">
@@ -1978,11 +1955,11 @@
         </is>
       </c>
       <c r="K40">
-        <f>IFERROR(VLOOKUP(J40, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(J40,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
       <c r="L40">
-        <f>IFERROR(VLOOKUP(J40, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(J40,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
     </row>
@@ -1993,7 +1970,7 @@
         </is>
       </c>
       <c r="F41">
-        <f>IFERROR(VLOOKUP(C41, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(C41,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
       <c r="I41" t="inlineStr">
@@ -2002,11 +1979,11 @@
         </is>
       </c>
       <c r="K41">
-        <f>IFERROR(VLOOKUP(J41, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(J41,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
       <c r="L41">
-        <f>IFERROR(VLOOKUP(J41, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(J41,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
     </row>
@@ -2022,11 +1999,11 @@
         </is>
       </c>
       <c r="E42">
-        <f>IFERROR(VLOOKUP(C42, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(C42,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
       <c r="F42">
-        <f>IFERROR(VLOOKUP(C42, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(C42,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
       <c r="H42" t="inlineStr">
@@ -2040,11 +2017,11 @@
         </is>
       </c>
       <c r="K42">
-        <f>IFERROR(VLOOKUP(J42, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(J42,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
       <c r="L42">
-        <f>IFERROR(VLOOKUP(J42, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(J42,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
     </row>
@@ -2055,11 +2032,11 @@
         </is>
       </c>
       <c r="E43">
-        <f>IFERROR(VLOOKUP(C43, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(C43,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
       <c r="F43">
-        <f>IFERROR(VLOOKUP(C43, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(C43,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
       <c r="I43" t="inlineStr">
@@ -2068,11 +2045,11 @@
         </is>
       </c>
       <c r="K43">
-        <f>IFERROR(VLOOKUP(J43, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(J43,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
       <c r="L43">
-        <f>IFERROR(VLOOKUP(J43, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(J43,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
     </row>
@@ -2083,11 +2060,11 @@
         </is>
       </c>
       <c r="E44">
-        <f>IFERROR(VLOOKUP(C44, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(C44,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
       <c r="F44">
-        <f>IFERROR(VLOOKUP(C44, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(C44,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
       <c r="I44" t="inlineStr">
@@ -2096,11 +2073,11 @@
         </is>
       </c>
       <c r="K44">
-        <f>IFERROR(VLOOKUP(J44, Recipes!$A$2:$C$1000, 2, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(J44,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
       <c r="L44">
-        <f>IFERROR(VLOOKUP(J44, Recipes!$A$2:$C$1000, 3, FALSE), "")</f>
+        <f>IFERROR(VLOOKUP(J44,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
     </row>
@@ -2192,7 +2169,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2201,212 +2178,260 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="7" t="inlineStr">
+      <c r="A1" s="6" t="inlineStr">
+        <is>
+          <t>Meal Type</t>
+        </is>
+      </c>
+      <c r="B1" s="6" t="inlineStr">
         <is>
           <t>Recipe Name</t>
         </is>
       </c>
-      <c r="B1" s="7" t="inlineStr">
-        <is>
-          <t>Meal Type</t>
-        </is>
-      </c>
-      <c r="C1" s="7" t="inlineStr">
-        <is>
-          <t>Image URL</t>
-        </is>
-      </c>
-      <c r="D1" s="7" t="inlineStr">
-        <is>
-          <t>Recipe URL</t>
-        </is>
-      </c>
-      <c r="E1" s="7" t="inlineStr">
+      <c r="C1" s="6" t="inlineStr">
+        <is>
+          <t>Calories Per Serving</t>
+        </is>
+      </c>
+      <c r="D1" s="6" t="inlineStr">
+        <is>
+          <t>Servings</t>
+        </is>
+      </c>
+      <c r="E1" s="6" t="inlineStr">
         <is>
           <t>Ingredients</t>
         </is>
       </c>
-      <c r="F1" s="7" t="inlineStr">
-        <is>
-          <t>Calories</t>
+      <c r="F1" s="6" t="inlineStr">
+        <is>
+          <t>Instructions</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Red Lentil Soup with Chicken and Turnips</t>
+          <t>Breakfast</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Dinner</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>https://img.spoonacular.com/recipes/715415-312x231.jpg</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>https://spoonacular.com/recipes/715415</t>
-        </is>
+          <t>Breakfast Sausage Puffs</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>201</v>
+      </c>
+      <c r="D2" t="n">
+        <v>8</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>additional toppings: diced avocado, micro greens, chopped basil), 3 medium carrots, peeled and diced, 3 celery stalks, diced, 2 cups fully-cooked chicken breast, shredded (may be omitted for a vegetarian version), ½ cup flat leaf Italian parsley, chopped (plus extra for garnish), 6 cloves of garlic, finely minced, 2 tablespoons olive oil, 28 ounce-can plum tomatoes, drained and rinsed, chopped, 2 cups dried red lentils, rinsed, salt and black pepper, to taste, 1 large turnip, peeled and diced, 8 cups vegetable stock, 1 medium yellow onion, diced</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr"/>
+          <t>1 sheet puff pastry, thawed, 2 tablespoons maple syrup, plus more for serving, 18 cooked breakfast sausages, about 1 pound, 1 egg</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>https://www.marthastewart.com/868891/breakfast-sausage-puffs</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Slow Cooker Beef Stew</t>
+          <t>Breakfast</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Dinner</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>https://img.spoonacular.com/recipes/715446-312x231.jpg</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>https://spoonacular.com/recipes/715446</t>
-        </is>
+          <t>Recipe: Muffin-Pan Breakfast Sliders</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>188</v>
+      </c>
+      <c r="D3" t="n">
+        <v>4</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>1 14.5oz can of Beef Broth, 2 large carrots, chopped, 2 stalks celery, chopped, 1 26oz can Cream of Mushroom Soup, 3 green onions, chopped, 10 new (red)potatoes, 1 small onion chopped, ½ cup Dale's Seasoning, 2 pounds stew meat, 2 cups water</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr"/>
+          <t>4 ounces uncooked breakfast sausage, casings removed, 4 large eggs, 2 slices American cheese, halved</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>http://www.thekitchn.com/recipe-muffin-pan-breakfast-sliders-234089</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Asparagus and Pea Soup: Real Convenience Food</t>
+          <t>Breakfast</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Breakfastr</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>https://spoonacular.com/recipes/716406</t>
-        </is>
+          <t>Pastrami Breakfast Biscuit</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>440</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>1 bag of frozen organic asparagus (preferably thawed), 1T EVOO (extra virgin olive oil), a couple of garlic cloves, 1/2 onion, 2-3c of frozen organic peas, 1 box low-sodium vegetable broth</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr"/>
+          <t>1 Breakfast Biscuit, 2 ounces warm pastrami</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>https://www.foodandwine.com/recipes/pastrami-breakfast-biscuit</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Garlicky Kale</t>
+          <t>Dinner</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Breakfastr</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>https://spoonacular.com/recipes/644387</t>
-        </is>
+          <t>After-dinner mint cream</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>361</v>
+      </c>
+      <c r="D5" t="n">
+        <v>6</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>3 tablespoons balsamic vinegar, 1 clove garlic, minced, 1 bunch curly kale, stems removed and chopped, Olive oil</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr"/>
+          <t>250g mascarpone, 300ml double cream, 2-3 tbsp caster sugar, 2-3 tbsp cream sherry (we used Harvey's Bristol Cream), 200g thin after-dinner mints, plus 6 extra to serve</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>https://www.bbcgoodfood.com/recipes/after-dinner-mint-cream</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Powerhouse Almond Matcha Superfood Smoothie</t>
+          <t>Dinner</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Breakfast</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>https://spoonacular.com/recipes/756814</t>
-        </is>
+          <t>Everything Dinner Rolls</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>582</v>
+      </c>
+      <c r="D6" t="n">
+        <v>10</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2 tablespoons unsalted natural almond butter, 1 1/2 cups unsweetened almond milk, 1 medium frozen banana, 2 teaspoons chia seeds, 1 cup baby kale, packed, 1/2 cup frozen mango pieces, 1 tablespoon matcha green tea powder, 3/4 cup frozen pineapple, 1/2 teaspoon vanilla extract</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr"/>
+          <t>Cooking spray, 20 frozen dinner rolls, 2 tablespoons unsalted butter, 1 tablespoon honey, 2 tablespoons everything bagel seasoning</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>https://www.realsimple.com/everything-dinner-rolls-recipe-6750835</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Butternut Squash Frittata</t>
+          <t>Dinner</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Breakfast</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>https://spoonacular.com/recipes/636589</t>
-        </is>
+          <t>Buttered Dinner Rolls</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>275</v>
+      </c>
+      <c r="D7" t="n">
+        <v>15</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>1 large butternut squash, peeled, seeded, thinly sliced (with a mandoline), 1/2 oz goat cheese, 1/2 cup liquid egg substitute, 2 tbsp. non-fat milk, Pepper to taste</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr"/>
+          <t>Melted butter, 15 frozen, unbaked, unrisen dinner rolls, Coarse sea salt, for sprinkling</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>https://www.foodnetwork.com/recipes/ree-drummond/buttered-dinner-rolls-recipe-2109635</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Doughnuts</t>
+          <t>Dinner</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Breakfast</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr"/>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>https://spoonacular.com/recipes/716276</t>
-        </is>
+          <t>Easy Dinner Rolls</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>571</v>
+      </c>
+      <c r="D8" t="n">
+        <v>6</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>1.5 cups of flour, 30 ml honey, 1 tablespoon of powdered milk, 1/2 teaspoon salt, 150 ml warm water, 1 teaspoon yeast</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr"/>
+          <t>12 frozen, unbaked dinner rolls (such as Bridgford Parkerhouse Style Rolls Dough), 1 egg, beaten, 1 tablespoons to 2 desired topping (such as Everything Bagel, Greek, or Old Bay seasoning), 1 ½ tablespoons melted unsalted butter</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>https://www.myrecipes.com/recipe/easy-dinner-rolls</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Dinner</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Dinner Tonight: Custardy Popovers</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>195</v>
+      </c>
+      <c r="D9" t="n">
+        <v>6</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>2 tablespoons butter, 3 large eggs, 1 1/4 cups milk, 1 1/4 cups flour, 1/2 teaspoon salt</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>http://www.seriouseats.com/recipes/2007/12/dinner-tonight-custardy-popovers-recipe.html</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
fix: week 1 drop down and calorie count fixed
</commit_message>
<xml_diff>
--- a/MealPrepTracker.xlsx
+++ b/MealPrepTracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/quinnreams/Documents/GitHub/Personal-Growth-Planner/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{481006CC-72A5-5A43-9F38-FAC9A2633947}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE816B56-220F-BD4A-BF99-ABAA7D8D4752}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3120" yWindow="540" windowWidth="38400" windowHeight="19620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Meal Calendar" sheetId="1" r:id="rId1"/>
@@ -217,12 +217,6 @@
     </font>
     <font>
       <sz val="16"/>
-      <color theme="1"/>
-      <name val="Helvetica Neue"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="16"/>
       <color rgb="FF000000"/>
       <name val="Inherit"/>
     </font>
@@ -230,6 +224,12 @@
       <b/>
       <sz val="12"/>
       <name val="Aptos Narrow"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -283,14 +283,14 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -805,8 +805,8 @@
   <dimension ref="A1:L59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I59" sqref="I59"/>
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -870,11 +870,11 @@
       <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="4" t="str">
-        <f>IFERROR(VLOOKUP(C2,#REF!, 2, FALSE), "")</f>
-        <v/>
-      </c>
-      <c r="F2" s="5" t="str">
+      <c r="E2" s="8">
+        <f>IFERROR(VLOOKUP(D2, Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="F2" s="4" t="str">
         <f>IFERROR(VLOOKUP(C2,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
@@ -887,11 +887,8 @@
       <c r="I2" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="5" t="str">
-        <f>IFERROR(VLOOKUP(J2,#REF!, 2, FALSE), "")</f>
-        <v/>
-      </c>
-      <c r="L2" s="5" t="str">
+      <c r="K2" s="4"/>
+      <c r="L2" s="4" t="str">
         <f>IFERROR(VLOOKUP(J2,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
@@ -900,9 +897,9 @@
       <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="E3" t="str">
-        <f>IFERROR(VLOOKUP(C3,#REF!, 2, FALSE), "")</f>
-        <v/>
+      <c r="E3">
+        <f>IFERROR(VLOOKUP(D3, Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
       </c>
       <c r="F3" t="str">
         <f>IFERROR(VLOOKUP(C3,#REF!, 3, FALSE), "")</f>
@@ -911,10 +908,6 @@
       <c r="I3" t="s">
         <v>10</v>
       </c>
-      <c r="K3" t="str">
-        <f>IFERROR(VLOOKUP(J3,#REF!, 2, FALSE), "")</f>
-        <v/>
-      </c>
       <c r="L3" t="str">
         <f>IFERROR(VLOOKUP(J3,#REF!, 3, FALSE), "")</f>
         <v/>
@@ -924,9 +917,9 @@
       <c r="C4" t="s">
         <v>11</v>
       </c>
-      <c r="E4" t="str">
-        <f>IFERROR(VLOOKUP(C4,#REF!, 2, FALSE), "")</f>
-        <v/>
+      <c r="E4">
+        <f>IFERROR(VLOOKUP(D4, Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
       </c>
       <c r="F4" t="str">
         <f>IFERROR(VLOOKUP(C4,#REF!, 3, FALSE), "")</f>
@@ -948,22 +941,22 @@
       <c r="C5" t="s">
         <v>51</v>
       </c>
-      <c r="E5" s="8" t="str">
-        <f>IFERROR(VLOOKUP(C5,#REF!, 2, FALSE), "")</f>
-        <v/>
-      </c>
-      <c r="F5" s="8" t="str">
+      <c r="E5" s="7">
+        <f>IFERROR(VLOOKUP(D5, Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="F5" s="7" t="str">
         <f>IFERROR(VLOOKUP(C5,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
       <c r="I5" t="s">
         <v>51</v>
       </c>
-      <c r="K5" s="8" t="str">
+      <c r="K5" s="7" t="str">
         <f>IFERROR(VLOOKUP(J5,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="L5" s="8" t="str">
+      <c r="L5" s="7" t="str">
         <f>IFERROR(VLOOKUP(J5,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
@@ -975,9 +968,9 @@
       <c r="C6" t="s">
         <v>8</v>
       </c>
-      <c r="E6" t="str">
-        <f>IFERROR(VLOOKUP(C6,#REF!, 2, FALSE), "")</f>
-        <v/>
+      <c r="E6">
+        <f>IFERROR(VLOOKUP(D6, Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
       </c>
       <c r="F6" t="str">
         <f>IFERROR(VLOOKUP(C6,#REF!, 3, FALSE), "")</f>
@@ -1002,9 +995,9 @@
       <c r="C7" t="s">
         <v>10</v>
       </c>
-      <c r="E7" t="str">
-        <f>IFERROR(VLOOKUP(C7,#REF!, 2, FALSE), "")</f>
-        <v/>
+      <c r="E7">
+        <f>IFERROR(VLOOKUP(D7, Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
       </c>
       <c r="F7" t="str">
         <f>IFERROR(VLOOKUP(C7,#REF!, 3, FALSE), "")</f>
@@ -1026,9 +1019,9 @@
       <c r="C8" t="s">
         <v>11</v>
       </c>
-      <c r="E8" t="str">
-        <f>IFERROR(VLOOKUP(C8,#REF!, 2, FALSE), "")</f>
-        <v/>
+      <c r="E8">
+        <f>IFERROR(VLOOKUP(D8, Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
       </c>
       <c r="F8" t="str">
         <f>IFERROR(VLOOKUP(C8,#REF!, 3, FALSE), "")</f>
@@ -1050,22 +1043,22 @@
       <c r="C9" t="s">
         <v>51</v>
       </c>
-      <c r="E9" s="8" t="str">
-        <f>IFERROR(VLOOKUP(C9,#REF!, 2, FALSE), "")</f>
-        <v/>
-      </c>
-      <c r="F9" s="8" t="str">
+      <c r="E9" s="7">
+        <f>IFERROR(VLOOKUP(D9, Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="F9" s="7" t="str">
         <f>IFERROR(VLOOKUP(C9,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
       <c r="I9" t="s">
         <v>51</v>
       </c>
-      <c r="K9" s="8" t="str">
+      <c r="K9" s="7" t="str">
         <f>IFERROR(VLOOKUP(J9,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="L9" s="8" t="str">
+      <c r="L9" s="7" t="str">
         <f>IFERROR(VLOOKUP(J9,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
@@ -1077,6 +1070,10 @@
       <c r="C10" t="s">
         <v>8</v>
       </c>
+      <c r="E10">
+        <f>IFERROR(VLOOKUP(D10, Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
+      </c>
       <c r="H10" t="s">
         <v>13</v>
       </c>
@@ -1096,9 +1093,9 @@
       <c r="C11" t="s">
         <v>10</v>
       </c>
-      <c r="E11" t="str">
-        <f>IFERROR(VLOOKUP(C11,#REF!, 2, FALSE), "")</f>
-        <v/>
+      <c r="E11">
+        <f>IFERROR(VLOOKUP(D11, Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
       </c>
       <c r="F11" t="str">
         <f>IFERROR(VLOOKUP(C11,#REF!, 3, FALSE), "")</f>
@@ -1120,9 +1117,9 @@
       <c r="C12" t="s">
         <v>11</v>
       </c>
-      <c r="E12" t="str">
-        <f>IFERROR(VLOOKUP(C12,#REF!, 2, FALSE), "")</f>
-        <v/>
+      <c r="E12">
+        <f>IFERROR(VLOOKUP(D12, Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
       </c>
       <c r="F12" t="str">
         <f>IFERROR(VLOOKUP(C12,#REF!, 3, FALSE), "")</f>
@@ -1144,22 +1141,22 @@
       <c r="C13" t="s">
         <v>51</v>
       </c>
-      <c r="E13" s="8" t="str">
-        <f>IFERROR(VLOOKUP(C13,#REF!, 2, FALSE), "")</f>
-        <v/>
-      </c>
-      <c r="F13" s="8" t="str">
+      <c r="E13" s="7">
+        <f>IFERROR(VLOOKUP(D13, Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="F13" s="7" t="str">
         <f>IFERROR(VLOOKUP(C13,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
       <c r="I13" t="s">
         <v>51</v>
       </c>
-      <c r="K13" s="8" t="str">
+      <c r="K13" s="7" t="str">
         <f>IFERROR(VLOOKUP(J13,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="L13" s="8" t="str">
+      <c r="L13" s="7" t="str">
         <f>IFERROR(VLOOKUP(J13,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
@@ -1171,9 +1168,9 @@
       <c r="C14" t="s">
         <v>8</v>
       </c>
-      <c r="E14" t="str">
-        <f>IFERROR(VLOOKUP(C14,#REF!, 2, FALSE), "")</f>
-        <v/>
+      <c r="E14">
+        <f>IFERROR(VLOOKUP(D14, Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
       </c>
       <c r="F14" t="str">
         <f>IFERROR(VLOOKUP(C14,#REF!, 3, FALSE), "")</f>
@@ -1198,9 +1195,9 @@
       <c r="C15" t="s">
         <v>10</v>
       </c>
-      <c r="E15" t="str">
-        <f>IFERROR(VLOOKUP(C15,#REF!, 2, FALSE), "")</f>
-        <v/>
+      <c r="E15">
+        <f>IFERROR(VLOOKUP(D15, Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
       </c>
       <c r="F15" t="str">
         <f>IFERROR(VLOOKUP(C15,#REF!, 3, FALSE), "")</f>
@@ -1222,9 +1219,9 @@
       <c r="C16" t="s">
         <v>11</v>
       </c>
-      <c r="E16" t="str">
-        <f>IFERROR(VLOOKUP(C16,#REF!, 2, FALSE), "")</f>
-        <v/>
+      <c r="E16">
+        <f>IFERROR(VLOOKUP(D16, Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
       </c>
       <c r="F16" t="str">
         <f>IFERROR(VLOOKUP(C16,#REF!, 3, FALSE), "")</f>
@@ -1246,22 +1243,22 @@
       <c r="C17" t="s">
         <v>51</v>
       </c>
-      <c r="E17" s="8" t="str">
-        <f>IFERROR(VLOOKUP(C17,#REF!, 2, FALSE), "")</f>
-        <v/>
-      </c>
-      <c r="F17" s="8" t="str">
+      <c r="E17" s="7">
+        <f>IFERROR(VLOOKUP(D17, Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="F17" s="7" t="str">
         <f>IFERROR(VLOOKUP(C17,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
       <c r="I17" t="s">
         <v>51</v>
       </c>
-      <c r="K17" s="8" t="str">
+      <c r="K17" s="7" t="str">
         <f>IFERROR(VLOOKUP(J17,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="L17" s="8" t="str">
+      <c r="L17" s="7" t="str">
         <f>IFERROR(VLOOKUP(J17,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
@@ -1273,9 +1270,9 @@
       <c r="C18" t="s">
         <v>8</v>
       </c>
-      <c r="E18" t="str">
-        <f>IFERROR(VLOOKUP(C18,#REF!, 2, FALSE), "")</f>
-        <v/>
+      <c r="E18">
+        <f>IFERROR(VLOOKUP(D18, Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
       </c>
       <c r="F18" t="str">
         <f>IFERROR(VLOOKUP(C18,#REF!, 3, FALSE), "")</f>
@@ -1300,9 +1297,9 @@
       <c r="C19" t="s">
         <v>10</v>
       </c>
-      <c r="E19" t="str">
-        <f>IFERROR(VLOOKUP(C19,#REF!, 2, FALSE), "")</f>
-        <v/>
+      <c r="E19">
+        <f>IFERROR(VLOOKUP(D19, Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
       </c>
       <c r="F19" t="str">
         <f>IFERROR(VLOOKUP(C19,#REF!, 3, FALSE), "")</f>
@@ -1324,9 +1321,9 @@
       <c r="C20" t="s">
         <v>11</v>
       </c>
-      <c r="E20" t="str">
-        <f>IFERROR(VLOOKUP(C20,#REF!, 2, FALSE), "")</f>
-        <v/>
+      <c r="E20">
+        <f>IFERROR(VLOOKUP(D20, Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
       </c>
       <c r="F20" t="str">
         <f>IFERROR(VLOOKUP(C20,#REF!, 3, FALSE), "")</f>
@@ -1348,22 +1345,22 @@
       <c r="C21" t="s">
         <v>51</v>
       </c>
-      <c r="E21" s="8" t="str">
-        <f>IFERROR(VLOOKUP(C21,#REF!, 2, FALSE), "")</f>
-        <v/>
-      </c>
-      <c r="F21" s="8" t="str">
+      <c r="E21" s="7">
+        <f>IFERROR(VLOOKUP(D21, Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="F21" s="7" t="str">
         <f>IFERROR(VLOOKUP(C21,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
       <c r="I21" t="s">
         <v>51</v>
       </c>
-      <c r="K21" s="8" t="str">
+      <c r="K21" s="7" t="str">
         <f>IFERROR(VLOOKUP(J21,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="L21" s="8" t="str">
+      <c r="L21" s="7" t="str">
         <f>IFERROR(VLOOKUP(J21,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
@@ -1375,9 +1372,9 @@
       <c r="C22" t="s">
         <v>8</v>
       </c>
-      <c r="E22" t="str">
-        <f>IFERROR(VLOOKUP(C22,#REF!, 2, FALSE), "")</f>
-        <v/>
+      <c r="E22">
+        <f>IFERROR(VLOOKUP(D22, Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
       </c>
       <c r="F22" t="str">
         <f>IFERROR(VLOOKUP(C22,#REF!, 3, FALSE), "")</f>
@@ -1402,9 +1399,9 @@
       <c r="C23" t="s">
         <v>10</v>
       </c>
-      <c r="E23" t="str">
-        <f>IFERROR(VLOOKUP(C23,#REF!, 2, FALSE), "")</f>
-        <v/>
+      <c r="E23">
+        <f>IFERROR(VLOOKUP(D23, Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
       </c>
       <c r="F23" t="str">
         <f>IFERROR(VLOOKUP(C23,#REF!, 3, FALSE), "")</f>
@@ -1426,9 +1423,9 @@
       <c r="C24" t="s">
         <v>11</v>
       </c>
-      <c r="E24" t="str">
-        <f>IFERROR(VLOOKUP(C24,#REF!, 2, FALSE), "")</f>
-        <v/>
+      <c r="E24">
+        <f>IFERROR(VLOOKUP(D24, Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
       </c>
       <c r="F24" t="str">
         <f>IFERROR(VLOOKUP(C24,#REF!, 3, FALSE), "")</f>
@@ -1446,22 +1443,22 @@
       <c r="C25" t="s">
         <v>51</v>
       </c>
-      <c r="E25" s="8" t="str">
-        <f>IFERROR(VLOOKUP(C25,#REF!, 2, FALSE), "")</f>
-        <v/>
-      </c>
-      <c r="F25" s="8" t="str">
+      <c r="E25" s="7">
+        <f>IFERROR(VLOOKUP(D25, Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="F25" s="7" t="str">
         <f>IFERROR(VLOOKUP(C25,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
       <c r="I25" t="s">
         <v>51</v>
       </c>
-      <c r="K25" s="8" t="str">
+      <c r="K25" s="7" t="str">
         <f>IFERROR(VLOOKUP(J25,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="L25" s="8" t="str">
+      <c r="L25" s="7" t="str">
         <f>IFERROR(VLOOKUP(J25,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
@@ -1473,9 +1470,9 @@
       <c r="C26" t="s">
         <v>8</v>
       </c>
-      <c r="E26" t="str">
-        <f>IFERROR(VLOOKUP(C26,#REF!, 2, FALSE), "")</f>
-        <v/>
+      <c r="E26">
+        <f>IFERROR(VLOOKUP(D26, Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
       </c>
       <c r="F26" t="str">
         <f>IFERROR(VLOOKUP(C26,#REF!, 3, FALSE), "")</f>
@@ -1496,6 +1493,10 @@
       <c r="C27" t="s">
         <v>10</v>
       </c>
+      <c r="E27">
+        <f>IFERROR(VLOOKUP(D27, Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
+      </c>
       <c r="F27" t="str">
         <f>IFERROR(VLOOKUP(C27,#REF!, 3, FALSE), "")</f>
         <v/>
@@ -1516,6 +1517,10 @@
       <c r="C28" t="s">
         <v>11</v>
       </c>
+      <c r="E28">
+        <f>IFERROR(VLOOKUP(D28, Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
+      </c>
       <c r="F28" t="str">
         <f>IFERROR(VLOOKUP(C28,#REF!, 3, FALSE), "")</f>
         <v/>
@@ -1536,22 +1541,22 @@
       <c r="C29" t="s">
         <v>51</v>
       </c>
-      <c r="E29" s="8" t="str">
-        <f>IFERROR(VLOOKUP(C29,#REF!, 2, FALSE), "")</f>
-        <v/>
-      </c>
-      <c r="F29" s="8" t="str">
+      <c r="E29" s="7">
+        <f>IFERROR(VLOOKUP(D29, Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="F29" s="7" t="str">
         <f>IFERROR(VLOOKUP(C29,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
       <c r="I29" t="s">
         <v>51</v>
       </c>
-      <c r="K29" s="8" t="str">
+      <c r="K29" s="7" t="str">
         <f>IFERROR(VLOOKUP(J29,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="L29" s="8" t="str">
+      <c r="L29" s="7" t="str">
         <f>IFERROR(VLOOKUP(J29,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
@@ -1561,11 +1566,11 @@
         <v>18</v>
       </c>
       <c r="E30">
-        <f>SUM(E2:E28)</f>
+        <f>SUM(E2:E29)</f>
         <v>0</v>
       </c>
       <c r="F30">
-        <f>SUM(F2:F28)</f>
+        <f>SUM(F2:F29)</f>
         <v>0</v>
       </c>
       <c r="H30" t="s">
@@ -1668,22 +1673,22 @@
       <c r="C34" t="s">
         <v>51</v>
       </c>
-      <c r="E34" s="8" t="str">
+      <c r="E34" s="7" t="str">
         <f>IFERROR(VLOOKUP(C34,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="F34" s="8" t="str">
+      <c r="F34" s="7" t="str">
         <f>IFERROR(VLOOKUP(C34,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
       <c r="I34" t="s">
         <v>51</v>
       </c>
-      <c r="K34" s="8" t="str">
+      <c r="K34" s="7" t="str">
         <f>IFERROR(VLOOKUP(J34,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="L34" s="8" t="str">
+      <c r="L34" s="7" t="str">
         <f>IFERROR(VLOOKUP(J34,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
@@ -1770,22 +1775,22 @@
       <c r="C38" t="s">
         <v>51</v>
       </c>
-      <c r="E38" s="8" t="str">
+      <c r="E38" s="7" t="str">
         <f>IFERROR(VLOOKUP(C38,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="F38" s="8" t="str">
+      <c r="F38" s="7" t="str">
         <f>IFERROR(VLOOKUP(C38,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
       <c r="I38" t="s">
         <v>51</v>
       </c>
-      <c r="K38" s="8" t="str">
+      <c r="K38" s="7" t="str">
         <f>IFERROR(VLOOKUP(J38,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="L38" s="8" t="str">
+      <c r="L38" s="7" t="str">
         <f>IFERROR(VLOOKUP(J38,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
@@ -1872,22 +1877,22 @@
       <c r="C42" t="s">
         <v>51</v>
       </c>
-      <c r="E42" s="8" t="str">
+      <c r="E42" s="7" t="str">
         <f>IFERROR(VLOOKUP(C42,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="F42" s="8" t="str">
+      <c r="F42" s="7" t="str">
         <f>IFERROR(VLOOKUP(C42,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
       <c r="I42" t="s">
         <v>51</v>
       </c>
-      <c r="K42" s="8" t="str">
+      <c r="K42" s="7" t="str">
         <f>IFERROR(VLOOKUP(J42,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="L42" s="8" t="str">
+      <c r="L42" s="7" t="str">
         <f>IFERROR(VLOOKUP(J42,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
@@ -1974,22 +1979,22 @@
       <c r="C46" t="s">
         <v>51</v>
       </c>
-      <c r="E46" s="8" t="str">
+      <c r="E46" s="7" t="str">
         <f>IFERROR(VLOOKUP(C46,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="F46" s="8" t="str">
+      <c r="F46" s="7" t="str">
         <f>IFERROR(VLOOKUP(C46,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
       <c r="I46" t="s">
         <v>51</v>
       </c>
-      <c r="K46" s="8" t="str">
+      <c r="K46" s="7" t="str">
         <f>IFERROR(VLOOKUP(J46,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="L46" s="8" t="str">
+      <c r="L46" s="7" t="str">
         <f>IFERROR(VLOOKUP(J46,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
@@ -2076,22 +2081,22 @@
       <c r="C50" t="s">
         <v>51</v>
       </c>
-      <c r="E50" s="8" t="str">
+      <c r="E50" s="7" t="str">
         <f>IFERROR(VLOOKUP(C50,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="F50" s="8" t="str">
+      <c r="F50" s="7" t="str">
         <f>IFERROR(VLOOKUP(C50,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
       <c r="I50" t="s">
         <v>51</v>
       </c>
-      <c r="K50" s="8" t="str">
+      <c r="K50" s="7" t="str">
         <f>IFERROR(VLOOKUP(J50,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="L50" s="8" t="str">
+      <c r="L50" s="7" t="str">
         <f>IFERROR(VLOOKUP(J50,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
@@ -2166,22 +2171,22 @@
       <c r="C54" t="s">
         <v>51</v>
       </c>
-      <c r="E54" s="8" t="str">
+      <c r="E54" s="7" t="str">
         <f>IFERROR(VLOOKUP(C54,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="F54" s="8" t="str">
+      <c r="F54" s="7" t="str">
         <f>IFERROR(VLOOKUP(C54,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
       <c r="I54" t="s">
         <v>51</v>
       </c>
-      <c r="K54" s="8" t="str">
+      <c r="K54" s="7" t="str">
         <f>IFERROR(VLOOKUP(J54,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="L54" s="8" t="str">
+      <c r="L54" s="7" t="str">
         <f>IFERROR(VLOOKUP(J54,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
@@ -2268,22 +2273,22 @@
       <c r="C58" t="s">
         <v>51</v>
       </c>
-      <c r="E58" s="8" t="str">
+      <c r="E58" s="7" t="str">
         <f>IFERROR(VLOOKUP(C58,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="F58" s="8" t="str">
+      <c r="F58" s="7" t="str">
         <f>IFERROR(VLOOKUP(C58,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
       <c r="I58" t="s">
         <v>51</v>
       </c>
-      <c r="K58" s="8" t="str">
+      <c r="K58" s="7" t="str">
         <f>IFERROR(VLOOKUP(J58,#REF!, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="L58" s="8" t="str">
+      <c r="L58" s="7" t="str">
         <f>IFERROR(VLOOKUP(J58,#REF!, 3, FALSE), "")</f>
         <v/>
       </c>
@@ -2384,22 +2389,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="17">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="6" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>

<commit_message>
wb: week 2 fixed on calories
</commit_message>
<xml_diff>
--- a/MealPrepTracker.xlsx
+++ b/MealPrepTracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/quinnreams/Documents/GitHub/Personal-Growth-Planner/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE816B56-220F-BD4A-BF99-ABAA7D8D4752}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B06DF14-9451-C543-A29E-DF17691679F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="540" windowWidth="38400" windowHeight="19620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="340" yWindow="500" windowWidth="38400" windowHeight="19620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Meal Calendar" sheetId="1" r:id="rId1"/>
@@ -805,8 +805,8 @@
   <dimension ref="A1:L59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G30" sqref="G30"/>
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E58" sqref="E58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1595,9 +1595,9 @@
       <c r="C31" t="s">
         <v>8</v>
       </c>
-      <c r="E31" t="str">
-        <f>IFERROR(VLOOKUP(C31,#REF!, 2, FALSE), "")</f>
-        <v/>
+      <c r="E31">
+        <f>IFERROR(VLOOKUP(D31, Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
       </c>
       <c r="F31" t="str">
         <f>IFERROR(VLOOKUP(C31,#REF!, 3, FALSE), "")</f>
@@ -1625,9 +1625,9 @@
       <c r="C32" t="s">
         <v>10</v>
       </c>
-      <c r="E32" t="str">
-        <f>IFERROR(VLOOKUP(C32,#REF!, 2, FALSE), "")</f>
-        <v/>
+      <c r="E32">
+        <f>IFERROR(VLOOKUP(D32, Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
       </c>
       <c r="F32" t="str">
         <f>IFERROR(VLOOKUP(C32,#REF!, 3, FALSE), "")</f>
@@ -1649,9 +1649,9 @@
       <c r="C33" t="s">
         <v>11</v>
       </c>
-      <c r="E33" t="str">
-        <f>IFERROR(VLOOKUP(C33,#REF!, 2, FALSE), "")</f>
-        <v/>
+      <c r="E33">
+        <f>IFERROR(VLOOKUP(D33, Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
       </c>
       <c r="F33" t="str">
         <f>IFERROR(VLOOKUP(C33,#REF!, 3, FALSE), "")</f>
@@ -1673,9 +1673,9 @@
       <c r="C34" t="s">
         <v>51</v>
       </c>
-      <c r="E34" s="7" t="str">
-        <f>IFERROR(VLOOKUP(C34,#REF!, 2, FALSE), "")</f>
-        <v/>
+      <c r="E34" s="7">
+        <f>IFERROR(VLOOKUP(D34, Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
       </c>
       <c r="F34" s="7" t="str">
         <f>IFERROR(VLOOKUP(C34,#REF!, 3, FALSE), "")</f>
@@ -1700,9 +1700,9 @@
       <c r="C35" t="s">
         <v>8</v>
       </c>
-      <c r="E35" t="str">
-        <f>IFERROR(VLOOKUP(C35,#REF!, 2, FALSE), "")</f>
-        <v/>
+      <c r="E35">
+        <f>IFERROR(VLOOKUP(D35, Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
       </c>
       <c r="F35" t="str">
         <f>IFERROR(VLOOKUP(C35,#REF!, 3, FALSE), "")</f>
@@ -1727,9 +1727,9 @@
       <c r="C36" t="s">
         <v>10</v>
       </c>
-      <c r="E36" t="str">
-        <f>IFERROR(VLOOKUP(C36,#REF!, 2, FALSE), "")</f>
-        <v/>
+      <c r="E36">
+        <f>IFERROR(VLOOKUP(D36, Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
       </c>
       <c r="F36" t="str">
         <f>IFERROR(VLOOKUP(C36,#REF!, 3, FALSE), "")</f>
@@ -1751,9 +1751,9 @@
       <c r="C37" t="s">
         <v>11</v>
       </c>
-      <c r="E37" t="str">
-        <f>IFERROR(VLOOKUP(C37,#REF!, 2, FALSE), "")</f>
-        <v/>
+      <c r="E37">
+        <f>IFERROR(VLOOKUP(D37, Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
       </c>
       <c r="F37" t="str">
         <f>IFERROR(VLOOKUP(C37,#REF!, 3, FALSE), "")</f>
@@ -1775,9 +1775,9 @@
       <c r="C38" t="s">
         <v>51</v>
       </c>
-      <c r="E38" s="7" t="str">
-        <f>IFERROR(VLOOKUP(C38,#REF!, 2, FALSE), "")</f>
-        <v/>
+      <c r="E38" s="7">
+        <f>IFERROR(VLOOKUP(D38, Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
       </c>
       <c r="F38" s="7" t="str">
         <f>IFERROR(VLOOKUP(C38,#REF!, 3, FALSE), "")</f>
@@ -1802,9 +1802,9 @@
       <c r="C39" t="s">
         <v>8</v>
       </c>
-      <c r="E39" t="str">
-        <f>IFERROR(VLOOKUP(C39,#REF!, 2, FALSE), "")</f>
-        <v/>
+      <c r="E39">
+        <f>IFERROR(VLOOKUP(D39, Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
       </c>
       <c r="F39" t="str">
         <f>IFERROR(VLOOKUP(C39,#REF!, 3, FALSE), "")</f>
@@ -1829,9 +1829,9 @@
       <c r="C40" t="s">
         <v>10</v>
       </c>
-      <c r="E40" t="str">
-        <f>IFERROR(VLOOKUP(C40,#REF!, 2, FALSE), "")</f>
-        <v/>
+      <c r="E40">
+        <f>IFERROR(VLOOKUP(D40, Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
       </c>
       <c r="F40" t="str">
         <f>IFERROR(VLOOKUP(C40,#REF!, 3, FALSE), "")</f>
@@ -1853,9 +1853,9 @@
       <c r="C41" t="s">
         <v>11</v>
       </c>
-      <c r="E41" t="str">
-        <f>IFERROR(VLOOKUP(C41,#REF!, 2, FALSE), "")</f>
-        <v/>
+      <c r="E41">
+        <f>IFERROR(VLOOKUP(D41, Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
       </c>
       <c r="F41" t="str">
         <f>IFERROR(VLOOKUP(C41,#REF!, 3, FALSE), "")</f>
@@ -1877,9 +1877,9 @@
       <c r="C42" t="s">
         <v>51</v>
       </c>
-      <c r="E42" s="7" t="str">
-        <f>IFERROR(VLOOKUP(C42,#REF!, 2, FALSE), "")</f>
-        <v/>
+      <c r="E42" s="7">
+        <f>IFERROR(VLOOKUP(D42, Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
       </c>
       <c r="F42" s="7" t="str">
         <f>IFERROR(VLOOKUP(C42,#REF!, 3, FALSE), "")</f>
@@ -1904,9 +1904,9 @@
       <c r="C43" t="s">
         <v>8</v>
       </c>
-      <c r="E43" t="str">
-        <f>IFERROR(VLOOKUP(C43,#REF!, 2, FALSE), "")</f>
-        <v/>
+      <c r="E43">
+        <f>IFERROR(VLOOKUP(D43, Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
       </c>
       <c r="F43" t="str">
         <f>IFERROR(VLOOKUP(C43,#REF!, 3, FALSE), "")</f>
@@ -1931,9 +1931,9 @@
       <c r="C44" t="s">
         <v>10</v>
       </c>
-      <c r="E44" t="str">
-        <f>IFERROR(VLOOKUP(C44,#REF!, 2, FALSE), "")</f>
-        <v/>
+      <c r="E44">
+        <f>IFERROR(VLOOKUP(D44, Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
       </c>
       <c r="F44" t="str">
         <f>IFERROR(VLOOKUP(C44,#REF!, 3, FALSE), "")</f>
@@ -1955,9 +1955,9 @@
       <c r="C45" t="s">
         <v>11</v>
       </c>
-      <c r="E45" t="str">
-        <f>IFERROR(VLOOKUP(C45,#REF!, 2, FALSE), "")</f>
-        <v/>
+      <c r="E45">
+        <f>IFERROR(VLOOKUP(D45, Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
       </c>
       <c r="F45" t="str">
         <f>IFERROR(VLOOKUP(C45,#REF!, 3, FALSE), "")</f>
@@ -1979,9 +1979,9 @@
       <c r="C46" t="s">
         <v>51</v>
       </c>
-      <c r="E46" s="7" t="str">
-        <f>IFERROR(VLOOKUP(C46,#REF!, 2, FALSE), "")</f>
-        <v/>
+      <c r="E46" s="7">
+        <f>IFERROR(VLOOKUP(D46, Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
       </c>
       <c r="F46" s="7" t="str">
         <f>IFERROR(VLOOKUP(C46,#REF!, 3, FALSE), "")</f>
@@ -2006,9 +2006,9 @@
       <c r="C47" t="s">
         <v>8</v>
       </c>
-      <c r="E47" t="str">
-        <f>IFERROR(VLOOKUP(C47,#REF!, 2, FALSE), "")</f>
-        <v/>
+      <c r="E47">
+        <f>IFERROR(VLOOKUP(D47, Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
       </c>
       <c r="F47" t="str">
         <f>IFERROR(VLOOKUP(C47,#REF!, 3, FALSE), "")</f>
@@ -2033,9 +2033,9 @@
       <c r="C48" t="s">
         <v>10</v>
       </c>
-      <c r="E48" t="str">
-        <f>IFERROR(VLOOKUP(C48,#REF!, 2, FALSE), "")</f>
-        <v/>
+      <c r="E48">
+        <f>IFERROR(VLOOKUP(D48, Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
       </c>
       <c r="F48" t="str">
         <f>IFERROR(VLOOKUP(C48,#REF!, 3, FALSE), "")</f>
@@ -2057,9 +2057,9 @@
       <c r="C49" t="s">
         <v>11</v>
       </c>
-      <c r="E49" t="str">
-        <f>IFERROR(VLOOKUP(C49,#REF!, 2, FALSE), "")</f>
-        <v/>
+      <c r="E49">
+        <f>IFERROR(VLOOKUP(D49, Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
       </c>
       <c r="F49" t="str">
         <f>IFERROR(VLOOKUP(C49,#REF!, 3, FALSE), "")</f>
@@ -2081,9 +2081,9 @@
       <c r="C50" t="s">
         <v>51</v>
       </c>
-      <c r="E50" s="7" t="str">
-        <f>IFERROR(VLOOKUP(C50,#REF!, 2, FALSE), "")</f>
-        <v/>
+      <c r="E50" s="7">
+        <f>IFERROR(VLOOKUP(D50, Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
       </c>
       <c r="F50" s="7" t="str">
         <f>IFERROR(VLOOKUP(C50,#REF!, 3, FALSE), "")</f>
@@ -2108,9 +2108,9 @@
       <c r="C51" t="s">
         <v>8</v>
       </c>
-      <c r="E51" t="str">
-        <f>IFERROR(VLOOKUP(C51,#REF!, 2, FALSE), "")</f>
-        <v/>
+      <c r="E51">
+        <f>IFERROR(VLOOKUP(D51, Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
       </c>
       <c r="F51" t="str">
         <f>IFERROR(VLOOKUP(C51,#REF!, 3, FALSE), "")</f>
@@ -2127,9 +2127,9 @@
       <c r="C52" t="s">
         <v>10</v>
       </c>
-      <c r="E52" t="str">
-        <f>IFERROR(VLOOKUP(C52,#REF!, 2, FALSE), "")</f>
-        <v/>
+      <c r="E52">
+        <f>IFERROR(VLOOKUP(D52, Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
       </c>
       <c r="F52" t="str">
         <f>IFERROR(VLOOKUP(C52,#REF!, 3, FALSE), "")</f>
@@ -2151,6 +2151,10 @@
       <c r="C53" t="s">
         <v>11</v>
       </c>
+      <c r="E53">
+        <f>IFERROR(VLOOKUP(D53, Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
+      </c>
       <c r="F53" t="str">
         <f>IFERROR(VLOOKUP(C53,#REF!, 3, FALSE), "")</f>
         <v/>
@@ -2171,9 +2175,9 @@
       <c r="C54" t="s">
         <v>51</v>
       </c>
-      <c r="E54" s="7" t="str">
-        <f>IFERROR(VLOOKUP(C54,#REF!, 2, FALSE), "")</f>
-        <v/>
+      <c r="E54" s="7">
+        <f>IFERROR(VLOOKUP(D54, Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
       </c>
       <c r="F54" s="7" t="str">
         <f>IFERROR(VLOOKUP(C54,#REF!, 3, FALSE), "")</f>
@@ -2198,9 +2202,9 @@
       <c r="C55" t="s">
         <v>8</v>
       </c>
-      <c r="E55" t="str">
-        <f>IFERROR(VLOOKUP(C55,#REF!, 2, FALSE), "")</f>
-        <v/>
+      <c r="E55">
+        <f>IFERROR(VLOOKUP(D55, Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
       </c>
       <c r="F55" t="str">
         <f>IFERROR(VLOOKUP(C55,#REF!, 3, FALSE), "")</f>
@@ -2225,9 +2229,9 @@
       <c r="C56" t="s">
         <v>10</v>
       </c>
-      <c r="E56" t="str">
-        <f>IFERROR(VLOOKUP(C56,#REF!, 2, FALSE), "")</f>
-        <v/>
+      <c r="E56">
+        <f>IFERROR(VLOOKUP(D56, Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
       </c>
       <c r="F56" t="str">
         <f>IFERROR(VLOOKUP(C56,#REF!, 3, FALSE), "")</f>
@@ -2249,9 +2253,9 @@
       <c r="C57" t="s">
         <v>11</v>
       </c>
-      <c r="E57" t="str">
-        <f>IFERROR(VLOOKUP(C57,#REF!, 2, FALSE), "")</f>
-        <v/>
+      <c r="E57">
+        <f>IFERROR(VLOOKUP(D57, Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
       </c>
       <c r="F57" t="str">
         <f>IFERROR(VLOOKUP(C57,#REF!, 3, FALSE), "")</f>
@@ -2273,9 +2277,9 @@
       <c r="C58" t="s">
         <v>51</v>
       </c>
-      <c r="E58" s="7" t="str">
-        <f>IFERROR(VLOOKUP(C58,#REF!, 2, FALSE), "")</f>
-        <v/>
+      <c r="E58" s="7">
+        <f>IFERROR(VLOOKUP(D58, Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
       </c>
       <c r="F58" s="7" t="str">
         <f>IFERROR(VLOOKUP(C58,#REF!, 3, FALSE), "")</f>

</xml_diff>

<commit_message>
wb:weeks 3/4 calories done
</commit_message>
<xml_diff>
--- a/MealPrepTracker.xlsx
+++ b/MealPrepTracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/quinnreams/Documents/GitHub/Personal-Growth-Planner/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B06DF14-9451-C543-A29E-DF17691679F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D21BE2AB-7684-C248-BF46-8ED62BE89816}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="340" yWindow="500" windowWidth="38400" windowHeight="19620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,6 +36,28 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="52">
   <si>
@@ -199,7 +221,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -228,6 +250,12 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
@@ -273,7 +301,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -291,6 +319,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -806,7 +835,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E58" sqref="E58"/>
+      <selection pane="bottomLeft" activeCell="J44" sqref="J44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -887,7 +916,10 @@
       <c r="I2" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="4"/>
+      <c r="K2" s="9" cm="1">
+        <f t="array" aca="1" ref="K2" ca="1">IFERROR(VLOOKUP(INDIRECT("R[0]C[-1]",0), Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
+      </c>
       <c r="L2" s="4" t="str">
         <f>IFERROR(VLOOKUP(J2,#REF!, 3, FALSE), "")</f>
         <v/>
@@ -908,6 +940,10 @@
       <c r="I3" t="s">
         <v>10</v>
       </c>
+      <c r="K3" cm="1">
+        <f t="array" aca="1" ref="K3" ca="1">IFERROR(VLOOKUP(INDIRECT("R[0]C[-1]",0), Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
+      </c>
       <c r="L3" t="str">
         <f>IFERROR(VLOOKUP(J3,#REF!, 3, FALSE), "")</f>
         <v/>
@@ -928,9 +964,9 @@
       <c r="I4" t="s">
         <v>11</v>
       </c>
-      <c r="K4" t="str">
-        <f>IFERROR(VLOOKUP(J4,#REF!, 2, FALSE), "")</f>
-        <v/>
+      <c r="K4" cm="1">
+        <f t="array" aca="1" ref="K4" ca="1">IFERROR(VLOOKUP(INDIRECT("R[0]C[-1]",0), Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
       </c>
       <c r="L4" t="str">
         <f>IFERROR(VLOOKUP(J4,#REF!, 3, FALSE), "")</f>
@@ -952,9 +988,9 @@
       <c r="I5" t="s">
         <v>51</v>
       </c>
-      <c r="K5" s="7" t="str">
-        <f>IFERROR(VLOOKUP(J5,#REF!, 2, FALSE), "")</f>
-        <v/>
+      <c r="K5" s="7" cm="1">
+        <f t="array" aca="1" ref="K5" ca="1">IFERROR(VLOOKUP(INDIRECT("R[0]C[-1]",0), Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
       </c>
       <c r="L5" s="7" t="str">
         <f>IFERROR(VLOOKUP(J5,#REF!, 3, FALSE), "")</f>
@@ -982,9 +1018,9 @@
       <c r="I6" t="s">
         <v>8</v>
       </c>
-      <c r="K6" t="str">
-        <f>IFERROR(VLOOKUP(J6,#REF!, 2, FALSE), "")</f>
-        <v/>
+      <c r="K6" cm="1">
+        <f t="array" aca="1" ref="K6" ca="1">IFERROR(VLOOKUP(INDIRECT("R[0]C[-1]",0), Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
       </c>
       <c r="L6" t="str">
         <f>IFERROR(VLOOKUP(J6,#REF!, 3, FALSE), "")</f>
@@ -1006,9 +1042,9 @@
       <c r="I7" t="s">
         <v>10</v>
       </c>
-      <c r="K7" t="str">
-        <f>IFERROR(VLOOKUP(J7,#REF!, 2, FALSE), "")</f>
-        <v/>
+      <c r="K7" cm="1">
+        <f t="array" aca="1" ref="K7" ca="1">IFERROR(VLOOKUP(INDIRECT("R[0]C[-1]",0), Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
       </c>
       <c r="L7" t="str">
         <f>IFERROR(VLOOKUP(J7,#REF!, 3, FALSE), "")</f>
@@ -1030,9 +1066,9 @@
       <c r="I8" t="s">
         <v>11</v>
       </c>
-      <c r="K8" t="str">
-        <f>IFERROR(VLOOKUP(J8,#REF!, 2, FALSE), "")</f>
-        <v/>
+      <c r="K8" cm="1">
+        <f t="array" aca="1" ref="K8" ca="1">IFERROR(VLOOKUP(INDIRECT("R[0]C[-1]",0), Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
       </c>
       <c r="L8" t="str">
         <f>IFERROR(VLOOKUP(J8,#REF!, 3, FALSE), "")</f>
@@ -1054,9 +1090,9 @@
       <c r="I9" t="s">
         <v>51</v>
       </c>
-      <c r="K9" s="7" t="str">
-        <f>IFERROR(VLOOKUP(J9,#REF!, 2, FALSE), "")</f>
-        <v/>
+      <c r="K9" s="7" cm="1">
+        <f t="array" aca="1" ref="K9" ca="1">IFERROR(VLOOKUP(INDIRECT("R[0]C[-1]",0), Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
       </c>
       <c r="L9" s="7" t="str">
         <f>IFERROR(VLOOKUP(J9,#REF!, 3, FALSE), "")</f>
@@ -1080,9 +1116,9 @@
       <c r="I10" t="s">
         <v>8</v>
       </c>
-      <c r="K10" t="str">
-        <f>IFERROR(VLOOKUP(J10,#REF!, 2, FALSE), "")</f>
-        <v/>
+      <c r="K10" cm="1">
+        <f t="array" aca="1" ref="K10" ca="1">IFERROR(VLOOKUP(INDIRECT("R[0]C[-1]",0), Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
       </c>
       <c r="L10" t="str">
         <f>IFERROR(VLOOKUP(J10,#REF!, 3, FALSE), "")</f>
@@ -1104,9 +1140,9 @@
       <c r="I11" t="s">
         <v>10</v>
       </c>
-      <c r="K11" t="str">
-        <f>IFERROR(VLOOKUP(J11,#REF!, 2, FALSE), "")</f>
-        <v/>
+      <c r="K11" cm="1">
+        <f t="array" aca="1" ref="K11" ca="1">IFERROR(VLOOKUP(INDIRECT("R[0]C[-1]",0), Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
       </c>
       <c r="L11" t="str">
         <f>IFERROR(VLOOKUP(J11,#REF!, 3, FALSE), "")</f>
@@ -1128,9 +1164,9 @@
       <c r="I12" t="s">
         <v>11</v>
       </c>
-      <c r="K12" t="str">
-        <f>IFERROR(VLOOKUP(J12,#REF!, 2, FALSE), "")</f>
-        <v/>
+      <c r="K12" cm="1">
+        <f t="array" aca="1" ref="K12" ca="1">IFERROR(VLOOKUP(INDIRECT("R[0]C[-1]",0), Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
       </c>
       <c r="L12" t="str">
         <f>IFERROR(VLOOKUP(J12,#REF!, 3, FALSE), "")</f>
@@ -1152,9 +1188,9 @@
       <c r="I13" t="s">
         <v>51</v>
       </c>
-      <c r="K13" s="7" t="str">
-        <f>IFERROR(VLOOKUP(J13,#REF!, 2, FALSE), "")</f>
-        <v/>
+      <c r="K13" s="7" cm="1">
+        <f t="array" aca="1" ref="K13" ca="1">IFERROR(VLOOKUP(INDIRECT("R[0]C[-1]",0), Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
       </c>
       <c r="L13" s="7" t="str">
         <f>IFERROR(VLOOKUP(J13,#REF!, 3, FALSE), "")</f>
@@ -1182,9 +1218,9 @@
       <c r="I14" t="s">
         <v>8</v>
       </c>
-      <c r="K14" t="str">
-        <f>IFERROR(VLOOKUP(J14,#REF!, 2, FALSE), "")</f>
-        <v/>
+      <c r="K14" cm="1">
+        <f t="array" aca="1" ref="K14" ca="1">IFERROR(VLOOKUP(INDIRECT("R[0]C[-1]",0), Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
       </c>
       <c r="L14" t="str">
         <f>IFERROR(VLOOKUP(J14,#REF!, 3, FALSE), "")</f>
@@ -1206,9 +1242,9 @@
       <c r="I15" t="s">
         <v>10</v>
       </c>
-      <c r="K15" t="str">
-        <f>IFERROR(VLOOKUP(J15,#REF!, 2, FALSE), "")</f>
-        <v/>
+      <c r="K15" cm="1">
+        <f t="array" aca="1" ref="K15" ca="1">IFERROR(VLOOKUP(INDIRECT("R[0]C[-1]",0), Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
       </c>
       <c r="L15" t="str">
         <f>IFERROR(VLOOKUP(J15,#REF!, 3, FALSE), "")</f>
@@ -1230,9 +1266,9 @@
       <c r="I16" t="s">
         <v>11</v>
       </c>
-      <c r="K16" t="str">
-        <f>IFERROR(VLOOKUP(J16,#REF!, 2, FALSE), "")</f>
-        <v/>
+      <c r="K16" cm="1">
+        <f t="array" aca="1" ref="K16" ca="1">IFERROR(VLOOKUP(INDIRECT("R[0]C[-1]",0), Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
       </c>
       <c r="L16" t="str">
         <f>IFERROR(VLOOKUP(J16,#REF!, 3, FALSE), "")</f>
@@ -1254,9 +1290,9 @@
       <c r="I17" t="s">
         <v>51</v>
       </c>
-      <c r="K17" s="7" t="str">
-        <f>IFERROR(VLOOKUP(J17,#REF!, 2, FALSE), "")</f>
-        <v/>
+      <c r="K17" s="7" cm="1">
+        <f t="array" aca="1" ref="K17" ca="1">IFERROR(VLOOKUP(INDIRECT("R[0]C[-1]",0), Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
       </c>
       <c r="L17" s="7" t="str">
         <f>IFERROR(VLOOKUP(J17,#REF!, 3, FALSE), "")</f>
@@ -1284,9 +1320,9 @@
       <c r="I18" t="s">
         <v>8</v>
       </c>
-      <c r="K18" t="str">
-        <f>IFERROR(VLOOKUP(J18,#REF!, 2, FALSE), "")</f>
-        <v/>
+      <c r="K18" cm="1">
+        <f t="array" aca="1" ref="K18" ca="1">IFERROR(VLOOKUP(INDIRECT("R[0]C[-1]",0), Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
       </c>
       <c r="L18" t="str">
         <f>IFERROR(VLOOKUP(J18,#REF!, 3, FALSE), "")</f>
@@ -1308,9 +1344,9 @@
       <c r="I19" t="s">
         <v>10</v>
       </c>
-      <c r="K19" t="str">
-        <f>IFERROR(VLOOKUP(J19,#REF!, 2, FALSE), "")</f>
-        <v/>
+      <c r="K19" cm="1">
+        <f t="array" aca="1" ref="K19" ca="1">IFERROR(VLOOKUP(INDIRECT("R[0]C[-1]",0), Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
       </c>
       <c r="L19" t="str">
         <f>IFERROR(VLOOKUP(J19,#REF!, 3, FALSE), "")</f>
@@ -1332,9 +1368,9 @@
       <c r="I20" t="s">
         <v>11</v>
       </c>
-      <c r="K20" t="str">
-        <f>IFERROR(VLOOKUP(J20,#REF!, 2, FALSE), "")</f>
-        <v/>
+      <c r="K20" cm="1">
+        <f t="array" aca="1" ref="K20" ca="1">IFERROR(VLOOKUP(INDIRECT("R[0]C[-1]",0), Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
       </c>
       <c r="L20" t="str">
         <f>IFERROR(VLOOKUP(J20,#REF!, 3, FALSE), "")</f>
@@ -1356,9 +1392,9 @@
       <c r="I21" t="s">
         <v>51</v>
       </c>
-      <c r="K21" s="7" t="str">
-        <f>IFERROR(VLOOKUP(J21,#REF!, 2, FALSE), "")</f>
-        <v/>
+      <c r="K21" s="7" cm="1">
+        <f t="array" aca="1" ref="K21" ca="1">IFERROR(VLOOKUP(INDIRECT("R[0]C[-1]",0), Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
       </c>
       <c r="L21" s="7" t="str">
         <f>IFERROR(VLOOKUP(J21,#REF!, 3, FALSE), "")</f>
@@ -1386,9 +1422,9 @@
       <c r="I22" t="s">
         <v>8</v>
       </c>
-      <c r="K22" t="str">
-        <f>IFERROR(VLOOKUP(J22,#REF!, 2, FALSE), "")</f>
-        <v/>
+      <c r="K22" cm="1">
+        <f t="array" aca="1" ref="K22" ca="1">IFERROR(VLOOKUP(INDIRECT("R[0]C[-1]",0), Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
       </c>
       <c r="L22" t="str">
         <f>IFERROR(VLOOKUP(J22,#REF!, 3, FALSE), "")</f>
@@ -1410,9 +1446,9 @@
       <c r="I23" t="s">
         <v>10</v>
       </c>
-      <c r="K23" t="str">
-        <f>IFERROR(VLOOKUP(J23,#REF!, 2, FALSE), "")</f>
-        <v/>
+      <c r="K23" cm="1">
+        <f t="array" aca="1" ref="K23" ca="1">IFERROR(VLOOKUP(INDIRECT("R[0]C[-1]",0), Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
       </c>
       <c r="L23" t="str">
         <f>IFERROR(VLOOKUP(J23,#REF!, 3, FALSE), "")</f>
@@ -1434,6 +1470,10 @@
       <c r="I24" t="s">
         <v>11</v>
       </c>
+      <c r="K24" cm="1">
+        <f t="array" aca="1" ref="K24" ca="1">IFERROR(VLOOKUP(INDIRECT("R[0]C[-1]",0), Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
+      </c>
       <c r="L24" t="str">
         <f>IFERROR(VLOOKUP(J24,#REF!, 3, FALSE), "")</f>
         <v/>
@@ -1454,9 +1494,9 @@
       <c r="I25" t="s">
         <v>51</v>
       </c>
-      <c r="K25" s="7" t="str">
-        <f>IFERROR(VLOOKUP(J25,#REF!, 2, FALSE), "")</f>
-        <v/>
+      <c r="K25" s="7" cm="1">
+        <f t="array" aca="1" ref="K25" ca="1">IFERROR(VLOOKUP(INDIRECT("R[0]C[-1]",0), Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
       </c>
       <c r="L25" s="7" t="str">
         <f>IFERROR(VLOOKUP(J25,#REF!, 3, FALSE), "")</f>
@@ -1484,6 +1524,10 @@
       <c r="I26" t="s">
         <v>8</v>
       </c>
+      <c r="K26" cm="1">
+        <f t="array" aca="1" ref="K26" ca="1">IFERROR(VLOOKUP(INDIRECT("R[0]C[-1]",0), Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
+      </c>
       <c r="L26" t="str">
         <f>IFERROR(VLOOKUP(J26,#REF!, 3, FALSE), "")</f>
         <v/>
@@ -1504,10 +1548,6 @@
       <c r="I27" t="s">
         <v>10</v>
       </c>
-      <c r="K27" t="str">
-        <f>IFERROR(VLOOKUP(J27,#REF!, 2, FALSE), "")</f>
-        <v/>
-      </c>
       <c r="L27" t="str">
         <f>IFERROR(VLOOKUP(J27,#REF!, 3, FALSE), "")</f>
         <v/>
@@ -1528,9 +1568,9 @@
       <c r="I28" t="s">
         <v>11</v>
       </c>
-      <c r="K28" t="str">
-        <f>IFERROR(VLOOKUP(J28,#REF!, 2, FALSE), "")</f>
-        <v/>
+      <c r="K28" cm="1">
+        <f t="array" aca="1" ref="K28" ca="1">IFERROR(VLOOKUP(INDIRECT("R[0]C[-1]",0), Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
       </c>
       <c r="L28" t="str">
         <f>IFERROR(VLOOKUP(J28,#REF!, 3, FALSE), "")</f>
@@ -1552,9 +1592,9 @@
       <c r="I29" t="s">
         <v>51</v>
       </c>
-      <c r="K29" s="7" t="str">
-        <f>IFERROR(VLOOKUP(J29,#REF!, 2, FALSE), "")</f>
-        <v/>
+      <c r="K29" s="7" cm="1">
+        <f t="array" aca="1" ref="K29" ca="1">IFERROR(VLOOKUP(INDIRECT("R[0]C[-1]",0), Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
       </c>
       <c r="L29" s="7" t="str">
         <f>IFERROR(VLOOKUP(J29,#REF!, 3, FALSE), "")</f>
@@ -1577,11 +1617,11 @@
         <v>18</v>
       </c>
       <c r="K30">
-        <f>SUM(K2:K28)</f>
+        <f ca="1">SUM(K2:K29)</f>
         <v>0</v>
       </c>
       <c r="L30">
-        <f>SUM(L2:L28)</f>
+        <f>SUM(L2:L29)</f>
         <v>0</v>
       </c>
     </row>
@@ -1612,9 +1652,9 @@
       <c r="I31" t="s">
         <v>8</v>
       </c>
-      <c r="K31" t="str">
-        <f>IFERROR(VLOOKUP(J31,#REF!, 2, FALSE), "")</f>
-        <v/>
+      <c r="K31" cm="1">
+        <f t="array" aca="1" ref="K31" ca="1">IFERROR(VLOOKUP(INDIRECT("R[0]C[-1]",0), Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
       </c>
       <c r="L31" t="str">
         <f>IFERROR(VLOOKUP(J31,#REF!, 3, FALSE), "")</f>
@@ -1636,9 +1676,9 @@
       <c r="I32" t="s">
         <v>10</v>
       </c>
-      <c r="K32" t="str">
-        <f>IFERROR(VLOOKUP(J32,#REF!, 2, FALSE), "")</f>
-        <v/>
+      <c r="K32" cm="1">
+        <f t="array" aca="1" ref="K32" ca="1">IFERROR(VLOOKUP(INDIRECT("R[0]C[-1]",0), Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
       </c>
       <c r="L32" t="str">
         <f>IFERROR(VLOOKUP(J32,#REF!, 3, FALSE), "")</f>
@@ -1660,9 +1700,9 @@
       <c r="I33" t="s">
         <v>11</v>
       </c>
-      <c r="K33" t="str">
-        <f>IFERROR(VLOOKUP(J33,#REF!, 2, FALSE), "")</f>
-        <v/>
+      <c r="K33" cm="1">
+        <f t="array" aca="1" ref="K33" ca="1">IFERROR(VLOOKUP(INDIRECT("R[0]C[-1]",0), Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
       </c>
       <c r="L33" t="str">
         <f>IFERROR(VLOOKUP(J33,#REF!, 3, FALSE), "")</f>
@@ -1684,9 +1724,9 @@
       <c r="I34" t="s">
         <v>51</v>
       </c>
-      <c r="K34" s="7" t="str">
-        <f>IFERROR(VLOOKUP(J34,#REF!, 2, FALSE), "")</f>
-        <v/>
+      <c r="K34" s="7" cm="1">
+        <f t="array" aca="1" ref="K34" ca="1">IFERROR(VLOOKUP(INDIRECT("R[0]C[-1]",0), Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
       </c>
       <c r="L34" s="7" t="str">
         <f>IFERROR(VLOOKUP(J34,#REF!, 3, FALSE), "")</f>
@@ -1714,9 +1754,9 @@
       <c r="I35" t="s">
         <v>8</v>
       </c>
-      <c r="K35" t="str">
-        <f>IFERROR(VLOOKUP(J35,#REF!, 2, FALSE), "")</f>
-        <v/>
+      <c r="K35" cm="1">
+        <f t="array" aca="1" ref="K35" ca="1">IFERROR(VLOOKUP(INDIRECT("R[0]C[-1]",0), Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
       </c>
       <c r="L35" t="str">
         <f>IFERROR(VLOOKUP(J35,#REF!, 3, FALSE), "")</f>
@@ -1738,9 +1778,9 @@
       <c r="I36" t="s">
         <v>10</v>
       </c>
-      <c r="K36" t="str">
-        <f>IFERROR(VLOOKUP(J36,#REF!, 2, FALSE), "")</f>
-        <v/>
+      <c r="K36" cm="1">
+        <f t="array" aca="1" ref="K36" ca="1">IFERROR(VLOOKUP(INDIRECT("R[0]C[-1]",0), Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
       </c>
       <c r="L36" t="str">
         <f>IFERROR(VLOOKUP(J36,#REF!, 3, FALSE), "")</f>
@@ -1762,9 +1802,9 @@
       <c r="I37" t="s">
         <v>11</v>
       </c>
-      <c r="K37" t="str">
-        <f>IFERROR(VLOOKUP(J37,#REF!, 2, FALSE), "")</f>
-        <v/>
+      <c r="K37" cm="1">
+        <f t="array" aca="1" ref="K37" ca="1">IFERROR(VLOOKUP(INDIRECT("R[0]C[-1]",0), Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
       </c>
       <c r="L37" t="str">
         <f>IFERROR(VLOOKUP(J37,#REF!, 3, FALSE), "")</f>
@@ -1786,9 +1826,9 @@
       <c r="I38" t="s">
         <v>51</v>
       </c>
-      <c r="K38" s="7" t="str">
-        <f>IFERROR(VLOOKUP(J38,#REF!, 2, FALSE), "")</f>
-        <v/>
+      <c r="K38" s="7" cm="1">
+        <f t="array" aca="1" ref="K38" ca="1">IFERROR(VLOOKUP(INDIRECT("R[0]C[-1]",0), Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
       </c>
       <c r="L38" s="7" t="str">
         <f>IFERROR(VLOOKUP(J38,#REF!, 3, FALSE), "")</f>
@@ -1816,9 +1856,9 @@
       <c r="I39" t="s">
         <v>8</v>
       </c>
-      <c r="K39" t="str">
-        <f>IFERROR(VLOOKUP(J39,#REF!, 2, FALSE), "")</f>
-        <v/>
+      <c r="K39" cm="1">
+        <f t="array" aca="1" ref="K39" ca="1">IFERROR(VLOOKUP(INDIRECT("R[0]C[-1]",0), Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
       </c>
       <c r="L39" t="str">
         <f>IFERROR(VLOOKUP(J39,#REF!, 3, FALSE), "")</f>
@@ -1840,9 +1880,9 @@
       <c r="I40" t="s">
         <v>10</v>
       </c>
-      <c r="K40" t="str">
-        <f>IFERROR(VLOOKUP(J40,#REF!, 2, FALSE), "")</f>
-        <v/>
+      <c r="K40" cm="1">
+        <f t="array" aca="1" ref="K40" ca="1">IFERROR(VLOOKUP(INDIRECT("R[0]C[-1]",0), Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
       </c>
       <c r="L40" t="str">
         <f>IFERROR(VLOOKUP(J40,#REF!, 3, FALSE), "")</f>
@@ -1864,9 +1904,9 @@
       <c r="I41" t="s">
         <v>11</v>
       </c>
-      <c r="K41" t="str">
-        <f>IFERROR(VLOOKUP(J41,#REF!, 2, FALSE), "")</f>
-        <v/>
+      <c r="K41" cm="1">
+        <f t="array" aca="1" ref="K41" ca="1">IFERROR(VLOOKUP(INDIRECT("R[0]C[-1]",0), Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
       </c>
       <c r="L41" t="str">
         <f>IFERROR(VLOOKUP(J41,#REF!, 3, FALSE), "")</f>
@@ -1888,9 +1928,9 @@
       <c r="I42" t="s">
         <v>51</v>
       </c>
-      <c r="K42" s="7" t="str">
-        <f>IFERROR(VLOOKUP(J42,#REF!, 2, FALSE), "")</f>
-        <v/>
+      <c r="K42" s="7" cm="1">
+        <f t="array" aca="1" ref="K42" ca="1">IFERROR(VLOOKUP(INDIRECT("R[0]C[-1]",0), Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
       </c>
       <c r="L42" s="7" t="str">
         <f>IFERROR(VLOOKUP(J42,#REF!, 3, FALSE), "")</f>
@@ -1918,9 +1958,9 @@
       <c r="I43" t="s">
         <v>8</v>
       </c>
-      <c r="K43" t="str">
-        <f>IFERROR(VLOOKUP(J43,#REF!, 2, FALSE), "")</f>
-        <v/>
+      <c r="K43" cm="1">
+        <f t="array" aca="1" ref="K43" ca="1">IFERROR(VLOOKUP(INDIRECT("R[0]C[-1]",0), Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
       </c>
       <c r="L43" t="str">
         <f>IFERROR(VLOOKUP(J43,#REF!, 3, FALSE), "")</f>
@@ -1942,9 +1982,9 @@
       <c r="I44" t="s">
         <v>10</v>
       </c>
-      <c r="K44" t="str">
-        <f>IFERROR(VLOOKUP(J44,#REF!, 2, FALSE), "")</f>
-        <v/>
+      <c r="K44" cm="1">
+        <f t="array" aca="1" ref="K44" ca="1">IFERROR(VLOOKUP(INDIRECT("R[0]C[-1]",0), Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
       </c>
       <c r="L44" t="str">
         <f>IFERROR(VLOOKUP(J44,#REF!, 3, FALSE), "")</f>
@@ -1966,9 +2006,9 @@
       <c r="I45" t="s">
         <v>11</v>
       </c>
-      <c r="K45" t="str">
-        <f>IFERROR(VLOOKUP(J45,#REF!, 2, FALSE), "")</f>
-        <v/>
+      <c r="K45" cm="1">
+        <f t="array" aca="1" ref="K45" ca="1">IFERROR(VLOOKUP(INDIRECT("R[0]C[-1]",0), Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
       </c>
       <c r="L45" t="str">
         <f>IFERROR(VLOOKUP(J45,#REF!, 3, FALSE), "")</f>
@@ -1990,9 +2030,9 @@
       <c r="I46" t="s">
         <v>51</v>
       </c>
-      <c r="K46" s="7" t="str">
-        <f>IFERROR(VLOOKUP(J46,#REF!, 2, FALSE), "")</f>
-        <v/>
+      <c r="K46" s="7" cm="1">
+        <f t="array" aca="1" ref="K46" ca="1">IFERROR(VLOOKUP(INDIRECT("R[0]C[-1]",0), Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
       </c>
       <c r="L46" s="7" t="str">
         <f>IFERROR(VLOOKUP(J46,#REF!, 3, FALSE), "")</f>
@@ -2020,9 +2060,9 @@
       <c r="I47" t="s">
         <v>8</v>
       </c>
-      <c r="K47" t="str">
-        <f>IFERROR(VLOOKUP(J47,#REF!, 2, FALSE), "")</f>
-        <v/>
+      <c r="K47" cm="1">
+        <f t="array" aca="1" ref="K47" ca="1">IFERROR(VLOOKUP(INDIRECT("R[0]C[-1]",0), Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
       </c>
       <c r="L47" t="str">
         <f>IFERROR(VLOOKUP(J47,#REF!, 3, FALSE), "")</f>
@@ -2044,9 +2084,9 @@
       <c r="I48" t="s">
         <v>10</v>
       </c>
-      <c r="K48" t="str">
-        <f>IFERROR(VLOOKUP(J48,#REF!, 2, FALSE), "")</f>
-        <v/>
+      <c r="K48" cm="1">
+        <f t="array" aca="1" ref="K48" ca="1">IFERROR(VLOOKUP(INDIRECT("R[0]C[-1]",0), Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
       </c>
       <c r="L48" t="str">
         <f>IFERROR(VLOOKUP(J48,#REF!, 3, FALSE), "")</f>
@@ -2068,9 +2108,9 @@
       <c r="I49" t="s">
         <v>11</v>
       </c>
-      <c r="K49" t="str">
-        <f>IFERROR(VLOOKUP(J49,#REF!, 2, FALSE), "")</f>
-        <v/>
+      <c r="K49" cm="1">
+        <f t="array" aca="1" ref="K49" ca="1">IFERROR(VLOOKUP(INDIRECT("R[0]C[-1]",0), Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
       </c>
       <c r="L49" t="str">
         <f>IFERROR(VLOOKUP(J49,#REF!, 3, FALSE), "")</f>
@@ -2092,9 +2132,9 @@
       <c r="I50" t="s">
         <v>51</v>
       </c>
-      <c r="K50" s="7" t="str">
-        <f>IFERROR(VLOOKUP(J50,#REF!, 2, FALSE), "")</f>
-        <v/>
+      <c r="K50" s="7" cm="1">
+        <f t="array" aca="1" ref="K50" ca="1">IFERROR(VLOOKUP(INDIRECT("R[0]C[-1]",0), Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
       </c>
       <c r="L50" s="7" t="str">
         <f>IFERROR(VLOOKUP(J50,#REF!, 3, FALSE), "")</f>
@@ -2122,6 +2162,10 @@
       <c r="I51" t="s">
         <v>8</v>
       </c>
+      <c r="K51" cm="1">
+        <f t="array" aca="1" ref="K51" ca="1">IFERROR(VLOOKUP(INDIRECT("R[0]C[-1]",0), Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="52" spans="2:12" ht="30" customHeight="1">
       <c r="C52" t="s">
@@ -2138,9 +2182,9 @@
       <c r="I52" t="s">
         <v>10</v>
       </c>
-      <c r="K52" t="str">
-        <f>IFERROR(VLOOKUP(J52,#REF!, 2, FALSE), "")</f>
-        <v/>
+      <c r="K52" cm="1">
+        <f t="array" aca="1" ref="K52" ca="1">IFERROR(VLOOKUP(INDIRECT("R[0]C[-1]",0), Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
       </c>
       <c r="L52" t="str">
         <f>IFERROR(VLOOKUP(J52,#REF!, 3, FALSE), "")</f>
@@ -2162,9 +2206,9 @@
       <c r="I53" t="s">
         <v>11</v>
       </c>
-      <c r="K53" t="str">
-        <f>IFERROR(VLOOKUP(J53,#REF!, 2, FALSE), "")</f>
-        <v/>
+      <c r="K53" cm="1">
+        <f t="array" aca="1" ref="K53" ca="1">IFERROR(VLOOKUP(INDIRECT("R[0]C[-1]",0), Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
       </c>
       <c r="L53" t="str">
         <f>IFERROR(VLOOKUP(J53,#REF!, 3, FALSE), "")</f>
@@ -2186,9 +2230,9 @@
       <c r="I54" t="s">
         <v>51</v>
       </c>
-      <c r="K54" s="7" t="str">
-        <f>IFERROR(VLOOKUP(J54,#REF!, 2, FALSE), "")</f>
-        <v/>
+      <c r="K54" s="7" cm="1">
+        <f t="array" aca="1" ref="K54" ca="1">IFERROR(VLOOKUP(INDIRECT("R[0]C[-1]",0), Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
       </c>
       <c r="L54" s="7" t="str">
         <f>IFERROR(VLOOKUP(J54,#REF!, 3, FALSE), "")</f>
@@ -2216,9 +2260,9 @@
       <c r="I55" t="s">
         <v>8</v>
       </c>
-      <c r="K55" t="str">
-        <f>IFERROR(VLOOKUP(J55,#REF!, 2, FALSE), "")</f>
-        <v/>
+      <c r="K55" cm="1">
+        <f t="array" aca="1" ref="K55" ca="1">IFERROR(VLOOKUP(INDIRECT("R[0]C[-1]",0), Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
       </c>
       <c r="L55" t="str">
         <f>IFERROR(VLOOKUP(J55,#REF!, 3, FALSE), "")</f>
@@ -2240,9 +2284,9 @@
       <c r="I56" t="s">
         <v>10</v>
       </c>
-      <c r="K56" t="str">
-        <f>IFERROR(VLOOKUP(J56,#REF!, 2, FALSE), "")</f>
-        <v/>
+      <c r="K56" cm="1">
+        <f t="array" aca="1" ref="K56" ca="1">IFERROR(VLOOKUP(INDIRECT("R[0]C[-1]",0), Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
       </c>
       <c r="L56" t="str">
         <f>IFERROR(VLOOKUP(J56,#REF!, 3, FALSE), "")</f>
@@ -2264,9 +2308,9 @@
       <c r="I57" t="s">
         <v>11</v>
       </c>
-      <c r="K57" t="str">
-        <f>IFERROR(VLOOKUP(J57,#REF!, 2, FALSE), "")</f>
-        <v/>
+      <c r="K57" cm="1">
+        <f t="array" aca="1" ref="K57" ca="1">IFERROR(VLOOKUP(INDIRECT("R[0]C[-1]",0), Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
       </c>
       <c r="L57" t="str">
         <f>IFERROR(VLOOKUP(J57,#REF!, 3, FALSE), "")</f>
@@ -2288,9 +2332,9 @@
       <c r="I58" t="s">
         <v>51</v>
       </c>
-      <c r="K58" s="7" t="str">
-        <f>IFERROR(VLOOKUP(J58,#REF!, 2, FALSE), "")</f>
-        <v/>
+      <c r="K58" s="7" cm="1">
+        <f t="array" aca="1" ref="K58" ca="1">IFERROR(VLOOKUP(INDIRECT("R[0]C[-1]",0), Recipes!$B$2:$F$1000, 2, FALSE), 0)</f>
+        <v>0</v>
       </c>
       <c r="L58" s="7" t="str">
         <f>IFERROR(VLOOKUP(J58,#REF!, 3, FALSE), "")</f>
@@ -2302,7 +2346,7 @@
         <v>18</v>
       </c>
       <c r="E59">
-        <f>SUM(E31:E57)</f>
+        <f>SUM(E31:E58)</f>
         <v>0</v>
       </c>
       <c r="F59">
@@ -2313,11 +2357,11 @@
         <v>18</v>
       </c>
       <c r="K59">
-        <f>SUM(K31:K57)</f>
+        <f ca="1">SUM(K31:K58)</f>
         <v>0</v>
       </c>
       <c r="L59">
-        <f>SUM(L31:L57)</f>
+        <f>SUM(L31:L58)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
wb:filters added to recipes sheet to make it easier
</commit_message>
<xml_diff>
--- a/MealPrepTracker.xlsx
+++ b/MealPrepTracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/quinnreams/Documents/GitHub/Personal-Growth-Planner/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D21BE2AB-7684-C248-BF46-8ED62BE89816}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FAE209E-9D52-3E4C-AD44-A7FB319A7B25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="340" yWindow="500" windowWidth="38400" windowHeight="19620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,12 @@
     <sheet name="Recipes" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Recipes!$A$1:$F$1</definedName>
+    <definedName name="Breakfast">_xlfn._xlws.FILTER(Recipes!$B$2:$B$1000, Recipes!$A$2:$A$1000="breakfast")</definedName>
+    <definedName name="Dinner">_xlfn._xlws.FILTER(Recipes!$B$2:$B$1000, Recipes!$A$2:$A$1000="dinner")</definedName>
+    <definedName name="Lunch">_xlfn._xlws.FILTER(Recipes!$B$2:$B$1000, Recipes!$A$2:$A$1000="lunch")</definedName>
     <definedName name="RecipeList">OFFSET(Recipes!$B$2, 0, 0, COUNTA(Recipes!$B:$B)-1, 1)</definedName>
+    <definedName name="Snacks">_xlfn._xlws.FILTER(Recipes!$B$2:$B$1000, Recipes!$A$2:$A$1000="snack")</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +42,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -325,6 +330,9 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="16">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" wrapText="1"/>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -441,9 +449,6 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" wrapText="1"/>
-    </dxf>
-    <dxf>
       <font>
         <b/>
         <strike val="0"/>
@@ -483,11 +488,11 @@
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Week"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Day"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Meal"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Meal Name" dataDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Calories" dataDxfId="13">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Meal Name" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Calories" dataDxfId="14">
       <calculatedColumnFormula>IFERROR(VLOOKUP(C2,#REF!, 2, FALSE), "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Cost" dataDxfId="12">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Cost" dataDxfId="13">
       <calculatedColumnFormula>IFERROR(VLOOKUP(C2,#REF!, 3, FALSE), "")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -496,17 +501,17 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table13" displayName="Table13" ref="G1:L59" totalsRowShown="0" headerRowDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table13" displayName="Table13" ref="G1:L59" totalsRowShown="0" headerRowDxfId="12">
   <autoFilter ref="G1:L59" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Week"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Day"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Meal"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Meal Name" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Calories" dataDxfId="9">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Meal Name" dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Calories" dataDxfId="10">
       <calculatedColumnFormula>IFERROR(VLOOKUP(J2,#REF!, 2, FALSE), "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Cost" dataDxfId="8">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Cost" dataDxfId="9">
       <calculatedColumnFormula>IFERROR(VLOOKUP(J2,#REF!, 3, FALSE), "")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -834,8 +839,8 @@
   <dimension ref="A1:L59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J44" sqref="J44"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2367,42 +2372,42 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E30">
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="8" operator="greaterThan">
       <formula>14000</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E59">
-    <cfRule type="cellIs" dxfId="6" priority="4" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="4" stopIfTrue="1" operator="greaterThan">
       <formula>14000</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F30">
-    <cfRule type="cellIs" dxfId="5" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="greaterThan">
       <formula>100</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F59">
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="greaterThan">
       <formula>100</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K30">
-    <cfRule type="cellIs" dxfId="3" priority="6" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="4" priority="6" stopIfTrue="1" operator="greaterThan">
       <formula>14000</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K59">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="greaterThan">
       <formula>14000</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L30">
-    <cfRule type="cellIs" dxfId="1" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="5" operator="greaterThan">
       <formula>100</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L59">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
       <formula>100</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2424,7 +2429,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
@@ -2434,6 +2439,7 @@
     <col min="3" max="3" width="20.83203125" customWidth="1"/>
     <col min="4" max="4" width="10.83203125" customWidth="1"/>
     <col min="5" max="6" width="50.83203125" style="3" customWidth="1"/>
+    <col min="10" max="10" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="17">
@@ -2617,6 +2623,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:F1" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
wb: helper table started for grocery list
</commit_message>
<xml_diff>
--- a/MealPrepTracker.xlsx
+++ b/MealPrepTracker.xlsx
@@ -8,16 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/quinnreams/Documents/GitHub/Personal-Growth-Planner/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE3C349F-9796-2948-B735-59C042BED304}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B755871-111C-2148-A21C-3C4E9DDC0118}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19620" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Meal Calendar" sheetId="1" r:id="rId1"/>
-    <sheet name="Recipes" sheetId="2" r:id="rId2"/>
+    <sheet name="Helper" sheetId="4" r:id="rId2"/>
+    <sheet name="Grocery List" sheetId="3" r:id="rId3"/>
+    <sheet name="Recipes" sheetId="2" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Recipes!$A$1:$F$387</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Recipes!$A$1:$F$387</definedName>
     <definedName name="Breakfast">_xlfn._xlws.FILTER(Recipes!$B$2:$B$1000, Recipes!$A$2:$A$1000="breakfast")</definedName>
     <definedName name="Dinner">_xlfn._xlws.FILTER(Recipes!$B$2:$B$1000, Recipes!$A$2:$A$1000="dinner")</definedName>
     <definedName name="Lunch">_xlfn._xlws.FILTER(Recipes!$B$2:$B$1000, Recipes!$A$2:$A$1000="lunch")</definedName>
@@ -42,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1710" uniqueCount="1186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1721" uniqueCount="1190">
   <si>
     <t>Week</t>
   </si>
@@ -3600,13 +3602,25 @@
   </si>
   <si>
     <t>https://www.delish.com/cooking/recipe-ideas/recipes/a20966/strawberry-fruit-roll-ups-recipe-del0313/</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>Ingredient</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Purchased</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -3649,6 +3663,14 @@
       <sz val="12"/>
       <name val="Aptos Narrow"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -3688,10 +3710,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3712,11 +3735,25 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="16">
+  <dxfs count="18">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -3798,6 +3835,16 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
@@ -3869,17 +3916,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:F59" totalsRowShown="0" headerRowDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:F59" totalsRowShown="0" headerRowDxfId="17">
   <autoFilter ref="A1:F59" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Week"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Day"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Meal"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Meal Name" dataDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Calories" dataDxfId="13">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Meal Name" dataDxfId="16"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Calories" dataDxfId="15">
       <calculatedColumnFormula>IFERROR(VLOOKUP(C2,#REF!, 2, FALSE), "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Cost" dataDxfId="12">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Cost" dataDxfId="14">
       <calculatedColumnFormula>IFERROR(VLOOKUP(C2,#REF!, 3, FALSE), "")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3888,17 +3935,17 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table13" displayName="Table13" ref="G1:L59" totalsRowShown="0" headerRowDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table13" displayName="Table13" ref="G1:L59" totalsRowShown="0" headerRowDxfId="13">
   <autoFilter ref="G1:L59" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Week"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Day"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Meal"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Meal Name" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Calories" dataDxfId="9">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Meal Name" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Calories" dataDxfId="11">
       <calculatedColumnFormula>IFERROR(VLOOKUP(J2,#REF!, 2, FALSE), "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Cost" dataDxfId="8">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Cost" dataDxfId="10">
       <calculatedColumnFormula>IFERROR(VLOOKUP(J2,#REF!, 3, FALSE), "")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4227,7 +4274,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J17" sqref="J17"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -5759,42 +5806,42 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E30">
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="8" operator="greaterThan">
       <formula>14000</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E59">
-    <cfRule type="cellIs" dxfId="6" priority="4" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="4" stopIfTrue="1" operator="greaterThan">
       <formula>14000</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F30">
-    <cfRule type="cellIs" dxfId="5" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="greaterThan">
       <formula>100</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F59">
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="greaterThan">
       <formula>100</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K30">
-    <cfRule type="cellIs" dxfId="3" priority="6" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="4" priority="6" stopIfTrue="1" operator="greaterThan">
       <formula>14000</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K59">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="greaterThan">
       <formula>14000</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L30">
-    <cfRule type="cellIs" dxfId="1" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="5" operator="greaterThan">
       <formula>100</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L59">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
       <formula>100</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5812,11 +5859,1973 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50723675-B2F4-E141-9E40-923361B6A99F}">
+  <dimension ref="A1:F201"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A153" workbookViewId="0">
+      <selection activeCell="C173" sqref="C173"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="str">
+        <f>IF('Meal Calendar'!D2&lt;&gt;"", 'Meal Calendar'!D2, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="str">
+        <f>IF('Meal Calendar'!D4&lt;&gt;"", 'Meal Calendar'!D4, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="str">
+        <f>IF('Meal Calendar'!D5&lt;&gt;"", 'Meal Calendar'!D5, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="str">
+        <f>IF('Meal Calendar'!D6&lt;&gt;"", 'Meal Calendar'!D6, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="C7" t="str">
+        <f>IF('Meal Calendar'!D7&lt;&gt;"", 'Meal Calendar'!D7, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="C8" t="str">
+        <f>IF('Meal Calendar'!D8&lt;&gt;"", 'Meal Calendar'!D8, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="C9" t="str">
+        <f>IF('Meal Calendar'!D9&lt;&gt;"", 'Meal Calendar'!D9, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="C10" t="str">
+        <f>IF('Meal Calendar'!D10&lt;&gt;"", 'Meal Calendar'!D10, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="C11" t="str">
+        <f>IF('Meal Calendar'!D11&lt;&gt;"", 'Meal Calendar'!D11, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="C12" t="str">
+        <f>IF('Meal Calendar'!D12&lt;&gt;"", 'Meal Calendar'!D12, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="C13" t="str">
+        <f>IF('Meal Calendar'!D13&lt;&gt;"", 'Meal Calendar'!D13, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="C14" t="str">
+        <f>IF('Meal Calendar'!D14&lt;&gt;"", 'Meal Calendar'!D14, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="C15" t="str">
+        <f>IF('Meal Calendar'!D15&lt;&gt;"", 'Meal Calendar'!D15, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="C16" t="str">
+        <f>IF('Meal Calendar'!D16&lt;&gt;"", 'Meal Calendar'!D16, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="C17" t="str">
+        <f>IF('Meal Calendar'!D17&lt;&gt;"", 'Meal Calendar'!D17, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="C18" t="str">
+        <f>IF('Meal Calendar'!D18&lt;&gt;"", 'Meal Calendar'!D18, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="C19" t="str">
+        <f>IF('Meal Calendar'!D19&lt;&gt;"", 'Meal Calendar'!D19, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="C20" t="str">
+        <f>IF('Meal Calendar'!D20&lt;&gt;"", 'Meal Calendar'!D20, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21">
+        <v>1</v>
+      </c>
+      <c r="C21" t="str">
+        <f>IF('Meal Calendar'!D21&lt;&gt;"", 'Meal Calendar'!D21, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="C22" t="str">
+        <f>IF('Meal Calendar'!D22&lt;&gt;"", 'Meal Calendar'!D22, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23">
+        <v>1</v>
+      </c>
+      <c r="C23" t="str">
+        <f>IF('Meal Calendar'!D23&lt;&gt;"", 'Meal Calendar'!D23, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24">
+        <v>1</v>
+      </c>
+      <c r="C24" t="str">
+        <f>IF('Meal Calendar'!D24&lt;&gt;"", 'Meal Calendar'!D24, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25">
+        <v>1</v>
+      </c>
+      <c r="C25" t="str">
+        <f>IF('Meal Calendar'!D25&lt;&gt;"", 'Meal Calendar'!D25, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26">
+        <v>1</v>
+      </c>
+      <c r="C26" t="str">
+        <f>IF('Meal Calendar'!D26&lt;&gt;"", 'Meal Calendar'!D26, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27">
+        <v>1</v>
+      </c>
+      <c r="C27" t="str">
+        <f>IF('Meal Calendar'!D27&lt;&gt;"", 'Meal Calendar'!D27, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28">
+        <v>1</v>
+      </c>
+      <c r="C28" t="str">
+        <f>IF('Meal Calendar'!D28&lt;&gt;"", 'Meal Calendar'!D28, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29">
+        <v>1</v>
+      </c>
+      <c r="C29" t="str">
+        <f>IF('Meal Calendar'!D29&lt;&gt;"", 'Meal Calendar'!D29, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30">
+        <v>1</v>
+      </c>
+      <c r="C30" t="str">
+        <f>IF('Meal Calendar'!D30&lt;&gt;"", 'Meal Calendar'!D30, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31">
+        <v>1</v>
+      </c>
+      <c r="C31" t="str">
+        <f>IF('Meal Calendar'!D31&lt;&gt;"", 'Meal Calendar'!D31, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32">
+        <v>1</v>
+      </c>
+      <c r="C32" t="str">
+        <f>IF('Meal Calendar'!D32&lt;&gt;"", 'Meal Calendar'!D32, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33">
+        <v>1</v>
+      </c>
+      <c r="C33" t="str">
+        <f>IF('Meal Calendar'!D33&lt;&gt;"", 'Meal Calendar'!D33, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34">
+        <v>1</v>
+      </c>
+      <c r="C34" t="str">
+        <f>IF('Meal Calendar'!D34&lt;&gt;"", 'Meal Calendar'!D34, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35">
+        <v>1</v>
+      </c>
+      <c r="C35" t="str">
+        <f>IF('Meal Calendar'!D35&lt;&gt;"", 'Meal Calendar'!D35, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36">
+        <v>1</v>
+      </c>
+      <c r="C36" t="str">
+        <f>IF('Meal Calendar'!D36&lt;&gt;"", 'Meal Calendar'!D36, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37">
+        <v>1</v>
+      </c>
+      <c r="C37" t="str">
+        <f>IF('Meal Calendar'!D37&lt;&gt;"", 'Meal Calendar'!D37, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38">
+        <v>1</v>
+      </c>
+      <c r="C38" t="str">
+        <f>IF('Meal Calendar'!D38&lt;&gt;"", 'Meal Calendar'!D38, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39">
+        <v>1</v>
+      </c>
+      <c r="C39" t="str">
+        <f>IF('Meal Calendar'!D39&lt;&gt;"", 'Meal Calendar'!D39, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40">
+        <v>1</v>
+      </c>
+      <c r="C40" t="str">
+        <f>IF('Meal Calendar'!D40&lt;&gt;"", 'Meal Calendar'!D40, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41">
+        <v>1</v>
+      </c>
+      <c r="C41" t="str">
+        <f>IF('Meal Calendar'!D41&lt;&gt;"", 'Meal Calendar'!D41, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42">
+        <v>1</v>
+      </c>
+      <c r="C42" t="str">
+        <f>IF('Meal Calendar'!D42&lt;&gt;"", 'Meal Calendar'!D42, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43">
+        <v>1</v>
+      </c>
+      <c r="C43" t="str">
+        <f>IF('Meal Calendar'!D43&lt;&gt;"", 'Meal Calendar'!D43, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44">
+        <v>1</v>
+      </c>
+      <c r="C44" t="str">
+        <f>IF('Meal Calendar'!D44&lt;&gt;"", 'Meal Calendar'!D44, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45">
+        <v>1</v>
+      </c>
+      <c r="C45" t="str">
+        <f>IF('Meal Calendar'!D45&lt;&gt;"", 'Meal Calendar'!D45, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46">
+        <v>1</v>
+      </c>
+      <c r="C46" t="str">
+        <f>IF('Meal Calendar'!D46&lt;&gt;"", 'Meal Calendar'!D46, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47">
+        <v>1</v>
+      </c>
+      <c r="C47" t="str">
+        <f>IF('Meal Calendar'!D47&lt;&gt;"", 'Meal Calendar'!D47, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48">
+        <v>1</v>
+      </c>
+      <c r="C48" t="str">
+        <f>IF('Meal Calendar'!D48&lt;&gt;"", 'Meal Calendar'!D48, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49">
+        <v>1</v>
+      </c>
+      <c r="C49" t="str">
+        <f>IF('Meal Calendar'!D49&lt;&gt;"", 'Meal Calendar'!D49, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50">
+        <v>1</v>
+      </c>
+      <c r="C50" t="str">
+        <f>IF('Meal Calendar'!D50&lt;&gt;"", 'Meal Calendar'!D50, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51">
+        <v>1</v>
+      </c>
+      <c r="C51" t="str">
+        <f>IF('Meal Calendar'!D51&lt;&gt;"", 'Meal Calendar'!D51, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52">
+        <v>2</v>
+      </c>
+      <c r="C52" t="str">
+        <f>IF('Meal Calendar'!D52&lt;&gt;"", 'Meal Calendar'!D52, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54">
+        <v>2</v>
+      </c>
+      <c r="C54" t="str">
+        <f>IF('Meal Calendar'!D54&lt;&gt;"", 'Meal Calendar'!D54, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55">
+        <v>2</v>
+      </c>
+      <c r="C55" t="str">
+        <f>IF('Meal Calendar'!D55&lt;&gt;"", 'Meal Calendar'!D55, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56">
+        <v>2</v>
+      </c>
+      <c r="C56" t="str">
+        <f>IF('Meal Calendar'!D56&lt;&gt;"", 'Meal Calendar'!D56, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57">
+        <v>2</v>
+      </c>
+      <c r="C57" t="str">
+        <f>IF('Meal Calendar'!D57&lt;&gt;"", 'Meal Calendar'!D57, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58">
+        <v>2</v>
+      </c>
+      <c r="C58" t="str">
+        <f>IF('Meal Calendar'!D58&lt;&gt;"", 'Meal Calendar'!D58, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59">
+        <v>2</v>
+      </c>
+      <c r="C59" t="str">
+        <f>IF('Meal Calendar'!D59&lt;&gt;"", 'Meal Calendar'!D59, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60">
+        <v>2</v>
+      </c>
+      <c r="C60" t="str">
+        <f>IF('Meal Calendar'!D60&lt;&gt;"", 'Meal Calendar'!D60, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61">
+        <v>2</v>
+      </c>
+      <c r="C61" t="str">
+        <f>IF('Meal Calendar'!D61&lt;&gt;"", 'Meal Calendar'!D61, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62">
+        <v>2</v>
+      </c>
+      <c r="C62" t="str">
+        <f>IF('Meal Calendar'!D62&lt;&gt;"", 'Meal Calendar'!D62, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63">
+        <v>2</v>
+      </c>
+      <c r="C63" t="str">
+        <f>IF('Meal Calendar'!D63&lt;&gt;"", 'Meal Calendar'!D63, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64">
+        <v>2</v>
+      </c>
+      <c r="C64" t="str">
+        <f>IF('Meal Calendar'!D64&lt;&gt;"", 'Meal Calendar'!D64, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65">
+        <v>2</v>
+      </c>
+      <c r="C65" t="str">
+        <f>IF('Meal Calendar'!D65&lt;&gt;"", 'Meal Calendar'!D65, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66">
+        <v>2</v>
+      </c>
+      <c r="C66" t="str">
+        <f>IF('Meal Calendar'!D66&lt;&gt;"", 'Meal Calendar'!D66, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67">
+        <v>2</v>
+      </c>
+      <c r="C67" t="str">
+        <f>IF('Meal Calendar'!D67&lt;&gt;"", 'Meal Calendar'!D67, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68">
+        <v>2</v>
+      </c>
+      <c r="C68" t="str">
+        <f>IF('Meal Calendar'!D68&lt;&gt;"", 'Meal Calendar'!D68, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69">
+        <v>2</v>
+      </c>
+      <c r="C69" t="str">
+        <f>IF('Meal Calendar'!D69&lt;&gt;"", 'Meal Calendar'!D69, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70">
+        <v>2</v>
+      </c>
+      <c r="C70" t="str">
+        <f>IF('Meal Calendar'!D70&lt;&gt;"", 'Meal Calendar'!D70, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71">
+        <v>2</v>
+      </c>
+      <c r="C71" t="str">
+        <f>IF('Meal Calendar'!D71&lt;&gt;"", 'Meal Calendar'!D71, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72">
+        <v>2</v>
+      </c>
+      <c r="C72" t="str">
+        <f>IF('Meal Calendar'!D72&lt;&gt;"", 'Meal Calendar'!D72, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73">
+        <v>2</v>
+      </c>
+      <c r="C73" t="str">
+        <f>IF('Meal Calendar'!D73&lt;&gt;"", 'Meal Calendar'!D73, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74">
+        <v>2</v>
+      </c>
+      <c r="C74" t="str">
+        <f>IF('Meal Calendar'!D74&lt;&gt;"", 'Meal Calendar'!D74, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75">
+        <v>2</v>
+      </c>
+      <c r="C75" t="str">
+        <f>IF('Meal Calendar'!D75&lt;&gt;"", 'Meal Calendar'!D75, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76">
+        <v>2</v>
+      </c>
+      <c r="C76" t="str">
+        <f>IF('Meal Calendar'!D76&lt;&gt;"", 'Meal Calendar'!D76, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77">
+        <v>2</v>
+      </c>
+      <c r="C77" t="str">
+        <f>IF('Meal Calendar'!D77&lt;&gt;"", 'Meal Calendar'!D77, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78">
+        <v>2</v>
+      </c>
+      <c r="C78" t="str">
+        <f>IF('Meal Calendar'!D78&lt;&gt;"", 'Meal Calendar'!D78, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="A79">
+        <v>2</v>
+      </c>
+      <c r="C79" t="str">
+        <f>IF('Meal Calendar'!D79&lt;&gt;"", 'Meal Calendar'!D79, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="A80">
+        <v>2</v>
+      </c>
+      <c r="C80" t="str">
+        <f>IF('Meal Calendar'!D80&lt;&gt;"", 'Meal Calendar'!D80, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81">
+        <v>2</v>
+      </c>
+      <c r="C81" t="str">
+        <f>IF('Meal Calendar'!D81&lt;&gt;"", 'Meal Calendar'!D81, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="A82">
+        <v>2</v>
+      </c>
+      <c r="C82" t="str">
+        <f>IF('Meal Calendar'!D82&lt;&gt;"", 'Meal Calendar'!D82, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
+      <c r="A83">
+        <v>2</v>
+      </c>
+      <c r="C83" t="str">
+        <f>IF('Meal Calendar'!D83&lt;&gt;"", 'Meal Calendar'!D83, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
+      <c r="A84">
+        <v>2</v>
+      </c>
+      <c r="C84" t="str">
+        <f>IF('Meal Calendar'!D84&lt;&gt;"", 'Meal Calendar'!D84, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
+      <c r="A85">
+        <v>2</v>
+      </c>
+      <c r="C85" t="str">
+        <f>IF('Meal Calendar'!D85&lt;&gt;"", 'Meal Calendar'!D85, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
+      <c r="A86">
+        <v>2</v>
+      </c>
+      <c r="C86" t="str">
+        <f>IF('Meal Calendar'!D86&lt;&gt;"", 'Meal Calendar'!D86, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
+      <c r="A87">
+        <v>2</v>
+      </c>
+      <c r="C87" t="str">
+        <f>IF('Meal Calendar'!D87&lt;&gt;"", 'Meal Calendar'!D87, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
+      <c r="A88">
+        <v>2</v>
+      </c>
+      <c r="C88" t="str">
+        <f>IF('Meal Calendar'!D88&lt;&gt;"", 'Meal Calendar'!D88, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="89" spans="1:3">
+      <c r="A89">
+        <v>2</v>
+      </c>
+      <c r="C89" t="str">
+        <f>IF('Meal Calendar'!D89&lt;&gt;"", 'Meal Calendar'!D89, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="90" spans="1:3">
+      <c r="A90">
+        <v>2</v>
+      </c>
+      <c r="C90" t="str">
+        <f>IF('Meal Calendar'!D90&lt;&gt;"", 'Meal Calendar'!D90, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="91" spans="1:3">
+      <c r="A91">
+        <v>2</v>
+      </c>
+      <c r="C91" t="str">
+        <f>IF('Meal Calendar'!D91&lt;&gt;"", 'Meal Calendar'!D91, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="92" spans="1:3">
+      <c r="A92">
+        <v>2</v>
+      </c>
+      <c r="C92" t="str">
+        <f>IF('Meal Calendar'!D92&lt;&gt;"", 'Meal Calendar'!D92, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="93" spans="1:3">
+      <c r="A93">
+        <v>2</v>
+      </c>
+      <c r="C93" t="str">
+        <f>IF('Meal Calendar'!D93&lt;&gt;"", 'Meal Calendar'!D93, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="94" spans="1:3">
+      <c r="A94">
+        <v>2</v>
+      </c>
+      <c r="C94" t="str">
+        <f>IF('Meal Calendar'!D94&lt;&gt;"", 'Meal Calendar'!D94, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="95" spans="1:3">
+      <c r="A95">
+        <v>2</v>
+      </c>
+      <c r="C95" t="str">
+        <f>IF('Meal Calendar'!D95&lt;&gt;"", 'Meal Calendar'!D95, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="96" spans="1:3">
+      <c r="A96">
+        <v>2</v>
+      </c>
+      <c r="C96" t="str">
+        <f>IF('Meal Calendar'!D96&lt;&gt;"", 'Meal Calendar'!D96, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="97" spans="1:3">
+      <c r="A97">
+        <v>2</v>
+      </c>
+      <c r="C97" t="str">
+        <f>IF('Meal Calendar'!D97&lt;&gt;"", 'Meal Calendar'!D97, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="98" spans="1:3">
+      <c r="A98">
+        <v>2</v>
+      </c>
+      <c r="C98" t="str">
+        <f>IF('Meal Calendar'!D98&lt;&gt;"", 'Meal Calendar'!D98, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="99" spans="1:3">
+      <c r="A99">
+        <v>2</v>
+      </c>
+      <c r="C99" t="str">
+        <f>IF('Meal Calendar'!D99&lt;&gt;"", 'Meal Calendar'!D99, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="100" spans="1:3">
+      <c r="A100">
+        <v>2</v>
+      </c>
+      <c r="C100" t="str">
+        <f>IF('Meal Calendar'!D100&lt;&gt;"", 'Meal Calendar'!D100, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="101" spans="1:3">
+      <c r="A101">
+        <v>2</v>
+      </c>
+      <c r="C101" t="str">
+        <f>IF('Meal Calendar'!D101&lt;&gt;"", 'Meal Calendar'!D101, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="102" spans="1:3">
+      <c r="A102">
+        <v>3</v>
+      </c>
+      <c r="C102" t="str">
+        <f>IF('Meal Calendar'!J2&lt;&gt;"", 'Meal Calendar'!J2, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="103" spans="1:3">
+      <c r="A103">
+        <v>3</v>
+      </c>
+      <c r="C103" t="str">
+        <f>IF('Meal Calendar'!J3&lt;&gt;"", 'Meal Calendar'!J3, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="104" spans="1:3">
+      <c r="A104">
+        <v>3</v>
+      </c>
+      <c r="C104" t="str">
+        <f>IF('Meal Calendar'!J4&lt;&gt;"", 'Meal Calendar'!J4, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="105" spans="1:3">
+      <c r="A105">
+        <v>3</v>
+      </c>
+      <c r="C105" t="str">
+        <f>IF('Meal Calendar'!J5&lt;&gt;"", 'Meal Calendar'!J5, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="106" spans="1:3">
+      <c r="A106">
+        <v>3</v>
+      </c>
+      <c r="C106" t="str">
+        <f>IF('Meal Calendar'!J6&lt;&gt;"", 'Meal Calendar'!J6, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="107" spans="1:3">
+      <c r="A107">
+        <v>3</v>
+      </c>
+      <c r="C107" t="str">
+        <f>IF('Meal Calendar'!J7&lt;&gt;"", 'Meal Calendar'!J7, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="108" spans="1:3">
+      <c r="A108">
+        <v>3</v>
+      </c>
+      <c r="C108" t="str">
+        <f>IF('Meal Calendar'!J8&lt;&gt;"", 'Meal Calendar'!J8, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="109" spans="1:3">
+      <c r="A109">
+        <v>3</v>
+      </c>
+      <c r="C109" t="str">
+        <f>IF('Meal Calendar'!J9&lt;&gt;"", 'Meal Calendar'!J9, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="110" spans="1:3">
+      <c r="A110">
+        <v>3</v>
+      </c>
+      <c r="C110" t="str">
+        <f>IF('Meal Calendar'!J10&lt;&gt;"", 'Meal Calendar'!J10, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="111" spans="1:3">
+      <c r="A111">
+        <v>3</v>
+      </c>
+      <c r="C111" t="str">
+        <f>IF('Meal Calendar'!J11&lt;&gt;"", 'Meal Calendar'!J11, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="112" spans="1:3">
+      <c r="A112">
+        <v>3</v>
+      </c>
+      <c r="C112" t="str">
+        <f>IF('Meal Calendar'!J12&lt;&gt;"", 'Meal Calendar'!J12, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="113" spans="1:3">
+      <c r="A113">
+        <v>3</v>
+      </c>
+      <c r="C113" t="str">
+        <f>IF('Meal Calendar'!J13&lt;&gt;"", 'Meal Calendar'!J13, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="114" spans="1:3">
+      <c r="A114">
+        <v>3</v>
+      </c>
+      <c r="C114" t="str">
+        <f>IF('Meal Calendar'!J14&lt;&gt;"", 'Meal Calendar'!J14, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="115" spans="1:3">
+      <c r="A115">
+        <v>3</v>
+      </c>
+      <c r="C115" t="str">
+        <f>IF('Meal Calendar'!J15&lt;&gt;"", 'Meal Calendar'!J15, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="116" spans="1:3">
+      <c r="A116">
+        <v>3</v>
+      </c>
+      <c r="C116" t="str">
+        <f>IF('Meal Calendar'!J16&lt;&gt;"", 'Meal Calendar'!J16, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="117" spans="1:3">
+      <c r="A117">
+        <v>3</v>
+      </c>
+      <c r="C117" t="str">
+        <f>IF('Meal Calendar'!J17&lt;&gt;"", 'Meal Calendar'!J17, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="118" spans="1:3">
+      <c r="A118">
+        <v>3</v>
+      </c>
+      <c r="C118" t="str">
+        <f>IF('Meal Calendar'!J18&lt;&gt;"", 'Meal Calendar'!J18, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="119" spans="1:3">
+      <c r="A119">
+        <v>3</v>
+      </c>
+      <c r="C119" t="str">
+        <f>IF('Meal Calendar'!J19&lt;&gt;"", 'Meal Calendar'!J19, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="120" spans="1:3">
+      <c r="A120">
+        <v>3</v>
+      </c>
+      <c r="C120" t="str">
+        <f>IF('Meal Calendar'!J20&lt;&gt;"", 'Meal Calendar'!J20, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="121" spans="1:3">
+      <c r="A121">
+        <v>3</v>
+      </c>
+      <c r="C121" t="str">
+        <f>IF('Meal Calendar'!J21&lt;&gt;"", 'Meal Calendar'!J21, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="122" spans="1:3">
+      <c r="A122">
+        <v>3</v>
+      </c>
+      <c r="C122" t="str">
+        <f>IF('Meal Calendar'!J22&lt;&gt;"", 'Meal Calendar'!J22, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="123" spans="1:3">
+      <c r="A123">
+        <v>3</v>
+      </c>
+      <c r="C123" t="str">
+        <f>IF('Meal Calendar'!J23&lt;&gt;"", 'Meal Calendar'!J23, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="124" spans="1:3">
+      <c r="A124">
+        <v>3</v>
+      </c>
+      <c r="C124" t="str">
+        <f>IF('Meal Calendar'!J24&lt;&gt;"", 'Meal Calendar'!J24, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="125" spans="1:3">
+      <c r="A125">
+        <v>3</v>
+      </c>
+      <c r="C125" t="str">
+        <f>IF('Meal Calendar'!J25&lt;&gt;"", 'Meal Calendar'!J25, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="126" spans="1:3">
+      <c r="A126">
+        <v>3</v>
+      </c>
+      <c r="C126" t="str">
+        <f>IF('Meal Calendar'!J26&lt;&gt;"", 'Meal Calendar'!J26, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="127" spans="1:3">
+      <c r="A127">
+        <v>3</v>
+      </c>
+      <c r="C127" t="str">
+        <f>IF('Meal Calendar'!J27&lt;&gt;"", 'Meal Calendar'!J27, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="128" spans="1:3">
+      <c r="A128">
+        <v>3</v>
+      </c>
+      <c r="C128" t="str">
+        <f>IF('Meal Calendar'!J28&lt;&gt;"", 'Meal Calendar'!J28, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="129" spans="1:3">
+      <c r="A129">
+        <v>3</v>
+      </c>
+      <c r="C129" t="str">
+        <f>IF('Meal Calendar'!J29&lt;&gt;"", 'Meal Calendar'!J29, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="130" spans="1:3">
+      <c r="A130">
+        <v>3</v>
+      </c>
+      <c r="C130" t="str">
+        <f>IF('Meal Calendar'!J30&lt;&gt;"", 'Meal Calendar'!J30, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="131" spans="1:3">
+      <c r="A131">
+        <v>3</v>
+      </c>
+      <c r="C131" t="str">
+        <f>IF('Meal Calendar'!J31&lt;&gt;"", 'Meal Calendar'!J31, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="132" spans="1:3">
+      <c r="A132">
+        <v>3</v>
+      </c>
+      <c r="C132" t="str">
+        <f>IF('Meal Calendar'!J32&lt;&gt;"", 'Meal Calendar'!J32, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="133" spans="1:3">
+      <c r="A133">
+        <v>3</v>
+      </c>
+      <c r="C133" t="str">
+        <f>IF('Meal Calendar'!J33&lt;&gt;"", 'Meal Calendar'!J33, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="134" spans="1:3">
+      <c r="A134">
+        <v>3</v>
+      </c>
+      <c r="C134" t="str">
+        <f>IF('Meal Calendar'!J34&lt;&gt;"", 'Meal Calendar'!J34, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="135" spans="1:3">
+      <c r="A135">
+        <v>3</v>
+      </c>
+      <c r="C135" t="str">
+        <f>IF('Meal Calendar'!J35&lt;&gt;"", 'Meal Calendar'!J35, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="136" spans="1:3">
+      <c r="A136">
+        <v>3</v>
+      </c>
+      <c r="C136" t="str">
+        <f>IF('Meal Calendar'!J36&lt;&gt;"", 'Meal Calendar'!J36, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="137" spans="1:3">
+      <c r="A137">
+        <v>3</v>
+      </c>
+      <c r="C137" t="str">
+        <f>IF('Meal Calendar'!J37&lt;&gt;"", 'Meal Calendar'!J37, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="138" spans="1:3">
+      <c r="A138">
+        <v>3</v>
+      </c>
+      <c r="C138" t="str">
+        <f>IF('Meal Calendar'!J38&lt;&gt;"", 'Meal Calendar'!J38, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="139" spans="1:3">
+      <c r="A139">
+        <v>3</v>
+      </c>
+      <c r="C139" t="str">
+        <f>IF('Meal Calendar'!J39&lt;&gt;"", 'Meal Calendar'!J39, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="140" spans="1:3">
+      <c r="A140">
+        <v>3</v>
+      </c>
+      <c r="C140" t="str">
+        <f>IF('Meal Calendar'!J40&lt;&gt;"", 'Meal Calendar'!J40, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="141" spans="1:3">
+      <c r="A141">
+        <v>3</v>
+      </c>
+      <c r="C141" t="str">
+        <f>IF('Meal Calendar'!J41&lt;&gt;"", 'Meal Calendar'!J41, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="142" spans="1:3">
+      <c r="A142">
+        <v>3</v>
+      </c>
+      <c r="C142" t="str">
+        <f>IF('Meal Calendar'!J42&lt;&gt;"", 'Meal Calendar'!J42, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="143" spans="1:3">
+      <c r="A143">
+        <v>3</v>
+      </c>
+      <c r="C143" t="str">
+        <f>IF('Meal Calendar'!J43&lt;&gt;"", 'Meal Calendar'!J43, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="144" spans="1:3">
+      <c r="A144">
+        <v>3</v>
+      </c>
+      <c r="C144" t="str">
+        <f>IF('Meal Calendar'!J44&lt;&gt;"", 'Meal Calendar'!J44, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="145" spans="1:3">
+      <c r="A145">
+        <v>3</v>
+      </c>
+      <c r="C145" t="str">
+        <f>IF('Meal Calendar'!J45&lt;&gt;"", 'Meal Calendar'!J45, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="146" spans="1:3">
+      <c r="A146">
+        <v>3</v>
+      </c>
+      <c r="C146" t="str">
+        <f>IF('Meal Calendar'!J46&lt;&gt;"", 'Meal Calendar'!J46, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="147" spans="1:3">
+      <c r="A147">
+        <v>3</v>
+      </c>
+      <c r="C147" t="str">
+        <f>IF('Meal Calendar'!J47&lt;&gt;"", 'Meal Calendar'!J47, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="148" spans="1:3">
+      <c r="A148">
+        <v>3</v>
+      </c>
+      <c r="C148" t="str">
+        <f>IF('Meal Calendar'!J48&lt;&gt;"", 'Meal Calendar'!J48, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="149" spans="1:3">
+      <c r="A149">
+        <v>3</v>
+      </c>
+      <c r="C149" t="str">
+        <f>IF('Meal Calendar'!J49&lt;&gt;"", 'Meal Calendar'!J49, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="150" spans="1:3">
+      <c r="A150">
+        <v>3</v>
+      </c>
+      <c r="C150" t="str">
+        <f>IF('Meal Calendar'!J50&lt;&gt;"", 'Meal Calendar'!J50, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="151" spans="1:3">
+      <c r="A151">
+        <v>3</v>
+      </c>
+      <c r="C151" t="str">
+        <f>IF('Meal Calendar'!J51&lt;&gt;"", 'Meal Calendar'!J51, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="152" spans="1:3">
+      <c r="A152">
+        <v>4</v>
+      </c>
+      <c r="C152" t="str">
+        <f>IF('Meal Calendar'!J52&lt;&gt;"", 'Meal Calendar'!J52, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="153" spans="1:3">
+      <c r="A153">
+        <v>4</v>
+      </c>
+      <c r="C153" t="str">
+        <f>IF('Meal Calendar'!J53&lt;&gt;"", 'Meal Calendar'!J53, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="154" spans="1:3">
+      <c r="A154">
+        <v>4</v>
+      </c>
+      <c r="C154" t="str">
+        <f>IF('Meal Calendar'!J54&lt;&gt;"", 'Meal Calendar'!J54, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="155" spans="1:3">
+      <c r="A155">
+        <v>4</v>
+      </c>
+      <c r="C155" t="str">
+        <f>IF('Meal Calendar'!J55&lt;&gt;"", 'Meal Calendar'!J55, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="156" spans="1:3">
+      <c r="A156">
+        <v>4</v>
+      </c>
+      <c r="C156" t="str">
+        <f>IF('Meal Calendar'!J56&lt;&gt;"", 'Meal Calendar'!J56, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="157" spans="1:3">
+      <c r="A157">
+        <v>4</v>
+      </c>
+      <c r="C157" t="str">
+        <f>IF('Meal Calendar'!J57&lt;&gt;"", 'Meal Calendar'!J57, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="158" spans="1:3">
+      <c r="A158">
+        <v>4</v>
+      </c>
+      <c r="C158" t="str">
+        <f>IF('Meal Calendar'!J58&lt;&gt;"", 'Meal Calendar'!J58, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="159" spans="1:3">
+      <c r="A159">
+        <v>4</v>
+      </c>
+      <c r="C159" t="str">
+        <f>IF('Meal Calendar'!J59&lt;&gt;"", 'Meal Calendar'!J59, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="160" spans="1:3">
+      <c r="A160">
+        <v>4</v>
+      </c>
+      <c r="C160" t="str">
+        <f>IF('Meal Calendar'!J60&lt;&gt;"", 'Meal Calendar'!J60, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="161" spans="1:3">
+      <c r="A161">
+        <v>4</v>
+      </c>
+      <c r="C161" t="str">
+        <f>IF('Meal Calendar'!J61&lt;&gt;"", 'Meal Calendar'!J61, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="162" spans="1:3">
+      <c r="A162">
+        <v>4</v>
+      </c>
+      <c r="C162" t="str">
+        <f>IF('Meal Calendar'!J62&lt;&gt;"", 'Meal Calendar'!J62, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="163" spans="1:3">
+      <c r="A163">
+        <v>4</v>
+      </c>
+      <c r="C163" t="str">
+        <f>IF('Meal Calendar'!J63&lt;&gt;"", 'Meal Calendar'!J63, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="164" spans="1:3">
+      <c r="A164">
+        <v>4</v>
+      </c>
+      <c r="C164" t="str">
+        <f>IF('Meal Calendar'!J64&lt;&gt;"", 'Meal Calendar'!J64, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="165" spans="1:3">
+      <c r="A165">
+        <v>4</v>
+      </c>
+      <c r="C165" t="str">
+        <f>IF('Meal Calendar'!J65&lt;&gt;"", 'Meal Calendar'!J65, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="166" spans="1:3">
+      <c r="A166">
+        <v>4</v>
+      </c>
+      <c r="C166" t="str">
+        <f>IF('Meal Calendar'!J66&lt;&gt;"", 'Meal Calendar'!J66, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="167" spans="1:3">
+      <c r="A167">
+        <v>4</v>
+      </c>
+      <c r="C167" t="str">
+        <f>IF('Meal Calendar'!J67&lt;&gt;"", 'Meal Calendar'!J67, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="168" spans="1:3">
+      <c r="A168">
+        <v>4</v>
+      </c>
+      <c r="C168" t="str">
+        <f>IF('Meal Calendar'!J68&lt;&gt;"", 'Meal Calendar'!J68, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="169" spans="1:3">
+      <c r="A169">
+        <v>4</v>
+      </c>
+      <c r="C169" t="str">
+        <f>IF('Meal Calendar'!J69&lt;&gt;"", 'Meal Calendar'!J69, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="170" spans="1:3">
+      <c r="A170">
+        <v>4</v>
+      </c>
+      <c r="C170" t="str">
+        <f>IF('Meal Calendar'!J70&lt;&gt;"", 'Meal Calendar'!J70, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="171" spans="1:3">
+      <c r="A171">
+        <v>4</v>
+      </c>
+      <c r="C171" t="str">
+        <f>IF('Meal Calendar'!J71&lt;&gt;"", 'Meal Calendar'!J71, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="172" spans="1:3">
+      <c r="A172">
+        <v>4</v>
+      </c>
+      <c r="C172" t="str">
+        <f>IF('Meal Calendar'!J72&lt;&gt;"", 'Meal Calendar'!J72, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="173" spans="1:3">
+      <c r="A173">
+        <v>4</v>
+      </c>
+      <c r="C173" t="str">
+        <f>IF('Meal Calendar'!J73&lt;&gt;"", 'Meal Calendar'!J73, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="174" spans="1:3">
+      <c r="A174">
+        <v>4</v>
+      </c>
+      <c r="C174" t="str">
+        <f>IF('Meal Calendar'!J74&lt;&gt;"", 'Meal Calendar'!J74, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="175" spans="1:3">
+      <c r="A175">
+        <v>4</v>
+      </c>
+      <c r="C175" t="str">
+        <f>IF('Meal Calendar'!J75&lt;&gt;"", 'Meal Calendar'!J75, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="176" spans="1:3">
+      <c r="A176">
+        <v>4</v>
+      </c>
+      <c r="C176" t="str">
+        <f>IF('Meal Calendar'!J76&lt;&gt;"", 'Meal Calendar'!J76, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="177" spans="1:3">
+      <c r="A177">
+        <v>4</v>
+      </c>
+      <c r="C177" t="str">
+        <f>IF('Meal Calendar'!J77&lt;&gt;"", 'Meal Calendar'!J77, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="178" spans="1:3">
+      <c r="A178">
+        <v>4</v>
+      </c>
+      <c r="C178" t="str">
+        <f>IF('Meal Calendar'!J78&lt;&gt;"", 'Meal Calendar'!J78, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="179" spans="1:3">
+      <c r="A179">
+        <v>4</v>
+      </c>
+      <c r="C179" t="str">
+        <f>IF('Meal Calendar'!J79&lt;&gt;"", 'Meal Calendar'!J79, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="180" spans="1:3">
+      <c r="A180">
+        <v>4</v>
+      </c>
+      <c r="C180" t="str">
+        <f>IF('Meal Calendar'!J80&lt;&gt;"", 'Meal Calendar'!J80, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="181" spans="1:3">
+      <c r="A181">
+        <v>4</v>
+      </c>
+      <c r="C181" t="str">
+        <f>IF('Meal Calendar'!J81&lt;&gt;"", 'Meal Calendar'!J81, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="182" spans="1:3">
+      <c r="A182">
+        <v>4</v>
+      </c>
+      <c r="C182" t="str">
+        <f>IF('Meal Calendar'!J82&lt;&gt;"", 'Meal Calendar'!J82, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="183" spans="1:3">
+      <c r="A183">
+        <v>4</v>
+      </c>
+      <c r="C183" t="str">
+        <f>IF('Meal Calendar'!J83&lt;&gt;"", 'Meal Calendar'!J83, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="184" spans="1:3">
+      <c r="A184">
+        <v>4</v>
+      </c>
+      <c r="C184" t="str">
+        <f>IF('Meal Calendar'!J84&lt;&gt;"", 'Meal Calendar'!J84, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="185" spans="1:3">
+      <c r="A185">
+        <v>4</v>
+      </c>
+      <c r="C185" t="str">
+        <f>IF('Meal Calendar'!J85&lt;&gt;"", 'Meal Calendar'!J85, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="186" spans="1:3">
+      <c r="A186">
+        <v>4</v>
+      </c>
+      <c r="C186" t="str">
+        <f>IF('Meal Calendar'!J86&lt;&gt;"", 'Meal Calendar'!J86, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="187" spans="1:3">
+      <c r="A187">
+        <v>4</v>
+      </c>
+      <c r="C187" t="str">
+        <f>IF('Meal Calendar'!J87&lt;&gt;"", 'Meal Calendar'!J87, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="188" spans="1:3">
+      <c r="A188">
+        <v>4</v>
+      </c>
+      <c r="C188" t="str">
+        <f>IF('Meal Calendar'!J88&lt;&gt;"", 'Meal Calendar'!J88, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="189" spans="1:3">
+      <c r="A189">
+        <v>4</v>
+      </c>
+      <c r="C189" t="str">
+        <f>IF('Meal Calendar'!J89&lt;&gt;"", 'Meal Calendar'!J89, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="190" spans="1:3">
+      <c r="A190">
+        <v>4</v>
+      </c>
+      <c r="C190" t="str">
+        <f>IF('Meal Calendar'!J90&lt;&gt;"", 'Meal Calendar'!J90, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="191" spans="1:3">
+      <c r="A191">
+        <v>4</v>
+      </c>
+      <c r="C191" t="str">
+        <f>IF('Meal Calendar'!J91&lt;&gt;"", 'Meal Calendar'!J91, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="192" spans="1:3">
+      <c r="A192">
+        <v>4</v>
+      </c>
+      <c r="C192" t="str">
+        <f>IF('Meal Calendar'!J92&lt;&gt;"", 'Meal Calendar'!J92, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="193" spans="1:3">
+      <c r="A193">
+        <v>4</v>
+      </c>
+      <c r="C193" t="str">
+        <f>IF('Meal Calendar'!J93&lt;&gt;"", 'Meal Calendar'!J93, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="194" spans="1:3">
+      <c r="A194">
+        <v>4</v>
+      </c>
+      <c r="C194" t="str">
+        <f>IF('Meal Calendar'!J94&lt;&gt;"", 'Meal Calendar'!J94, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="195" spans="1:3">
+      <c r="A195">
+        <v>4</v>
+      </c>
+      <c r="C195" t="str">
+        <f>IF('Meal Calendar'!J95&lt;&gt;"", 'Meal Calendar'!J95, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="196" spans="1:3">
+      <c r="A196">
+        <v>4</v>
+      </c>
+      <c r="C196" t="str">
+        <f>IF('Meal Calendar'!J96&lt;&gt;"", 'Meal Calendar'!J96, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="197" spans="1:3">
+      <c r="A197">
+        <v>4</v>
+      </c>
+      <c r="C197" t="str">
+        <f>IF('Meal Calendar'!J97&lt;&gt;"", 'Meal Calendar'!J97, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="198" spans="1:3">
+      <c r="A198">
+        <v>4</v>
+      </c>
+      <c r="C198" t="str">
+        <f>IF('Meal Calendar'!J98&lt;&gt;"", 'Meal Calendar'!J98, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="199" spans="1:3">
+      <c r="A199">
+        <v>4</v>
+      </c>
+      <c r="C199" t="str">
+        <f>IF('Meal Calendar'!J99&lt;&gt;"", 'Meal Calendar'!J99, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="200" spans="1:3">
+      <c r="A200">
+        <v>4</v>
+      </c>
+      <c r="C200" t="str">
+        <f>IF('Meal Calendar'!J100&lt;&gt;"", 'Meal Calendar'!J100, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="201" spans="1:3">
+      <c r="A201">
+        <v>4</v>
+      </c>
+      <c r="C201" t="str">
+        <f>IF('Meal Calendar'!J101&lt;&gt;"", 'Meal Calendar'!J101, "")</f>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA4164A3-C298-314D-8211-F5B8F16F83E1}">
+  <dimension ref="A1:E100"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="5" width="20.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="30" customHeight="1">
+      <c r="A1" t="s">
+        <v>1189</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1187</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1188</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1186</v>
+      </c>
+      <c r="E1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="30" customHeight="1"/>
+    <row r="3" spans="1:5" ht="30" customHeight="1"/>
+    <row r="4" spans="1:5" ht="30" customHeight="1"/>
+    <row r="5" spans="1:5" ht="30" customHeight="1"/>
+    <row r="6" spans="1:5" ht="30" customHeight="1"/>
+    <row r="7" spans="1:5" ht="30" customHeight="1"/>
+    <row r="8" spans="1:5" ht="30" customHeight="1"/>
+    <row r="9" spans="1:5" ht="30" customHeight="1"/>
+    <row r="10" spans="1:5" ht="30" customHeight="1"/>
+    <row r="11" spans="1:5" ht="30" customHeight="1"/>
+    <row r="12" spans="1:5" ht="30" customHeight="1"/>
+    <row r="13" spans="1:5" ht="30" customHeight="1"/>
+    <row r="14" spans="1:5" ht="30" customHeight="1"/>
+    <row r="15" spans="1:5" ht="30" customHeight="1"/>
+    <row r="16" spans="1:5" ht="30" customHeight="1"/>
+    <row r="17" ht="30" customHeight="1"/>
+    <row r="18" ht="30" customHeight="1"/>
+    <row r="19" ht="30" customHeight="1"/>
+    <row r="20" ht="30" customHeight="1"/>
+    <row r="21" ht="30" customHeight="1"/>
+    <row r="22" ht="30" customHeight="1"/>
+    <row r="23" ht="30" customHeight="1"/>
+    <row r="24" ht="30" customHeight="1"/>
+    <row r="25" ht="30" customHeight="1"/>
+    <row r="26" ht="30" customHeight="1"/>
+    <row r="27" ht="30" customHeight="1"/>
+    <row r="28" ht="30" customHeight="1"/>
+    <row r="29" ht="30" customHeight="1"/>
+    <row r="30" ht="30" customHeight="1"/>
+    <row r="31" ht="30" customHeight="1"/>
+    <row r="32" ht="30" customHeight="1"/>
+    <row r="33" ht="30" customHeight="1"/>
+    <row r="34" ht="30" customHeight="1"/>
+    <row r="35" ht="30" customHeight="1"/>
+    <row r="36" ht="30" customHeight="1"/>
+    <row r="37" ht="30" customHeight="1"/>
+    <row r="38" ht="30" customHeight="1"/>
+    <row r="39" ht="30" customHeight="1"/>
+    <row r="40" ht="30" customHeight="1"/>
+    <row r="41" ht="30" customHeight="1"/>
+    <row r="42" ht="30" customHeight="1"/>
+    <row r="43" ht="30" customHeight="1"/>
+    <row r="44" ht="30" customHeight="1"/>
+    <row r="45" ht="30" customHeight="1"/>
+    <row r="46" ht="30" customHeight="1"/>
+    <row r="47" ht="30" customHeight="1"/>
+    <row r="48" ht="30" customHeight="1"/>
+    <row r="49" ht="30" customHeight="1"/>
+    <row r="50" ht="30" customHeight="1"/>
+    <row r="51" ht="30" customHeight="1"/>
+    <row r="52" ht="30" customHeight="1"/>
+    <row r="53" ht="30" customHeight="1"/>
+    <row r="54" ht="30" customHeight="1"/>
+    <row r="55" ht="30" customHeight="1"/>
+    <row r="56" ht="30" customHeight="1"/>
+    <row r="57" ht="30" customHeight="1"/>
+    <row r="58" ht="30" customHeight="1"/>
+    <row r="59" ht="30" customHeight="1"/>
+    <row r="60" ht="30" customHeight="1"/>
+    <row r="61" ht="30" customHeight="1"/>
+    <row r="62" ht="30" customHeight="1"/>
+    <row r="63" ht="30" customHeight="1"/>
+    <row r="64" ht="30" customHeight="1"/>
+    <row r="65" ht="30" customHeight="1"/>
+    <row r="66" ht="30" customHeight="1"/>
+    <row r="67" ht="30" customHeight="1"/>
+    <row r="68" ht="30" customHeight="1"/>
+    <row r="69" ht="30" customHeight="1"/>
+    <row r="70" ht="30" customHeight="1"/>
+    <row r="71" ht="30" customHeight="1"/>
+    <row r="72" ht="30" customHeight="1"/>
+    <row r="73" ht="30" customHeight="1"/>
+    <row r="74" ht="30" customHeight="1"/>
+    <row r="75" ht="30" customHeight="1"/>
+    <row r="76" ht="30" customHeight="1"/>
+    <row r="77" ht="30" customHeight="1"/>
+    <row r="78" ht="30" customHeight="1"/>
+    <row r="79" ht="30" customHeight="1"/>
+    <row r="80" ht="30" customHeight="1"/>
+    <row r="81" ht="30" customHeight="1"/>
+    <row r="82" ht="30" customHeight="1"/>
+    <row r="83" ht="30" customHeight="1"/>
+    <row r="84" ht="30" customHeight="1"/>
+    <row r="85" ht="30" customHeight="1"/>
+    <row r="86" ht="30" customHeight="1"/>
+    <row r="87" ht="30" customHeight="1"/>
+    <row r="88" ht="30" customHeight="1"/>
+    <row r="89" ht="30" customHeight="1"/>
+    <row r="90" ht="30" customHeight="1"/>
+    <row r="91" ht="30" customHeight="1"/>
+    <row r="92" ht="30" customHeight="1"/>
+    <row r="93" ht="30" customHeight="1"/>
+    <row r="94" ht="30" customHeight="1"/>
+    <row r="95" ht="30" customHeight="1"/>
+    <row r="96" ht="30" customHeight="1"/>
+    <row r="97" ht="30" customHeight="1"/>
+    <row r="98" ht="30" customHeight="1"/>
+    <row r="99" ht="30" customHeight="1"/>
+    <row r="100" ht="30" customHeight="1"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:F387"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
@@ -6584,7 +8593,7 @@
       <c r="E38" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="F38" s="3" t="s">
+      <c r="F38" s="10" t="s">
         <v>153</v>
       </c>
     </row>
@@ -7748,7 +9757,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="97" spans="1:6" ht="51">
+    <row r="97" spans="1:6" ht="51" hidden="1">
       <c r="A97" t="s">
         <v>11</v>
       </c>
@@ -7768,7 +9777,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="98" spans="1:6" ht="51">
+    <row r="98" spans="1:6" ht="51" hidden="1">
       <c r="A98" t="s">
         <v>11</v>
       </c>
@@ -7788,7 +9797,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="99" spans="1:6" ht="34">
+    <row r="99" spans="1:6" ht="34" hidden="1">
       <c r="A99" t="s">
         <v>11</v>
       </c>
@@ -7808,7 +9817,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="100" spans="1:6" ht="68">
+    <row r="100" spans="1:6" ht="68" hidden="1">
       <c r="A100" t="s">
         <v>11</v>
       </c>
@@ -7828,7 +9837,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="101" spans="1:6" ht="34">
+    <row r="101" spans="1:6" ht="34" hidden="1">
       <c r="A101" t="s">
         <v>11</v>
       </c>
@@ -7848,7 +9857,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="102" spans="1:6" ht="34">
+    <row r="102" spans="1:6" ht="34" hidden="1">
       <c r="A102" t="s">
         <v>11</v>
       </c>
@@ -7868,7 +9877,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="103" spans="1:6" ht="51">
+    <row r="103" spans="1:6" ht="51" hidden="1">
       <c r="A103" t="s">
         <v>11</v>
       </c>
@@ -7888,7 +9897,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="104" spans="1:6" ht="102">
+    <row r="104" spans="1:6" ht="102" hidden="1">
       <c r="A104" t="s">
         <v>11</v>
       </c>
@@ -7908,7 +9917,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="105" spans="1:6" ht="34">
+    <row r="105" spans="1:6" ht="34" hidden="1">
       <c r="A105" t="s">
         <v>11</v>
       </c>
@@ -7928,7 +9937,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="106" spans="1:6" ht="68">
+    <row r="106" spans="1:6" ht="68" hidden="1">
       <c r="A106" t="s">
         <v>11</v>
       </c>
@@ -7948,7 +9957,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="107" spans="1:6" ht="34">
+    <row r="107" spans="1:6" ht="34" hidden="1">
       <c r="A107" t="s">
         <v>11</v>
       </c>
@@ -7968,7 +9977,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="108" spans="1:6" ht="51">
+    <row r="108" spans="1:6" ht="51" hidden="1">
       <c r="A108" t="s">
         <v>11</v>
       </c>
@@ -7988,7 +9997,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="109" spans="1:6" ht="51">
+    <row r="109" spans="1:6" ht="51" hidden="1">
       <c r="A109" t="s">
         <v>11</v>
       </c>
@@ -8008,7 +10017,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="110" spans="1:6" ht="136">
+    <row r="110" spans="1:6" ht="136" hidden="1">
       <c r="A110" t="s">
         <v>11</v>
       </c>
@@ -8028,7 +10037,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="111" spans="1:6" ht="68">
+    <row r="111" spans="1:6" ht="68" hidden="1">
       <c r="A111" t="s">
         <v>11</v>
       </c>
@@ -8048,7 +10057,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="112" spans="1:6" ht="51">
+    <row r="112" spans="1:6" ht="51" hidden="1">
       <c r="A112" t="s">
         <v>11</v>
       </c>
@@ -8068,7 +10077,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="113" spans="1:6" ht="34">
+    <row r="113" spans="1:6" ht="34" hidden="1">
       <c r="A113" t="s">
         <v>11</v>
       </c>
@@ -8088,7 +10097,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="114" spans="1:6" ht="51">
+    <row r="114" spans="1:6" ht="51" hidden="1">
       <c r="A114" t="s">
         <v>11</v>
       </c>
@@ -8108,7 +10117,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="115" spans="1:6" ht="34">
+    <row r="115" spans="1:6" ht="34" hidden="1">
       <c r="A115" t="s">
         <v>11</v>
       </c>
@@ -8128,7 +10137,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="116" spans="1:6" ht="68">
+    <row r="116" spans="1:6" ht="68" hidden="1">
       <c r="A116" t="s">
         <v>11</v>
       </c>
@@ -8148,7 +10157,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="117" spans="1:6" ht="68">
+    <row r="117" spans="1:6" ht="68" hidden="1">
       <c r="A117" t="s">
         <v>11</v>
       </c>
@@ -8168,7 +10177,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="118" spans="1:6" ht="68">
+    <row r="118" spans="1:6" ht="68" hidden="1">
       <c r="A118" t="s">
         <v>11</v>
       </c>
@@ -8188,7 +10197,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="119" spans="1:6" ht="51">
+    <row r="119" spans="1:6" ht="51" hidden="1">
       <c r="A119" t="s">
         <v>11</v>
       </c>
@@ -8208,7 +10217,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="120" spans="1:6" ht="85">
+    <row r="120" spans="1:6" ht="85" hidden="1">
       <c r="A120" t="s">
         <v>11</v>
       </c>
@@ -8228,7 +10237,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="121" spans="1:6" ht="85">
+    <row r="121" spans="1:6" ht="85" hidden="1">
       <c r="A121" t="s">
         <v>11</v>
       </c>
@@ -8248,7 +10257,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="122" spans="1:6" ht="85">
+    <row r="122" spans="1:6" ht="85" hidden="1">
       <c r="A122" t="s">
         <v>11</v>
       </c>
@@ -8268,7 +10277,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="123" spans="1:6" ht="153">
+    <row r="123" spans="1:6" ht="153" hidden="1">
       <c r="A123" t="s">
         <v>11</v>
       </c>
@@ -8288,7 +10297,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="124" spans="1:6" ht="102">
+    <row r="124" spans="1:6" ht="102" hidden="1">
       <c r="A124" t="s">
         <v>11</v>
       </c>
@@ -8308,7 +10317,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="125" spans="1:6" ht="68">
+    <row r="125" spans="1:6" ht="68" hidden="1">
       <c r="A125" t="s">
         <v>11</v>
       </c>
@@ -8328,7 +10337,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="126" spans="1:6" ht="85">
+    <row r="126" spans="1:6" ht="85" hidden="1">
       <c r="A126" t="s">
         <v>11</v>
       </c>
@@ -8348,7 +10357,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="127" spans="1:6" ht="85">
+    <row r="127" spans="1:6" ht="85" hidden="1">
       <c r="A127" t="s">
         <v>11</v>
       </c>
@@ -8368,7 +10377,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="128" spans="1:6" ht="170">
+    <row r="128" spans="1:6" ht="170" hidden="1">
       <c r="A128" t="s">
         <v>11</v>
       </c>
@@ -8388,7 +10397,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="129" spans="1:6" ht="68">
+    <row r="129" spans="1:6" ht="68" hidden="1">
       <c r="A129" t="s">
         <v>11</v>
       </c>
@@ -8408,7 +10417,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="130" spans="1:6" ht="51">
+    <row r="130" spans="1:6" ht="51" hidden="1">
       <c r="A130" t="s">
         <v>11</v>
       </c>
@@ -8428,7 +10437,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="131" spans="1:6" ht="51">
+    <row r="131" spans="1:6" ht="51" hidden="1">
       <c r="A131" t="s">
         <v>11</v>
       </c>
@@ -8448,7 +10457,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="132" spans="1:6" ht="136">
+    <row r="132" spans="1:6" ht="136" hidden="1">
       <c r="A132" t="s">
         <v>11</v>
       </c>
@@ -8468,7 +10477,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="133" spans="1:6" ht="51">
+    <row r="133" spans="1:6" ht="51" hidden="1">
       <c r="A133" t="s">
         <v>11</v>
       </c>
@@ -8488,7 +10497,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="134" spans="1:6" ht="102">
+    <row r="134" spans="1:6" ht="102" hidden="1">
       <c r="A134" t="s">
         <v>11</v>
       </c>
@@ -8508,7 +10517,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="135" spans="1:6" ht="68">
+    <row r="135" spans="1:6" ht="68" hidden="1">
       <c r="A135" t="s">
         <v>11</v>
       </c>
@@ -8528,7 +10537,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="136" spans="1:6" ht="85">
+    <row r="136" spans="1:6" ht="85" hidden="1">
       <c r="A136" t="s">
         <v>11</v>
       </c>
@@ -8548,7 +10557,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="137" spans="1:6" ht="85">
+    <row r="137" spans="1:6" ht="85" hidden="1">
       <c r="A137" t="s">
         <v>11</v>
       </c>
@@ -8568,7 +10577,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="138" spans="1:6" ht="51">
+    <row r="138" spans="1:6" ht="51" hidden="1">
       <c r="A138" t="s">
         <v>11</v>
       </c>
@@ -8588,7 +10597,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="139" spans="1:6" ht="68">
+    <row r="139" spans="1:6" ht="68" hidden="1">
       <c r="A139" t="s">
         <v>11</v>
       </c>
@@ -8608,7 +10617,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="140" spans="1:6" ht="85">
+    <row r="140" spans="1:6" ht="85" hidden="1">
       <c r="A140" t="s">
         <v>11</v>
       </c>
@@ -8628,7 +10637,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="141" spans="1:6" ht="68">
+    <row r="141" spans="1:6" ht="68" hidden="1">
       <c r="A141" t="s">
         <v>11</v>
       </c>
@@ -8648,7 +10657,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="142" spans="1:6" ht="119">
+    <row r="142" spans="1:6" ht="119" hidden="1">
       <c r="A142" t="s">
         <v>11</v>
       </c>
@@ -8668,7 +10677,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="143" spans="1:6" ht="68">
+    <row r="143" spans="1:6" ht="68" hidden="1">
       <c r="A143" t="s">
         <v>11</v>
       </c>
@@ -8688,7 +10697,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="144" spans="1:6" ht="68">
+    <row r="144" spans="1:6" ht="68" hidden="1">
       <c r="A144" t="s">
         <v>11</v>
       </c>
@@ -8708,7 +10717,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="145" spans="1:6" ht="85">
+    <row r="145" spans="1:6" ht="85" hidden="1">
       <c r="A145" t="s">
         <v>11</v>
       </c>
@@ -8728,7 +10737,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="146" spans="1:6" ht="68">
+    <row r="146" spans="1:6" ht="68" hidden="1">
       <c r="A146" t="s">
         <v>11</v>
       </c>
@@ -8748,7 +10757,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="147" spans="1:6" ht="119">
+    <row r="147" spans="1:6" ht="119" hidden="1">
       <c r="A147" t="s">
         <v>11</v>
       </c>
@@ -8768,7 +10777,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="148" spans="1:6" ht="68">
+    <row r="148" spans="1:6" ht="68" hidden="1">
       <c r="A148" t="s">
         <v>11</v>
       </c>
@@ -8788,7 +10797,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="149" spans="1:6" ht="34">
+    <row r="149" spans="1:6" ht="34" hidden="1">
       <c r="A149" t="s">
         <v>11</v>
       </c>
@@ -8808,7 +10817,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="150" spans="1:6" ht="102">
+    <row r="150" spans="1:6" ht="102" hidden="1">
       <c r="A150" t="s">
         <v>11</v>
       </c>
@@ -8828,7 +10837,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="151" spans="1:6" ht="119">
+    <row r="151" spans="1:6" ht="119" hidden="1">
       <c r="A151" t="s">
         <v>11</v>
       </c>
@@ -8848,7 +10857,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="152" spans="1:6" ht="68">
+    <row r="152" spans="1:6" ht="68" hidden="1">
       <c r="A152" t="s">
         <v>11</v>
       </c>
@@ -8868,7 +10877,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="153" spans="1:6" ht="51">
+    <row r="153" spans="1:6" ht="51" hidden="1">
       <c r="A153" t="s">
         <v>11</v>
       </c>
@@ -8888,7 +10897,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="154" spans="1:6" ht="68">
+    <row r="154" spans="1:6" ht="68" hidden="1">
       <c r="A154" t="s">
         <v>11</v>
       </c>
@@ -8908,7 +10917,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="155" spans="1:6" ht="102">
+    <row r="155" spans="1:6" ht="102" hidden="1">
       <c r="A155" t="s">
         <v>11</v>
       </c>
@@ -8928,7 +10937,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="156" spans="1:6" ht="68">
+    <row r="156" spans="1:6" ht="68" hidden="1">
       <c r="A156" t="s">
         <v>11</v>
       </c>
@@ -8948,7 +10957,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="157" spans="1:6" ht="102">
+    <row r="157" spans="1:6" ht="102" hidden="1">
       <c r="A157" t="s">
         <v>11</v>
       </c>
@@ -8968,7 +10977,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="158" spans="1:6" ht="51">
+    <row r="158" spans="1:6" ht="51" hidden="1">
       <c r="A158" t="s">
         <v>11</v>
       </c>
@@ -8988,7 +10997,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="159" spans="1:6" ht="51">
+    <row r="159" spans="1:6" ht="51" hidden="1">
       <c r="A159" t="s">
         <v>11</v>
       </c>
@@ -9008,7 +11017,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="160" spans="1:6" ht="51">
+    <row r="160" spans="1:6" ht="51" hidden="1">
       <c r="A160" t="s">
         <v>11</v>
       </c>
@@ -9028,7 +11037,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="161" spans="1:6" ht="102">
+    <row r="161" spans="1:6" ht="102" hidden="1">
       <c r="A161" t="s">
         <v>11</v>
       </c>
@@ -9048,7 +11057,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="162" spans="1:6" ht="68">
+    <row r="162" spans="1:6" ht="68" hidden="1">
       <c r="A162" t="s">
         <v>11</v>
       </c>
@@ -9068,7 +11077,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="163" spans="1:6" ht="102">
+    <row r="163" spans="1:6" ht="102" hidden="1">
       <c r="A163" t="s">
         <v>11</v>
       </c>
@@ -9088,7 +11097,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="164" spans="1:6" ht="85">
+    <row r="164" spans="1:6" ht="85" hidden="1">
       <c r="A164" t="s">
         <v>11</v>
       </c>
@@ -9108,7 +11117,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="165" spans="1:6" ht="85">
+    <row r="165" spans="1:6" ht="85" hidden="1">
       <c r="A165" t="s">
         <v>11</v>
       </c>
@@ -9128,7 +11137,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="166" spans="1:6" ht="34">
+    <row r="166" spans="1:6" ht="34" hidden="1">
       <c r="A166" t="s">
         <v>11</v>
       </c>
@@ -9148,7 +11157,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="167" spans="1:6" ht="68">
+    <row r="167" spans="1:6" ht="68" hidden="1">
       <c r="A167" t="s">
         <v>11</v>
       </c>
@@ -9168,7 +11177,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="168" spans="1:6" ht="68">
+    <row r="168" spans="1:6" ht="68" hidden="1">
       <c r="A168" t="s">
         <v>11</v>
       </c>
@@ -9188,7 +11197,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="169" spans="1:6" ht="102">
+    <row r="169" spans="1:6" ht="102" hidden="1">
       <c r="A169" t="s">
         <v>11</v>
       </c>
@@ -9208,7 +11217,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="170" spans="1:6" ht="68">
+    <row r="170" spans="1:6" ht="68" hidden="1">
       <c r="A170" t="s">
         <v>11</v>
       </c>
@@ -9228,7 +11237,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="171" spans="1:6" ht="68">
+    <row r="171" spans="1:6" ht="68" hidden="1">
       <c r="A171" t="s">
         <v>11</v>
       </c>
@@ -9248,7 +11257,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="172" spans="1:6" ht="68">
+    <row r="172" spans="1:6" ht="68" hidden="1">
       <c r="A172" t="s">
         <v>11</v>
       </c>
@@ -9268,7 +11277,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="173" spans="1:6" ht="119">
+    <row r="173" spans="1:6" ht="119" hidden="1">
       <c r="A173" t="s">
         <v>11</v>
       </c>
@@ -9288,7 +11297,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="174" spans="1:6" ht="51">
+    <row r="174" spans="1:6" ht="51" hidden="1">
       <c r="A174" t="s">
         <v>11</v>
       </c>
@@ -9308,7 +11317,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="175" spans="1:6" ht="51">
+    <row r="175" spans="1:6" ht="51" hidden="1">
       <c r="A175" t="s">
         <v>11</v>
       </c>
@@ -9328,7 +11337,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="176" spans="1:6" ht="119">
+    <row r="176" spans="1:6" ht="119" hidden="1">
       <c r="A176" t="s">
         <v>11</v>
       </c>
@@ -9348,7 +11357,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="177" spans="1:6" ht="34">
+    <row r="177" spans="1:6" ht="34" hidden="1">
       <c r="A177" t="s">
         <v>11</v>
       </c>
@@ -9368,7 +11377,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="178" spans="1:6" ht="34">
+    <row r="178" spans="1:6" ht="34" hidden="1">
       <c r="A178" t="s">
         <v>11</v>
       </c>
@@ -9388,7 +11397,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="179" spans="1:6" ht="136">
+    <row r="179" spans="1:6" ht="136" hidden="1">
       <c r="A179" t="s">
         <v>11</v>
       </c>
@@ -9408,7 +11417,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="180" spans="1:6" ht="68">
+    <row r="180" spans="1:6" ht="68" hidden="1">
       <c r="A180" t="s">
         <v>11</v>
       </c>
@@ -9428,7 +11437,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="181" spans="1:6" ht="170">
+    <row r="181" spans="1:6" ht="170" hidden="1">
       <c r="A181" t="s">
         <v>11</v>
       </c>
@@ -9448,7 +11457,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="182" spans="1:6" ht="68">
+    <row r="182" spans="1:6" ht="68" hidden="1">
       <c r="A182" t="s">
         <v>11</v>
       </c>
@@ -9468,7 +11477,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="183" spans="1:6" ht="85">
+    <row r="183" spans="1:6" ht="85" hidden="1">
       <c r="A183" t="s">
         <v>11</v>
       </c>
@@ -9488,7 +11497,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="184" spans="1:6" ht="85">
+    <row r="184" spans="1:6" ht="85" hidden="1">
       <c r="A184" t="s">
         <v>11</v>
       </c>
@@ -9508,7 +11517,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="185" spans="1:6" ht="85">
+    <row r="185" spans="1:6" ht="85" hidden="1">
       <c r="A185" t="s">
         <v>11</v>
       </c>
@@ -9528,7 +11537,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="186" spans="1:6" ht="51">
+    <row r="186" spans="1:6" ht="51" hidden="1">
       <c r="A186" t="s">
         <v>11</v>
       </c>
@@ -9548,7 +11557,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="187" spans="1:6" ht="68">
+    <row r="187" spans="1:6" ht="68" hidden="1">
       <c r="A187" t="s">
         <v>11</v>
       </c>
@@ -9568,7 +11577,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="188" spans="1:6" ht="34">
+    <row r="188" spans="1:6" ht="34" hidden="1">
       <c r="A188" t="s">
         <v>11</v>
       </c>
@@ -9588,7 +11597,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="189" spans="1:6" ht="85">
+    <row r="189" spans="1:6" ht="85" hidden="1">
       <c r="A189" t="s">
         <v>11</v>
       </c>
@@ -9608,7 +11617,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="190" spans="1:6" ht="68">
+    <row r="190" spans="1:6" ht="68" hidden="1">
       <c r="A190" t="s">
         <v>11</v>
       </c>
@@ -9628,7 +11637,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="191" spans="1:6" ht="68">
+    <row r="191" spans="1:6" ht="68" hidden="1">
       <c r="A191" t="s">
         <v>11</v>
       </c>
@@ -9648,7 +11657,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="192" spans="1:6" ht="102">
+    <row r="192" spans="1:6" ht="102" hidden="1">
       <c r="A192" t="s">
         <v>11</v>
       </c>
@@ -9668,7 +11677,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="193" spans="1:6" ht="85">
+    <row r="193" spans="1:6" ht="85" hidden="1">
       <c r="A193" t="s">
         <v>11</v>
       </c>
@@ -13570,10 +15579,20 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:F387" xr:uid="{00000000-0001-0000-0100-000000000000}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="Breakfast"/>
+        <filter val="Lunch"/>
+        <filter val="Snack"/>
+      </filters>
+    </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F387">
       <sortCondition ref="A1:A387"/>
     </sortState>
   </autoFilter>
+  <hyperlinks>
+    <hyperlink ref="F38" r:id="rId1" xr:uid="{31309CCA-E10F-7A42-91B6-5F69157E9D55}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix: simplified wb format
</commit_message>
<xml_diff>
--- a/MealPrepTracker.xlsx
+++ b/MealPrepTracker.xlsx
@@ -8,18 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/quinnreams/Documents/GitHub/Personal-Growth-Planner/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B755871-111C-2148-A21C-3C4E9DDC0118}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77082618-2F95-FD44-A89D-40D31A56965D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19620" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Meal Calendar" sheetId="1" r:id="rId1"/>
-    <sheet name="Helper" sheetId="4" r:id="rId2"/>
-    <sheet name="Grocery List" sheetId="3" r:id="rId3"/>
-    <sheet name="Recipes" sheetId="2" r:id="rId4"/>
+    <sheet name="Recipes" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Recipes!$A$1:$F$387</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Recipes!$A$1:$F$387</definedName>
     <definedName name="Breakfast">_xlfn._xlws.FILTER(Recipes!$B$2:$B$1000, Recipes!$A$2:$A$1000="breakfast")</definedName>
     <definedName name="Dinner">_xlfn._xlws.FILTER(Recipes!$B$2:$B$1000, Recipes!$A$2:$A$1000="dinner")</definedName>
     <definedName name="Lunch">_xlfn._xlws.FILTER(Recipes!$B$2:$B$1000, Recipes!$A$2:$A$1000="lunch")</definedName>
@@ -44,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1721" uniqueCount="1190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1710" uniqueCount="1186">
   <si>
     <t>Week</t>
   </si>
@@ -3602,18 +3600,6 @@
   </si>
   <si>
     <t>https://www.delish.com/cooking/recipe-ideas/recipes/a20966/strawberry-fruit-roll-ups-recipe-del0313/</t>
-  </si>
-  <si>
-    <t>Unit</t>
-  </si>
-  <si>
-    <t>Ingredient</t>
-  </si>
-  <si>
-    <t>Quantity</t>
-  </si>
-  <si>
-    <t>Purchased</t>
   </si>
 </sst>
 </file>
@@ -3743,17 +3729,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="16">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -3835,16 +3811,6 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
@@ -3916,17 +3882,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:F59" totalsRowShown="0" headerRowDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:F59" totalsRowShown="0" headerRowDxfId="15">
   <autoFilter ref="A1:F59" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Week"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Day"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Meal"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Meal Name" dataDxfId="16"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Calories" dataDxfId="15">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Meal Name" dataDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Calories" dataDxfId="13">
       <calculatedColumnFormula>IFERROR(VLOOKUP(C2,#REF!, 2, FALSE), "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Cost" dataDxfId="14">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Cost" dataDxfId="12">
       <calculatedColumnFormula>IFERROR(VLOOKUP(C2,#REF!, 3, FALSE), "")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3935,17 +3901,17 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table13" displayName="Table13" ref="G1:L59" totalsRowShown="0" headerRowDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table13" displayName="Table13" ref="G1:L59" totalsRowShown="0" headerRowDxfId="11">
   <autoFilter ref="G1:L59" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Week"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Day"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Meal"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Meal Name" dataDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Calories" dataDxfId="11">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Meal Name" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Calories" dataDxfId="9">
       <calculatedColumnFormula>IFERROR(VLOOKUP(J2,#REF!, 2, FALSE), "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Cost" dataDxfId="10">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Cost" dataDxfId="8">
       <calculatedColumnFormula>IFERROR(VLOOKUP(J2,#REF!, 3, FALSE), "")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5806,42 +5772,42 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E30">
-    <cfRule type="cellIs" dxfId="8" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="greaterThan">
       <formula>14000</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E59">
-    <cfRule type="cellIs" dxfId="7" priority="4" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="4" stopIfTrue="1" operator="greaterThan">
       <formula>14000</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F30">
-    <cfRule type="cellIs" dxfId="6" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="greaterThan">
       <formula>100</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F59">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="greaterThan">
       <formula>100</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K30">
-    <cfRule type="cellIs" dxfId="4" priority="6" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="6" stopIfTrue="1" operator="greaterThan">
       <formula>14000</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K59">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="greaterThan">
       <formula>14000</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L30">
-    <cfRule type="cellIs" dxfId="2" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="5" operator="greaterThan">
       <formula>100</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L59">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>100</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5859,1972 +5825,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50723675-B2F4-E141-9E40-923361B6A99F}">
-  <dimension ref="A1:F201"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A153" workbookViewId="0">
-      <selection activeCell="C173" sqref="C173"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="C2" t="str">
-        <f>IF('Meal Calendar'!D2&lt;&gt;"", 'Meal Calendar'!D2, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="C4" t="str">
-        <f>IF('Meal Calendar'!D4&lt;&gt;"", 'Meal Calendar'!D4, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="C5" t="str">
-        <f>IF('Meal Calendar'!D5&lt;&gt;"", 'Meal Calendar'!D5, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6">
-        <v>1</v>
-      </c>
-      <c r="C6" t="str">
-        <f>IF('Meal Calendar'!D6&lt;&gt;"", 'Meal Calendar'!D6, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7">
-        <v>1</v>
-      </c>
-      <c r="C7" t="str">
-        <f>IF('Meal Calendar'!D7&lt;&gt;"", 'Meal Calendar'!D7, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8">
-        <v>1</v>
-      </c>
-      <c r="C8" t="str">
-        <f>IF('Meal Calendar'!D8&lt;&gt;"", 'Meal Calendar'!D8, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9">
-        <v>1</v>
-      </c>
-      <c r="C9" t="str">
-        <f>IF('Meal Calendar'!D9&lt;&gt;"", 'Meal Calendar'!D9, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10">
-        <v>1</v>
-      </c>
-      <c r="C10" t="str">
-        <f>IF('Meal Calendar'!D10&lt;&gt;"", 'Meal Calendar'!D10, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11">
-        <v>1</v>
-      </c>
-      <c r="C11" t="str">
-        <f>IF('Meal Calendar'!D11&lt;&gt;"", 'Meal Calendar'!D11, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12">
-        <v>1</v>
-      </c>
-      <c r="C12" t="str">
-        <f>IF('Meal Calendar'!D12&lt;&gt;"", 'Meal Calendar'!D12, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13">
-        <v>1</v>
-      </c>
-      <c r="C13" t="str">
-        <f>IF('Meal Calendar'!D13&lt;&gt;"", 'Meal Calendar'!D13, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14">
-        <v>1</v>
-      </c>
-      <c r="C14" t="str">
-        <f>IF('Meal Calendar'!D14&lt;&gt;"", 'Meal Calendar'!D14, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15">
-        <v>1</v>
-      </c>
-      <c r="C15" t="str">
-        <f>IF('Meal Calendar'!D15&lt;&gt;"", 'Meal Calendar'!D15, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16">
-        <v>1</v>
-      </c>
-      <c r="C16" t="str">
-        <f>IF('Meal Calendar'!D16&lt;&gt;"", 'Meal Calendar'!D16, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17">
-        <v>1</v>
-      </c>
-      <c r="C17" t="str">
-        <f>IF('Meal Calendar'!D17&lt;&gt;"", 'Meal Calendar'!D17, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18">
-        <v>1</v>
-      </c>
-      <c r="C18" t="str">
-        <f>IF('Meal Calendar'!D18&lt;&gt;"", 'Meal Calendar'!D18, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19">
-        <v>1</v>
-      </c>
-      <c r="C19" t="str">
-        <f>IF('Meal Calendar'!D19&lt;&gt;"", 'Meal Calendar'!D19, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20">
-        <v>1</v>
-      </c>
-      <c r="C20" t="str">
-        <f>IF('Meal Calendar'!D20&lt;&gt;"", 'Meal Calendar'!D20, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21">
-        <v>1</v>
-      </c>
-      <c r="C21" t="str">
-        <f>IF('Meal Calendar'!D21&lt;&gt;"", 'Meal Calendar'!D21, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22">
-        <v>1</v>
-      </c>
-      <c r="C22" t="str">
-        <f>IF('Meal Calendar'!D22&lt;&gt;"", 'Meal Calendar'!D22, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23">
-        <v>1</v>
-      </c>
-      <c r="C23" t="str">
-        <f>IF('Meal Calendar'!D23&lt;&gt;"", 'Meal Calendar'!D23, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24">
-        <v>1</v>
-      </c>
-      <c r="C24" t="str">
-        <f>IF('Meal Calendar'!D24&lt;&gt;"", 'Meal Calendar'!D24, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25">
-        <v>1</v>
-      </c>
-      <c r="C25" t="str">
-        <f>IF('Meal Calendar'!D25&lt;&gt;"", 'Meal Calendar'!D25, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26">
-        <v>1</v>
-      </c>
-      <c r="C26" t="str">
-        <f>IF('Meal Calendar'!D26&lt;&gt;"", 'Meal Calendar'!D26, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27">
-        <v>1</v>
-      </c>
-      <c r="C27" t="str">
-        <f>IF('Meal Calendar'!D27&lt;&gt;"", 'Meal Calendar'!D27, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28">
-        <v>1</v>
-      </c>
-      <c r="C28" t="str">
-        <f>IF('Meal Calendar'!D28&lt;&gt;"", 'Meal Calendar'!D28, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29">
-        <v>1</v>
-      </c>
-      <c r="C29" t="str">
-        <f>IF('Meal Calendar'!D29&lt;&gt;"", 'Meal Calendar'!D29, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30">
-        <v>1</v>
-      </c>
-      <c r="C30" t="str">
-        <f>IF('Meal Calendar'!D30&lt;&gt;"", 'Meal Calendar'!D30, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="A31">
-        <v>1</v>
-      </c>
-      <c r="C31" t="str">
-        <f>IF('Meal Calendar'!D31&lt;&gt;"", 'Meal Calendar'!D31, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="A32">
-        <v>1</v>
-      </c>
-      <c r="C32" t="str">
-        <f>IF('Meal Calendar'!D32&lt;&gt;"", 'Meal Calendar'!D32, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="A33">
-        <v>1</v>
-      </c>
-      <c r="C33" t="str">
-        <f>IF('Meal Calendar'!D33&lt;&gt;"", 'Meal Calendar'!D33, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34">
-        <v>1</v>
-      </c>
-      <c r="C34" t="str">
-        <f>IF('Meal Calendar'!D34&lt;&gt;"", 'Meal Calendar'!D34, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35">
-        <v>1</v>
-      </c>
-      <c r="C35" t="str">
-        <f>IF('Meal Calendar'!D35&lt;&gt;"", 'Meal Calendar'!D35, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="A36">
-        <v>1</v>
-      </c>
-      <c r="C36" t="str">
-        <f>IF('Meal Calendar'!D36&lt;&gt;"", 'Meal Calendar'!D36, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="A37">
-        <v>1</v>
-      </c>
-      <c r="C37" t="str">
-        <f>IF('Meal Calendar'!D37&lt;&gt;"", 'Meal Calendar'!D37, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
-      <c r="A38">
-        <v>1</v>
-      </c>
-      <c r="C38" t="str">
-        <f>IF('Meal Calendar'!D38&lt;&gt;"", 'Meal Calendar'!D38, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="39" spans="1:3">
-      <c r="A39">
-        <v>1</v>
-      </c>
-      <c r="C39" t="str">
-        <f>IF('Meal Calendar'!D39&lt;&gt;"", 'Meal Calendar'!D39, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="40" spans="1:3">
-      <c r="A40">
-        <v>1</v>
-      </c>
-      <c r="C40" t="str">
-        <f>IF('Meal Calendar'!D40&lt;&gt;"", 'Meal Calendar'!D40, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="41" spans="1:3">
-      <c r="A41">
-        <v>1</v>
-      </c>
-      <c r="C41" t="str">
-        <f>IF('Meal Calendar'!D41&lt;&gt;"", 'Meal Calendar'!D41, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="42" spans="1:3">
-      <c r="A42">
-        <v>1</v>
-      </c>
-      <c r="C42" t="str">
-        <f>IF('Meal Calendar'!D42&lt;&gt;"", 'Meal Calendar'!D42, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="43" spans="1:3">
-      <c r="A43">
-        <v>1</v>
-      </c>
-      <c r="C43" t="str">
-        <f>IF('Meal Calendar'!D43&lt;&gt;"", 'Meal Calendar'!D43, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="44" spans="1:3">
-      <c r="A44">
-        <v>1</v>
-      </c>
-      <c r="C44" t="str">
-        <f>IF('Meal Calendar'!D44&lt;&gt;"", 'Meal Calendar'!D44, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="45" spans="1:3">
-      <c r="A45">
-        <v>1</v>
-      </c>
-      <c r="C45" t="str">
-        <f>IF('Meal Calendar'!D45&lt;&gt;"", 'Meal Calendar'!D45, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="46" spans="1:3">
-      <c r="A46">
-        <v>1</v>
-      </c>
-      <c r="C46" t="str">
-        <f>IF('Meal Calendar'!D46&lt;&gt;"", 'Meal Calendar'!D46, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="47" spans="1:3">
-      <c r="A47">
-        <v>1</v>
-      </c>
-      <c r="C47" t="str">
-        <f>IF('Meal Calendar'!D47&lt;&gt;"", 'Meal Calendar'!D47, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="48" spans="1:3">
-      <c r="A48">
-        <v>1</v>
-      </c>
-      <c r="C48" t="str">
-        <f>IF('Meal Calendar'!D48&lt;&gt;"", 'Meal Calendar'!D48, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="49" spans="1:3">
-      <c r="A49">
-        <v>1</v>
-      </c>
-      <c r="C49" t="str">
-        <f>IF('Meal Calendar'!D49&lt;&gt;"", 'Meal Calendar'!D49, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="50" spans="1:3">
-      <c r="A50">
-        <v>1</v>
-      </c>
-      <c r="C50" t="str">
-        <f>IF('Meal Calendar'!D50&lt;&gt;"", 'Meal Calendar'!D50, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="51" spans="1:3">
-      <c r="A51">
-        <v>1</v>
-      </c>
-      <c r="C51" t="str">
-        <f>IF('Meal Calendar'!D51&lt;&gt;"", 'Meal Calendar'!D51, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="52" spans="1:3">
-      <c r="A52">
-        <v>2</v>
-      </c>
-      <c r="C52" t="str">
-        <f>IF('Meal Calendar'!D52&lt;&gt;"", 'Meal Calendar'!D52, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="53" spans="1:3">
-      <c r="A53">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3">
-      <c r="A54">
-        <v>2</v>
-      </c>
-      <c r="C54" t="str">
-        <f>IF('Meal Calendar'!D54&lt;&gt;"", 'Meal Calendar'!D54, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="55" spans="1:3">
-      <c r="A55">
-        <v>2</v>
-      </c>
-      <c r="C55" t="str">
-        <f>IF('Meal Calendar'!D55&lt;&gt;"", 'Meal Calendar'!D55, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="56" spans="1:3">
-      <c r="A56">
-        <v>2</v>
-      </c>
-      <c r="C56" t="str">
-        <f>IF('Meal Calendar'!D56&lt;&gt;"", 'Meal Calendar'!D56, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="57" spans="1:3">
-      <c r="A57">
-        <v>2</v>
-      </c>
-      <c r="C57" t="str">
-        <f>IF('Meal Calendar'!D57&lt;&gt;"", 'Meal Calendar'!D57, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="58" spans="1:3">
-      <c r="A58">
-        <v>2</v>
-      </c>
-      <c r="C58" t="str">
-        <f>IF('Meal Calendar'!D58&lt;&gt;"", 'Meal Calendar'!D58, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="59" spans="1:3">
-      <c r="A59">
-        <v>2</v>
-      </c>
-      <c r="C59" t="str">
-        <f>IF('Meal Calendar'!D59&lt;&gt;"", 'Meal Calendar'!D59, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="60" spans="1:3">
-      <c r="A60">
-        <v>2</v>
-      </c>
-      <c r="C60" t="str">
-        <f>IF('Meal Calendar'!D60&lt;&gt;"", 'Meal Calendar'!D60, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="61" spans="1:3">
-      <c r="A61">
-        <v>2</v>
-      </c>
-      <c r="C61" t="str">
-        <f>IF('Meal Calendar'!D61&lt;&gt;"", 'Meal Calendar'!D61, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="62" spans="1:3">
-      <c r="A62">
-        <v>2</v>
-      </c>
-      <c r="C62" t="str">
-        <f>IF('Meal Calendar'!D62&lt;&gt;"", 'Meal Calendar'!D62, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="63" spans="1:3">
-      <c r="A63">
-        <v>2</v>
-      </c>
-      <c r="C63" t="str">
-        <f>IF('Meal Calendar'!D63&lt;&gt;"", 'Meal Calendar'!D63, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="64" spans="1:3">
-      <c r="A64">
-        <v>2</v>
-      </c>
-      <c r="C64" t="str">
-        <f>IF('Meal Calendar'!D64&lt;&gt;"", 'Meal Calendar'!D64, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="65" spans="1:3">
-      <c r="A65">
-        <v>2</v>
-      </c>
-      <c r="C65" t="str">
-        <f>IF('Meal Calendar'!D65&lt;&gt;"", 'Meal Calendar'!D65, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="66" spans="1:3">
-      <c r="A66">
-        <v>2</v>
-      </c>
-      <c r="C66" t="str">
-        <f>IF('Meal Calendar'!D66&lt;&gt;"", 'Meal Calendar'!D66, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="67" spans="1:3">
-      <c r="A67">
-        <v>2</v>
-      </c>
-      <c r="C67" t="str">
-        <f>IF('Meal Calendar'!D67&lt;&gt;"", 'Meal Calendar'!D67, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="68" spans="1:3">
-      <c r="A68">
-        <v>2</v>
-      </c>
-      <c r="C68" t="str">
-        <f>IF('Meal Calendar'!D68&lt;&gt;"", 'Meal Calendar'!D68, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="69" spans="1:3">
-      <c r="A69">
-        <v>2</v>
-      </c>
-      <c r="C69" t="str">
-        <f>IF('Meal Calendar'!D69&lt;&gt;"", 'Meal Calendar'!D69, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="70" spans="1:3">
-      <c r="A70">
-        <v>2</v>
-      </c>
-      <c r="C70" t="str">
-        <f>IF('Meal Calendar'!D70&lt;&gt;"", 'Meal Calendar'!D70, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="71" spans="1:3">
-      <c r="A71">
-        <v>2</v>
-      </c>
-      <c r="C71" t="str">
-        <f>IF('Meal Calendar'!D71&lt;&gt;"", 'Meal Calendar'!D71, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="72" spans="1:3">
-      <c r="A72">
-        <v>2</v>
-      </c>
-      <c r="C72" t="str">
-        <f>IF('Meal Calendar'!D72&lt;&gt;"", 'Meal Calendar'!D72, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="73" spans="1:3">
-      <c r="A73">
-        <v>2</v>
-      </c>
-      <c r="C73" t="str">
-        <f>IF('Meal Calendar'!D73&lt;&gt;"", 'Meal Calendar'!D73, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="74" spans="1:3">
-      <c r="A74">
-        <v>2</v>
-      </c>
-      <c r="C74" t="str">
-        <f>IF('Meal Calendar'!D74&lt;&gt;"", 'Meal Calendar'!D74, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="75" spans="1:3">
-      <c r="A75">
-        <v>2</v>
-      </c>
-      <c r="C75" t="str">
-        <f>IF('Meal Calendar'!D75&lt;&gt;"", 'Meal Calendar'!D75, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="76" spans="1:3">
-      <c r="A76">
-        <v>2</v>
-      </c>
-      <c r="C76" t="str">
-        <f>IF('Meal Calendar'!D76&lt;&gt;"", 'Meal Calendar'!D76, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="77" spans="1:3">
-      <c r="A77">
-        <v>2</v>
-      </c>
-      <c r="C77" t="str">
-        <f>IF('Meal Calendar'!D77&lt;&gt;"", 'Meal Calendar'!D77, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="78" spans="1:3">
-      <c r="A78">
-        <v>2</v>
-      </c>
-      <c r="C78" t="str">
-        <f>IF('Meal Calendar'!D78&lt;&gt;"", 'Meal Calendar'!D78, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="79" spans="1:3">
-      <c r="A79">
-        <v>2</v>
-      </c>
-      <c r="C79" t="str">
-        <f>IF('Meal Calendar'!D79&lt;&gt;"", 'Meal Calendar'!D79, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="80" spans="1:3">
-      <c r="A80">
-        <v>2</v>
-      </c>
-      <c r="C80" t="str">
-        <f>IF('Meal Calendar'!D80&lt;&gt;"", 'Meal Calendar'!D80, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="81" spans="1:3">
-      <c r="A81">
-        <v>2</v>
-      </c>
-      <c r="C81" t="str">
-        <f>IF('Meal Calendar'!D81&lt;&gt;"", 'Meal Calendar'!D81, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="82" spans="1:3">
-      <c r="A82">
-        <v>2</v>
-      </c>
-      <c r="C82" t="str">
-        <f>IF('Meal Calendar'!D82&lt;&gt;"", 'Meal Calendar'!D82, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="83" spans="1:3">
-      <c r="A83">
-        <v>2</v>
-      </c>
-      <c r="C83" t="str">
-        <f>IF('Meal Calendar'!D83&lt;&gt;"", 'Meal Calendar'!D83, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="84" spans="1:3">
-      <c r="A84">
-        <v>2</v>
-      </c>
-      <c r="C84" t="str">
-        <f>IF('Meal Calendar'!D84&lt;&gt;"", 'Meal Calendar'!D84, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="85" spans="1:3">
-      <c r="A85">
-        <v>2</v>
-      </c>
-      <c r="C85" t="str">
-        <f>IF('Meal Calendar'!D85&lt;&gt;"", 'Meal Calendar'!D85, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="86" spans="1:3">
-      <c r="A86">
-        <v>2</v>
-      </c>
-      <c r="C86" t="str">
-        <f>IF('Meal Calendar'!D86&lt;&gt;"", 'Meal Calendar'!D86, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="87" spans="1:3">
-      <c r="A87">
-        <v>2</v>
-      </c>
-      <c r="C87" t="str">
-        <f>IF('Meal Calendar'!D87&lt;&gt;"", 'Meal Calendar'!D87, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="88" spans="1:3">
-      <c r="A88">
-        <v>2</v>
-      </c>
-      <c r="C88" t="str">
-        <f>IF('Meal Calendar'!D88&lt;&gt;"", 'Meal Calendar'!D88, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="89" spans="1:3">
-      <c r="A89">
-        <v>2</v>
-      </c>
-      <c r="C89" t="str">
-        <f>IF('Meal Calendar'!D89&lt;&gt;"", 'Meal Calendar'!D89, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="90" spans="1:3">
-      <c r="A90">
-        <v>2</v>
-      </c>
-      <c r="C90" t="str">
-        <f>IF('Meal Calendar'!D90&lt;&gt;"", 'Meal Calendar'!D90, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="91" spans="1:3">
-      <c r="A91">
-        <v>2</v>
-      </c>
-      <c r="C91" t="str">
-        <f>IF('Meal Calendar'!D91&lt;&gt;"", 'Meal Calendar'!D91, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="92" spans="1:3">
-      <c r="A92">
-        <v>2</v>
-      </c>
-      <c r="C92" t="str">
-        <f>IF('Meal Calendar'!D92&lt;&gt;"", 'Meal Calendar'!D92, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="93" spans="1:3">
-      <c r="A93">
-        <v>2</v>
-      </c>
-      <c r="C93" t="str">
-        <f>IF('Meal Calendar'!D93&lt;&gt;"", 'Meal Calendar'!D93, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="94" spans="1:3">
-      <c r="A94">
-        <v>2</v>
-      </c>
-      <c r="C94" t="str">
-        <f>IF('Meal Calendar'!D94&lt;&gt;"", 'Meal Calendar'!D94, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="95" spans="1:3">
-      <c r="A95">
-        <v>2</v>
-      </c>
-      <c r="C95" t="str">
-        <f>IF('Meal Calendar'!D95&lt;&gt;"", 'Meal Calendar'!D95, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="96" spans="1:3">
-      <c r="A96">
-        <v>2</v>
-      </c>
-      <c r="C96" t="str">
-        <f>IF('Meal Calendar'!D96&lt;&gt;"", 'Meal Calendar'!D96, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="97" spans="1:3">
-      <c r="A97">
-        <v>2</v>
-      </c>
-      <c r="C97" t="str">
-        <f>IF('Meal Calendar'!D97&lt;&gt;"", 'Meal Calendar'!D97, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="98" spans="1:3">
-      <c r="A98">
-        <v>2</v>
-      </c>
-      <c r="C98" t="str">
-        <f>IF('Meal Calendar'!D98&lt;&gt;"", 'Meal Calendar'!D98, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="99" spans="1:3">
-      <c r="A99">
-        <v>2</v>
-      </c>
-      <c r="C99" t="str">
-        <f>IF('Meal Calendar'!D99&lt;&gt;"", 'Meal Calendar'!D99, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="100" spans="1:3">
-      <c r="A100">
-        <v>2</v>
-      </c>
-      <c r="C100" t="str">
-        <f>IF('Meal Calendar'!D100&lt;&gt;"", 'Meal Calendar'!D100, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="101" spans="1:3">
-      <c r="A101">
-        <v>2</v>
-      </c>
-      <c r="C101" t="str">
-        <f>IF('Meal Calendar'!D101&lt;&gt;"", 'Meal Calendar'!D101, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="102" spans="1:3">
-      <c r="A102">
-        <v>3</v>
-      </c>
-      <c r="C102" t="str">
-        <f>IF('Meal Calendar'!J2&lt;&gt;"", 'Meal Calendar'!J2, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="103" spans="1:3">
-      <c r="A103">
-        <v>3</v>
-      </c>
-      <c r="C103" t="str">
-        <f>IF('Meal Calendar'!J3&lt;&gt;"", 'Meal Calendar'!J3, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="104" spans="1:3">
-      <c r="A104">
-        <v>3</v>
-      </c>
-      <c r="C104" t="str">
-        <f>IF('Meal Calendar'!J4&lt;&gt;"", 'Meal Calendar'!J4, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="105" spans="1:3">
-      <c r="A105">
-        <v>3</v>
-      </c>
-      <c r="C105" t="str">
-        <f>IF('Meal Calendar'!J5&lt;&gt;"", 'Meal Calendar'!J5, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="106" spans="1:3">
-      <c r="A106">
-        <v>3</v>
-      </c>
-      <c r="C106" t="str">
-        <f>IF('Meal Calendar'!J6&lt;&gt;"", 'Meal Calendar'!J6, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="107" spans="1:3">
-      <c r="A107">
-        <v>3</v>
-      </c>
-      <c r="C107" t="str">
-        <f>IF('Meal Calendar'!J7&lt;&gt;"", 'Meal Calendar'!J7, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="108" spans="1:3">
-      <c r="A108">
-        <v>3</v>
-      </c>
-      <c r="C108" t="str">
-        <f>IF('Meal Calendar'!J8&lt;&gt;"", 'Meal Calendar'!J8, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="109" spans="1:3">
-      <c r="A109">
-        <v>3</v>
-      </c>
-      <c r="C109" t="str">
-        <f>IF('Meal Calendar'!J9&lt;&gt;"", 'Meal Calendar'!J9, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="110" spans="1:3">
-      <c r="A110">
-        <v>3</v>
-      </c>
-      <c r="C110" t="str">
-        <f>IF('Meal Calendar'!J10&lt;&gt;"", 'Meal Calendar'!J10, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="111" spans="1:3">
-      <c r="A111">
-        <v>3</v>
-      </c>
-      <c r="C111" t="str">
-        <f>IF('Meal Calendar'!J11&lt;&gt;"", 'Meal Calendar'!J11, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="112" spans="1:3">
-      <c r="A112">
-        <v>3</v>
-      </c>
-      <c r="C112" t="str">
-        <f>IF('Meal Calendar'!J12&lt;&gt;"", 'Meal Calendar'!J12, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="113" spans="1:3">
-      <c r="A113">
-        <v>3</v>
-      </c>
-      <c r="C113" t="str">
-        <f>IF('Meal Calendar'!J13&lt;&gt;"", 'Meal Calendar'!J13, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="114" spans="1:3">
-      <c r="A114">
-        <v>3</v>
-      </c>
-      <c r="C114" t="str">
-        <f>IF('Meal Calendar'!J14&lt;&gt;"", 'Meal Calendar'!J14, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="115" spans="1:3">
-      <c r="A115">
-        <v>3</v>
-      </c>
-      <c r="C115" t="str">
-        <f>IF('Meal Calendar'!J15&lt;&gt;"", 'Meal Calendar'!J15, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="116" spans="1:3">
-      <c r="A116">
-        <v>3</v>
-      </c>
-      <c r="C116" t="str">
-        <f>IF('Meal Calendar'!J16&lt;&gt;"", 'Meal Calendar'!J16, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="117" spans="1:3">
-      <c r="A117">
-        <v>3</v>
-      </c>
-      <c r="C117" t="str">
-        <f>IF('Meal Calendar'!J17&lt;&gt;"", 'Meal Calendar'!J17, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="118" spans="1:3">
-      <c r="A118">
-        <v>3</v>
-      </c>
-      <c r="C118" t="str">
-        <f>IF('Meal Calendar'!J18&lt;&gt;"", 'Meal Calendar'!J18, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="119" spans="1:3">
-      <c r="A119">
-        <v>3</v>
-      </c>
-      <c r="C119" t="str">
-        <f>IF('Meal Calendar'!J19&lt;&gt;"", 'Meal Calendar'!J19, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="120" spans="1:3">
-      <c r="A120">
-        <v>3</v>
-      </c>
-      <c r="C120" t="str">
-        <f>IF('Meal Calendar'!J20&lt;&gt;"", 'Meal Calendar'!J20, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="121" spans="1:3">
-      <c r="A121">
-        <v>3</v>
-      </c>
-      <c r="C121" t="str">
-        <f>IF('Meal Calendar'!J21&lt;&gt;"", 'Meal Calendar'!J21, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="122" spans="1:3">
-      <c r="A122">
-        <v>3</v>
-      </c>
-      <c r="C122" t="str">
-        <f>IF('Meal Calendar'!J22&lt;&gt;"", 'Meal Calendar'!J22, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="123" spans="1:3">
-      <c r="A123">
-        <v>3</v>
-      </c>
-      <c r="C123" t="str">
-        <f>IF('Meal Calendar'!J23&lt;&gt;"", 'Meal Calendar'!J23, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="124" spans="1:3">
-      <c r="A124">
-        <v>3</v>
-      </c>
-      <c r="C124" t="str">
-        <f>IF('Meal Calendar'!J24&lt;&gt;"", 'Meal Calendar'!J24, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="125" spans="1:3">
-      <c r="A125">
-        <v>3</v>
-      </c>
-      <c r="C125" t="str">
-        <f>IF('Meal Calendar'!J25&lt;&gt;"", 'Meal Calendar'!J25, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="126" spans="1:3">
-      <c r="A126">
-        <v>3</v>
-      </c>
-      <c r="C126" t="str">
-        <f>IF('Meal Calendar'!J26&lt;&gt;"", 'Meal Calendar'!J26, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="127" spans="1:3">
-      <c r="A127">
-        <v>3</v>
-      </c>
-      <c r="C127" t="str">
-        <f>IF('Meal Calendar'!J27&lt;&gt;"", 'Meal Calendar'!J27, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="128" spans="1:3">
-      <c r="A128">
-        <v>3</v>
-      </c>
-      <c r="C128" t="str">
-        <f>IF('Meal Calendar'!J28&lt;&gt;"", 'Meal Calendar'!J28, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="129" spans="1:3">
-      <c r="A129">
-        <v>3</v>
-      </c>
-      <c r="C129" t="str">
-        <f>IF('Meal Calendar'!J29&lt;&gt;"", 'Meal Calendar'!J29, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="130" spans="1:3">
-      <c r="A130">
-        <v>3</v>
-      </c>
-      <c r="C130" t="str">
-        <f>IF('Meal Calendar'!J30&lt;&gt;"", 'Meal Calendar'!J30, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="131" spans="1:3">
-      <c r="A131">
-        <v>3</v>
-      </c>
-      <c r="C131" t="str">
-        <f>IF('Meal Calendar'!J31&lt;&gt;"", 'Meal Calendar'!J31, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="132" spans="1:3">
-      <c r="A132">
-        <v>3</v>
-      </c>
-      <c r="C132" t="str">
-        <f>IF('Meal Calendar'!J32&lt;&gt;"", 'Meal Calendar'!J32, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="133" spans="1:3">
-      <c r="A133">
-        <v>3</v>
-      </c>
-      <c r="C133" t="str">
-        <f>IF('Meal Calendar'!J33&lt;&gt;"", 'Meal Calendar'!J33, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="134" spans="1:3">
-      <c r="A134">
-        <v>3</v>
-      </c>
-      <c r="C134" t="str">
-        <f>IF('Meal Calendar'!J34&lt;&gt;"", 'Meal Calendar'!J34, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="135" spans="1:3">
-      <c r="A135">
-        <v>3</v>
-      </c>
-      <c r="C135" t="str">
-        <f>IF('Meal Calendar'!J35&lt;&gt;"", 'Meal Calendar'!J35, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="136" spans="1:3">
-      <c r="A136">
-        <v>3</v>
-      </c>
-      <c r="C136" t="str">
-        <f>IF('Meal Calendar'!J36&lt;&gt;"", 'Meal Calendar'!J36, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="137" spans="1:3">
-      <c r="A137">
-        <v>3</v>
-      </c>
-      <c r="C137" t="str">
-        <f>IF('Meal Calendar'!J37&lt;&gt;"", 'Meal Calendar'!J37, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="138" spans="1:3">
-      <c r="A138">
-        <v>3</v>
-      </c>
-      <c r="C138" t="str">
-        <f>IF('Meal Calendar'!J38&lt;&gt;"", 'Meal Calendar'!J38, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="139" spans="1:3">
-      <c r="A139">
-        <v>3</v>
-      </c>
-      <c r="C139" t="str">
-        <f>IF('Meal Calendar'!J39&lt;&gt;"", 'Meal Calendar'!J39, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="140" spans="1:3">
-      <c r="A140">
-        <v>3</v>
-      </c>
-      <c r="C140" t="str">
-        <f>IF('Meal Calendar'!J40&lt;&gt;"", 'Meal Calendar'!J40, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="141" spans="1:3">
-      <c r="A141">
-        <v>3</v>
-      </c>
-      <c r="C141" t="str">
-        <f>IF('Meal Calendar'!J41&lt;&gt;"", 'Meal Calendar'!J41, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="142" spans="1:3">
-      <c r="A142">
-        <v>3</v>
-      </c>
-      <c r="C142" t="str">
-        <f>IF('Meal Calendar'!J42&lt;&gt;"", 'Meal Calendar'!J42, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="143" spans="1:3">
-      <c r="A143">
-        <v>3</v>
-      </c>
-      <c r="C143" t="str">
-        <f>IF('Meal Calendar'!J43&lt;&gt;"", 'Meal Calendar'!J43, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="144" spans="1:3">
-      <c r="A144">
-        <v>3</v>
-      </c>
-      <c r="C144" t="str">
-        <f>IF('Meal Calendar'!J44&lt;&gt;"", 'Meal Calendar'!J44, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="145" spans="1:3">
-      <c r="A145">
-        <v>3</v>
-      </c>
-      <c r="C145" t="str">
-        <f>IF('Meal Calendar'!J45&lt;&gt;"", 'Meal Calendar'!J45, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="146" spans="1:3">
-      <c r="A146">
-        <v>3</v>
-      </c>
-      <c r="C146" t="str">
-        <f>IF('Meal Calendar'!J46&lt;&gt;"", 'Meal Calendar'!J46, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="147" spans="1:3">
-      <c r="A147">
-        <v>3</v>
-      </c>
-      <c r="C147" t="str">
-        <f>IF('Meal Calendar'!J47&lt;&gt;"", 'Meal Calendar'!J47, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="148" spans="1:3">
-      <c r="A148">
-        <v>3</v>
-      </c>
-      <c r="C148" t="str">
-        <f>IF('Meal Calendar'!J48&lt;&gt;"", 'Meal Calendar'!J48, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="149" spans="1:3">
-      <c r="A149">
-        <v>3</v>
-      </c>
-      <c r="C149" t="str">
-        <f>IF('Meal Calendar'!J49&lt;&gt;"", 'Meal Calendar'!J49, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="150" spans="1:3">
-      <c r="A150">
-        <v>3</v>
-      </c>
-      <c r="C150" t="str">
-        <f>IF('Meal Calendar'!J50&lt;&gt;"", 'Meal Calendar'!J50, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="151" spans="1:3">
-      <c r="A151">
-        <v>3</v>
-      </c>
-      <c r="C151" t="str">
-        <f>IF('Meal Calendar'!J51&lt;&gt;"", 'Meal Calendar'!J51, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="152" spans="1:3">
-      <c r="A152">
-        <v>4</v>
-      </c>
-      <c r="C152" t="str">
-        <f>IF('Meal Calendar'!J52&lt;&gt;"", 'Meal Calendar'!J52, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="153" spans="1:3">
-      <c r="A153">
-        <v>4</v>
-      </c>
-      <c r="C153" t="str">
-        <f>IF('Meal Calendar'!J53&lt;&gt;"", 'Meal Calendar'!J53, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="154" spans="1:3">
-      <c r="A154">
-        <v>4</v>
-      </c>
-      <c r="C154" t="str">
-        <f>IF('Meal Calendar'!J54&lt;&gt;"", 'Meal Calendar'!J54, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="155" spans="1:3">
-      <c r="A155">
-        <v>4</v>
-      </c>
-      <c r="C155" t="str">
-        <f>IF('Meal Calendar'!J55&lt;&gt;"", 'Meal Calendar'!J55, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="156" spans="1:3">
-      <c r="A156">
-        <v>4</v>
-      </c>
-      <c r="C156" t="str">
-        <f>IF('Meal Calendar'!J56&lt;&gt;"", 'Meal Calendar'!J56, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="157" spans="1:3">
-      <c r="A157">
-        <v>4</v>
-      </c>
-      <c r="C157" t="str">
-        <f>IF('Meal Calendar'!J57&lt;&gt;"", 'Meal Calendar'!J57, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="158" spans="1:3">
-      <c r="A158">
-        <v>4</v>
-      </c>
-      <c r="C158" t="str">
-        <f>IF('Meal Calendar'!J58&lt;&gt;"", 'Meal Calendar'!J58, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="159" spans="1:3">
-      <c r="A159">
-        <v>4</v>
-      </c>
-      <c r="C159" t="str">
-        <f>IF('Meal Calendar'!J59&lt;&gt;"", 'Meal Calendar'!J59, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="160" spans="1:3">
-      <c r="A160">
-        <v>4</v>
-      </c>
-      <c r="C160" t="str">
-        <f>IF('Meal Calendar'!J60&lt;&gt;"", 'Meal Calendar'!J60, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="161" spans="1:3">
-      <c r="A161">
-        <v>4</v>
-      </c>
-      <c r="C161" t="str">
-        <f>IF('Meal Calendar'!J61&lt;&gt;"", 'Meal Calendar'!J61, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="162" spans="1:3">
-      <c r="A162">
-        <v>4</v>
-      </c>
-      <c r="C162" t="str">
-        <f>IF('Meal Calendar'!J62&lt;&gt;"", 'Meal Calendar'!J62, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="163" spans="1:3">
-      <c r="A163">
-        <v>4</v>
-      </c>
-      <c r="C163" t="str">
-        <f>IF('Meal Calendar'!J63&lt;&gt;"", 'Meal Calendar'!J63, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="164" spans="1:3">
-      <c r="A164">
-        <v>4</v>
-      </c>
-      <c r="C164" t="str">
-        <f>IF('Meal Calendar'!J64&lt;&gt;"", 'Meal Calendar'!J64, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="165" spans="1:3">
-      <c r="A165">
-        <v>4</v>
-      </c>
-      <c r="C165" t="str">
-        <f>IF('Meal Calendar'!J65&lt;&gt;"", 'Meal Calendar'!J65, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="166" spans="1:3">
-      <c r="A166">
-        <v>4</v>
-      </c>
-      <c r="C166" t="str">
-        <f>IF('Meal Calendar'!J66&lt;&gt;"", 'Meal Calendar'!J66, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="167" spans="1:3">
-      <c r="A167">
-        <v>4</v>
-      </c>
-      <c r="C167" t="str">
-        <f>IF('Meal Calendar'!J67&lt;&gt;"", 'Meal Calendar'!J67, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="168" spans="1:3">
-      <c r="A168">
-        <v>4</v>
-      </c>
-      <c r="C168" t="str">
-        <f>IF('Meal Calendar'!J68&lt;&gt;"", 'Meal Calendar'!J68, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="169" spans="1:3">
-      <c r="A169">
-        <v>4</v>
-      </c>
-      <c r="C169" t="str">
-        <f>IF('Meal Calendar'!J69&lt;&gt;"", 'Meal Calendar'!J69, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="170" spans="1:3">
-      <c r="A170">
-        <v>4</v>
-      </c>
-      <c r="C170" t="str">
-        <f>IF('Meal Calendar'!J70&lt;&gt;"", 'Meal Calendar'!J70, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="171" spans="1:3">
-      <c r="A171">
-        <v>4</v>
-      </c>
-      <c r="C171" t="str">
-        <f>IF('Meal Calendar'!J71&lt;&gt;"", 'Meal Calendar'!J71, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="172" spans="1:3">
-      <c r="A172">
-        <v>4</v>
-      </c>
-      <c r="C172" t="str">
-        <f>IF('Meal Calendar'!J72&lt;&gt;"", 'Meal Calendar'!J72, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="173" spans="1:3">
-      <c r="A173">
-        <v>4</v>
-      </c>
-      <c r="C173" t="str">
-        <f>IF('Meal Calendar'!J73&lt;&gt;"", 'Meal Calendar'!J73, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="174" spans="1:3">
-      <c r="A174">
-        <v>4</v>
-      </c>
-      <c r="C174" t="str">
-        <f>IF('Meal Calendar'!J74&lt;&gt;"", 'Meal Calendar'!J74, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="175" spans="1:3">
-      <c r="A175">
-        <v>4</v>
-      </c>
-      <c r="C175" t="str">
-        <f>IF('Meal Calendar'!J75&lt;&gt;"", 'Meal Calendar'!J75, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="176" spans="1:3">
-      <c r="A176">
-        <v>4</v>
-      </c>
-      <c r="C176" t="str">
-        <f>IF('Meal Calendar'!J76&lt;&gt;"", 'Meal Calendar'!J76, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="177" spans="1:3">
-      <c r="A177">
-        <v>4</v>
-      </c>
-      <c r="C177" t="str">
-        <f>IF('Meal Calendar'!J77&lt;&gt;"", 'Meal Calendar'!J77, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="178" spans="1:3">
-      <c r="A178">
-        <v>4</v>
-      </c>
-      <c r="C178" t="str">
-        <f>IF('Meal Calendar'!J78&lt;&gt;"", 'Meal Calendar'!J78, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="179" spans="1:3">
-      <c r="A179">
-        <v>4</v>
-      </c>
-      <c r="C179" t="str">
-        <f>IF('Meal Calendar'!J79&lt;&gt;"", 'Meal Calendar'!J79, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="180" spans="1:3">
-      <c r="A180">
-        <v>4</v>
-      </c>
-      <c r="C180" t="str">
-        <f>IF('Meal Calendar'!J80&lt;&gt;"", 'Meal Calendar'!J80, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="181" spans="1:3">
-      <c r="A181">
-        <v>4</v>
-      </c>
-      <c r="C181" t="str">
-        <f>IF('Meal Calendar'!J81&lt;&gt;"", 'Meal Calendar'!J81, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="182" spans="1:3">
-      <c r="A182">
-        <v>4</v>
-      </c>
-      <c r="C182" t="str">
-        <f>IF('Meal Calendar'!J82&lt;&gt;"", 'Meal Calendar'!J82, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="183" spans="1:3">
-      <c r="A183">
-        <v>4</v>
-      </c>
-      <c r="C183" t="str">
-        <f>IF('Meal Calendar'!J83&lt;&gt;"", 'Meal Calendar'!J83, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="184" spans="1:3">
-      <c r="A184">
-        <v>4</v>
-      </c>
-      <c r="C184" t="str">
-        <f>IF('Meal Calendar'!J84&lt;&gt;"", 'Meal Calendar'!J84, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="185" spans="1:3">
-      <c r="A185">
-        <v>4</v>
-      </c>
-      <c r="C185" t="str">
-        <f>IF('Meal Calendar'!J85&lt;&gt;"", 'Meal Calendar'!J85, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="186" spans="1:3">
-      <c r="A186">
-        <v>4</v>
-      </c>
-      <c r="C186" t="str">
-        <f>IF('Meal Calendar'!J86&lt;&gt;"", 'Meal Calendar'!J86, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="187" spans="1:3">
-      <c r="A187">
-        <v>4</v>
-      </c>
-      <c r="C187" t="str">
-        <f>IF('Meal Calendar'!J87&lt;&gt;"", 'Meal Calendar'!J87, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="188" spans="1:3">
-      <c r="A188">
-        <v>4</v>
-      </c>
-      <c r="C188" t="str">
-        <f>IF('Meal Calendar'!J88&lt;&gt;"", 'Meal Calendar'!J88, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="189" spans="1:3">
-      <c r="A189">
-        <v>4</v>
-      </c>
-      <c r="C189" t="str">
-        <f>IF('Meal Calendar'!J89&lt;&gt;"", 'Meal Calendar'!J89, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="190" spans="1:3">
-      <c r="A190">
-        <v>4</v>
-      </c>
-      <c r="C190" t="str">
-        <f>IF('Meal Calendar'!J90&lt;&gt;"", 'Meal Calendar'!J90, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="191" spans="1:3">
-      <c r="A191">
-        <v>4</v>
-      </c>
-      <c r="C191" t="str">
-        <f>IF('Meal Calendar'!J91&lt;&gt;"", 'Meal Calendar'!J91, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="192" spans="1:3">
-      <c r="A192">
-        <v>4</v>
-      </c>
-      <c r="C192" t="str">
-        <f>IF('Meal Calendar'!J92&lt;&gt;"", 'Meal Calendar'!J92, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="193" spans="1:3">
-      <c r="A193">
-        <v>4</v>
-      </c>
-      <c r="C193" t="str">
-        <f>IF('Meal Calendar'!J93&lt;&gt;"", 'Meal Calendar'!J93, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="194" spans="1:3">
-      <c r="A194">
-        <v>4</v>
-      </c>
-      <c r="C194" t="str">
-        <f>IF('Meal Calendar'!J94&lt;&gt;"", 'Meal Calendar'!J94, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="195" spans="1:3">
-      <c r="A195">
-        <v>4</v>
-      </c>
-      <c r="C195" t="str">
-        <f>IF('Meal Calendar'!J95&lt;&gt;"", 'Meal Calendar'!J95, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="196" spans="1:3">
-      <c r="A196">
-        <v>4</v>
-      </c>
-      <c r="C196" t="str">
-        <f>IF('Meal Calendar'!J96&lt;&gt;"", 'Meal Calendar'!J96, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="197" spans="1:3">
-      <c r="A197">
-        <v>4</v>
-      </c>
-      <c r="C197" t="str">
-        <f>IF('Meal Calendar'!J97&lt;&gt;"", 'Meal Calendar'!J97, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="198" spans="1:3">
-      <c r="A198">
-        <v>4</v>
-      </c>
-      <c r="C198" t="str">
-        <f>IF('Meal Calendar'!J98&lt;&gt;"", 'Meal Calendar'!J98, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="199" spans="1:3">
-      <c r="A199">
-        <v>4</v>
-      </c>
-      <c r="C199" t="str">
-        <f>IF('Meal Calendar'!J99&lt;&gt;"", 'Meal Calendar'!J99, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="200" spans="1:3">
-      <c r="A200">
-        <v>4</v>
-      </c>
-      <c r="C200" t="str">
-        <f>IF('Meal Calendar'!J100&lt;&gt;"", 'Meal Calendar'!J100, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="201" spans="1:3">
-      <c r="A201">
-        <v>4</v>
-      </c>
-      <c r="C201" t="str">
-        <f>IF('Meal Calendar'!J101&lt;&gt;"", 'Meal Calendar'!J101, "")</f>
-        <v/>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA4164A3-C298-314D-8211-F5B8F16F83E1}">
-  <dimension ref="A1:E100"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <cols>
-    <col min="1" max="5" width="20.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="30" customHeight="1">
-      <c r="A1" t="s">
-        <v>1189</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1187</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1188</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1186</v>
-      </c>
-      <c r="E1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="30" customHeight="1"/>
-    <row r="3" spans="1:5" ht="30" customHeight="1"/>
-    <row r="4" spans="1:5" ht="30" customHeight="1"/>
-    <row r="5" spans="1:5" ht="30" customHeight="1"/>
-    <row r="6" spans="1:5" ht="30" customHeight="1"/>
-    <row r="7" spans="1:5" ht="30" customHeight="1"/>
-    <row r="8" spans="1:5" ht="30" customHeight="1"/>
-    <row r="9" spans="1:5" ht="30" customHeight="1"/>
-    <row r="10" spans="1:5" ht="30" customHeight="1"/>
-    <row r="11" spans="1:5" ht="30" customHeight="1"/>
-    <row r="12" spans="1:5" ht="30" customHeight="1"/>
-    <row r="13" spans="1:5" ht="30" customHeight="1"/>
-    <row r="14" spans="1:5" ht="30" customHeight="1"/>
-    <row r="15" spans="1:5" ht="30" customHeight="1"/>
-    <row r="16" spans="1:5" ht="30" customHeight="1"/>
-    <row r="17" ht="30" customHeight="1"/>
-    <row r="18" ht="30" customHeight="1"/>
-    <row r="19" ht="30" customHeight="1"/>
-    <row r="20" ht="30" customHeight="1"/>
-    <row r="21" ht="30" customHeight="1"/>
-    <row r="22" ht="30" customHeight="1"/>
-    <row r="23" ht="30" customHeight="1"/>
-    <row r="24" ht="30" customHeight="1"/>
-    <row r="25" ht="30" customHeight="1"/>
-    <row r="26" ht="30" customHeight="1"/>
-    <row r="27" ht="30" customHeight="1"/>
-    <row r="28" ht="30" customHeight="1"/>
-    <row r="29" ht="30" customHeight="1"/>
-    <row r="30" ht="30" customHeight="1"/>
-    <row r="31" ht="30" customHeight="1"/>
-    <row r="32" ht="30" customHeight="1"/>
-    <row r="33" ht="30" customHeight="1"/>
-    <row r="34" ht="30" customHeight="1"/>
-    <row r="35" ht="30" customHeight="1"/>
-    <row r="36" ht="30" customHeight="1"/>
-    <row r="37" ht="30" customHeight="1"/>
-    <row r="38" ht="30" customHeight="1"/>
-    <row r="39" ht="30" customHeight="1"/>
-    <row r="40" ht="30" customHeight="1"/>
-    <row r="41" ht="30" customHeight="1"/>
-    <row r="42" ht="30" customHeight="1"/>
-    <row r="43" ht="30" customHeight="1"/>
-    <row r="44" ht="30" customHeight="1"/>
-    <row r="45" ht="30" customHeight="1"/>
-    <row r="46" ht="30" customHeight="1"/>
-    <row r="47" ht="30" customHeight="1"/>
-    <row r="48" ht="30" customHeight="1"/>
-    <row r="49" ht="30" customHeight="1"/>
-    <row r="50" ht="30" customHeight="1"/>
-    <row r="51" ht="30" customHeight="1"/>
-    <row r="52" ht="30" customHeight="1"/>
-    <row r="53" ht="30" customHeight="1"/>
-    <row r="54" ht="30" customHeight="1"/>
-    <row r="55" ht="30" customHeight="1"/>
-    <row r="56" ht="30" customHeight="1"/>
-    <row r="57" ht="30" customHeight="1"/>
-    <row r="58" ht="30" customHeight="1"/>
-    <row r="59" ht="30" customHeight="1"/>
-    <row r="60" ht="30" customHeight="1"/>
-    <row r="61" ht="30" customHeight="1"/>
-    <row r="62" ht="30" customHeight="1"/>
-    <row r="63" ht="30" customHeight="1"/>
-    <row r="64" ht="30" customHeight="1"/>
-    <row r="65" ht="30" customHeight="1"/>
-    <row r="66" ht="30" customHeight="1"/>
-    <row r="67" ht="30" customHeight="1"/>
-    <row r="68" ht="30" customHeight="1"/>
-    <row r="69" ht="30" customHeight="1"/>
-    <row r="70" ht="30" customHeight="1"/>
-    <row r="71" ht="30" customHeight="1"/>
-    <row r="72" ht="30" customHeight="1"/>
-    <row r="73" ht="30" customHeight="1"/>
-    <row r="74" ht="30" customHeight="1"/>
-    <row r="75" ht="30" customHeight="1"/>
-    <row r="76" ht="30" customHeight="1"/>
-    <row r="77" ht="30" customHeight="1"/>
-    <row r="78" ht="30" customHeight="1"/>
-    <row r="79" ht="30" customHeight="1"/>
-    <row r="80" ht="30" customHeight="1"/>
-    <row r="81" ht="30" customHeight="1"/>
-    <row r="82" ht="30" customHeight="1"/>
-    <row r="83" ht="30" customHeight="1"/>
-    <row r="84" ht="30" customHeight="1"/>
-    <row r="85" ht="30" customHeight="1"/>
-    <row r="86" ht="30" customHeight="1"/>
-    <row r="87" ht="30" customHeight="1"/>
-    <row r="88" ht="30" customHeight="1"/>
-    <row r="89" ht="30" customHeight="1"/>
-    <row r="90" ht="30" customHeight="1"/>
-    <row r="91" ht="30" customHeight="1"/>
-    <row r="92" ht="30" customHeight="1"/>
-    <row r="93" ht="30" customHeight="1"/>
-    <row r="94" ht="30" customHeight="1"/>
-    <row r="95" ht="30" customHeight="1"/>
-    <row r="96" ht="30" customHeight="1"/>
-    <row r="97" ht="30" customHeight="1"/>
-    <row r="98" ht="30" customHeight="1"/>
-    <row r="99" ht="30" customHeight="1"/>
-    <row r="100" ht="30" customHeight="1"/>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:F387"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
       <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fix:reformatted recipes after scraping
</commit_message>
<xml_diff>
--- a/MealPrepTracker.xlsx
+++ b/MealPrepTracker.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/quinnreams/Documents/GitHub/Personal-Growth-Planner/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{468D3260-D247-D24E-833E-C0F61543912D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3D26196-D6E8-9D49-915C-C2ECC3489BCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19620" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19580" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Meal Calendar" sheetId="1" r:id="rId1"/>
     <sheet name="Recipes" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Recipes!$A$1:$F$387</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Recipes!$A$1:$F$1</definedName>
     <definedName name="Breakfast">_xlfn._xlws.FILTER(Recipes!$B$2:$B$1000, Recipes!$A$2:$A$1000="breakfast")</definedName>
     <definedName name="Dinner">_xlfn._xlws.FILTER(Recipes!$B$2:$B$1000, Recipes!$A$2:$A$1000="dinner")</definedName>
     <definedName name="Lunch">_xlfn._xlws.FILTER(Recipes!$B$2:$B$1000, Recipes!$A$2:$A$1000="lunch")</definedName>
@@ -155,6 +155,834 @@
     <t>https://www.foodandwine.com/recipes/pastrami-breakfast-biscuit</t>
   </si>
   <si>
+    <t>Breakfast Sausage, Mushroom, and Cheddar Rolls Recipe</t>
+  </si>
+  <si>
+    <t>1/2 pound breakfast sausage (about 10 links), 10 ounces button mushrooms, finely chopped, 4 sprigs thyme, 1/2 cup grated sharp Cheddar cheese, 1 pound puff pastry, thawed if frozen, 1 egg, beaten, Kosher salt and freshly ground black pepper, Hot English or Dijon mustard for serving</t>
+  </si>
+  <si>
+    <t>http://www.seriouseats.com/recipes/2014/01/breakfast-sausage-mushroom-cheddar-roll-recipe.html</t>
+  </si>
+  <si>
+    <t>Mini Breakfast Cookie &amp; Yogurt</t>
+  </si>
+  <si>
+    <t>1 oatmeal raisin mini breakfast cookie, 5 ⅓ ounces nonfat organic vanilla Greek yogurt, 1 cup raspberries</t>
+  </si>
+  <si>
+    <t>http://www.eatingwell.com/recipe/266418/mini-breakfast-cookie-yogurt/</t>
+  </si>
+  <si>
+    <t>Sausage and Potato Breakfast Casserole</t>
+  </si>
+  <si>
+    <t>1 pound bulk breakfast sausage, 2 tablespoons all purpose flour, 1 1/2 cups milk (do not use low-fat or nonfat), 1 1-pound package frozen shredded hash brown potatoes, 4 green onions, finely chopped, 1 1/4 cups grated sharp cheddar cheese</t>
+  </si>
+  <si>
+    <t>https://www.epicurious.com/recipes/food/views/sausage-and-potato-breakfast-casserole-4387</t>
+  </si>
+  <si>
+    <t>BA's Best Breakfast Sandwich</t>
+  </si>
+  <si>
+    <t>Unsalted butter, 1 English muffin, split, 1 BA Breakfast Sausage patty, 2 slices American cheese, 2 large eggs, beaten to blend, Kosher salt and freshly ground black pepper, Handful of chopped fresh chives, Hot sauce and honey (for serving; optional)</t>
+  </si>
+  <si>
+    <t>https://www.bonappetit.com/recipe/bas-best-breakfast-sandwich</t>
+  </si>
+  <si>
+    <t>Sausage and Cheddar Breakfast Casserole</t>
+  </si>
+  <si>
+    <t>1 tbsp. unsalted butter, for greasing, 6 slices white bread, 1 lb. bulk breakfast sausage, casing removed, 10 oz. grated cheddar cheese, 2 cups milk, 1⁄2 tsp. dry mustard, 6 eggs, lightly beaten, Kosher salt and freshly ground black pepper, to taste</t>
+  </si>
+  <si>
+    <t>https://www.saveur.com/article/recipes/sausage-and-cheddar-breakfast-casserole/</t>
+  </si>
+  <si>
+    <t>Paleo Sweet Potato Breakfast Hash</t>
+  </si>
+  <si>
+    <t>3 Large Sweet Potatoes (washed, peeled, and cubed), 1 tablespoon Olive Oil, 1 teaspoon Garlic Powder, 1 teaspoon Onion Powder, 1/2 teaspoon Paprika, 1 pinch Salt and Pepper, 4 Breakfast Sausage Links, 1/4 cup Red Onion (chopped), 1/2 cup Cherry Tomatoes, 1/2 tablespoon Organic Sriracha</t>
+  </si>
+  <si>
+    <t>https://food52.com/recipes/78306-paleo-sweet-potato-breakfast-hash</t>
+  </si>
+  <si>
+    <t>Breakfast Pigs in a Blanket</t>
+  </si>
+  <si>
+    <t>16 cooked or uncooked breakfast sausage links (do not thaw if frozen), 1 (8-ounce) can refrigerated crescent rolls</t>
+  </si>
+  <si>
+    <t>https://www.thekitchn.com/breakfast-pigs-in-a-blanket-recipe-23524373</t>
+  </si>
+  <si>
+    <t>Breakfast Fried Rice</t>
+  </si>
+  <si>
+    <t>1/2 yellow onion, finely chopped, 2 cloves garlic, minced, 1 tablespoon olive oil, 4 small breakfast sausages, 2 cup cooked rice, 2 tablespoons soy sauce, 1 teaspoon rice vinegar, 1 teaspoon toasted sesame oil, 1 teaspoon sriracha, 3 eggs, 3 tablespoons scallions, Salt and pepper</t>
+  </si>
+  <si>
+    <t>https://www.realsimple.com/food-recipes/browse-all-recipes/breakfast-fried-rice</t>
+  </si>
+  <si>
+    <t>Strawberry Jam Breakfast Biscuit</t>
+  </si>
+  <si>
+    <t>1 Breakfast Biscuit, 1 rounded tablespoon of strawberry jam</t>
+  </si>
+  <si>
+    <t>https://www.foodandwine.com/recipes/strawberry-jam-breakfast-biscuit</t>
+  </si>
+  <si>
+    <t>Dinner Tonight: Breakfast Sausage, Home Fries, and Eggs Recipe</t>
+  </si>
+  <si>
+    <t>1 pound breakfast sausage, 1 pound baking potatoes, peeled and cut into 1-inch cubes, 1/2 cup chopped onion, 1/3 cup chopped green bell pepper, 1 teaspoon garlic, minced, 3/4 teaspoon Creole seasoning, plus more for sprinkling, Canola oil, Salt and pepper, 4 eggs</t>
+  </si>
+  <si>
+    <t>http://www.seriouseats.com/recipes/2010/06/breakfast-sausage-home-fries-eggs-recipe.html</t>
+  </si>
+  <si>
+    <t>Sausage Breakfast Casserole</t>
+  </si>
+  <si>
+    <t>1 tablespoon olive oil, 14 to 16 ounces uncooked pork breakfast sausage, Cooking spray or olive oil, 12 large eggs, 2 cups half-and-half, 2 teaspoons dry mustard, 1 1/2 teaspoons kosher salt, 1/2 teaspoon freshly ground black pepper, 8 ounces sharp cheddar cheese, shredded (2 cups), preferably white, 6 slices hearty white sandwich bread (8 to 9 ounces)</t>
+  </si>
+  <si>
+    <t>https://www.thekitchn.com/sausage-breakfast-casserole-recipe-23218282</t>
+  </si>
+  <si>
+    <t>Recipe: Breakfast Fried Rice</t>
+  </si>
+  <si>
+    <t>2 tablespoons vegetable oil, divided, 3 large eggs, lightly beaten, 1 ounces uncooked breakfast sausage, casings removed, 1/2 medium onion, finely diced, 5 cups cooked rice, preferably cold, 2 tablespoons tamari or soy sauce, 1/2 teaspoon kosher salt, Freshly ground black pepper, 1/2 cup shredded sharp cheddar cheese, 1/2 cup frozen peas, 1 tablespoon coarsely chopped fresh parsley leaves</t>
+  </si>
+  <si>
+    <t>https://www.thekitchn.com/recipe-breakfast-fried-rice-253305</t>
+  </si>
+  <si>
+    <t>Recipe: Breakfast Stromboli</t>
+  </si>
+  <si>
+    <t>1 teaspoon olive oil, 8 ounces uncooked breakfast sausage, casings removed, 1/4 medium yellow onion, finely chopped, 4 large eggs, 1 tablespoon whole or 2% milk, 1/4 teaspoon kosher salt, Freshly ground black pepper, 1 pound pizza dough, at room temperature for at least 1 hour, 1 cup shredded sharp cheddar cheese, divided, 1 tablespoon coarsely chopped fresh parsley leaves</t>
+  </si>
+  <si>
+    <t>https://www.thekitchn.com/breakfast-hot-pocket-257232</t>
+  </si>
+  <si>
+    <t>Recipe: Sheet-Pan “Half English” Breakfast</t>
+  </si>
+  <si>
+    <t>Cooking spray or olive oil, 2 medium plum tomatoes, 2 tablespoons olive oil, divided, 1/4 teaspoon dried thyme, divided, Kosher salt, Freshly ground black pepper, 12 medium cremini mushrooms, 8 small uncooked breakfast link sausages (about 8 ounces), 4 large eggs, Toast, for serving (optional)</t>
+  </si>
+  <si>
+    <t>https://www.thekitchn.com/recipe-sheet-pan-half-english-breakfast-228390</t>
+  </si>
+  <si>
+    <t>Recipe: Easy Paleo Breakfast Egg Muffins</t>
+  </si>
+  <si>
+    <t>Cooking spray or olive oil, 8 ounces sugar-free uncooked pork breakfast sausage, casings removed, 1 cup thinly sliced cremini mushrooms (about 3 ounces), 1/2 cup diced yellow onion, 1 cup baby spinach (about 1 ounce), coarsely chopped, 8 large eggs, 3 tablespoons ghee, melted and cooled, 1 teaspoon kosher salt, 1/4 teaspoon freshly ground black pepper</t>
+  </si>
+  <si>
+    <t>https://www.thekitchn.com/recipe-easy-paleo-breakfast-egg-muffins-258351</t>
+  </si>
+  <si>
+    <t>Breakfast Meatballs</t>
+  </si>
+  <si>
+    <t>Cooking spray, 4 slices thick-cut bacon (about 5 ounces), 1 medium Pink Lady or Granny Smith apple, 1/2 medium yellow onion, 1 large egg, 1/2 cup shredded sharp cheddar cheese (2 ounces), 1/2 medium bunch fresh chives, 1 1/2 teaspoons kosher salt, 1/2 teaspoon freshly ground black pepper, 1/2 cup fine, dry breadcrumbs, 1/2 cup whole or 2% milk, 1 pound uncooked breakfast sausage, 2 tablespoons maple syrup, plus more for drizzling, Serving suggestions: creamy polenta , cheesy grits , or buttered noodles</t>
+  </si>
+  <si>
+    <t>https://www.thekitchn.com/breakfast-meatballs-23326125</t>
+  </si>
+  <si>
+    <t>The Ultimate Make-Ahead Breakfast Casserole</t>
+  </si>
+  <si>
+    <t>8 ounces crusty French bread or baguette, 4 teaspoons olive oil, divided, 2 medium scallions, 4 ounces cheddar cheese, 8 ounces uncooked breakfast sausage, 6 large eggs, 1 cup whole milk or 2% milk, 1 teaspoon smoked paprika, plus more for sprinkling, 1/2 teaspoon kosher salt, 1/4 teaspoon freshly ground black pepper</t>
+  </si>
+  <si>
+    <t>https://www.thekitchn.com/breakfast-casserole-recipe-23421081</t>
+  </si>
+  <si>
+    <t>Breakfast Burritos Plain</t>
+  </si>
+  <si>
+    <t>18 flour tortillas, 1 pound breakfast sausage, 4 tablespoons salted butter, 18 large eggs, 1/2 teaspoon kosher salt, 1/2 teaspoon freshly ground black pepper</t>
+  </si>
+  <si>
+    <t>https://www.foodnetwork.com/recipes/ree-drummond/breakfast-burritos-plain-8741035</t>
+  </si>
+  <si>
+    <t>Double Pork Sausage</t>
+  </si>
+  <si>
+    <t>4 slices bacon, cut in half crosswise, 8 pork breakfast sausages</t>
+  </si>
+  <si>
+    <t>https://www.marthastewart.com/964328/double-pork-sausage</t>
+  </si>
+  <si>
+    <t>Bison Breakfast Patties</t>
+  </si>
+  <si>
+    <t>1 Tablespoon dried sage, 1 Tablespoon onion powder, 1/2 Teaspoon fennel seeds, crushed, 2 Teaspoons brown sugar, 1 Pound bison breakfast sausage, 1 egg white, Salt and pepper, to taste, Vegetable oil, as needed</t>
+  </si>
+  <si>
+    <t>http://www.thedailymeal.com/bison-breakfast-patties-recipe</t>
+  </si>
+  <si>
+    <t>Breakfast Taquitos</t>
+  </si>
+  <si>
+    <t>12 small breakfast sausage links, 2 tbsp. butter, 6 eggs, 1/4 c. milk, 1/4 c. Chopped chives, 1/2 c. shredded Cheddar, 12 small corn tortillas, warmed, Hot sauce, for serving (optional)</t>
+  </si>
+  <si>
+    <t>http://www.delish.com/cooking/recipe-ideas/recipes/a48242/breakfast-taquitos-recipe/</t>
+  </si>
+  <si>
+    <t>Cider-Glazed Sausage</t>
+  </si>
+  <si>
+    <t>12 ounces (1 package) frozen breakfast sausage links, 1 cup apple cider</t>
+  </si>
+  <si>
+    <t>https://www.marthastewart.com/313789/cider-glazed-sausage</t>
+  </si>
+  <si>
+    <t>Breakfast Casserole with Mushroom "Gravy" (Made with Cream of Mushroom Soup)</t>
+  </si>
+  <si>
+    <t>1 pound breakfast sausage, 4 cups shredded cheddar cheese, 8 slices of bread, 6 eggs, 2 cups milk + 1/2 cup milk, reserved, 1 can of Cream of Mushroom soup, 1/2 tablespoon dried Italian Herbs, 3/4 teaspoon dry mustard powder, 1/2 teaspoon salt, Freshly cracked black pepper</t>
+  </si>
+  <si>
+    <t>https://food52.com/recipes/40963-breakfast-casserole-with-mushroom-gravy</t>
+  </si>
+  <si>
+    <t>Recipe: Egg, Sausage, and Cheese Bundt Breakfast Sandwich</t>
+  </si>
+  <si>
+    <t>Cooking spray, 1 pound frozen bread dough, thawed according to package directions, 8 ounces uncooked breakfast sausage, casings removed, 8 large eggs, 1/2 teaspoon kosher salt, Large pinch freshly ground black pepper, 1 (12-ounce) jar roasted red peppers, drained, 4 to 5 slices sharp cheddar cheese (about 4 ounces)</t>
+  </si>
+  <si>
+    <t>https://www.thekitchn.com/recipe-egg-sausage-and-cheese-bundt-breakfast-sandwich-235022</t>
+  </si>
+  <si>
+    <t>Potato, Sausage, and Spinach Breakfast Casserole</t>
+  </si>
+  <si>
+    <t>16 large eggs, 1 1/4 cups heavy cream, 1 1/2 teaspoons kosher salt plus more, 3/4 teaspoon freshly ground black pepper plus more, 5 tablespoons unsalted butter, divided, 12 ounces fresh breakfast sausage links, 2 cups sliced leeks, white and pale-green parts only, 2 russet potatoes (1 1/2 pounds), peeled, shredded, lightly squeezed, 1 pound frozen spinach, thawed, squeezed dry, roughly chopped, 1 1/2 cups (4 ounces) grated Gruyère, 1/2 cup (1 1/2 ounces) grated Parmesan</t>
+  </si>
+  <si>
+    <t>https://www.epicurious.com/recipes/food/views/potato-sausage-and-spinach-breakfast-casserole-368302</t>
+  </si>
+  <si>
+    <t>McDonald’s Breakfast Burrito</t>
+  </si>
+  <si>
+    <t>5 Ounces breakfast sausage, crumbled, 2 Tablespoons white onion, minced, 4 eggs, beaten, Salt, to taste, Black pepper, to taste, 4 flour tortillas, 4 slices of American cheese</t>
+  </si>
+  <si>
+    <t>http://www.thedailymeal.com/recipes/mcdonald-s-breakfast-burrito-recipe</t>
+  </si>
+  <si>
+    <t>Recipe: Sausage and Greens Breakfast Casserole</t>
+  </si>
+  <si>
+    <t>1 pound frozen diced potatoes (about 4 cups, do not thaw), 1 tablespoon olive oil, plus more for the baking dish, 1 pound uncooked breakfast sausage, casings removed, 1 medium yellow onion, diced, 1 1/2 teaspoons dried oregano, 5 ounces baby spinach (about 5 packed cups), 8 large eggs, 1 1/2 cups whole or 2% milk, 1 1/2 teaspoons kosher salt, 1/4 teaspoon freshly ground black pepper, 2 cups shredded Italian blend cheese (such as Parmesan, mozzarella, provolone)</t>
+  </si>
+  <si>
+    <t>https://www.thekitchn.com/recipe-sausage-and-greens-breakfast-casserole-243967</t>
+  </si>
+  <si>
+    <t>Polenta for Breakfast</t>
+  </si>
+  <si>
+    <t>For the Polenta, 1 tablespoon butter, 4 cups boiling water, 1 cup coarse cornmeal or polenta, preferably from Bob's Red Mill, 1 cup cold water, 1 teaspoon Kosher salt, 1/4 cup butter or light olive oil, 1/4-1/2 cups freshly grated Parmesan or shredded sharp Cheddar (optional), 1/4-1/2 cups milk, cream or half-and-half, Kosher salt and fresh-ground pepper, For Serving, 4-6 poached or fried eggs, 1 pound Breakfast sausage, ham or bacon, cooked as desired, 8-12 Toasted and buttered ciabatta squares (2 slices per person), 2 tablespoons chopped fresh parsley, chives or green onion</t>
+  </si>
+  <si>
+    <t>https://food52.com/recipes/1987-polenta-for-breakfast</t>
+  </si>
+  <si>
+    <t>Easy Breakfast Casserole</t>
+  </si>
+  <si>
+    <t>For the breakfast casserole base:, 6 to 10 large eggs, 2 to 3 cups grated cheddar cheese, 6 slices day-old bread, cut into 3/4-inch to 1-inch-wide cubes, 2 cups milk, Salt, Pepper, For the possible additions:, 1 cup corn (cooked or frozen), 1/2 cup chopped broccoli (cooked or raw, raw will turn out crunchier), 1/2 cup sliced mushrooms, 1/4 cup sliced green onions, 1 cup cubed ham and/or cooked Italian sausage, A few slices cooked bacon, chopped, 1 teaspoon Herbes de Provence, or other dried herbs, (or 1 tablespoon of fresh chopped herbs such as basil, rosemary, or thyme), 1/4 to 1/2 teaspoon of cumin or curry powder</t>
+  </si>
+  <si>
+    <t>https://www.simplyrecipes.com/recipes/as_you_like_it_breakfast_casserole/</t>
+  </si>
+  <si>
+    <t>Breakfast Burritos with Cheese</t>
+  </si>
+  <si>
+    <t>18 flour tortillas, 1 pound breakfast sausage, 1/3 stick (about 2 1/2 tablespoons) salted butter, 18 large eggs, 1/2 teaspoon kosher salt, 1/2 teaspoon freshly ground black pepper, 3 cups grated cheese</t>
+  </si>
+  <si>
+    <t>https://www.foodnetwork.com/recipes/ree-drummond/breakfast-burritos-with-cheese-8741043</t>
+  </si>
+  <si>
+    <t>Creamy Turkey Breakfast Casserole</t>
+  </si>
+  <si>
+    <t>6 slices turkey bacon, such as JENNIE-O® Turkey Bacon, 1 (12-ounce) package turkey breakfast sausage links, such as JENNIE-O® Lean Turkey Breakfast Sausage Links, 1/2 Cup butter, divided, 1/2 Cup flour, 4 Cups milk, 1/2 Cup sliced fresh mushrooms, 1/4 Teaspoon black pepper, 4 Cups egg substitute or 16 eggs, 1 (7.5-ounce) package refrigerated biscuit dough</t>
+  </si>
+  <si>
+    <t>http://www.thedailymeal.com/recipes/creamy-turkey-breakfast-casserole-recipe</t>
+  </si>
+  <si>
+    <t>Recipe: Cheesy Hash Brown Breakfast Casserole</t>
+  </si>
+  <si>
+    <t>Cooking spray or oil, 1 tablespoon olive oil, 1 pound uncooked breakfast sausage, casings removed, 1 medium onion, diced, 1 medium red bell pepper, cored, seeded, and diced, 3/4 teaspoon kosher salt, divided, 1 (20-ounce) bag frozen shredded potatoes (do not thaw), 10 large eggs, 1 cup sour cream, 1 cup whole or 2% milk, 2 tablespoons Dijon mustard, 1 1/2 cups shredded sharp cheddar cheese (about 6 ounces), 1/4 teaspoon freshly ground black pepper</t>
+  </si>
+  <si>
+    <t>https://www.thekitchn.com/recipe-cheesy-hashbrown-breakfast-casserole-241992</t>
+  </si>
+  <si>
+    <t>Cowboy Breakfast Casserole With Sausage and Spinach</t>
+  </si>
+  <si>
+    <t>7 slices white sandwich bread, 1 pound bulk breakfast sausage, Softened unsalted butter or nonstick vegetable cooking spray (for pan), 4 scallions, white and pale green and dark green parts separated, thinly sliced, 1 (10-ounce) package frozen spinach, thawed, squeezed dry, 8 ounces cheddar cheese, shredded (about 2 cups), 8 large eggs, 1 1/2 cups milk, 1/2 cup full-fat Greek yogurt, 1 teaspoon mustard powder, 1/2 teaspoon kosher salt, 1/2 teaspoon freshly ground black pepper, 1/4 teaspoon ground nutmeg</t>
+  </si>
+  <si>
+    <t>https://www.epicurious.com/recipes/food/views/cowboy-breakfast-casserole-with-sausage-and-spinach</t>
+  </si>
+  <si>
+    <t>Tea Vodka</t>
+  </si>
+  <si>
+    <t>12 ounces vodka, 1 English Breakfast tea bag</t>
+  </si>
+  <si>
+    <t>https://www.foodandwine.com/recipes/tea-vodka-cocktails-2011</t>
+  </si>
+  <si>
+    <t>Breakfast Taco Bar</t>
+  </si>
+  <si>
+    <t>14 six-inch mission tortillas, 2 packages Johnsonville breakfast sausage links, cooked, 1 dozen eggs, scrambled, 1/2 Teaspoon salt, 1/2 Teaspoon pepper, 2 Cups Cheddar cheese, shredded, 2 medium tomatoes, chopped, Toppings: sour cream, salsa, and chopped avocado, optional</t>
+  </si>
+  <si>
+    <t>http://www.thedailymeal.com/recipes/breakfast-taco-bar-recipe</t>
+  </si>
+  <si>
+    <t>Radish With Butter And Sea Salt And Radish Greens Salad</t>
+  </si>
+  <si>
+    <t>16-20 French breakfast radishes, scrubbed, Coarse sea salt, Best-quality butter, slighty softened, 1/4 cup Dijon Vinaigrette</t>
+  </si>
+  <si>
+    <t>http://www.bonappetit.com/recipes/2011/06/radish-with-butter-and-sea-salt-and-radish-greens-salad</t>
+  </si>
+  <si>
+    <t>Radish with Butter and Sea Salt and Radish Greens Salad</t>
+  </si>
+  <si>
+    <t>16-20 French breakfast radishes, scrubbed, Coarse sea salt, Best-quality butter, slighty softened, 1 /4 cup Dijon Vinaigrette</t>
+  </si>
+  <si>
+    <t>https://www.bonappetit.com/recipe/radish-with-butter-and-sea-salt-and-radish-greens-salad</t>
+  </si>
+  <si>
+    <t>Country Breakfast Casserole</t>
+  </si>
+  <si>
+    <t>1 tablespoon oil, 4 potatoes, diced, 1 ½ teaspoons salt, divided, 1 red pepper, diced, 1 green pepper, diced, 1 onion, minced, 8-oz. pkg. breakfast link sausage, chopped, browned and drained, 1 ½ cups egg substitute, 1 cup milk, 2 tablespoons all-purpose flour, ½ teaspoon pepper, 1 cup shredded Cheddar cheese</t>
+  </si>
+  <si>
+    <t>https://www.myrecipes.com/recipe/country-breakfast-casserole</t>
+  </si>
+  <si>
+    <t>Recipe: Apple, Sausage, and Smoked Cheddar Breakfast Casserole</t>
+  </si>
+  <si>
+    <t>1 tablespoon olive oil, 1 pound uncooked breakfast sausage links, 3 cups sourdough bread, cut into 1/2-inch cubes, 2 medium firm apples, peeled, cored, and cut into 1/2-inch chunks, 8 ounces smoked cheddar cheese, cut into 1/4-inch cubes, 10 large eggs, 1 cup whole or 2% milk, 1/2 cup heavy cream, 2 tablespoons Dijon mustard, 1/2 teaspoon kosher salt, 1/4 teaspoon freshly ground black pepper, 3 scallions, green part only, sliced thin</t>
+  </si>
+  <si>
+    <t>https://www.thekitchn.com/recipe-apple-sausage-and-smoked-cheddar-breakfast-casserole-238197</t>
+  </si>
+  <si>
+    <t>Breakfast Pizza: Shashuka Pizza</t>
+  </si>
+  <si>
+    <t>1 package Green Giant Cauliflower Crust, 1 Tablespoon olive oil, 1/4 cup sweet onion chopped, 1/4 cup red bell pepper chopped, 1/2 teaspoon minced garlic, 1 Tablespoon cilantro chopped, 1/4 teaspoon paprika, 1/4 teaspoon cumin, 1/4 teaspoon chili powder, 1/4-1/2 jalapeno minced optional, 2 to matoes diced or 1/2 cup canned diced tomatoes, 2-3 Tablespoons tomato sauce, 1/4 teaspoon sugar, 4 oz breakfast sausage mild Italian sausage 4 slices bacon, cooked and crumbled or a meat alternative, 1 cup mozzarella cheese shredded or a combination of your favorite cheeses, 4 small eggs, Garnish: chopped parsley or cilantro</t>
+  </si>
+  <si>
+    <t>https://honestcooking.com/shashuka-pizza/</t>
+  </si>
+  <si>
+    <t>Biscuits And Gravy</t>
+  </si>
+  <si>
+    <t>1 lb Breakfast Sausage, 1 can 16 Oz Canned Biscuits, 2 tbsp Flour, 1 cup Milk, Salt, Pepper</t>
+  </si>
+  <si>
+    <t>http://thepioneerwoman.com/cooking/2007/09/biscuits_and_gr/</t>
+  </si>
+  <si>
+    <t>Breakfast Garbage Bread</t>
+  </si>
+  <si>
+    <t>2 1/2 cups frozen potato tots, One 12-ounce package pork breakfast sausage, 10 strips bacon (8 ounces), 5 large eggs, 2 cups grated American cheese (6 ounces), 2 cups grated white Cheddar (6 ounces), All-purpose flour, for dusting 1 1/2 pounds store-bought pizza dough (see Cook's Note), Ketchup and/or hot sauce, for serving</t>
+  </si>
+  <si>
+    <t>https://www.foodnetwork.com/recipes/food-network-kitchen/breakfast-garbage-bread-3513751</t>
+  </si>
+  <si>
+    <t>Breakfast Foil Packs With Hash Brown Potatoes, Sausage, and Scallions</t>
+  </si>
+  <si>
+    <t>3 scallions, trimmed, sliced, 1 (16-ounce) package frozen shredded hash brown potatoes, defrosted, 12 ounces cooked breakfast sausages (about 16 sausage links), cut into ¾" pieces, ¼ cup olive oil, 1 teaspoon kosher salt, plus more to taste, ½ teaspoon freshly ground black pepper, plus more to taste, 3 (packed) cups baby spinach, 6 large eggs, ½ cup shredded cheddar (optional)</t>
+  </si>
+  <si>
+    <t>https://www.epicurious.com/recipes/food/views/breakfast-hobo-packs-with-hash-brown-potatoes-sausage-and-scallions-56389750</t>
+  </si>
+  <si>
+    <t>Cinnamon Sugar Breakfast Puffs</t>
+  </si>
+  <si>
+    <t>Breakfast puffs, 1/3 cup unsalted butter, 1/2 cup sugar, 1 large egg, at room temperature, 1 1/2 cups all purpose flour, 1 1/2 teaspoons baking powder, 1/2 teaspoon salt, 1/4 teaspoon nutmeg, 1/4 teaspoon allspice, 1 pinch ground cloves, 1 pinch ground ginger, 1 teaspoon orange zest, 1/2 cup whole milk, at room temperature, Cinnamon-sugar coating, 6 tablespoons butter, melted, 1/2 cup granulated sugar, 1 teaspoon ground cinnamon</t>
+  </si>
+  <si>
+    <t>https://food52.com/recipes/15110-cinnamon-sugar-breakfast-puffs</t>
+  </si>
+  <si>
+    <t>Recipe: Loaded Savory Breakfast Muffins</t>
+  </si>
+  <si>
+    <t>1 tablespoon vegetable oil, 8 ounces uncooked breakfast sausage, casings removed, 3 cups baby spinach (about 3 ounces), Cooking spray, 2 cups all-purpose flour, 2 teaspoons baking powder, 1/2 teaspoon baking soda, 1/2 teaspoon salt, 1/4 teaspoon freshly ground black pepper, 6 tablespoons unsalted butter, 1 1/4 cups buttermilk, 2 large eggs, 1 cup shredded sharp cheddar cheese (about 4 ounces), 2/3 cup small-dice apple, 1 tablespoon finely chopped fresh chives</t>
+  </si>
+  <si>
+    <t>https://www.thekitchn.com/recipe-loaded-breakfast-muffins-253421</t>
+  </si>
+  <si>
+    <t>Sausage, Cheese And Potato Breakfast Casserole</t>
+  </si>
+  <si>
+    <t>1 lb bulk breakfast sausage, 2 tbsp all purpose flour, 1 1/2 cup milk (do not use low-fat or nonfat), 1/1 pound package frozen shredded hash brown potatoes, 4 x green onions, finely chopped, 1 1/4 cup grated sharp cheddar cheese</t>
+  </si>
+  <si>
+    <t>http://whippedtheblog.com/2009/07/20/sausage-cheese-and-potato-breakfast-casserole/</t>
+  </si>
+  <si>
+    <t>Breakfast Crescent Ring</t>
+  </si>
+  <si>
+    <t>16 frozen potato tots, 1/2 cup heavy cream, 12 large eggs, Kosher salt and freshly ground black pepper, 6 strips bacon, cut into 1/2-inch-wide pieces, 6 ounces pork breakfast sausage, removed from casings and chopped, Nonstick cooking spray, for greasing the pan, 2 ounces American cheese, grated, 1/2 cup grated white Cheddar (about 2 ounces), Maple syrup, ketchup, hot sauce or white gravy, for dipping, optional</t>
+  </si>
+  <si>
+    <t>https://www.foodnetwork.com/recipes/food-network-kitchen/breakfast-crescent-ring-5232578</t>
+  </si>
+  <si>
+    <t>Wagyu Breakfast Sausage Biscuits and Gravy</t>
+  </si>
+  <si>
+    <t>1 pound Double 8 Cattle Company Fullblood Wagyu Breakfast Sausage (broken into pieces), 1/2 cup Unsalted Butter, 1/2 cup All Purpose Flour, 1 Yellow Onion (small, diced), 6 cups Whole Milk, 1/2 teaspoon Crushed Red Pepper Flakes, Kosher Salt and Freshly Ground Black Pepper (to taste), 1 1/2 tablespoons Hot Sauce, 20 ounces All Purpose Flour, 2 tablespoons Sugar, 2 tablespoons Baking Powder, 2 teaspoons Kosher Salt, 6 ounces Cold Unsalted Butter (grated), 10 ounces Half and Half</t>
+  </si>
+  <si>
+    <t>https://food52.com/recipes/83986-wagyu-breakfast-sausage-biscuits-and-gravy</t>
+  </si>
+  <si>
+    <t>Holiday Breakfast Casserole</t>
+  </si>
+  <si>
+    <t>2 packages (12 ounces each) Johnsonville® Original Breakfast Sausage Links, 6 English muffins, cut into 1-in. cubes, 1/4 cup butter, melted, 1 cup (4 ounces) Cheddar cheese, shredded, 1 cup (4 ounces) mozzarella cheese, shredded, 1/2 cup onion, chopped, 1/2 cup red pepper, chopped, 12 large eggs, 2 cups milk, 1/4 teaspoon salt, 1/4 cup bacon bits</t>
+  </si>
+  <si>
+    <t>https://www.foodnetwork.com/recipes/holiday-breakfast-casserole-3415289</t>
+  </si>
+  <si>
+    <t>Chicken Piccata with Radishes</t>
+  </si>
+  <si>
+    <t>1 tablespoon extra-virgin olive oil, 8 breakfast radishes, Kosher salt</t>
+  </si>
+  <si>
+    <t>https://www.foodandwine.com/recipes/chicken-piccata-radishes</t>
+  </si>
+  <si>
+    <t>Dinner Tonight: Sausage and Biscuit Sandwich Recipe</t>
+  </si>
+  <si>
+    <t>1 cup flour, 1/2 tablespoon baking powder, 1/2 teaspoon sugar, 1/4 teaspoon salt, 4 tablespoons butter, cold, 6 tablespoons buttermilk, 1 pound breakfast sausage, 6 slices American cheese, Canola oil</t>
+  </si>
+  <si>
+    <t>http://www.seriouseats.com/recipes/2010/05/sausage-and-biscuit-sandwich-recipe.html</t>
+  </si>
+  <si>
+    <t>Overnight Breakfast Casserole</t>
+  </si>
+  <si>
+    <t>1 package (12 ounce each) Johnsonville® Original Breakfast Sausage Links, 6 English muffins, cut into 1-in. cubes, 1/4 cup butter, melted, 1 cup (4 ounce) cheddar cheese, shredded, 1 cup (4 ounce) mozzarella cheese, shredded, 1/2 cup onion, chopped, 1/2 cup red pepper, chopped, 12 eggs, 2 cups milk, 1/4 tsp. salt, 1/8 tsp. pepper, 1/4 cup bacon bits</t>
+  </si>
+  <si>
+    <t>https://www.foodnetwork.com/recipes/overnight-breakfast-casserole-3415701</t>
+  </si>
+  <si>
+    <t>Wagyu Beef Breakfast Sausage Kolaches</t>
+  </si>
+  <si>
+    <t>1 pound Double 8 Cattle Company Fullblood Wagyu Ground Breakfast Sausage, 3 tablespoons Grapeseed Oil, 1 Sweet Onion (minced), 2 Garlic Cloves (minced), 3/4 cup Butter, 3/4 cup Flour, 1 cup Whole Milk, 1/2 cup Heavy Cream, 1 sprig Thyme (leaves minced), 1/2 teaspoon Crushed Red Pepper, 2 teaspoons Kosher Salt, 5 1/2 cups All Purpose Flour, 1 1/2 cups Warm Milk (80°F), 3/4 cup Butter (softened), 2 Eggs, 1 1/2 tablespoons Instant Yeast, 1/3 cup Sugar, 1 tablespoon Kosher Salt, 1 Egg, 1 tablespoon Water</t>
+  </si>
+  <si>
+    <t>https://food52.com/recipes/86040-wagyu-beef-breakfast-sausage-kolaches</t>
+  </si>
+  <si>
+    <t>Breakfast Sausage Cornbread</t>
+  </si>
+  <si>
+    <t>Nonstick cooking spray, for spraying the baking dish, 1 1/2 cups yellow cornmeal, 1/4 cup all-purpose flour, 2 tablespoons sugar, 1 teaspoon baking powder, 1/2 teaspoon baking soda, 1/4 teaspoon fine salt, 1 cup milk, 1 cup sour cream or 2 percent Greek yogurt, 2 tablespoons unsalted butter, melted, 1 large egg, 1 cup cooked and crumbled breakfast sausage, 1 teaspoon chopped fresh sage</t>
+  </si>
+  <si>
+    <t>https://www.foodnetwork.com/recipes/food-network-kitchen/breakfast-sausage-cornbread-5496989</t>
+  </si>
+  <si>
+    <t>Breakfast-for-Dinner Egg Boats</t>
+  </si>
+  <si>
+    <t>1/3 pound breakfast (country) sausage, 6 large eggs, 1 cup milk, 1 teaspoon Dijon mustard, Coarse salt, Four 7-inch mini baguettes or bolillo rolls, 1/2 cup finely chopped kale, 1/2 cup shredded Cheddar, Parsley leaves, for garnish</t>
+  </si>
+  <si>
+    <t>https://www.foodnetwork.com/recipes/breakfast-for-dinner-egg-boats-5426546</t>
+  </si>
+  <si>
+    <t>Radish and Basil Compound Butter</t>
+  </si>
+  <si>
+    <t>3 small breakfast radishes, minced, 4 fresh basil leaves, minced, 1/4 teaspoon sea salt, or more to taste, 1/2 cup unsalted butter, softened</t>
+  </si>
+  <si>
+    <t>https://food52.com/recipes/28751-radish-and-basil-compound-butter</t>
+  </si>
+  <si>
+    <t>Awesome Breakfast Burritos</t>
+  </si>
+  <si>
+    <t>12 slices bacon, chopped, 1 onion, chopped, 1 pound loose breakfast sausage, 10 slices ham, chopped, 12 large eggs, whisked, 2 cups grated pepper jack cheese, 1/2 cup store-bought salsa verde, Two 4-ounce cans diced green chiles, Kosher salt and freshly ground black pepper, Twelve 8-inch flour tortillas</t>
+  </si>
+  <si>
+    <t>https://www.foodnetwork.com/recipes/ree-drummond/awesome-breakfast-burritos-5117356</t>
+  </si>
+  <si>
+    <t>Sausage and Cheese Breakfast Casserole</t>
+  </si>
+  <si>
+    <t>1 teaspoon canola oil, 12 ounces turkey breakfast sausage, 2 cups 1% low-fat milk, 2 cups egg substitute, 1 teaspoon dry mustard, ½ teaspoon freshly ground black pepper, ¼ teaspoon salt, ¼ teaspoon ground red pepper, 3 large eggs, 16 (1-ounce) slices white bread, 1 cup (4 ounces) finely shredded reduced-fat extrasharp cheddar cheese, Cooking spray</t>
+  </si>
+  <si>
+    <t>https://www.myrecipes.com/recipe/sausage-cheese-breakfast-casserole</t>
+  </si>
+  <si>
+    <t>Peach and Blackberry Iced Tea</t>
+  </si>
+  <si>
+    <t>2 black-tea bags, such as English breakfast, 8 cups boiling water, 4 peaches, 1/4 cup sugar, 1/2 cup peach nectar, Blackberries, for garnish</t>
+  </si>
+  <si>
+    <t>https://www.marthastewart.com/1142785/peach-iced-tea</t>
+  </si>
+  <si>
+    <t>Savory Breakfast Kabobs</t>
+  </si>
+  <si>
+    <t>2 tablespoons olive oil, 6 breakfast sausage links, cut into 1-inch pieces, 1 small onion, cut into chunks, 1 small red bell pepper, cut into chunks, 1 small green bell pepper, cut into chunks, 1 tablespoon Montreal steak seasoning, 1/3 cup half-and-half, 2 teaspoons kosher salt, 1 teaspoon freshly ground black pepper, 6 large eggs, 2 tablespoons butter, 1 cup shredded Cheddar cheese</t>
+  </si>
+  <si>
+    <t>https://www.foodnetwork.com/recipes/ree-drummond/savory-breakfast-kabobs-5478046</t>
+  </si>
+  <si>
+    <t>Sausage and Cilantro Omelete</t>
+  </si>
+  <si>
+    <t>1 Breakfast sausage, cut into rounds, 1/2 Onion, small dice, 2 tablespoons Fresh cilantro, chopped, 3 Large eggs, whisked, 1/4 cup Cheese, shredded</t>
+  </si>
+  <si>
+    <t>https://food52.com/recipes/37426-sausage-and-cilantro-omelete</t>
+  </si>
+  <si>
+    <t>Recipe: Slow Cooker Sausage and Spinach Breakfast Casserole</t>
+  </si>
+  <si>
+    <t>Cooking spray, 1 pound uncooked pork breakfast sausage, casings removed, 1 small yellow onion, diced, 1 1/2 teaspoons dried oregano, 5 ounces baby spinach (about 5 packed cups), 1 pound frozen diced potatoes (do not thaw, about 4 cups), 1 1/4 cups shredded Swiss cheese, divided, 1/4 cup grated Parmesan cheese, plus more for serving, 8 large eggs, 2 cups whole or 2% milk, 2 teaspoons Dijon mustard, 1 1/2 teaspoons kosher salt, 1/4 teaspoon freshly ground black pepper, Red pepper flakes or hot sauce, for serving</t>
+  </si>
+  <si>
+    <t>https://www.thekitchn.com/slow-cooker-sausage-breakfast-casserole-256182</t>
+  </si>
+  <si>
+    <t>Cucumber, Feta and Watermelon Salad</t>
+  </si>
+  <si>
+    <t>1/2 watermelon, 1/2 pound north american feta, 2 cucumbers, 1 bunch radishes, french breakfast are the best, 1 bunch fresh mint, 1/4 cup Balsamic vinegar</t>
+  </si>
+  <si>
+    <t>https://food52.com/recipes/4922-cucumber-feta-and-watermelon-salad</t>
+  </si>
+  <si>
+    <t>Breakfast Nachos</t>
+  </si>
+  <si>
+    <t>8 homemade or thawed frozen waffles, cut into triangles (like tortilla chips), 1 pound breakfast sausage, casings removed and meat crumbled, 1 tablespoon olive oil, 6 large eggs, Kosher salt and freshly ground black pepper, 1 tablespoon maple syrup, 2 cups shredded sharp Cheddar, 1 avocado, thinly sliced, 1/2 cup quartered cherry tomatoes, 3 scallions, white and light green parts only, thinly sliced, 1 jalapeno, thinly sliced, 1/4 cup chopped fresh cilantro, Hot sauce, for serving, optional, Sour cream, for garnish</t>
+  </si>
+  <si>
+    <t>https://www.foodnetwork.com/recipes/katie-lee/breakfast-nachos-3513869</t>
+  </si>
+  <si>
+    <t>Meat Lover’s Breakfast Sandwich</t>
+  </si>
+  <si>
+    <t>2 teaspoons canola oil, 5 ounces bulk breakfast sausage, 2 large eggs, 1 1/2 tablespoons cream cheese, at room temperature, 1 tablespoon finely chopped fresh chives, 1 tablespoon finely chopped fresh cilantro, 1 tablespoon finely chopped fresh parsley, Kosher salt and freshly ground black pepper, 1 deli slice sharp Cheddar, 1/4 avocado, cut into 1/4-inch slices</t>
+  </si>
+  <si>
+    <t>https://www.foodnetwork.com/recipes/food-network-kitchen/meat-lovers-breakfast-sandwich-5463144</t>
+  </si>
+  <si>
+    <t>Cheesy Sausage and Potato Breakfast Casserole</t>
+  </si>
+  <si>
+    <t>2 packages (12 ounces each) Johnsonville® Cheesy Breakfast Sausage Links, 1 package (20 ounces) frozen roasted potatoes, 1/2 cup chopped onion, 1/2 cup chopped green pepper, 2 cups (8 ounces) shredded cheddar cheese, divided, 9 eggs, 3 cups milk, 1 tablespoon Dijon mustard, 1/4 teaspoon salt, 1/4 teaspoon pepper</t>
+  </si>
+  <si>
+    <t>https://www.foodnetwork.com/recipes/cheesy-sausage-and-potato-breakfast-casserole-3414393</t>
+  </si>
+  <si>
+    <t>Cheesy Sausage Breakfast Grits</t>
+  </si>
+  <si>
+    <t>1 pound ground breakfast sausage, 3 cups lowfat (2 percent) milk, 1 cup quick-cooking grits, 3 cups grated Cheddar, 4 large eggs, 1 tablespoon hot sauce, 4 scallions, white and light green parts, thinly sliced, dark green tops reserved for garnish, 4 scallions, white and light green parts, thinly sliced, dark green tops reserved for garnish, 1 jalapeno, minced, Kosher salt and freshly cracked black pepper</t>
+  </si>
+  <si>
+    <t>https://www.foodnetwork.com/recipes/cheesy-sausage-breakfast-grits-3209099</t>
+  </si>
+  <si>
+    <t>Slow-Cooker Overnight Breakfast Casserole</t>
+  </si>
+  <si>
+    <t>24 Ounces Johnsonville Hot and Spicy Breakfast sausage, 1 Cup greens onions, chopped, 1 sweet red bell pepper, chopped, 4 Ounces mild green chiles, diced, 1/4 Cup fresh cilantro, chopped, 30 Ounces frozen shredded hash brown potatoes, 1 1/2 Cup Cheddar cheese, shredded, 12 eggs, 1 Cup milk, 1/2 Teaspoon salt, 1/8 Teaspoon black pepper</t>
+  </si>
+  <si>
+    <t>http://www.thedailymeal.com/recipes/slow-cooker-overnight-breakfast-casserole-recipe</t>
+  </si>
+  <si>
+    <t>Breakfast Bread Pudding</t>
+  </si>
+  <si>
+    <t>Butter, for greasing, 1 tablespoon olive oil, 1 medium yellow onion, minced, 1 pound breakfast sausage, crumbled, 10 large eggs, 3 cups milk, 1 teaspoon salt, 1/2 teaspoon freshly ground black pepper, 1/2 teaspoon garlic powder, 1 loaf day-old brioche or country white bread, cut into 1 1/2-inch cubes (about 12 cups), 2 cups shredded Cheddar (about 6 ounces)</t>
+  </si>
+  <si>
+    <t>https://www.foodnetwork.com/recipes/katie-lee/breakfast-bread-pudding-2396291</t>
+  </si>
+  <si>
+    <t>Peppery kohlrabi slaw</t>
+  </si>
+  <si>
+    <t>2 whole kohlrabi, peeled, head of spring greens, finely shredded, 2 bunches spring onions, very finely shredded, small bunch French breakfast radishes, quartered, leaves attached, juice 0.5 lemon</t>
+  </si>
+  <si>
+    <t>https://www.bbcgoodfood.com/recipes/peppery-kohlrabi-slaw</t>
+  </si>
+  <si>
+    <t>Sheet Pan Sausage and Egg Breakfast Bake</t>
+  </si>
+  <si>
+    <t>4 uncooked breakfast sausages (6 oz total), 4 slices bacon, 8 oz. small cremini mushrooms, halved or quartered if large, 16 Campari or cocktail tomatoes, halved, 2 cloves garlic, finely chopped, 1 tbsp. olive oil, Kosher salt and pepper, 4 large eggs, 1/2 c. flat-leaf parsley, chopped, Toast, for serving</t>
+  </si>
+  <si>
+    <t>https://www.goodhousekeeping.com/food-recipes/a34464150/sheet-pan-breakfast-bake-recipe/</t>
+  </si>
+  <si>
+    <t>Hangover Breakfast Sausage-and-Egg Burger</t>
+  </si>
+  <si>
+    <t>1 tablespoon mayonnaise, 1/2 teaspoon Sriracha, 1/2 teaspoon pure maple syrup, 1 sesame-seed hamburger bun, 1 lettuce leaf, 1 tomato slice, 3 to 4 thin rings red onion, 4 ounces bulk breakfast sausage, 1 teaspoon vegetable oil, 1 slice Cheddar, 1 large egg, Kosher salt and freshly ground black pepper</t>
+  </si>
+  <si>
+    <t>https://www.foodnetwork.com/recipes/food-network-kitchen/hangover-breakfast-sausage-and-egg-burger-3363856</t>
+  </si>
+  <si>
+    <t>Breakfast Sausage and Rice Brunch Ring</t>
+  </si>
+  <si>
+    <t>2 rolls breakfast sausage, mild, 1/2 pound lean ground beef, 1 cup chopped onions, 1/2 cup chopped green bell pepper, 1 cup sliced fresh mushrooms, 1 teaspoon garlic salt, 2 tablespoons dark brown sugar, 2 cups cooked rice, medium grain (cooked in chicken broth), 2 cans refrigerated crescent rolls, 2 cups shredded cheese, Mexican style with jalapenos, 1 package Canadian bacon</t>
+  </si>
+  <si>
+    <t>https://www.foodnetwork.com/recipes/breakfast-sausage-and-rice-brunch-ring-recipe-1940202</t>
+  </si>
+  <si>
+    <t>Breakfast Sausage With Red-Pepper Gravy</t>
+  </si>
+  <si>
+    <t>1 tablespoon extra-virgin olive oil, 1 pound breakfast sausage, 3 scallions, sliced, white and green parts separated, 1 red bell pepper, diced, Kosher salt and freshly ground pepper, 1 tablespoon flour, 1 clove garlic, minced, 1/2 teaspoon Worcestershire sauce, 1/8 teaspoon ground allspice, 3/4 cup low-sodium chicken broth, 1 1/4 cups milk</t>
+  </si>
+  <si>
+    <t>https://www.foodnetwork.com/recipes/food-network-kitchen/breakfast-sausage-with-red-pepper-gravy-recipe-1973877</t>
+  </si>
+  <si>
+    <t>Bagel Breakfast Casserole</t>
+  </si>
+  <si>
+    <t>Unsalted butter or nonstick cooking spray, for greasing the baking dish, 1 tablespoon olive oil, 8 ounces breakfast sausage, casing removed (8 sausages) (see Cook's Note), 2 cups whole milk, 3/4 cup half-and-half, Pinch of cayenne, 8 large eggs, Kosher salt and freshly ground black pepper, 1 1/3 cups packed baby spinach, 2 large plain bagels, split and cut into 1-inch pieces, 1 1/3 cups shredded provolone, 8 ounces cream cheese, cut into 1/2-inch cubes, 2 tablespoons everything bagel seasoning</t>
+  </si>
+  <si>
+    <t>https://www.foodnetwork.com/recipes/food-network-kitchen/bagel-breakfast-casserole-3814175</t>
+  </si>
+  <si>
+    <t>Fast and Easy Breakfast Cups</t>
+  </si>
+  <si>
+    <t>1 package (9.6 ounces) Johnsonville® Fully Cooked Original Recipe or Turkey Breakfast Sausage Links, cut into ¼-inch pieces, 1 1/2 cup frozen shredded hash brown potatoes, 1/4 cup finely chopped onion, 1 cup shredded Cheddar cheese, divided, 2 eggs, 1 cup milk, 1/2 cup biscuit/baking mix, 1/4 teaspoon pepper, 1/8 teaspoon salt</t>
+  </si>
+  <si>
+    <t>https://www.foodnetwork.com/recipes/fast-and-easy-breakfast-cups-3416649</t>
+  </si>
+  <si>
+    <t>Chai tea</t>
+  </si>
+  <si>
+    <t>2 mugs milk (or use almond milk), 2 English Breakfast tea bags, 6 cracked cardamom pods, ½ cinnamon stick, a grating of fresh nutmeg, 2 cloves, 2-4 tsp light brown soft sugar</t>
+  </si>
+  <si>
+    <t>https://www.bbcgoodfood.com/recipes/cassies-chai-tea</t>
+  </si>
+  <si>
+    <t>Double D Sliders</t>
+  </si>
+  <si>
+    <t>1 glazed doughnut, halved, One 2-ounce breakfast sausage patty, such as Delia's chicken breakfast sausage, 1 tablespoon sour cherry cream cheese</t>
+  </si>
+  <si>
+    <t>https://www.foodnetwork.com/recipes/double-d-sliders-3078779</t>
+  </si>
+  <si>
+    <t>Sausage Gravy and Cheddar Biscuit Pot Pie</t>
+  </si>
+  <si>
+    <t>12 oz. pork breakfast sausage, ½ cups flour, 3½ cups milk, 1 cup heavy cream, 1 tbsp. apple cider vinegar, ¼ tsp. cayenne, Kosher salt and freshly ground black pepper, to taste</t>
+  </si>
+  <si>
+    <t>https://www.saveur.com/article/Recipes/Sausage-Gravy-and-Cheddar-Biscuit-Pot-Pie/</t>
+  </si>
+  <si>
+    <t>Sweet Iced Black Tea With Cream</t>
+  </si>
+  <si>
+    <t>4 cups boiling water, 8 teaspoons loose English breakfast tea (or 8 tea bags), 1/2 cup sugar, Crushed ice, for serving, 1/2 cup heavy cream</t>
+  </si>
+  <si>
+    <t>https://www.marthastewart.com/1142446/sweet-iced-black-tea-cream</t>
+  </si>
+  <si>
+    <t>Breakfast quinoa</t>
+  </si>
+  <si>
+    <t>1 cup quinoa, 1.5 cups milk, 2 tablespoons maple syrup (more to taste if you like it sweeter), 4 ounces blueberries, can use fresh or frozen, 1/2 cup walnuts, 1/2 teaspoon cinnamon (optional)</t>
+  </si>
+  <si>
+    <t>https://food52.com/recipes/23503-breakfast-quinoa</t>
+  </si>
+  <si>
+    <t>Poached duck egg with hot smoked salmon &amp; mustard hollandaise</t>
+  </si>
+  <si>
+    <t>2 x 150g pieces hot smoked salmon, 4 duck eggs, splash of white wine vinegar, 60g watercress, a little rapeseed oil, 2 breakfast muffins, cut in half and toasted</t>
+  </si>
+  <si>
+    <t>https://www.bbcgoodfood.com/recipes/poached-duck-egg-hot-smoked-salmon-mustard-hollandaise</t>
+  </si>
+  <si>
+    <t>1-Minute Sausage and Cheese Omelette recipes</t>
+  </si>
+  <si>
+    <t>1 egg, beaten, 1 Tablespoon milk, 2 Tablespoons fully-cooked breakfast sausage crumbles or one fully-cooked breakfast sausage link or patty, chopped, 2 Tablespoons shredded Cheddar cheese, 1 flatbread (six-inch), toasted</t>
+  </si>
+  <si>
+    <t>http://www.thedailymeal.com/recipes/1-minute-sausage-and-cheese-omelette-recipe</t>
+  </si>
+  <si>
+    <t>The Breakfast Martini Recipe</t>
+  </si>
+  <si>
+    <t>1 3/4 ounces gin, 1/2 ounce fresh lemon juice from one lemon, 1/2 ounce Cointreau, 1 teaspoon orange marmalade, Quarter-sized piece of orange zest, or strip cut with a channel knife</t>
+  </si>
+  <si>
+    <t>https://www.seriouseats.com/the-breakfast-martini-marmalade-cocktail-recipe</t>
+  </si>
+  <si>
+    <t>Radishes with Spicy Mayo and Sesame Salt</t>
+  </si>
+  <si>
+    <t>½ cup black sesame seeds, preferably Japanese, 2 tablespoons sugar, ¾ teaspoon kosher salt, 1 cup homemade or purchased mayonnaise, 2 teaspoons gochujang (Korean hot pepper paste), 2 bunches breakfast radishes</t>
+  </si>
+  <si>
+    <t>https://www.bonappetit.com/recipe/radishes-with-spicy-mayo-and-sesame-salt</t>
+  </si>
+  <si>
+    <t>Spicy Breakfast Burritos with Cheese</t>
+  </si>
+  <si>
+    <t>18 flour tortillas, 1 pound breakfast sausage, 1/3 stick (about 2 1/2 tablespoons) salted butter, 18 large eggs, 1/2 teaspoon kosher salt, 1/2 teaspoon freshly ground black pepper, 1 tablespoon hot sauce, plus more for serving, 1/4 of a 16-ounce jar jalapenos plus liquid from the jar, plus more jalapenos for serving, 3 cups grated cheese, Salsa, for serving</t>
+  </si>
+  <si>
+    <t>https://www.foodnetwork.com/recipes/ree-drummond/spicy-breakfast-burritos-with-cheese-8741045</t>
+  </si>
+  <si>
+    <t>Breakfast smoothie</t>
+  </si>
+  <si>
+    <t>1 small ripe banana, about 140g blackberries, blueberries, raspberries or strawberries (or use a mix), plus extra to serve, apple juice or mineral water, optional, runny honey, to serve</t>
+  </si>
+  <si>
+    <t>https://www.bbcgoodfood.com/recipes/breakfast-smoothie</t>
+  </si>
+  <si>
+    <t>Sticky bourbon BBQ wings with blue cheese dip</t>
+  </si>
+  <si>
+    <t>1kg whole chicken wings, 2 tbsp olive oil, 4 celery sticks, each cut into 4 small sticks (keep some with their leaves), bunch French breakfast radishes (with their leaves if you can get them)</t>
+  </si>
+  <si>
+    <t>https://www.bbcgoodfood.com/recipes/sticky-bourbon-bbq-wings-blue-cheese-dip</t>
+  </si>
+  <si>
+    <t>Black Tea Jelly</t>
+  </si>
+  <si>
+    <t>2 cups of your favorite black tea (I use Taylor's of Harrogate Scottish Breakfast), strongly brewed and cooled to room temperature, 2 packets (1/2 an ounce) powdered gelatin, 1/4 cup sugar</t>
+  </si>
+  <si>
+    <t>https://food52.com/recipes/4167-black-tea-jelly</t>
+  </si>
+  <si>
+    <t>Breakfast Burrito Casserole</t>
+  </si>
+  <si>
+    <t>Nonstick cooking spray, oil or butter, for the baking dish, One 20-ounce bag refrigerated diced potatoes with onions, 2 tablespoons olive oil, 1 pound bulk breakfast sausage, 1 cup milk, 1/2 cup sour cream, 1/2 teaspoon seasoned salt, such as Lawry’s, 1/4 teaspoon freshly ground black pepper, 4 large eggs, 4 scallions, sliced, 1 red bell pepper, diced, 2 cups grated pepper jack, 1 cup grated sharp Cheddar, 1/2 cup jarred pickled jalapeno slices, Tortillas and salsa, for serving</t>
+  </si>
+  <si>
+    <t>https://www.foodnetwork.com/recipes/ree-drummond/breakfast-burrito-casserole-13402856</t>
+  </si>
+  <si>
+    <t>Apple, Sausage, and Cheddar Monkey Bread</t>
+  </si>
+  <si>
+    <t>8 ounces crumbled breakfast sausage, 2 red apples, diced, 16 ounce can of biscuit dough, cut into 1-inch pieces, 1½ cups grated cheddar</t>
+  </si>
+  <si>
+    <t>https://www.realsimple.com/food-recipes/browse-all-recipes/apple-sausage-cheddar-monkey-bread</t>
+  </si>
+  <si>
+    <t>Sausage Gravy</t>
+  </si>
+  <si>
+    <t>1/2 pound breakfast sausage, 1/2 cup (1 stick) unsalted butter, 1/2 cup all-purpose flour, 6 cups whole milk, 1/2 teaspoon crushed red pepper flakes, Kosher salt, Freshly ground pepper</t>
+  </si>
+  <si>
+    <t>https://www.epicurious.com/recipes/food/views/sausage-gravy-367139</t>
+  </si>
+  <si>
     <t>After-dinner mint cream</t>
   </si>
   <si>
@@ -198,834 +1026,6 @@
   </si>
   <si>
     <t>http://www.seriouseats.com/recipes/2007/12/dinner-tonight-custardy-popovers-recipe.html</t>
-  </si>
-  <si>
-    <t>Breakfast Sausage, Mushroom, and Cheddar Rolls Recipe</t>
-  </si>
-  <si>
-    <t>1/2 pound breakfast sausage (about 10 links), 10 ounces button mushrooms, finely chopped, 4 sprigs thyme, 1/2 cup grated sharp Cheddar cheese, 1 pound puff pastry, thawed if frozen, 1 egg, beaten, Kosher salt and freshly ground black pepper, Hot English or Dijon mustard for serving</t>
-  </si>
-  <si>
-    <t>http://www.seriouseats.com/recipes/2014/01/breakfast-sausage-mushroom-cheddar-roll-recipe.html</t>
-  </si>
-  <si>
-    <t>Mini Breakfast Cookie &amp; Yogurt</t>
-  </si>
-  <si>
-    <t>1 oatmeal raisin mini breakfast cookie, 5 ⅓ ounces nonfat organic vanilla Greek yogurt, 1 cup raspberries</t>
-  </si>
-  <si>
-    <t>http://www.eatingwell.com/recipe/266418/mini-breakfast-cookie-yogurt/</t>
-  </si>
-  <si>
-    <t>Sausage and Potato Breakfast Casserole</t>
-  </si>
-  <si>
-    <t>1 pound bulk breakfast sausage, 2 tablespoons all purpose flour, 1 1/2 cups milk (do not use low-fat or nonfat), 1 1-pound package frozen shredded hash brown potatoes, 4 green onions, finely chopped, 1 1/4 cups grated sharp cheddar cheese</t>
-  </si>
-  <si>
-    <t>https://www.epicurious.com/recipes/food/views/sausage-and-potato-breakfast-casserole-4387</t>
-  </si>
-  <si>
-    <t>BA's Best Breakfast Sandwich</t>
-  </si>
-  <si>
-    <t>Unsalted butter, 1 English muffin, split, 1 BA Breakfast Sausage patty, 2 slices American cheese, 2 large eggs, beaten to blend, Kosher salt and freshly ground black pepper, Handful of chopped fresh chives, Hot sauce and honey (for serving; optional)</t>
-  </si>
-  <si>
-    <t>https://www.bonappetit.com/recipe/bas-best-breakfast-sandwich</t>
-  </si>
-  <si>
-    <t>Sausage and Cheddar Breakfast Casserole</t>
-  </si>
-  <si>
-    <t>1 tbsp. unsalted butter, for greasing, 6 slices white bread, 1 lb. bulk breakfast sausage, casing removed, 10 oz. grated cheddar cheese, 2 cups milk, 1⁄2 tsp. dry mustard, 6 eggs, lightly beaten, Kosher salt and freshly ground black pepper, to taste</t>
-  </si>
-  <si>
-    <t>https://www.saveur.com/article/recipes/sausage-and-cheddar-breakfast-casserole/</t>
-  </si>
-  <si>
-    <t>Paleo Sweet Potato Breakfast Hash</t>
-  </si>
-  <si>
-    <t>3 Large Sweet Potatoes (washed, peeled, and cubed), 1 tablespoon Olive Oil, 1 teaspoon Garlic Powder, 1 teaspoon Onion Powder, 1/2 teaspoon Paprika, 1 pinch Salt and Pepper, 4 Breakfast Sausage Links, 1/4 cup Red Onion (chopped), 1/2 cup Cherry Tomatoes, 1/2 tablespoon Organic Sriracha</t>
-  </si>
-  <si>
-    <t>https://food52.com/recipes/78306-paleo-sweet-potato-breakfast-hash</t>
-  </si>
-  <si>
-    <t>Breakfast Pigs in a Blanket</t>
-  </si>
-  <si>
-    <t>16 cooked or uncooked breakfast sausage links (do not thaw if frozen), 1 (8-ounce) can refrigerated crescent rolls</t>
-  </si>
-  <si>
-    <t>https://www.thekitchn.com/breakfast-pigs-in-a-blanket-recipe-23524373</t>
-  </si>
-  <si>
-    <t>Breakfast Fried Rice</t>
-  </si>
-  <si>
-    <t>1/2 yellow onion, finely chopped, 2 cloves garlic, minced, 1 tablespoon olive oil, 4 small breakfast sausages, 2 cup cooked rice, 2 tablespoons soy sauce, 1 teaspoon rice vinegar, 1 teaspoon toasted sesame oil, 1 teaspoon sriracha, 3 eggs, 3 tablespoons scallions, Salt and pepper</t>
-  </si>
-  <si>
-    <t>https://www.realsimple.com/food-recipes/browse-all-recipes/breakfast-fried-rice</t>
-  </si>
-  <si>
-    <t>Strawberry Jam Breakfast Biscuit</t>
-  </si>
-  <si>
-    <t>1 Breakfast Biscuit, 1 rounded tablespoon of strawberry jam</t>
-  </si>
-  <si>
-    <t>https://www.foodandwine.com/recipes/strawberry-jam-breakfast-biscuit</t>
-  </si>
-  <si>
-    <t>Dinner Tonight: Breakfast Sausage, Home Fries, and Eggs Recipe</t>
-  </si>
-  <si>
-    <t>1 pound breakfast sausage, 1 pound baking potatoes, peeled and cut into 1-inch cubes, 1/2 cup chopped onion, 1/3 cup chopped green bell pepper, 1 teaspoon garlic, minced, 3/4 teaspoon Creole seasoning, plus more for sprinkling, Canola oil, Salt and pepper, 4 eggs</t>
-  </si>
-  <si>
-    <t>http://www.seriouseats.com/recipes/2010/06/breakfast-sausage-home-fries-eggs-recipe.html</t>
-  </si>
-  <si>
-    <t>Sausage Breakfast Casserole</t>
-  </si>
-  <si>
-    <t>1 tablespoon olive oil, 14 to 16 ounces uncooked pork breakfast sausage, Cooking spray or olive oil, 12 large eggs, 2 cups half-and-half, 2 teaspoons dry mustard, 1 1/2 teaspoons kosher salt, 1/2 teaspoon freshly ground black pepper, 8 ounces sharp cheddar cheese, shredded (2 cups), preferably white, 6 slices hearty white sandwich bread (8 to 9 ounces)</t>
-  </si>
-  <si>
-    <t>https://www.thekitchn.com/sausage-breakfast-casserole-recipe-23218282</t>
-  </si>
-  <si>
-    <t>Recipe: Breakfast Fried Rice</t>
-  </si>
-  <si>
-    <t>2 tablespoons vegetable oil, divided, 3 large eggs, lightly beaten, 1 ounces uncooked breakfast sausage, casings removed, 1/2 medium onion, finely diced, 5 cups cooked rice, preferably cold, 2 tablespoons tamari or soy sauce, 1/2 teaspoon kosher salt, Freshly ground black pepper, 1/2 cup shredded sharp cheddar cheese, 1/2 cup frozen peas, 1 tablespoon coarsely chopped fresh parsley leaves</t>
-  </si>
-  <si>
-    <t>https://www.thekitchn.com/recipe-breakfast-fried-rice-253305</t>
-  </si>
-  <si>
-    <t>Recipe: Breakfast Stromboli</t>
-  </si>
-  <si>
-    <t>1 teaspoon olive oil, 8 ounces uncooked breakfast sausage, casings removed, 1/4 medium yellow onion, finely chopped, 4 large eggs, 1 tablespoon whole or 2% milk, 1/4 teaspoon kosher salt, Freshly ground black pepper, 1 pound pizza dough, at room temperature for at least 1 hour, 1 cup shredded sharp cheddar cheese, divided, 1 tablespoon coarsely chopped fresh parsley leaves</t>
-  </si>
-  <si>
-    <t>https://www.thekitchn.com/breakfast-hot-pocket-257232</t>
-  </si>
-  <si>
-    <t>Recipe: Sheet-Pan “Half English” Breakfast</t>
-  </si>
-  <si>
-    <t>Cooking spray or olive oil, 2 medium plum tomatoes, 2 tablespoons olive oil, divided, 1/4 teaspoon dried thyme, divided, Kosher salt, Freshly ground black pepper, 12 medium cremini mushrooms, 8 small uncooked breakfast link sausages (about 8 ounces), 4 large eggs, Toast, for serving (optional)</t>
-  </si>
-  <si>
-    <t>https://www.thekitchn.com/recipe-sheet-pan-half-english-breakfast-228390</t>
-  </si>
-  <si>
-    <t>Recipe: Easy Paleo Breakfast Egg Muffins</t>
-  </si>
-  <si>
-    <t>Cooking spray or olive oil, 8 ounces sugar-free uncooked pork breakfast sausage, casings removed, 1 cup thinly sliced cremini mushrooms (about 3 ounces), 1/2 cup diced yellow onion, 1 cup baby spinach (about 1 ounce), coarsely chopped, 8 large eggs, 3 tablespoons ghee, melted and cooled, 1 teaspoon kosher salt, 1/4 teaspoon freshly ground black pepper</t>
-  </si>
-  <si>
-    <t>https://www.thekitchn.com/recipe-easy-paleo-breakfast-egg-muffins-258351</t>
-  </si>
-  <si>
-    <t>Breakfast Meatballs</t>
-  </si>
-  <si>
-    <t>Cooking spray, 4 slices thick-cut bacon (about 5 ounces), 1 medium Pink Lady or Granny Smith apple, 1/2 medium yellow onion, 1 large egg, 1/2 cup shredded sharp cheddar cheese (2 ounces), 1/2 medium bunch fresh chives, 1 1/2 teaspoons kosher salt, 1/2 teaspoon freshly ground black pepper, 1/2 cup fine, dry breadcrumbs, 1/2 cup whole or 2% milk, 1 pound uncooked breakfast sausage, 2 tablespoons maple syrup, plus more for drizzling, Serving suggestions: creamy polenta , cheesy grits , or buttered noodles</t>
-  </si>
-  <si>
-    <t>https://www.thekitchn.com/breakfast-meatballs-23326125</t>
-  </si>
-  <si>
-    <t>The Ultimate Make-Ahead Breakfast Casserole</t>
-  </si>
-  <si>
-    <t>8 ounces crusty French bread or baguette, 4 teaspoons olive oil, divided, 2 medium scallions, 4 ounces cheddar cheese, 8 ounces uncooked breakfast sausage, 6 large eggs, 1 cup whole milk or 2% milk, 1 teaspoon smoked paprika, plus more for sprinkling, 1/2 teaspoon kosher salt, 1/4 teaspoon freshly ground black pepper</t>
-  </si>
-  <si>
-    <t>https://www.thekitchn.com/breakfast-casserole-recipe-23421081</t>
-  </si>
-  <si>
-    <t>Breakfast Burritos Plain</t>
-  </si>
-  <si>
-    <t>18 flour tortillas, 1 pound breakfast sausage, 4 tablespoons salted butter, 18 large eggs, 1/2 teaspoon kosher salt, 1/2 teaspoon freshly ground black pepper</t>
-  </si>
-  <si>
-    <t>https://www.foodnetwork.com/recipes/ree-drummond/breakfast-burritos-plain-8741035</t>
-  </si>
-  <si>
-    <t>Double Pork Sausage</t>
-  </si>
-  <si>
-    <t>4 slices bacon, cut in half crosswise, 8 pork breakfast sausages</t>
-  </si>
-  <si>
-    <t>https://www.marthastewart.com/964328/double-pork-sausage</t>
-  </si>
-  <si>
-    <t>Bison Breakfast Patties</t>
-  </si>
-  <si>
-    <t>1 Tablespoon dried sage, 1 Tablespoon onion powder, 1/2 Teaspoon fennel seeds, crushed, 2 Teaspoons brown sugar, 1 Pound bison breakfast sausage, 1 egg white, Salt and pepper, to taste, Vegetable oil, as needed</t>
-  </si>
-  <si>
-    <t>http://www.thedailymeal.com/bison-breakfast-patties-recipe</t>
-  </si>
-  <si>
-    <t>Breakfast Taquitos</t>
-  </si>
-  <si>
-    <t>12 small breakfast sausage links, 2 tbsp. butter, 6 eggs, 1/4 c. milk, 1/4 c. Chopped chives, 1/2 c. shredded Cheddar, 12 small corn tortillas, warmed, Hot sauce, for serving (optional)</t>
-  </si>
-  <si>
-    <t>http://www.delish.com/cooking/recipe-ideas/recipes/a48242/breakfast-taquitos-recipe/</t>
-  </si>
-  <si>
-    <t>Cider-Glazed Sausage</t>
-  </si>
-  <si>
-    <t>12 ounces (1 package) frozen breakfast sausage links, 1 cup apple cider</t>
-  </si>
-  <si>
-    <t>https://www.marthastewart.com/313789/cider-glazed-sausage</t>
-  </si>
-  <si>
-    <t>Breakfast Casserole with Mushroom "Gravy" (Made with Cream of Mushroom Soup)</t>
-  </si>
-  <si>
-    <t>1 pound breakfast sausage, 4 cups shredded cheddar cheese, 8 slices of bread, 6 eggs, 2 cups milk + 1/2 cup milk, reserved, 1 can of Cream of Mushroom soup, 1/2 tablespoon dried Italian Herbs, 3/4 teaspoon dry mustard powder, 1/2 teaspoon salt, Freshly cracked black pepper</t>
-  </si>
-  <si>
-    <t>https://food52.com/recipes/40963-breakfast-casserole-with-mushroom-gravy</t>
-  </si>
-  <si>
-    <t>Recipe: Egg, Sausage, and Cheese Bundt Breakfast Sandwich</t>
-  </si>
-  <si>
-    <t>Cooking spray, 1 pound frozen bread dough, thawed according to package directions, 8 ounces uncooked breakfast sausage, casings removed, 8 large eggs, 1/2 teaspoon kosher salt, Large pinch freshly ground black pepper, 1 (12-ounce) jar roasted red peppers, drained, 4 to 5 slices sharp cheddar cheese (about 4 ounces)</t>
-  </si>
-  <si>
-    <t>https://www.thekitchn.com/recipe-egg-sausage-and-cheese-bundt-breakfast-sandwich-235022</t>
-  </si>
-  <si>
-    <t>Potato, Sausage, and Spinach Breakfast Casserole</t>
-  </si>
-  <si>
-    <t>16 large eggs, 1 1/4 cups heavy cream, 1 1/2 teaspoons kosher salt plus more, 3/4 teaspoon freshly ground black pepper plus more, 5 tablespoons unsalted butter, divided, 12 ounces fresh breakfast sausage links, 2 cups sliced leeks, white and pale-green parts only, 2 russet potatoes (1 1/2 pounds), peeled, shredded, lightly squeezed, 1 pound frozen spinach, thawed, squeezed dry, roughly chopped, 1 1/2 cups (4 ounces) grated Gruyère, 1/2 cup (1 1/2 ounces) grated Parmesan</t>
-  </si>
-  <si>
-    <t>https://www.epicurious.com/recipes/food/views/potato-sausage-and-spinach-breakfast-casserole-368302</t>
-  </si>
-  <si>
-    <t>McDonald’s Breakfast Burrito</t>
-  </si>
-  <si>
-    <t>5 Ounces breakfast sausage, crumbled, 2 Tablespoons white onion, minced, 4 eggs, beaten, Salt, to taste, Black pepper, to taste, 4 flour tortillas, 4 slices of American cheese</t>
-  </si>
-  <si>
-    <t>http://www.thedailymeal.com/recipes/mcdonald-s-breakfast-burrito-recipe</t>
-  </si>
-  <si>
-    <t>Recipe: Sausage and Greens Breakfast Casserole</t>
-  </si>
-  <si>
-    <t>1 pound frozen diced potatoes (about 4 cups, do not thaw), 1 tablespoon olive oil, plus more for the baking dish, 1 pound uncooked breakfast sausage, casings removed, 1 medium yellow onion, diced, 1 1/2 teaspoons dried oregano, 5 ounces baby spinach (about 5 packed cups), 8 large eggs, 1 1/2 cups whole or 2% milk, 1 1/2 teaspoons kosher salt, 1/4 teaspoon freshly ground black pepper, 2 cups shredded Italian blend cheese (such as Parmesan, mozzarella, provolone)</t>
-  </si>
-  <si>
-    <t>https://www.thekitchn.com/recipe-sausage-and-greens-breakfast-casserole-243967</t>
-  </si>
-  <si>
-    <t>Polenta for Breakfast</t>
-  </si>
-  <si>
-    <t>For the Polenta, 1 tablespoon butter, 4 cups boiling water, 1 cup coarse cornmeal or polenta, preferably from Bob's Red Mill, 1 cup cold water, 1 teaspoon Kosher salt, 1/4 cup butter or light olive oil, 1/4-1/2 cups freshly grated Parmesan or shredded sharp Cheddar (optional), 1/4-1/2 cups milk, cream or half-and-half, Kosher salt and fresh-ground pepper, For Serving, 4-6 poached or fried eggs, 1 pound Breakfast sausage, ham or bacon, cooked as desired, 8-12 Toasted and buttered ciabatta squares (2 slices per person), 2 tablespoons chopped fresh parsley, chives or green onion</t>
-  </si>
-  <si>
-    <t>https://food52.com/recipes/1987-polenta-for-breakfast</t>
-  </si>
-  <si>
-    <t>Easy Breakfast Casserole</t>
-  </si>
-  <si>
-    <t>For the breakfast casserole base:, 6 to 10 large eggs, 2 to 3 cups grated cheddar cheese, 6 slices day-old bread, cut into 3/4-inch to 1-inch-wide cubes, 2 cups milk, Salt, Pepper, For the possible additions:, 1 cup corn (cooked or frozen), 1/2 cup chopped broccoli (cooked or raw, raw will turn out crunchier), 1/2 cup sliced mushrooms, 1/4 cup sliced green onions, 1 cup cubed ham and/or cooked Italian sausage, A few slices cooked bacon, chopped, 1 teaspoon Herbes de Provence, or other dried herbs, (or 1 tablespoon of fresh chopped herbs such as basil, rosemary, or thyme), 1/4 to 1/2 teaspoon of cumin or curry powder</t>
-  </si>
-  <si>
-    <t>https://www.simplyrecipes.com/recipes/as_you_like_it_breakfast_casserole/</t>
-  </si>
-  <si>
-    <t>Breakfast Burritos with Cheese</t>
-  </si>
-  <si>
-    <t>18 flour tortillas, 1 pound breakfast sausage, 1/3 stick (about 2 1/2 tablespoons) salted butter, 18 large eggs, 1/2 teaspoon kosher salt, 1/2 teaspoon freshly ground black pepper, 3 cups grated cheese</t>
-  </si>
-  <si>
-    <t>https://www.foodnetwork.com/recipes/ree-drummond/breakfast-burritos-with-cheese-8741043</t>
-  </si>
-  <si>
-    <t>Creamy Turkey Breakfast Casserole</t>
-  </si>
-  <si>
-    <t>6 slices turkey bacon, such as JENNIE-O® Turkey Bacon, 1 (12-ounce) package turkey breakfast sausage links, such as JENNIE-O® Lean Turkey Breakfast Sausage Links, 1/2 Cup butter, divided, 1/2 Cup flour, 4 Cups milk, 1/2 Cup sliced fresh mushrooms, 1/4 Teaspoon black pepper, 4 Cups egg substitute or 16 eggs, 1 (7.5-ounce) package refrigerated biscuit dough</t>
-  </si>
-  <si>
-    <t>http://www.thedailymeal.com/recipes/creamy-turkey-breakfast-casserole-recipe</t>
-  </si>
-  <si>
-    <t>Recipe: Cheesy Hash Brown Breakfast Casserole</t>
-  </si>
-  <si>
-    <t>Cooking spray or oil, 1 tablespoon olive oil, 1 pound uncooked breakfast sausage, casings removed, 1 medium onion, diced, 1 medium red bell pepper, cored, seeded, and diced, 3/4 teaspoon kosher salt, divided, 1 (20-ounce) bag frozen shredded potatoes (do not thaw), 10 large eggs, 1 cup sour cream, 1 cup whole or 2% milk, 2 tablespoons Dijon mustard, 1 1/2 cups shredded sharp cheddar cheese (about 6 ounces), 1/4 teaspoon freshly ground black pepper</t>
-  </si>
-  <si>
-    <t>https://www.thekitchn.com/recipe-cheesy-hashbrown-breakfast-casserole-241992</t>
-  </si>
-  <si>
-    <t>Cowboy Breakfast Casserole With Sausage and Spinach</t>
-  </si>
-  <si>
-    <t>7 slices white sandwich bread, 1 pound bulk breakfast sausage, Softened unsalted butter or nonstick vegetable cooking spray (for pan), 4 scallions, white and pale green and dark green parts separated, thinly sliced, 1 (10-ounce) package frozen spinach, thawed, squeezed dry, 8 ounces cheddar cheese, shredded (about 2 cups), 8 large eggs, 1 1/2 cups milk, 1/2 cup full-fat Greek yogurt, 1 teaspoon mustard powder, 1/2 teaspoon kosher salt, 1/2 teaspoon freshly ground black pepper, 1/4 teaspoon ground nutmeg</t>
-  </si>
-  <si>
-    <t>https://www.epicurious.com/recipes/food/views/cowboy-breakfast-casserole-with-sausage-and-spinach</t>
-  </si>
-  <si>
-    <t>Tea Vodka</t>
-  </si>
-  <si>
-    <t>12 ounces vodka, 1 English Breakfast tea bag</t>
-  </si>
-  <si>
-    <t>https://www.foodandwine.com/recipes/tea-vodka-cocktails-2011</t>
-  </si>
-  <si>
-    <t>Breakfast Taco Bar</t>
-  </si>
-  <si>
-    <t>14 six-inch mission tortillas, 2 packages Johnsonville breakfast sausage links, cooked, 1 dozen eggs, scrambled, 1/2 Teaspoon salt, 1/2 Teaspoon pepper, 2 Cups Cheddar cheese, shredded, 2 medium tomatoes, chopped, Toppings: sour cream, salsa, and chopped avocado, optional</t>
-  </si>
-  <si>
-    <t>http://www.thedailymeal.com/recipes/breakfast-taco-bar-recipe</t>
-  </si>
-  <si>
-    <t>Radish With Butter And Sea Salt And Radish Greens Salad</t>
-  </si>
-  <si>
-    <t>16-20 French breakfast radishes, scrubbed, Coarse sea salt, Best-quality butter, slighty softened, 1/4 cup Dijon Vinaigrette</t>
-  </si>
-  <si>
-    <t>http://www.bonappetit.com/recipes/2011/06/radish-with-butter-and-sea-salt-and-radish-greens-salad</t>
-  </si>
-  <si>
-    <t>Radish with Butter and Sea Salt and Radish Greens Salad</t>
-  </si>
-  <si>
-    <t>16-20 French breakfast radishes, scrubbed, Coarse sea salt, Best-quality butter, slighty softened, 1 /4 cup Dijon Vinaigrette</t>
-  </si>
-  <si>
-    <t>https://www.bonappetit.com/recipe/radish-with-butter-and-sea-salt-and-radish-greens-salad</t>
-  </si>
-  <si>
-    <t>Country Breakfast Casserole</t>
-  </si>
-  <si>
-    <t>1 tablespoon oil, 4 potatoes, diced, 1 ½ teaspoons salt, divided, 1 red pepper, diced, 1 green pepper, diced, 1 onion, minced, 8-oz. pkg. breakfast link sausage, chopped, browned and drained, 1 ½ cups egg substitute, 1 cup milk, 2 tablespoons all-purpose flour, ½ teaspoon pepper, 1 cup shredded Cheddar cheese</t>
-  </si>
-  <si>
-    <t>https://www.myrecipes.com/recipe/country-breakfast-casserole</t>
-  </si>
-  <si>
-    <t>Recipe: Apple, Sausage, and Smoked Cheddar Breakfast Casserole</t>
-  </si>
-  <si>
-    <t>1 tablespoon olive oil, 1 pound uncooked breakfast sausage links, 3 cups sourdough bread, cut into 1/2-inch cubes, 2 medium firm apples, peeled, cored, and cut into 1/2-inch chunks, 8 ounces smoked cheddar cheese, cut into 1/4-inch cubes, 10 large eggs, 1 cup whole or 2% milk, 1/2 cup heavy cream, 2 tablespoons Dijon mustard, 1/2 teaspoon kosher salt, 1/4 teaspoon freshly ground black pepper, 3 scallions, green part only, sliced thin</t>
-  </si>
-  <si>
-    <t>https://www.thekitchn.com/recipe-apple-sausage-and-smoked-cheddar-breakfast-casserole-238197</t>
-  </si>
-  <si>
-    <t>Breakfast Pizza: Shashuka Pizza</t>
-  </si>
-  <si>
-    <t>1 package Green Giant Cauliflower Crust, 1 Tablespoon olive oil, 1/4 cup sweet onion chopped, 1/4 cup red bell pepper chopped, 1/2 teaspoon minced garlic, 1 Tablespoon cilantro chopped, 1/4 teaspoon paprika, 1/4 teaspoon cumin, 1/4 teaspoon chili powder, 1/4-1/2 jalapeno minced optional, 2 to matoes diced or 1/2 cup canned diced tomatoes, 2-3 Tablespoons tomato sauce, 1/4 teaspoon sugar, 4 oz breakfast sausage mild Italian sausage 4 slices bacon, cooked and crumbled or a meat alternative, 1 cup mozzarella cheese shredded or a combination of your favorite cheeses, 4 small eggs, Garnish: chopped parsley or cilantro</t>
-  </si>
-  <si>
-    <t>https://honestcooking.com/shashuka-pizza/</t>
-  </si>
-  <si>
-    <t>Biscuits And Gravy</t>
-  </si>
-  <si>
-    <t>1 lb Breakfast Sausage, 1 can 16 Oz Canned Biscuits, 2 tbsp Flour, 1 cup Milk, Salt, Pepper</t>
-  </si>
-  <si>
-    <t>http://thepioneerwoman.com/cooking/2007/09/biscuits_and_gr/</t>
-  </si>
-  <si>
-    <t>Breakfast Garbage Bread</t>
-  </si>
-  <si>
-    <t>2 1/2 cups frozen potato tots, One 12-ounce package pork breakfast sausage, 10 strips bacon (8 ounces), 5 large eggs, 2 cups grated American cheese (6 ounces), 2 cups grated white Cheddar (6 ounces), All-purpose flour, for dusting 1 1/2 pounds store-bought pizza dough (see Cook's Note), Ketchup and/or hot sauce, for serving</t>
-  </si>
-  <si>
-    <t>https://www.foodnetwork.com/recipes/food-network-kitchen/breakfast-garbage-bread-3513751</t>
-  </si>
-  <si>
-    <t>Breakfast Foil Packs With Hash Brown Potatoes, Sausage, and Scallions</t>
-  </si>
-  <si>
-    <t>3 scallions, trimmed, sliced, 1 (16-ounce) package frozen shredded hash brown potatoes, defrosted, 12 ounces cooked breakfast sausages (about 16 sausage links), cut into ¾" pieces, ¼ cup olive oil, 1 teaspoon kosher salt, plus more to taste, ½ teaspoon freshly ground black pepper, plus more to taste, 3 (packed) cups baby spinach, 6 large eggs, ½ cup shredded cheddar (optional)</t>
-  </si>
-  <si>
-    <t>https://www.epicurious.com/recipes/food/views/breakfast-hobo-packs-with-hash-brown-potatoes-sausage-and-scallions-56389750</t>
-  </si>
-  <si>
-    <t>Cinnamon Sugar Breakfast Puffs</t>
-  </si>
-  <si>
-    <t>Breakfast puffs, 1/3 cup unsalted butter, 1/2 cup sugar, 1 large egg, at room temperature, 1 1/2 cups all purpose flour, 1 1/2 teaspoons baking powder, 1/2 teaspoon salt, 1/4 teaspoon nutmeg, 1/4 teaspoon allspice, 1 pinch ground cloves, 1 pinch ground ginger, 1 teaspoon orange zest, 1/2 cup whole milk, at room temperature, Cinnamon-sugar coating, 6 tablespoons butter, melted, 1/2 cup granulated sugar, 1 teaspoon ground cinnamon</t>
-  </si>
-  <si>
-    <t>https://food52.com/recipes/15110-cinnamon-sugar-breakfast-puffs</t>
-  </si>
-  <si>
-    <t>Recipe: Loaded Savory Breakfast Muffins</t>
-  </si>
-  <si>
-    <t>1 tablespoon vegetable oil, 8 ounces uncooked breakfast sausage, casings removed, 3 cups baby spinach (about 3 ounces), Cooking spray, 2 cups all-purpose flour, 2 teaspoons baking powder, 1/2 teaspoon baking soda, 1/2 teaspoon salt, 1/4 teaspoon freshly ground black pepper, 6 tablespoons unsalted butter, 1 1/4 cups buttermilk, 2 large eggs, 1 cup shredded sharp cheddar cheese (about 4 ounces), 2/3 cup small-dice apple, 1 tablespoon finely chopped fresh chives</t>
-  </si>
-  <si>
-    <t>https://www.thekitchn.com/recipe-loaded-breakfast-muffins-253421</t>
-  </si>
-  <si>
-    <t>Sausage, Cheese And Potato Breakfast Casserole</t>
-  </si>
-  <si>
-    <t>1 lb bulk breakfast sausage, 2 tbsp all purpose flour, 1 1/2 cup milk (do not use low-fat or nonfat), 1/1 pound package frozen shredded hash brown potatoes, 4 x green onions, finely chopped, 1 1/4 cup grated sharp cheddar cheese</t>
-  </si>
-  <si>
-    <t>http://whippedtheblog.com/2009/07/20/sausage-cheese-and-potato-breakfast-casserole/</t>
-  </si>
-  <si>
-    <t>Breakfast Crescent Ring</t>
-  </si>
-  <si>
-    <t>16 frozen potato tots, 1/2 cup heavy cream, 12 large eggs, Kosher salt and freshly ground black pepper, 6 strips bacon, cut into 1/2-inch-wide pieces, 6 ounces pork breakfast sausage, removed from casings and chopped, Nonstick cooking spray, for greasing the pan, 2 ounces American cheese, grated, 1/2 cup grated white Cheddar (about 2 ounces), Maple syrup, ketchup, hot sauce or white gravy, for dipping, optional</t>
-  </si>
-  <si>
-    <t>https://www.foodnetwork.com/recipes/food-network-kitchen/breakfast-crescent-ring-5232578</t>
-  </si>
-  <si>
-    <t>Wagyu Breakfast Sausage Biscuits and Gravy</t>
-  </si>
-  <si>
-    <t>1 pound Double 8 Cattle Company Fullblood Wagyu Breakfast Sausage (broken into pieces), 1/2 cup Unsalted Butter, 1/2 cup All Purpose Flour, 1 Yellow Onion (small, diced), 6 cups Whole Milk, 1/2 teaspoon Crushed Red Pepper Flakes, Kosher Salt and Freshly Ground Black Pepper (to taste), 1 1/2 tablespoons Hot Sauce, 20 ounces All Purpose Flour, 2 tablespoons Sugar, 2 tablespoons Baking Powder, 2 teaspoons Kosher Salt, 6 ounces Cold Unsalted Butter (grated), 10 ounces Half and Half</t>
-  </si>
-  <si>
-    <t>https://food52.com/recipes/83986-wagyu-breakfast-sausage-biscuits-and-gravy</t>
-  </si>
-  <si>
-    <t>Holiday Breakfast Casserole</t>
-  </si>
-  <si>
-    <t>2 packages (12 ounces each) Johnsonville® Original Breakfast Sausage Links, 6 English muffins, cut into 1-in. cubes, 1/4 cup butter, melted, 1 cup (4 ounces) Cheddar cheese, shredded, 1 cup (4 ounces) mozzarella cheese, shredded, 1/2 cup onion, chopped, 1/2 cup red pepper, chopped, 12 large eggs, 2 cups milk, 1/4 teaspoon salt, 1/4 cup bacon bits</t>
-  </si>
-  <si>
-    <t>https://www.foodnetwork.com/recipes/holiday-breakfast-casserole-3415289</t>
-  </si>
-  <si>
-    <t>Chicken Piccata with Radishes</t>
-  </si>
-  <si>
-    <t>1 tablespoon extra-virgin olive oil, 8 breakfast radishes, Kosher salt</t>
-  </si>
-  <si>
-    <t>https://www.foodandwine.com/recipes/chicken-piccata-radishes</t>
-  </si>
-  <si>
-    <t>Dinner Tonight: Sausage and Biscuit Sandwich Recipe</t>
-  </si>
-  <si>
-    <t>1 cup flour, 1/2 tablespoon baking powder, 1/2 teaspoon sugar, 1/4 teaspoon salt, 4 tablespoons butter, cold, 6 tablespoons buttermilk, 1 pound breakfast sausage, 6 slices American cheese, Canola oil</t>
-  </si>
-  <si>
-    <t>http://www.seriouseats.com/recipes/2010/05/sausage-and-biscuit-sandwich-recipe.html</t>
-  </si>
-  <si>
-    <t>Overnight Breakfast Casserole</t>
-  </si>
-  <si>
-    <t>1 package (12 ounce each) Johnsonville® Original Breakfast Sausage Links, 6 English muffins, cut into 1-in. cubes, 1/4 cup butter, melted, 1 cup (4 ounce) cheddar cheese, shredded, 1 cup (4 ounce) mozzarella cheese, shredded, 1/2 cup onion, chopped, 1/2 cup red pepper, chopped, 12 eggs, 2 cups milk, 1/4 tsp. salt, 1/8 tsp. pepper, 1/4 cup bacon bits</t>
-  </si>
-  <si>
-    <t>https://www.foodnetwork.com/recipes/overnight-breakfast-casserole-3415701</t>
-  </si>
-  <si>
-    <t>Wagyu Beef Breakfast Sausage Kolaches</t>
-  </si>
-  <si>
-    <t>1 pound Double 8 Cattle Company Fullblood Wagyu Ground Breakfast Sausage, 3 tablespoons Grapeseed Oil, 1 Sweet Onion (minced), 2 Garlic Cloves (minced), 3/4 cup Butter, 3/4 cup Flour, 1 cup Whole Milk, 1/2 cup Heavy Cream, 1 sprig Thyme (leaves minced), 1/2 teaspoon Crushed Red Pepper, 2 teaspoons Kosher Salt, 5 1/2 cups All Purpose Flour, 1 1/2 cups Warm Milk (80°F), 3/4 cup Butter (softened), 2 Eggs, 1 1/2 tablespoons Instant Yeast, 1/3 cup Sugar, 1 tablespoon Kosher Salt, 1 Egg, 1 tablespoon Water</t>
-  </si>
-  <si>
-    <t>https://food52.com/recipes/86040-wagyu-beef-breakfast-sausage-kolaches</t>
-  </si>
-  <si>
-    <t>Breakfast Sausage Cornbread</t>
-  </si>
-  <si>
-    <t>Nonstick cooking spray, for spraying the baking dish, 1 1/2 cups yellow cornmeal, 1/4 cup all-purpose flour, 2 tablespoons sugar, 1 teaspoon baking powder, 1/2 teaspoon baking soda, 1/4 teaspoon fine salt, 1 cup milk, 1 cup sour cream or 2 percent Greek yogurt, 2 tablespoons unsalted butter, melted, 1 large egg, 1 cup cooked and crumbled breakfast sausage, 1 teaspoon chopped fresh sage</t>
-  </si>
-  <si>
-    <t>https://www.foodnetwork.com/recipes/food-network-kitchen/breakfast-sausage-cornbread-5496989</t>
-  </si>
-  <si>
-    <t>Breakfast-for-Dinner Egg Boats</t>
-  </si>
-  <si>
-    <t>1/3 pound breakfast (country) sausage, 6 large eggs, 1 cup milk, 1 teaspoon Dijon mustard, Coarse salt, Four 7-inch mini baguettes or bolillo rolls, 1/2 cup finely chopped kale, 1/2 cup shredded Cheddar, Parsley leaves, for garnish</t>
-  </si>
-  <si>
-    <t>https://www.foodnetwork.com/recipes/breakfast-for-dinner-egg-boats-5426546</t>
-  </si>
-  <si>
-    <t>Radish and Basil Compound Butter</t>
-  </si>
-  <si>
-    <t>3 small breakfast radishes, minced, 4 fresh basil leaves, minced, 1/4 teaspoon sea salt, or more to taste, 1/2 cup unsalted butter, softened</t>
-  </si>
-  <si>
-    <t>https://food52.com/recipes/28751-radish-and-basil-compound-butter</t>
-  </si>
-  <si>
-    <t>Awesome Breakfast Burritos</t>
-  </si>
-  <si>
-    <t>12 slices bacon, chopped, 1 onion, chopped, 1 pound loose breakfast sausage, 10 slices ham, chopped, 12 large eggs, whisked, 2 cups grated pepper jack cheese, 1/2 cup store-bought salsa verde, Two 4-ounce cans diced green chiles, Kosher salt and freshly ground black pepper, Twelve 8-inch flour tortillas</t>
-  </si>
-  <si>
-    <t>https://www.foodnetwork.com/recipes/ree-drummond/awesome-breakfast-burritos-5117356</t>
-  </si>
-  <si>
-    <t>Sausage and Cheese Breakfast Casserole</t>
-  </si>
-  <si>
-    <t>1 teaspoon canola oil, 12 ounces turkey breakfast sausage, 2 cups 1% low-fat milk, 2 cups egg substitute, 1 teaspoon dry mustard, ½ teaspoon freshly ground black pepper, ¼ teaspoon salt, ¼ teaspoon ground red pepper, 3 large eggs, 16 (1-ounce) slices white bread, 1 cup (4 ounces) finely shredded reduced-fat extrasharp cheddar cheese, Cooking spray</t>
-  </si>
-  <si>
-    <t>https://www.myrecipes.com/recipe/sausage-cheese-breakfast-casserole</t>
-  </si>
-  <si>
-    <t>Peach and Blackberry Iced Tea</t>
-  </si>
-  <si>
-    <t>2 black-tea bags, such as English breakfast, 8 cups boiling water, 4 peaches, 1/4 cup sugar, 1/2 cup peach nectar, Blackberries, for garnish</t>
-  </si>
-  <si>
-    <t>https://www.marthastewart.com/1142785/peach-iced-tea</t>
-  </si>
-  <si>
-    <t>Savory Breakfast Kabobs</t>
-  </si>
-  <si>
-    <t>2 tablespoons olive oil, 6 breakfast sausage links, cut into 1-inch pieces, 1 small onion, cut into chunks, 1 small red bell pepper, cut into chunks, 1 small green bell pepper, cut into chunks, 1 tablespoon Montreal steak seasoning, 1/3 cup half-and-half, 2 teaspoons kosher salt, 1 teaspoon freshly ground black pepper, 6 large eggs, 2 tablespoons butter, 1 cup shredded Cheddar cheese</t>
-  </si>
-  <si>
-    <t>https://www.foodnetwork.com/recipes/ree-drummond/savory-breakfast-kabobs-5478046</t>
-  </si>
-  <si>
-    <t>Sausage and Cilantro Omelete</t>
-  </si>
-  <si>
-    <t>1 Breakfast sausage, cut into rounds, 1/2 Onion, small dice, 2 tablespoons Fresh cilantro, chopped, 3 Large eggs, whisked, 1/4 cup Cheese, shredded</t>
-  </si>
-  <si>
-    <t>https://food52.com/recipes/37426-sausage-and-cilantro-omelete</t>
-  </si>
-  <si>
-    <t>Recipe: Slow Cooker Sausage and Spinach Breakfast Casserole</t>
-  </si>
-  <si>
-    <t>Cooking spray, 1 pound uncooked pork breakfast sausage, casings removed, 1 small yellow onion, diced, 1 1/2 teaspoons dried oregano, 5 ounces baby spinach (about 5 packed cups), 1 pound frozen diced potatoes (do not thaw, about 4 cups), 1 1/4 cups shredded Swiss cheese, divided, 1/4 cup grated Parmesan cheese, plus more for serving, 8 large eggs, 2 cups whole or 2% milk, 2 teaspoons Dijon mustard, 1 1/2 teaspoons kosher salt, 1/4 teaspoon freshly ground black pepper, Red pepper flakes or hot sauce, for serving</t>
-  </si>
-  <si>
-    <t>https://www.thekitchn.com/slow-cooker-sausage-breakfast-casserole-256182</t>
-  </si>
-  <si>
-    <t>Cucumber, Feta and Watermelon Salad</t>
-  </si>
-  <si>
-    <t>1/2 watermelon, 1/2 pound north american feta, 2 cucumbers, 1 bunch radishes, french breakfast are the best, 1 bunch fresh mint, 1/4 cup Balsamic vinegar</t>
-  </si>
-  <si>
-    <t>https://food52.com/recipes/4922-cucumber-feta-and-watermelon-salad</t>
-  </si>
-  <si>
-    <t>Breakfast Nachos</t>
-  </si>
-  <si>
-    <t>8 homemade or thawed frozen waffles, cut into triangles (like tortilla chips), 1 pound breakfast sausage, casings removed and meat crumbled, 1 tablespoon olive oil, 6 large eggs, Kosher salt and freshly ground black pepper, 1 tablespoon maple syrup, 2 cups shredded sharp Cheddar, 1 avocado, thinly sliced, 1/2 cup quartered cherry tomatoes, 3 scallions, white and light green parts only, thinly sliced, 1 jalapeno, thinly sliced, 1/4 cup chopped fresh cilantro, Hot sauce, for serving, optional, Sour cream, for garnish</t>
-  </si>
-  <si>
-    <t>https://www.foodnetwork.com/recipes/katie-lee/breakfast-nachos-3513869</t>
-  </si>
-  <si>
-    <t>Meat Lover’s Breakfast Sandwich</t>
-  </si>
-  <si>
-    <t>2 teaspoons canola oil, 5 ounces bulk breakfast sausage, 2 large eggs, 1 1/2 tablespoons cream cheese, at room temperature, 1 tablespoon finely chopped fresh chives, 1 tablespoon finely chopped fresh cilantro, 1 tablespoon finely chopped fresh parsley, Kosher salt and freshly ground black pepper, 1 deli slice sharp Cheddar, 1/4 avocado, cut into 1/4-inch slices</t>
-  </si>
-  <si>
-    <t>https://www.foodnetwork.com/recipes/food-network-kitchen/meat-lovers-breakfast-sandwich-5463144</t>
-  </si>
-  <si>
-    <t>Cheesy Sausage and Potato Breakfast Casserole</t>
-  </si>
-  <si>
-    <t>2 packages (12 ounces each) Johnsonville® Cheesy Breakfast Sausage Links, 1 package (20 ounces) frozen roasted potatoes, 1/2 cup chopped onion, 1/2 cup chopped green pepper, 2 cups (8 ounces) shredded cheddar cheese, divided, 9 eggs, 3 cups milk, 1 tablespoon Dijon mustard, 1/4 teaspoon salt, 1/4 teaspoon pepper</t>
-  </si>
-  <si>
-    <t>https://www.foodnetwork.com/recipes/cheesy-sausage-and-potato-breakfast-casserole-3414393</t>
-  </si>
-  <si>
-    <t>Cheesy Sausage Breakfast Grits</t>
-  </si>
-  <si>
-    <t>1 pound ground breakfast sausage, 3 cups lowfat (2 percent) milk, 1 cup quick-cooking grits, 3 cups grated Cheddar, 4 large eggs, 1 tablespoon hot sauce, 4 scallions, white and light green parts, thinly sliced, dark green tops reserved for garnish, 4 scallions, white and light green parts, thinly sliced, dark green tops reserved for garnish, 1 jalapeno, minced, Kosher salt and freshly cracked black pepper</t>
-  </si>
-  <si>
-    <t>https://www.foodnetwork.com/recipes/cheesy-sausage-breakfast-grits-3209099</t>
-  </si>
-  <si>
-    <t>Slow-Cooker Overnight Breakfast Casserole</t>
-  </si>
-  <si>
-    <t>24 Ounces Johnsonville Hot and Spicy Breakfast sausage, 1 Cup greens onions, chopped, 1 sweet red bell pepper, chopped, 4 Ounces mild green chiles, diced, 1/4 Cup fresh cilantro, chopped, 30 Ounces frozen shredded hash brown potatoes, 1 1/2 Cup Cheddar cheese, shredded, 12 eggs, 1 Cup milk, 1/2 Teaspoon salt, 1/8 Teaspoon black pepper</t>
-  </si>
-  <si>
-    <t>http://www.thedailymeal.com/recipes/slow-cooker-overnight-breakfast-casserole-recipe</t>
-  </si>
-  <si>
-    <t>Breakfast Bread Pudding</t>
-  </si>
-  <si>
-    <t>Butter, for greasing, 1 tablespoon olive oil, 1 medium yellow onion, minced, 1 pound breakfast sausage, crumbled, 10 large eggs, 3 cups milk, 1 teaspoon salt, 1/2 teaspoon freshly ground black pepper, 1/2 teaspoon garlic powder, 1 loaf day-old brioche or country white bread, cut into 1 1/2-inch cubes (about 12 cups), 2 cups shredded Cheddar (about 6 ounces)</t>
-  </si>
-  <si>
-    <t>https://www.foodnetwork.com/recipes/katie-lee/breakfast-bread-pudding-2396291</t>
-  </si>
-  <si>
-    <t>Peppery kohlrabi slaw</t>
-  </si>
-  <si>
-    <t>2 whole kohlrabi, peeled, head of spring greens, finely shredded, 2 bunches spring onions, very finely shredded, small bunch French breakfast radishes, quartered, leaves attached, juice 0.5 lemon</t>
-  </si>
-  <si>
-    <t>https://www.bbcgoodfood.com/recipes/peppery-kohlrabi-slaw</t>
-  </si>
-  <si>
-    <t>Sheet Pan Sausage and Egg Breakfast Bake</t>
-  </si>
-  <si>
-    <t>4 uncooked breakfast sausages (6 oz total), 4 slices bacon, 8 oz. small cremini mushrooms, halved or quartered if large, 16 Campari or cocktail tomatoes, halved, 2 cloves garlic, finely chopped, 1 tbsp. olive oil, Kosher salt and pepper, 4 large eggs, 1/2 c. flat-leaf parsley, chopped, Toast, for serving</t>
-  </si>
-  <si>
-    <t>https://www.goodhousekeeping.com/food-recipes/a34464150/sheet-pan-breakfast-bake-recipe/</t>
-  </si>
-  <si>
-    <t>Hangover Breakfast Sausage-and-Egg Burger</t>
-  </si>
-  <si>
-    <t>1 tablespoon mayonnaise, 1/2 teaspoon Sriracha, 1/2 teaspoon pure maple syrup, 1 sesame-seed hamburger bun, 1 lettuce leaf, 1 tomato slice, 3 to 4 thin rings red onion, 4 ounces bulk breakfast sausage, 1 teaspoon vegetable oil, 1 slice Cheddar, 1 large egg, Kosher salt and freshly ground black pepper</t>
-  </si>
-  <si>
-    <t>https://www.foodnetwork.com/recipes/food-network-kitchen/hangover-breakfast-sausage-and-egg-burger-3363856</t>
-  </si>
-  <si>
-    <t>Breakfast Sausage and Rice Brunch Ring</t>
-  </si>
-  <si>
-    <t>2 rolls breakfast sausage, mild, 1/2 pound lean ground beef, 1 cup chopped onions, 1/2 cup chopped green bell pepper, 1 cup sliced fresh mushrooms, 1 teaspoon garlic salt, 2 tablespoons dark brown sugar, 2 cups cooked rice, medium grain (cooked in chicken broth), 2 cans refrigerated crescent rolls, 2 cups shredded cheese, Mexican style with jalapenos, 1 package Canadian bacon</t>
-  </si>
-  <si>
-    <t>https://www.foodnetwork.com/recipes/breakfast-sausage-and-rice-brunch-ring-recipe-1940202</t>
-  </si>
-  <si>
-    <t>Breakfast Sausage With Red-Pepper Gravy</t>
-  </si>
-  <si>
-    <t>1 tablespoon extra-virgin olive oil, 1 pound breakfast sausage, 3 scallions, sliced, white and green parts separated, 1 red bell pepper, diced, Kosher salt and freshly ground pepper, 1 tablespoon flour, 1 clove garlic, minced, 1/2 teaspoon Worcestershire sauce, 1/8 teaspoon ground allspice, 3/4 cup low-sodium chicken broth, 1 1/4 cups milk</t>
-  </si>
-  <si>
-    <t>https://www.foodnetwork.com/recipes/food-network-kitchen/breakfast-sausage-with-red-pepper-gravy-recipe-1973877</t>
-  </si>
-  <si>
-    <t>Bagel Breakfast Casserole</t>
-  </si>
-  <si>
-    <t>Unsalted butter or nonstick cooking spray, for greasing the baking dish, 1 tablespoon olive oil, 8 ounces breakfast sausage, casing removed (8 sausages) (see Cook's Note), 2 cups whole milk, 3/4 cup half-and-half, Pinch of cayenne, 8 large eggs, Kosher salt and freshly ground black pepper, 1 1/3 cups packed baby spinach, 2 large plain bagels, split and cut into 1-inch pieces, 1 1/3 cups shredded provolone, 8 ounces cream cheese, cut into 1/2-inch cubes, 2 tablespoons everything bagel seasoning</t>
-  </si>
-  <si>
-    <t>https://www.foodnetwork.com/recipes/food-network-kitchen/bagel-breakfast-casserole-3814175</t>
-  </si>
-  <si>
-    <t>Fast and Easy Breakfast Cups</t>
-  </si>
-  <si>
-    <t>1 package (9.6 ounces) Johnsonville® Fully Cooked Original Recipe or Turkey Breakfast Sausage Links, cut into ¼-inch pieces, 1 1/2 cup frozen shredded hash brown potatoes, 1/4 cup finely chopped onion, 1 cup shredded Cheddar cheese, divided, 2 eggs, 1 cup milk, 1/2 cup biscuit/baking mix, 1/4 teaspoon pepper, 1/8 teaspoon salt</t>
-  </si>
-  <si>
-    <t>https://www.foodnetwork.com/recipes/fast-and-easy-breakfast-cups-3416649</t>
-  </si>
-  <si>
-    <t>Chai tea</t>
-  </si>
-  <si>
-    <t>2 mugs milk (or use almond milk), 2 English Breakfast tea bags, 6 cracked cardamom pods, ½ cinnamon stick, a grating of fresh nutmeg, 2 cloves, 2-4 tsp light brown soft sugar</t>
-  </si>
-  <si>
-    <t>https://www.bbcgoodfood.com/recipes/cassies-chai-tea</t>
-  </si>
-  <si>
-    <t>Double D Sliders</t>
-  </si>
-  <si>
-    <t>1 glazed doughnut, halved, One 2-ounce breakfast sausage patty, such as Delia's chicken breakfast sausage, 1 tablespoon sour cherry cream cheese</t>
-  </si>
-  <si>
-    <t>https://www.foodnetwork.com/recipes/double-d-sliders-3078779</t>
-  </si>
-  <si>
-    <t>Sausage Gravy and Cheddar Biscuit Pot Pie</t>
-  </si>
-  <si>
-    <t>12 oz. pork breakfast sausage, ½ cups flour, 3½ cups milk, 1 cup heavy cream, 1 tbsp. apple cider vinegar, ¼ tsp. cayenne, Kosher salt and freshly ground black pepper, to taste</t>
-  </si>
-  <si>
-    <t>https://www.saveur.com/article/Recipes/Sausage-Gravy-and-Cheddar-Biscuit-Pot-Pie/</t>
-  </si>
-  <si>
-    <t>Sweet Iced Black Tea With Cream</t>
-  </si>
-  <si>
-    <t>4 cups boiling water, 8 teaspoons loose English breakfast tea (or 8 tea bags), 1/2 cup sugar, Crushed ice, for serving, 1/2 cup heavy cream</t>
-  </si>
-  <si>
-    <t>https://www.marthastewart.com/1142446/sweet-iced-black-tea-cream</t>
-  </si>
-  <si>
-    <t>Breakfast quinoa</t>
-  </si>
-  <si>
-    <t>1 cup quinoa, 1.5 cups milk, 2 tablespoons maple syrup (more to taste if you like it sweeter), 4 ounces blueberries, can use fresh or frozen, 1/2 cup walnuts, 1/2 teaspoon cinnamon (optional)</t>
-  </si>
-  <si>
-    <t>https://food52.com/recipes/23503-breakfast-quinoa</t>
-  </si>
-  <si>
-    <t>Poached duck egg with hot smoked salmon &amp; mustard hollandaise</t>
-  </si>
-  <si>
-    <t>2 x 150g pieces hot smoked salmon, 4 duck eggs, splash of white wine vinegar, 60g watercress, a little rapeseed oil, 2 breakfast muffins, cut in half and toasted</t>
-  </si>
-  <si>
-    <t>https://www.bbcgoodfood.com/recipes/poached-duck-egg-hot-smoked-salmon-mustard-hollandaise</t>
-  </si>
-  <si>
-    <t>1-Minute Sausage and Cheese Omelette recipes</t>
-  </si>
-  <si>
-    <t>1 egg, beaten, 1 Tablespoon milk, 2 Tablespoons fully-cooked breakfast sausage crumbles or one fully-cooked breakfast sausage link or patty, chopped, 2 Tablespoons shredded Cheddar cheese, 1 flatbread (six-inch), toasted</t>
-  </si>
-  <si>
-    <t>http://www.thedailymeal.com/recipes/1-minute-sausage-and-cheese-omelette-recipe</t>
-  </si>
-  <si>
-    <t>The Breakfast Martini Recipe</t>
-  </si>
-  <si>
-    <t>1 3/4 ounces gin, 1/2 ounce fresh lemon juice from one lemon, 1/2 ounce Cointreau, 1 teaspoon orange marmalade, Quarter-sized piece of orange zest, or strip cut with a channel knife</t>
-  </si>
-  <si>
-    <t>https://www.seriouseats.com/the-breakfast-martini-marmalade-cocktail-recipe</t>
-  </si>
-  <si>
-    <t>Radishes with Spicy Mayo and Sesame Salt</t>
-  </si>
-  <si>
-    <t>½ cup black sesame seeds, preferably Japanese, 2 tablespoons sugar, ¾ teaspoon kosher salt, 1 cup homemade or purchased mayonnaise, 2 teaspoons gochujang (Korean hot pepper paste), 2 bunches breakfast radishes</t>
-  </si>
-  <si>
-    <t>https://www.bonappetit.com/recipe/radishes-with-spicy-mayo-and-sesame-salt</t>
-  </si>
-  <si>
-    <t>Spicy Breakfast Burritos with Cheese</t>
-  </si>
-  <si>
-    <t>18 flour tortillas, 1 pound breakfast sausage, 1/3 stick (about 2 1/2 tablespoons) salted butter, 18 large eggs, 1/2 teaspoon kosher salt, 1/2 teaspoon freshly ground black pepper, 1 tablespoon hot sauce, plus more for serving, 1/4 of a 16-ounce jar jalapenos plus liquid from the jar, plus more jalapenos for serving, 3 cups grated cheese, Salsa, for serving</t>
-  </si>
-  <si>
-    <t>https://www.foodnetwork.com/recipes/ree-drummond/spicy-breakfast-burritos-with-cheese-8741045</t>
-  </si>
-  <si>
-    <t>Breakfast smoothie</t>
-  </si>
-  <si>
-    <t>1 small ripe banana, about 140g blackberries, blueberries, raspberries or strawberries (or use a mix), plus extra to serve, apple juice or mineral water, optional, runny honey, to serve</t>
-  </si>
-  <si>
-    <t>https://www.bbcgoodfood.com/recipes/breakfast-smoothie</t>
-  </si>
-  <si>
-    <t>Sticky bourbon BBQ wings with blue cheese dip</t>
-  </si>
-  <si>
-    <t>1kg whole chicken wings, 2 tbsp olive oil, 4 celery sticks, each cut into 4 small sticks (keep some with their leaves), bunch French breakfast radishes (with their leaves if you can get them)</t>
-  </si>
-  <si>
-    <t>https://www.bbcgoodfood.com/recipes/sticky-bourbon-bbq-wings-blue-cheese-dip</t>
-  </si>
-  <si>
-    <t>Black Tea Jelly</t>
-  </si>
-  <si>
-    <t>2 cups of your favorite black tea (I use Taylor's of Harrogate Scottish Breakfast), strongly brewed and cooled to room temperature, 2 packets (1/2 an ounce) powdered gelatin, 1/4 cup sugar</t>
-  </si>
-  <si>
-    <t>https://food52.com/recipes/4167-black-tea-jelly</t>
-  </si>
-  <si>
-    <t>Breakfast Burrito Casserole</t>
-  </si>
-  <si>
-    <t>Nonstick cooking spray, oil or butter, for the baking dish, One 20-ounce bag refrigerated diced potatoes with onions, 2 tablespoons olive oil, 1 pound bulk breakfast sausage, 1 cup milk, 1/2 cup sour cream, 1/2 teaspoon seasoned salt, such as Lawry’s, 1/4 teaspoon freshly ground black pepper, 4 large eggs, 4 scallions, sliced, 1 red bell pepper, diced, 2 cups grated pepper jack, 1 cup grated sharp Cheddar, 1/2 cup jarred pickled jalapeno slices, Tortillas and salsa, for serving</t>
-  </si>
-  <si>
-    <t>https://www.foodnetwork.com/recipes/ree-drummond/breakfast-burrito-casserole-13402856</t>
-  </si>
-  <si>
-    <t>Apple, Sausage, and Cheddar Monkey Bread</t>
-  </si>
-  <si>
-    <t>8 ounces crumbled breakfast sausage, 2 red apples, diced, 16 ounce can of biscuit dough, cut into 1-inch pieces, 1½ cups grated cheddar</t>
-  </si>
-  <si>
-    <t>https://www.realsimple.com/food-recipes/browse-all-recipes/apple-sausage-cheddar-monkey-bread</t>
-  </si>
-  <si>
-    <t>Sausage Gravy</t>
-  </si>
-  <si>
-    <t>1/2 pound breakfast sausage, 1/2 cup (1 stick) unsalted butter, 1/2 cup all-purpose flour, 6 cups whole milk, 1/2 teaspoon crushed red pepper flakes, Kosher salt, Freshly ground pepper</t>
-  </si>
-  <si>
-    <t>https://www.epicurious.com/recipes/food/views/sausage-gravy-367139</t>
   </si>
   <si>
     <t>Sweet Lemon Pull-Apart Bread</t>
@@ -3606,7 +3606,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -3643,19 +3643,6 @@
       <b/>
       <sz val="12"/>
       <name val="Aptos Narrow"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <name val="Aptos Narrow"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -3696,11 +3683,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3712,21 +3698,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="16">
@@ -5826,11 +5805,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:F387"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
@@ -5838,7 +5816,7 @@
     <col min="1" max="1" width="15.83203125" customWidth="1"/>
     <col min="2" max="2" width="30.83203125" style="3" customWidth="1"/>
     <col min="3" max="3" width="20.83203125" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" customWidth="1"/>
+    <col min="4" max="4" width="15.83203125" customWidth="1"/>
     <col min="5" max="6" width="50.83203125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5852,7 +5830,7 @@
       <c r="C1" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="7" t="s">
         <v>25</v>
       </c>
       <c r="E1" s="8" t="s">
@@ -5927,7 +5905,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="C5">
         <v>365</v>
@@ -5936,10 +5914,10 @@
         <v>10</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="34">
@@ -5947,7 +5925,7 @@
         <v>8</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="C6">
         <v>274</v>
@@ -5956,10 +5934,10 @@
         <v>1</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="85">
@@ -5967,7 +5945,7 @@
         <v>8</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="C7">
         <v>436</v>
@@ -5976,10 +5954,10 @@
         <v>6</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="85">
@@ -5987,7 +5965,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="C8">
         <v>508</v>
@@ -5996,10 +5974,10 @@
         <v>1</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="85">
@@ -6007,7 +5985,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="C9">
         <v>371</v>
@@ -6016,10 +5994,10 @@
         <v>10</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="102">
@@ -6027,7 +6005,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="C10">
         <v>220</v>
@@ -6036,10 +6014,10 @@
         <v>4</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="34">
@@ -6047,7 +6025,7 @@
         <v>8</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="C11">
         <v>114</v>
@@ -6056,10 +6034,10 @@
         <v>16</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="85">
@@ -6067,7 +6045,7 @@
         <v>8</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="C12">
         <v>517</v>
@@ -6076,10 +6054,10 @@
         <v>2</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="34">
@@ -6087,7 +6065,7 @@
         <v>8</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="C13">
         <v>103</v>
@@ -6096,10 +6074,10 @@
         <v>4</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="85">
@@ -6107,7 +6085,7 @@
         <v>8</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="C14">
         <v>529</v>
@@ -6116,10 +6094,10 @@
         <v>4</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="102">
@@ -6127,7 +6105,7 @@
         <v>8</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
       <c r="C15">
         <v>465</v>
@@ -6136,10 +6114,10 @@
         <v>10</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="119">
@@ -6147,7 +6125,7 @@
         <v>8</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="C16">
         <v>484</v>
@@ -6156,10 +6134,10 @@
         <v>4</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>86</v>
+        <v>71</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="119">
@@ -6167,7 +6145,7 @@
         <v>8</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
       <c r="C17">
         <v>452</v>
@@ -6176,10 +6154,10 @@
         <v>6</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="102">
@@ -6187,7 +6165,7 @@
         <v>8</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="C18">
         <v>348</v>
@@ -6196,10 +6174,10 @@
         <v>4</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="119">
@@ -6207,7 +6185,7 @@
         <v>8</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="C19">
         <v>143</v>
@@ -6216,10 +6194,10 @@
         <v>12</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="153">
@@ -6227,7 +6205,7 @@
         <v>8</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="C20">
         <v>515</v>
@@ -6236,10 +6214,10 @@
         <v>6</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="102">
@@ -6247,7 +6225,7 @@
         <v>8</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="C21">
         <v>414</v>
@@ -6256,10 +6234,10 @@
         <v>6</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>102</v>
+        <v>87</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="51">
@@ -6267,7 +6245,7 @@
         <v>8</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
       <c r="C22">
         <v>312</v>
@@ -6276,10 +6254,10 @@
         <v>18</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>104</v>
+        <v>89</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="34">
@@ -6287,7 +6265,7 @@
         <v>8</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="C23">
         <v>258</v>
@@ -6296,10 +6274,10 @@
         <v>4</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>107</v>
+        <v>92</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>108</v>
+        <v>93</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="68">
@@ -6307,7 +6285,7 @@
         <v>8</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>109</v>
+        <v>94</v>
       </c>
       <c r="C24">
         <v>360</v>
@@ -6316,10 +6294,10 @@
         <v>4</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>111</v>
+        <v>96</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="68">
@@ -6327,7 +6305,7 @@
         <v>8</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>112</v>
+        <v>97</v>
       </c>
       <c r="C25">
         <v>529</v>
@@ -6336,10 +6314,10 @@
         <v>4</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>113</v>
+        <v>98</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>114</v>
+        <v>99</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="34">
@@ -6347,7 +6325,7 @@
         <v>8</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="C26">
         <v>273</v>
@@ -6356,10 +6334,10 @@
         <v>4</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>116</v>
+        <v>101</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>117</v>
+        <v>102</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="85">
@@ -6367,7 +6345,7 @@
         <v>8</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>118</v>
+        <v>103</v>
       </c>
       <c r="C27">
         <v>470</v>
@@ -6376,10 +6354,10 @@
         <v>10</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>119</v>
+        <v>104</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>120</v>
+        <v>105</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="102">
@@ -6387,7 +6365,7 @@
         <v>8</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>121</v>
+        <v>106</v>
       </c>
       <c r="C28">
         <v>390</v>
@@ -6396,10 +6374,10 @@
         <v>8</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>122</v>
+        <v>107</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>123</v>
+        <v>108</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="153">
@@ -6407,7 +6385,7 @@
         <v>8</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="C29">
         <v>490</v>
@@ -6416,10 +6394,10 @@
         <v>10</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>126</v>
+        <v>111</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="51">
@@ -6427,7 +6405,7 @@
         <v>8</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>127</v>
+        <v>112</v>
       </c>
       <c r="C30">
         <v>191</v>
@@ -6436,10 +6414,10 @@
         <v>8</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>128</v>
+        <v>113</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>129</v>
+        <v>114</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="136">
@@ -6447,7 +6425,7 @@
         <v>8</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>130</v>
+        <v>115</v>
       </c>
       <c r="C31">
         <v>457</v>
@@ -6456,10 +6434,10 @@
         <v>8</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>131</v>
+        <v>116</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>132</v>
+        <v>117</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="170">
@@ -6467,7 +6445,7 @@
         <v>8</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>133</v>
+        <v>118</v>
       </c>
       <c r="C32">
         <v>585</v>
@@ -6476,10 +6454,10 @@
         <v>6</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="187">
@@ -6487,7 +6465,7 @@
         <v>8</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
       <c r="C33">
         <v>444</v>
@@ -6496,10 +6474,10 @@
         <v>8</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>137</v>
+        <v>122</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>138</v>
+        <v>123</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="68">
@@ -6507,7 +6485,7 @@
         <v>8</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>139</v>
+        <v>124</v>
       </c>
       <c r="C34">
         <v>393</v>
@@ -6516,10 +6494,10 @@
         <v>18</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>140</v>
+        <v>125</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>141</v>
+        <v>126</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="119">
@@ -6527,7 +6505,7 @@
         <v>8</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="C35">
         <v>439</v>
@@ -6536,10 +6514,10 @@
         <v>12</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>143</v>
+        <v>128</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>144</v>
+        <v>129</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="136">
@@ -6547,7 +6525,7 @@
         <v>8</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>145</v>
+        <v>130</v>
       </c>
       <c r="C36">
         <v>525</v>
@@ -6556,10 +6534,10 @@
         <v>8</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>146</v>
+        <v>131</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>147</v>
+        <v>132</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="153">
@@ -6567,7 +6545,7 @@
         <v>8</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="C37">
         <v>286</v>
@@ -6576,10 +6554,10 @@
         <v>14</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="34">
@@ -6587,7 +6565,7 @@
         <v>8</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>151</v>
+        <v>136</v>
       </c>
       <c r="C38">
         <v>393</v>
@@ -6596,10 +6574,10 @@
         <v>2</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="F38" s="10" t="s">
-        <v>153</v>
+        <v>137</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="85">
@@ -6607,7 +6585,7 @@
         <v>8</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>154</v>
+        <v>139</v>
       </c>
       <c r="C39">
         <v>368</v>
@@ -6616,10 +6594,10 @@
         <v>7</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>155</v>
+        <v>140</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>156</v>
+        <v>141</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="51">
@@ -6627,7 +6605,7 @@
         <v>8</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>157</v>
+        <v>142</v>
       </c>
       <c r="C40">
         <v>76</v>
@@ -6636,10 +6614,10 @@
         <v>4</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>158</v>
+        <v>143</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>159</v>
+        <v>144</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="51">
@@ -6647,7 +6625,7 @@
         <v>8</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>160</v>
+        <v>145</v>
       </c>
       <c r="C41">
         <v>76</v>
@@ -6656,10 +6634,10 @@
         <v>4</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>161</v>
+        <v>146</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>162</v>
+        <v>147</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="102">
@@ -6667,7 +6645,7 @@
         <v>8</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
       <c r="C42">
         <v>365</v>
@@ -6676,10 +6654,10 @@
         <v>8</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>164</v>
+        <v>149</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>165</v>
+        <v>150</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="136">
@@ -6687,7 +6665,7 @@
         <v>8</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>166</v>
+        <v>151</v>
       </c>
       <c r="C43">
         <v>511</v>
@@ -6696,10 +6674,10 @@
         <v>8</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>167</v>
+        <v>152</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>168</v>
+        <v>153</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="187">
@@ -6707,7 +6685,7 @@
         <v>8</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="C44">
         <v>461</v>
@@ -6716,10 +6694,10 @@
         <v>4</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>170</v>
+        <v>155</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>171</v>
+        <v>156</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="34">
@@ -6727,7 +6705,7 @@
         <v>8</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>172</v>
+        <v>157</v>
       </c>
       <c r="C45">
         <v>503</v>
@@ -6736,10 +6714,10 @@
         <v>4</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>173</v>
+        <v>158</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>174</v>
+        <v>159</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="102">
@@ -6747,7 +6725,7 @@
         <v>8</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>175</v>
+        <v>160</v>
       </c>
       <c r="C46">
         <v>386</v>
@@ -6756,10 +6734,10 @@
         <v>10</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>176</v>
+        <v>161</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>177</v>
+        <v>162</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="119">
@@ -6767,7 +6745,7 @@
         <v>8</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>178</v>
+        <v>163</v>
       </c>
       <c r="C47">
         <v>263</v>
@@ -6776,10 +6754,10 @@
         <v>6</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>179</v>
+        <v>164</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>180</v>
+        <v>165</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="136">
@@ -6787,7 +6765,7 @@
         <v>8</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>181</v>
+        <v>166</v>
       </c>
       <c r="C48">
         <v>234</v>
@@ -6796,10 +6774,10 @@
         <v>12</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>182</v>
+        <v>167</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>183</v>
+        <v>168</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="136">
@@ -6807,7 +6785,7 @@
         <v>8</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>184</v>
+        <v>169</v>
       </c>
       <c r="C49">
         <v>268</v>
@@ -6816,10 +6794,10 @@
         <v>12</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>185</v>
+        <v>170</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>186</v>
+        <v>171</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="68">
@@ -6827,7 +6805,7 @@
         <v>8</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>187</v>
+        <v>172</v>
       </c>
       <c r="C50">
         <v>524</v>
@@ -6836,10 +6814,10 @@
         <v>5</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>188</v>
+        <v>173</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>189</v>
+        <v>174</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="136">
@@ -6847,7 +6825,7 @@
         <v>8</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>190</v>
+        <v>175</v>
       </c>
       <c r="C51">
         <v>600</v>
@@ -6856,10 +6834,10 @@
         <v>10</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>191</v>
+        <v>176</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="153">
@@ -6867,7 +6845,7 @@
         <v>8</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>193</v>
+        <v>178</v>
       </c>
       <c r="C52">
         <v>590</v>
@@ -6876,10 +6854,10 @@
         <v>12</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>194</v>
+        <v>179</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>195</v>
+        <v>180</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="119">
@@ -6887,7 +6865,7 @@
         <v>8</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="C53">
         <v>442</v>
@@ -6896,10 +6874,10 @@
         <v>12</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="34">
@@ -6907,7 +6885,7 @@
         <v>8</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>199</v>
+        <v>184</v>
       </c>
       <c r="C54">
         <v>31</v>
@@ -6916,10 +6894,10 @@
         <v>4</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>200</v>
+        <v>185</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>201</v>
+        <v>186</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="68">
@@ -6927,7 +6905,7 @@
         <v>8</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>202</v>
+        <v>187</v>
       </c>
       <c r="C55">
         <v>274</v>
@@ -6936,10 +6914,10 @@
         <v>10</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>204</v>
+        <v>189</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="102">
@@ -6947,7 +6925,7 @@
         <v>8</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>205</v>
+        <v>190</v>
       </c>
       <c r="C56">
         <v>351</v>
@@ -6956,10 +6934,10 @@
         <v>12</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>207</v>
+        <v>192</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="153">
@@ -6967,7 +6945,7 @@
         <v>8</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>208</v>
+        <v>193</v>
       </c>
       <c r="C57">
         <v>522</v>
@@ -6976,10 +6954,10 @@
         <v>16</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="119">
@@ -6987,7 +6965,7 @@
         <v>8</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>211</v>
+        <v>196</v>
       </c>
       <c r="C58">
         <v>323</v>
@@ -6996,10 +6974,10 @@
         <v>6</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>212</v>
+        <v>197</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>213</v>
+        <v>198</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="68">
@@ -7007,7 +6985,7 @@
         <v>8</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>214</v>
+        <v>199</v>
       </c>
       <c r="C59">
         <v>417</v>
@@ -7016,10 +6994,10 @@
         <v>4</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>215</v>
+        <v>200</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>216</v>
+        <v>201</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="51">
@@ -7027,7 +7005,7 @@
         <v>8</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>217</v>
+        <v>202</v>
       </c>
       <c r="C60">
         <v>204</v>
@@ -7036,10 +7014,10 @@
         <v>4</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>218</v>
+        <v>203</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>219</v>
+        <v>204</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="102">
@@ -7047,7 +7025,7 @@
         <v>8</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>220</v>
+        <v>205</v>
       </c>
       <c r="C61">
         <v>574</v>
@@ -7056,10 +7034,10 @@
         <v>12</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>221</v>
+        <v>206</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>222</v>
+        <v>207</v>
       </c>
     </row>
     <row r="62" spans="1:6" ht="119">
@@ -7067,7 +7045,7 @@
         <v>8</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="C62">
         <v>359</v>
@@ -7076,10 +7054,10 @@
         <v>12</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>224</v>
+        <v>209</v>
       </c>
       <c r="F62" s="3" t="s">
-        <v>225</v>
+        <v>210</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="51">
@@ -7087,7 +7065,7 @@
         <v>8</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>226</v>
+        <v>211</v>
       </c>
       <c r="C63">
         <v>62</v>
@@ -7096,10 +7074,10 @@
         <v>8</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>227</v>
+        <v>212</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>228</v>
+        <v>213</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="119">
@@ -7107,7 +7085,7 @@
         <v>8</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>229</v>
+        <v>214</v>
       </c>
       <c r="C64">
         <v>324</v>
@@ -7116,10 +7094,10 @@
         <v>6</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>230</v>
+        <v>215</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>231</v>
+        <v>216</v>
       </c>
     </row>
     <row r="65" spans="1:6" ht="51">
@@ -7127,7 +7105,7 @@
         <v>8</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>232</v>
+        <v>217</v>
       </c>
       <c r="C65">
         <v>415</v>
@@ -7136,10 +7114,10 @@
         <v>1</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>233</v>
+        <v>218</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>234</v>
+        <v>219</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="170">
@@ -7147,7 +7125,7 @@
         <v>8</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>235</v>
+        <v>220</v>
       </c>
       <c r="C66">
         <v>429</v>
@@ -7156,10 +7134,10 @@
         <v>8</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>236</v>
+        <v>221</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>237</v>
+        <v>222</v>
       </c>
     </row>
     <row r="67" spans="1:6" ht="51">
@@ -7167,7 +7145,7 @@
         <v>8</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>238</v>
+        <v>223</v>
       </c>
       <c r="C67">
         <v>112</v>
@@ -7176,10 +7154,10 @@
         <v>10</v>
       </c>
       <c r="E67" s="3" t="s">
-        <v>239</v>
+        <v>224</v>
       </c>
       <c r="F67" s="3" t="s">
-        <v>240</v>
+        <v>225</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="153">
@@ -7187,7 +7165,7 @@
         <v>8</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>241</v>
+        <v>226</v>
       </c>
       <c r="C68">
         <v>485</v>
@@ -7196,10 +7174,10 @@
         <v>10</v>
       </c>
       <c r="E68" s="3" t="s">
-        <v>242</v>
+        <v>227</v>
       </c>
       <c r="F68" s="3" t="s">
-        <v>243</v>
+        <v>228</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="119">
@@ -7207,7 +7185,7 @@
         <v>8</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>244</v>
+        <v>229</v>
       </c>
       <c r="C69">
         <v>151</v>
@@ -7216,10 +7194,10 @@
         <v>6</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>245</v>
+        <v>230</v>
       </c>
       <c r="F69" s="3" t="s">
-        <v>246</v>
+        <v>231</v>
       </c>
     </row>
     <row r="70" spans="1:6" ht="102">
@@ -7227,7 +7205,7 @@
         <v>8</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>247</v>
+        <v>232</v>
       </c>
       <c r="C70">
         <v>273</v>
@@ -7236,10 +7214,10 @@
         <v>16</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>248</v>
+        <v>233</v>
       </c>
       <c r="F70" s="3" t="s">
-        <v>249</v>
+        <v>234</v>
       </c>
     </row>
     <row r="71" spans="1:6" ht="119">
@@ -7247,7 +7225,7 @@
         <v>8</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>250</v>
+        <v>235</v>
       </c>
       <c r="C71">
         <v>427</v>
@@ -7256,10 +7234,10 @@
         <v>10</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="F71" s="3" t="s">
-        <v>252</v>
+        <v>237</v>
       </c>
     </row>
     <row r="72" spans="1:6" ht="102">
@@ -7267,7 +7245,7 @@
         <v>8</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>253</v>
+        <v>238</v>
       </c>
       <c r="C72">
         <v>358</v>
@@ -7276,10 +7254,10 @@
         <v>12</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="F72" s="3" t="s">
-        <v>255</v>
+        <v>240</v>
       </c>
     </row>
     <row r="73" spans="1:6" ht="102">
@@ -7287,7 +7265,7 @@
         <v>8</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>256</v>
+        <v>241</v>
       </c>
       <c r="C73">
         <v>461</v>
@@ -7296,10 +7274,10 @@
         <v>10</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>257</v>
+        <v>242</v>
       </c>
       <c r="F73" s="3" t="s">
-        <v>258</v>
+        <v>243</v>
       </c>
     </row>
     <row r="74" spans="1:6" ht="68">
@@ -7307,7 +7285,7 @@
         <v>8</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>259</v>
+        <v>244</v>
       </c>
       <c r="C74">
         <v>39</v>
@@ -7316,10 +7294,10 @@
         <v>6</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>260</v>
+        <v>245</v>
       </c>
       <c r="F74" s="3" t="s">
-        <v>261</v>
+        <v>246</v>
       </c>
     </row>
     <row r="75" spans="1:6" ht="85">
@@ -7327,7 +7305,7 @@
         <v>8</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>262</v>
+        <v>247</v>
       </c>
       <c r="C75">
         <v>338</v>
@@ -7336,10 +7314,10 @@
         <v>4</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>263</v>
+        <v>248</v>
       </c>
       <c r="F75" s="3" t="s">
-        <v>264</v>
+        <v>249</v>
       </c>
     </row>
     <row r="76" spans="1:6" ht="102">
@@ -7347,7 +7325,7 @@
         <v>8</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>265</v>
+        <v>250</v>
       </c>
       <c r="C76">
         <v>199</v>
@@ -7356,10 +7334,10 @@
         <v>4</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>266</v>
+        <v>251</v>
       </c>
       <c r="F76" s="3" t="s">
-        <v>267</v>
+        <v>252</v>
       </c>
     </row>
     <row r="77" spans="1:6" ht="119">
@@ -7367,7 +7345,7 @@
         <v>8</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>268</v>
+        <v>253</v>
       </c>
       <c r="C77">
         <v>473</v>
@@ -7376,10 +7354,10 @@
         <v>10</v>
       </c>
       <c r="E77" s="3" t="s">
-        <v>269</v>
+        <v>254</v>
       </c>
       <c r="F77" s="3" t="s">
-        <v>270</v>
+        <v>255</v>
       </c>
     </row>
     <row r="78" spans="1:6" ht="102">
@@ -7387,7 +7365,7 @@
         <v>8</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="C78">
         <v>288</v>
@@ -7396,10 +7374,10 @@
         <v>6</v>
       </c>
       <c r="E78" s="3" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="F78" s="3" t="s">
-        <v>273</v>
+        <v>258</v>
       </c>
     </row>
     <row r="79" spans="1:6" ht="153">
@@ -7407,7 +7385,7 @@
         <v>8</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>274</v>
+        <v>259</v>
       </c>
       <c r="C79">
         <v>517</v>
@@ -7416,10 +7394,10 @@
         <v>10</v>
       </c>
       <c r="E79" s="3" t="s">
-        <v>275</v>
+        <v>260</v>
       </c>
       <c r="F79" s="3" t="s">
-        <v>276</v>
+        <v>261</v>
       </c>
     </row>
     <row r="80" spans="1:6" ht="102">
@@ -7427,7 +7405,7 @@
         <v>8</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>277</v>
+        <v>262</v>
       </c>
       <c r="C80">
         <v>163</v>
@@ -7436,10 +7414,10 @@
         <v>12</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>278</v>
+        <v>263</v>
       </c>
       <c r="F80" s="3" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
     </row>
     <row r="81" spans="1:6" ht="51">
@@ -7447,7 +7425,7 @@
         <v>8</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>280</v>
+        <v>265</v>
       </c>
       <c r="C81">
         <v>91</v>
@@ -7456,10 +7434,10 @@
         <v>4</v>
       </c>
       <c r="E81" s="3" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="F81" s="3" t="s">
-        <v>282</v>
+        <v>267</v>
       </c>
     </row>
     <row r="82" spans="1:6" ht="51">
@@ -7467,7 +7445,7 @@
         <v>8</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>283</v>
+        <v>268</v>
       </c>
       <c r="C82">
         <v>406</v>
@@ -7476,10 +7454,10 @@
         <v>1</v>
       </c>
       <c r="E82" s="3" t="s">
-        <v>284</v>
+        <v>269</v>
       </c>
       <c r="F82" s="3" t="s">
-        <v>285</v>
+        <v>270</v>
       </c>
     </row>
     <row r="83" spans="1:6" ht="51">
@@ -7487,7 +7465,7 @@
         <v>8</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>286</v>
+        <v>271</v>
       </c>
       <c r="C83">
         <v>319</v>
@@ -7496,10 +7474,10 @@
         <v>8</v>
       </c>
       <c r="E83" s="3" t="s">
-        <v>287</v>
+        <v>272</v>
       </c>
       <c r="F83" s="3" t="s">
-        <v>288</v>
+        <v>273</v>
       </c>
     </row>
     <row r="84" spans="1:6" ht="51">
@@ -7507,7 +7485,7 @@
         <v>8</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>289</v>
+        <v>274</v>
       </c>
       <c r="C84">
         <v>198</v>
@@ -7516,10 +7494,10 @@
         <v>4</v>
       </c>
       <c r="E84" s="3" t="s">
-        <v>290</v>
+        <v>275</v>
       </c>
       <c r="F84" s="3" t="s">
-        <v>291</v>
+        <v>276</v>
       </c>
     </row>
     <row r="85" spans="1:6" ht="68">
@@ -7527,7 +7505,7 @@
         <v>8</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>292</v>
+        <v>277</v>
       </c>
       <c r="C85">
         <v>236</v>
@@ -7536,10 +7514,10 @@
         <v>6</v>
       </c>
       <c r="E85" s="3" t="s">
-        <v>293</v>
+        <v>278</v>
       </c>
       <c r="F85" s="3" t="s">
-        <v>294</v>
+        <v>279</v>
       </c>
     </row>
     <row r="86" spans="1:6" ht="51">
@@ -7547,7 +7525,7 @@
         <v>8</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>295</v>
+        <v>280</v>
       </c>
       <c r="C86">
         <v>327</v>
@@ -7556,10 +7534,10 @@
         <v>4</v>
       </c>
       <c r="E86" s="3" t="s">
-        <v>296</v>
+        <v>281</v>
       </c>
       <c r="F86" s="3" t="s">
-        <v>297</v>
+        <v>282</v>
       </c>
     </row>
     <row r="87" spans="1:6" ht="68">
@@ -7567,7 +7545,7 @@
         <v>8</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>298</v>
+        <v>283</v>
       </c>
       <c r="C87">
         <v>309</v>
@@ -7576,10 +7554,10 @@
         <v>4</v>
       </c>
       <c r="E87" s="3" t="s">
-        <v>299</v>
+        <v>284</v>
       </c>
       <c r="F87" s="3" t="s">
-        <v>300</v>
+        <v>285</v>
       </c>
     </row>
     <row r="88" spans="1:6" ht="68">
@@ -7587,7 +7565,7 @@
         <v>8</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>301</v>
+        <v>286</v>
       </c>
       <c r="C88">
         <v>185</v>
@@ -7596,10 +7574,10 @@
         <v>1</v>
       </c>
       <c r="E88" s="3" t="s">
-        <v>302</v>
+        <v>287</v>
       </c>
       <c r="F88" s="3" t="s">
-        <v>303</v>
+        <v>288</v>
       </c>
     </row>
     <row r="89" spans="1:6" ht="68">
@@ -7607,7 +7585,7 @@
         <v>8</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>304</v>
+        <v>289</v>
       </c>
       <c r="C89">
         <v>271</v>
@@ -7616,10 +7594,10 @@
         <v>8</v>
       </c>
       <c r="E89" s="3" t="s">
-        <v>305</v>
+        <v>290</v>
       </c>
       <c r="F89" s="3" t="s">
-        <v>306</v>
+        <v>291</v>
       </c>
     </row>
     <row r="90" spans="1:6" ht="102">
@@ -7627,7 +7605,7 @@
         <v>8</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>307</v>
+        <v>292</v>
       </c>
       <c r="C90">
         <v>395</v>
@@ -7636,10 +7614,10 @@
         <v>18</v>
       </c>
       <c r="E90" s="3" t="s">
-        <v>308</v>
+        <v>293</v>
       </c>
       <c r="F90" s="3" t="s">
-        <v>309</v>
+        <v>294</v>
       </c>
     </row>
     <row r="91" spans="1:6" ht="51">
@@ -7647,7 +7625,7 @@
         <v>8</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>310</v>
+        <v>295</v>
       </c>
       <c r="C91">
         <v>150</v>
@@ -7656,10 +7634,10 @@
         <v>1</v>
       </c>
       <c r="E91" s="3" t="s">
-        <v>311</v>
+        <v>296</v>
       </c>
       <c r="F91" s="3" t="s">
-        <v>312</v>
+        <v>297</v>
       </c>
     </row>
     <row r="92" spans="1:6" ht="68">
@@ -7667,7 +7645,7 @@
         <v>8</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>313</v>
+        <v>298</v>
       </c>
       <c r="C92">
         <v>55</v>
@@ -7676,10 +7654,10 @@
         <v>40</v>
       </c>
       <c r="E92" s="3" t="s">
-        <v>314</v>
+        <v>299</v>
       </c>
       <c r="F92" s="3" t="s">
-        <v>315</v>
+        <v>300</v>
       </c>
     </row>
     <row r="93" spans="1:6" ht="68">
@@ -7687,7 +7665,7 @@
         <v>8</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>316</v>
+        <v>301</v>
       </c>
       <c r="C93">
         <v>246</v>
@@ -7696,10 +7674,10 @@
         <v>1</v>
       </c>
       <c r="E93" s="3" t="s">
-        <v>317</v>
+        <v>302</v>
       </c>
       <c r="F93" s="3" t="s">
-        <v>318</v>
+        <v>303</v>
       </c>
     </row>
     <row r="94" spans="1:6" ht="136">
@@ -7707,7 +7685,7 @@
         <v>8</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>319</v>
+        <v>304</v>
       </c>
       <c r="C94">
         <v>511</v>
@@ -7716,10 +7694,10 @@
         <v>8</v>
       </c>
       <c r="E94" s="3" t="s">
-        <v>320</v>
+        <v>305</v>
       </c>
       <c r="F94" s="3" t="s">
-        <v>321</v>
+        <v>306</v>
       </c>
     </row>
     <row r="95" spans="1:6" ht="51">
@@ -7727,7 +7705,7 @@
         <v>8</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>322</v>
+        <v>307</v>
       </c>
       <c r="C95">
         <v>235</v>
@@ -7736,10 +7714,10 @@
         <v>12</v>
       </c>
       <c r="E95" s="3" t="s">
-        <v>323</v>
+        <v>308</v>
       </c>
       <c r="F95" s="3" t="s">
-        <v>324</v>
+        <v>309</v>
       </c>
     </row>
     <row r="96" spans="1:6" ht="68">
@@ -7747,7 +7725,7 @@
         <v>8</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>325</v>
+        <v>310</v>
       </c>
       <c r="C96">
         <v>259</v>
@@ -7756,18 +7734,18 @@
         <v>10</v>
       </c>
       <c r="E96" s="3" t="s">
-        <v>326</v>
+        <v>311</v>
       </c>
       <c r="F96" s="3" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="97" spans="1:6" ht="51" hidden="1">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" ht="51">
       <c r="A97" t="s">
         <v>11</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>37</v>
+        <v>313</v>
       </c>
       <c r="C97">
         <v>361</v>
@@ -7776,18 +7754,18 @@
         <v>6</v>
       </c>
       <c r="E97" s="3" t="s">
-        <v>38</v>
+        <v>314</v>
       </c>
       <c r="F97" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="98" spans="1:6" ht="51" hidden="1">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" ht="51">
       <c r="A98" t="s">
         <v>11</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>40</v>
+        <v>316</v>
       </c>
       <c r="C98">
         <v>582</v>
@@ -7796,18 +7774,18 @@
         <v>10</v>
       </c>
       <c r="E98" s="3" t="s">
-        <v>41</v>
+        <v>317</v>
       </c>
       <c r="F98" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="99" spans="1:6" ht="34" hidden="1">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" ht="34">
       <c r="A99" t="s">
         <v>11</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>43</v>
+        <v>319</v>
       </c>
       <c r="C99">
         <v>275</v>
@@ -7816,18 +7794,18 @@
         <v>15</v>
       </c>
       <c r="E99" s="3" t="s">
-        <v>44</v>
+        <v>320</v>
       </c>
       <c r="F99" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="100" spans="1:6" ht="68" hidden="1">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" ht="68">
       <c r="A100" t="s">
         <v>11</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>46</v>
+        <v>322</v>
       </c>
       <c r="C100">
         <v>571</v>
@@ -7836,18 +7814,18 @@
         <v>6</v>
       </c>
       <c r="E100" s="3" t="s">
-        <v>47</v>
+        <v>323</v>
       </c>
       <c r="F100" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="101" spans="1:6" ht="34" hidden="1">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" ht="34">
       <c r="A101" t="s">
         <v>11</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>49</v>
+        <v>325</v>
       </c>
       <c r="C101">
         <v>195</v>
@@ -7856,13 +7834,13 @@
         <v>6</v>
       </c>
       <c r="E101" s="3" t="s">
-        <v>50</v>
+        <v>326</v>
       </c>
       <c r="F101" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="102" spans="1:6" ht="34" hidden="1">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" ht="34">
       <c r="A102" t="s">
         <v>11</v>
       </c>
@@ -7882,7 +7860,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="103" spans="1:6" ht="51" hidden="1">
+    <row r="103" spans="1:6" ht="51">
       <c r="A103" t="s">
         <v>11</v>
       </c>
@@ -7902,7 +7880,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="104" spans="1:6" ht="102" hidden="1">
+    <row r="104" spans="1:6" ht="102">
       <c r="A104" t="s">
         <v>11</v>
       </c>
@@ -7922,7 +7900,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="105" spans="1:6" ht="34" hidden="1">
+    <row r="105" spans="1:6" ht="34">
       <c r="A105" t="s">
         <v>11</v>
       </c>
@@ -7942,7 +7920,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="106" spans="1:6" ht="68" hidden="1">
+    <row r="106" spans="1:6" ht="68">
       <c r="A106" t="s">
         <v>11</v>
       </c>
@@ -7962,7 +7940,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="107" spans="1:6" ht="34" hidden="1">
+    <row r="107" spans="1:6" ht="34">
       <c r="A107" t="s">
         <v>11</v>
       </c>
@@ -7982,7 +7960,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="108" spans="1:6" ht="51" hidden="1">
+    <row r="108" spans="1:6" ht="51">
       <c r="A108" t="s">
         <v>11</v>
       </c>
@@ -8002,7 +7980,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="109" spans="1:6" ht="51" hidden="1">
+    <row r="109" spans="1:6" ht="51">
       <c r="A109" t="s">
         <v>11</v>
       </c>
@@ -8022,7 +8000,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="110" spans="1:6" ht="136" hidden="1">
+    <row r="110" spans="1:6" ht="136">
       <c r="A110" t="s">
         <v>11</v>
       </c>
@@ -8042,7 +8020,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="111" spans="1:6" ht="68" hidden="1">
+    <row r="111" spans="1:6" ht="68">
       <c r="A111" t="s">
         <v>11</v>
       </c>
@@ -8062,7 +8040,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="112" spans="1:6" ht="51" hidden="1">
+    <row r="112" spans="1:6" ht="51">
       <c r="A112" t="s">
         <v>11</v>
       </c>
@@ -8082,7 +8060,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="113" spans="1:6" ht="34" hidden="1">
+    <row r="113" spans="1:6" ht="34">
       <c r="A113" t="s">
         <v>11</v>
       </c>
@@ -8102,7 +8080,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="114" spans="1:6" ht="51" hidden="1">
+    <row r="114" spans="1:6" ht="51">
       <c r="A114" t="s">
         <v>11</v>
       </c>
@@ -8122,7 +8100,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="115" spans="1:6" ht="34" hidden="1">
+    <row r="115" spans="1:6" ht="34">
       <c r="A115" t="s">
         <v>11</v>
       </c>
@@ -8142,7 +8120,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="116" spans="1:6" ht="68" hidden="1">
+    <row r="116" spans="1:6" ht="68">
       <c r="A116" t="s">
         <v>11</v>
       </c>
@@ -8162,7 +8140,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="117" spans="1:6" ht="68" hidden="1">
+    <row r="117" spans="1:6" ht="68">
       <c r="A117" t="s">
         <v>11</v>
       </c>
@@ -8182,7 +8160,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="118" spans="1:6" ht="68" hidden="1">
+    <row r="118" spans="1:6" ht="68">
       <c r="A118" t="s">
         <v>11</v>
       </c>
@@ -8202,7 +8180,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="119" spans="1:6" ht="51" hidden="1">
+    <row r="119" spans="1:6" ht="51">
       <c r="A119" t="s">
         <v>11</v>
       </c>
@@ -8222,7 +8200,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="120" spans="1:6" ht="85" hidden="1">
+    <row r="120" spans="1:6" ht="85">
       <c r="A120" t="s">
         <v>11</v>
       </c>
@@ -8242,7 +8220,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="121" spans="1:6" ht="85" hidden="1">
+    <row r="121" spans="1:6" ht="85">
       <c r="A121" t="s">
         <v>11</v>
       </c>
@@ -8262,7 +8240,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="122" spans="1:6" ht="85" hidden="1">
+    <row r="122" spans="1:6" ht="85">
       <c r="A122" t="s">
         <v>11</v>
       </c>
@@ -8282,7 +8260,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="123" spans="1:6" ht="153" hidden="1">
+    <row r="123" spans="1:6" ht="153">
       <c r="A123" t="s">
         <v>11</v>
       </c>
@@ -8302,7 +8280,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="124" spans="1:6" ht="102" hidden="1">
+    <row r="124" spans="1:6" ht="102">
       <c r="A124" t="s">
         <v>11</v>
       </c>
@@ -8322,7 +8300,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="125" spans="1:6" ht="68" hidden="1">
+    <row r="125" spans="1:6" ht="68">
       <c r="A125" t="s">
         <v>11</v>
       </c>
@@ -8342,7 +8320,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="126" spans="1:6" ht="85" hidden="1">
+    <row r="126" spans="1:6" ht="85">
       <c r="A126" t="s">
         <v>11</v>
       </c>
@@ -8362,7 +8340,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="127" spans="1:6" ht="85" hidden="1">
+    <row r="127" spans="1:6" ht="85">
       <c r="A127" t="s">
         <v>11</v>
       </c>
@@ -8382,7 +8360,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="128" spans="1:6" ht="170" hidden="1">
+    <row r="128" spans="1:6" ht="170">
       <c r="A128" t="s">
         <v>11</v>
       </c>
@@ -8402,7 +8380,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="129" spans="1:6" ht="68" hidden="1">
+    <row r="129" spans="1:6" ht="68">
       <c r="A129" t="s">
         <v>11</v>
       </c>
@@ -8422,7 +8400,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="130" spans="1:6" ht="51" hidden="1">
+    <row r="130" spans="1:6" ht="51">
       <c r="A130" t="s">
         <v>11</v>
       </c>
@@ -8442,7 +8420,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="131" spans="1:6" ht="51" hidden="1">
+    <row r="131" spans="1:6" ht="51">
       <c r="A131" t="s">
         <v>11</v>
       </c>
@@ -8462,7 +8440,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="132" spans="1:6" ht="136" hidden="1">
+    <row r="132" spans="1:6" ht="136">
       <c r="A132" t="s">
         <v>11</v>
       </c>
@@ -8482,7 +8460,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="133" spans="1:6" ht="51" hidden="1">
+    <row r="133" spans="1:6" ht="51">
       <c r="A133" t="s">
         <v>11</v>
       </c>
@@ -8502,7 +8480,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="134" spans="1:6" ht="102" hidden="1">
+    <row r="134" spans="1:6" ht="102">
       <c r="A134" t="s">
         <v>11</v>
       </c>
@@ -8522,7 +8500,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="135" spans="1:6" ht="68" hidden="1">
+    <row r="135" spans="1:6" ht="68">
       <c r="A135" t="s">
         <v>11</v>
       </c>
@@ -8542,7 +8520,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="136" spans="1:6" ht="85" hidden="1">
+    <row r="136" spans="1:6" ht="85">
       <c r="A136" t="s">
         <v>11</v>
       </c>
@@ -8562,7 +8540,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="137" spans="1:6" ht="85" hidden="1">
+    <row r="137" spans="1:6" ht="85">
       <c r="A137" t="s">
         <v>11</v>
       </c>
@@ -8582,7 +8560,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="138" spans="1:6" ht="51" hidden="1">
+    <row r="138" spans="1:6" ht="51">
       <c r="A138" t="s">
         <v>11</v>
       </c>
@@ -8602,7 +8580,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="139" spans="1:6" ht="68" hidden="1">
+    <row r="139" spans="1:6" ht="68">
       <c r="A139" t="s">
         <v>11</v>
       </c>
@@ -8622,7 +8600,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="140" spans="1:6" ht="85" hidden="1">
+    <row r="140" spans="1:6" ht="85">
       <c r="A140" t="s">
         <v>11</v>
       </c>
@@ -8642,7 +8620,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="141" spans="1:6" ht="68" hidden="1">
+    <row r="141" spans="1:6" ht="68">
       <c r="A141" t="s">
         <v>11</v>
       </c>
@@ -8662,7 +8640,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="142" spans="1:6" ht="119" hidden="1">
+    <row r="142" spans="1:6" ht="119">
       <c r="A142" t="s">
         <v>11</v>
       </c>
@@ -8682,7 +8660,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="143" spans="1:6" ht="68" hidden="1">
+    <row r="143" spans="1:6" ht="68">
       <c r="A143" t="s">
         <v>11</v>
       </c>
@@ -8702,7 +8680,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="144" spans="1:6" ht="68" hidden="1">
+    <row r="144" spans="1:6" ht="68">
       <c r="A144" t="s">
         <v>11</v>
       </c>
@@ -8722,7 +8700,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="145" spans="1:6" ht="85" hidden="1">
+    <row r="145" spans="1:6" ht="85">
       <c r="A145" t="s">
         <v>11</v>
       </c>
@@ -8742,7 +8720,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="146" spans="1:6" ht="68" hidden="1">
+    <row r="146" spans="1:6" ht="68">
       <c r="A146" t="s">
         <v>11</v>
       </c>
@@ -8762,7 +8740,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="147" spans="1:6" ht="119" hidden="1">
+    <row r="147" spans="1:6" ht="119">
       <c r="A147" t="s">
         <v>11</v>
       </c>
@@ -8782,7 +8760,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="148" spans="1:6" ht="68" hidden="1">
+    <row r="148" spans="1:6" ht="68">
       <c r="A148" t="s">
         <v>11</v>
       </c>
@@ -8802,7 +8780,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="149" spans="1:6" ht="34" hidden="1">
+    <row r="149" spans="1:6" ht="34">
       <c r="A149" t="s">
         <v>11</v>
       </c>
@@ -8822,7 +8800,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="150" spans="1:6" ht="102" hidden="1">
+    <row r="150" spans="1:6" ht="102">
       <c r="A150" t="s">
         <v>11</v>
       </c>
@@ -8842,7 +8820,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="151" spans="1:6" ht="119" hidden="1">
+    <row r="151" spans="1:6" ht="119">
       <c r="A151" t="s">
         <v>11</v>
       </c>
@@ -8862,7 +8840,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="152" spans="1:6" ht="68" hidden="1">
+    <row r="152" spans="1:6" ht="68">
       <c r="A152" t="s">
         <v>11</v>
       </c>
@@ -8882,7 +8860,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="153" spans="1:6" ht="51" hidden="1">
+    <row r="153" spans="1:6" ht="51">
       <c r="A153" t="s">
         <v>11</v>
       </c>
@@ -8902,7 +8880,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="154" spans="1:6" ht="68" hidden="1">
+    <row r="154" spans="1:6" ht="68">
       <c r="A154" t="s">
         <v>11</v>
       </c>
@@ -8922,7 +8900,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="155" spans="1:6" ht="102" hidden="1">
+    <row r="155" spans="1:6" ht="102">
       <c r="A155" t="s">
         <v>11</v>
       </c>
@@ -8942,7 +8920,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="156" spans="1:6" ht="68" hidden="1">
+    <row r="156" spans="1:6" ht="68">
       <c r="A156" t="s">
         <v>11</v>
       </c>
@@ -8962,7 +8940,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="157" spans="1:6" ht="102" hidden="1">
+    <row r="157" spans="1:6" ht="102">
       <c r="A157" t="s">
         <v>11</v>
       </c>
@@ -8982,7 +8960,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="158" spans="1:6" ht="51" hidden="1">
+    <row r="158" spans="1:6" ht="51">
       <c r="A158" t="s">
         <v>11</v>
       </c>
@@ -9002,7 +8980,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="159" spans="1:6" ht="51" hidden="1">
+    <row r="159" spans="1:6" ht="51">
       <c r="A159" t="s">
         <v>11</v>
       </c>
@@ -9022,7 +9000,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="160" spans="1:6" ht="51" hidden="1">
+    <row r="160" spans="1:6" ht="51">
       <c r="A160" t="s">
         <v>11</v>
       </c>
@@ -9042,7 +9020,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="161" spans="1:6" ht="102" hidden="1">
+    <row r="161" spans="1:6" ht="102">
       <c r="A161" t="s">
         <v>11</v>
       </c>
@@ -9062,7 +9040,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="162" spans="1:6" ht="68" hidden="1">
+    <row r="162" spans="1:6" ht="68">
       <c r="A162" t="s">
         <v>11</v>
       </c>
@@ -9082,7 +9060,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="163" spans="1:6" ht="102" hidden="1">
+    <row r="163" spans="1:6" ht="102">
       <c r="A163" t="s">
         <v>11</v>
       </c>
@@ -9102,7 +9080,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="164" spans="1:6" ht="85" hidden="1">
+    <row r="164" spans="1:6" ht="85">
       <c r="A164" t="s">
         <v>11</v>
       </c>
@@ -9122,7 +9100,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="165" spans="1:6" ht="85" hidden="1">
+    <row r="165" spans="1:6" ht="85">
       <c r="A165" t="s">
         <v>11</v>
       </c>
@@ -9142,7 +9120,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="166" spans="1:6" ht="34" hidden="1">
+    <row r="166" spans="1:6" ht="34">
       <c r="A166" t="s">
         <v>11</v>
       </c>
@@ -9162,7 +9140,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="167" spans="1:6" ht="68" hidden="1">
+    <row r="167" spans="1:6" ht="68">
       <c r="A167" t="s">
         <v>11</v>
       </c>
@@ -9182,7 +9160,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="168" spans="1:6" ht="68" hidden="1">
+    <row r="168" spans="1:6" ht="68">
       <c r="A168" t="s">
         <v>11</v>
       </c>
@@ -9202,7 +9180,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="169" spans="1:6" ht="102" hidden="1">
+    <row r="169" spans="1:6" ht="102">
       <c r="A169" t="s">
         <v>11</v>
       </c>
@@ -9222,7 +9200,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="170" spans="1:6" ht="68" hidden="1">
+    <row r="170" spans="1:6" ht="68">
       <c r="A170" t="s">
         <v>11</v>
       </c>
@@ -9242,7 +9220,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="171" spans="1:6" ht="68" hidden="1">
+    <row r="171" spans="1:6" ht="68">
       <c r="A171" t="s">
         <v>11</v>
       </c>
@@ -9262,7 +9240,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="172" spans="1:6" ht="68" hidden="1">
+    <row r="172" spans="1:6" ht="68">
       <c r="A172" t="s">
         <v>11</v>
       </c>
@@ -9282,7 +9260,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="173" spans="1:6" ht="119" hidden="1">
+    <row r="173" spans="1:6" ht="119">
       <c r="A173" t="s">
         <v>11</v>
       </c>
@@ -9302,7 +9280,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="174" spans="1:6" ht="51" hidden="1">
+    <row r="174" spans="1:6" ht="51">
       <c r="A174" t="s">
         <v>11</v>
       </c>
@@ -9322,7 +9300,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="175" spans="1:6" ht="51" hidden="1">
+    <row r="175" spans="1:6" ht="51">
       <c r="A175" t="s">
         <v>11</v>
       </c>
@@ -9342,7 +9320,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="176" spans="1:6" ht="119" hidden="1">
+    <row r="176" spans="1:6" ht="119">
       <c r="A176" t="s">
         <v>11</v>
       </c>
@@ -9362,7 +9340,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="177" spans="1:6" ht="34" hidden="1">
+    <row r="177" spans="1:6" ht="34">
       <c r="A177" t="s">
         <v>11</v>
       </c>
@@ -9382,7 +9360,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="178" spans="1:6" ht="34" hidden="1">
+    <row r="178" spans="1:6" ht="34">
       <c r="A178" t="s">
         <v>11</v>
       </c>
@@ -9402,7 +9380,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="179" spans="1:6" ht="136" hidden="1">
+    <row r="179" spans="1:6" ht="136">
       <c r="A179" t="s">
         <v>11</v>
       </c>
@@ -9422,7 +9400,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="180" spans="1:6" ht="68" hidden="1">
+    <row r="180" spans="1:6" ht="68">
       <c r="A180" t="s">
         <v>11</v>
       </c>
@@ -9442,7 +9420,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="181" spans="1:6" ht="170" hidden="1">
+    <row r="181" spans="1:6" ht="170">
       <c r="A181" t="s">
         <v>11</v>
       </c>
@@ -9462,7 +9440,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="182" spans="1:6" ht="68" hidden="1">
+    <row r="182" spans="1:6" ht="68">
       <c r="A182" t="s">
         <v>11</v>
       </c>
@@ -9482,7 +9460,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="183" spans="1:6" ht="85" hidden="1">
+    <row r="183" spans="1:6" ht="85">
       <c r="A183" t="s">
         <v>11</v>
       </c>
@@ -9502,7 +9480,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="184" spans="1:6" ht="85" hidden="1">
+    <row r="184" spans="1:6" ht="85">
       <c r="A184" t="s">
         <v>11</v>
       </c>
@@ -9522,7 +9500,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="185" spans="1:6" ht="85" hidden="1">
+    <row r="185" spans="1:6" ht="85">
       <c r="A185" t="s">
         <v>11</v>
       </c>
@@ -9542,7 +9520,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="186" spans="1:6" ht="51" hidden="1">
+    <row r="186" spans="1:6" ht="51">
       <c r="A186" t="s">
         <v>11</v>
       </c>
@@ -9562,7 +9540,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="187" spans="1:6" ht="68" hidden="1">
+    <row r="187" spans="1:6" ht="68">
       <c r="A187" t="s">
         <v>11</v>
       </c>
@@ -9582,7 +9560,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="188" spans="1:6" ht="34" hidden="1">
+    <row r="188" spans="1:6" ht="34">
       <c r="A188" t="s">
         <v>11</v>
       </c>
@@ -9602,7 +9580,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="189" spans="1:6" ht="85" hidden="1">
+    <row r="189" spans="1:6" ht="85">
       <c r="A189" t="s">
         <v>11</v>
       </c>
@@ -9622,7 +9600,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="190" spans="1:6" ht="68" hidden="1">
+    <row r="190" spans="1:6" ht="68">
       <c r="A190" t="s">
         <v>11</v>
       </c>
@@ -9642,7 +9620,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="191" spans="1:6" ht="68" hidden="1">
+    <row r="191" spans="1:6" ht="68">
       <c r="A191" t="s">
         <v>11</v>
       </c>
@@ -9662,7 +9640,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="192" spans="1:6" ht="102" hidden="1">
+    <row r="192" spans="1:6" ht="102">
       <c r="A192" t="s">
         <v>11</v>
       </c>
@@ -9682,7 +9660,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="193" spans="1:6" ht="85" hidden="1">
+    <row r="193" spans="1:6" ht="85">
       <c r="A193" t="s">
         <v>11</v>
       </c>
@@ -13583,21 +13561,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F387" xr:uid="{00000000-0001-0000-0100-000000000000}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="Breakfast"/>
-        <filter val="Lunch"/>
-        <filter val="Snack"/>
-      </filters>
-    </filterColumn>
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F387">
-      <sortCondition ref="A1:A387"/>
-    </sortState>
-  </autoFilter>
-  <hyperlinks>
-    <hyperlink ref="F38" r:id="rId1" xr:uid="{31309CCA-E10F-7A42-91B6-5F69157E9D55}"/>
-  </hyperlinks>
+  <autoFilter ref="A1:F1" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>